<commit_message>
update SRS & CRS & RTM
</commit_message>
<xml_diff>
--- a/RTM/Traceability_Matrix learning hub ver 2.xlsx
+++ b/RTM/Traceability_Matrix learning hub ver 2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti\QA\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alaa Osama\Documents\GitHub\learning-hub\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E78FCD1-3D81-4207-9547-4186FF6E2D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028132BE-D214-47CB-A306-A8C3C26551D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" state="hidden" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Requirement_Traceability_Matrix!$A$5:$L$8</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Requirement_Traceability_Matrix!$A$1:$L$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Requirement_Traceability_Matrix!$A$1:$L$30</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Requirement_Traceability_Matrix!$1:$5</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="277">
   <si>
     <t>For detail regarding the practice of Requirements Management, please refer to the Requirements Management Practices Guide</t>
   </si>
@@ -605,12 +605,6 @@
     <t>SRS_LOGIN_004</t>
   </si>
   <si>
-    <t>014</t>
-  </si>
-  <si>
-    <t>SRS_LOGIN_005</t>
-  </si>
-  <si>
     <t>015</t>
   </si>
   <si>
@@ -641,12 +635,6 @@
     <t>SRS_NAV_004</t>
   </si>
   <si>
-    <t>019</t>
-  </si>
-  <si>
-    <t>SRS_NAV_005</t>
-  </si>
-  <si>
     <t>020</t>
   </si>
   <si>
@@ -704,60 +692,12 @@
     <t>SRS-ADD-009</t>
   </si>
   <si>
-    <t>029</t>
-  </si>
-  <si>
-    <t>SRS-ADD-010</t>
-  </si>
-  <si>
-    <t>032</t>
-  </si>
-  <si>
-    <t>SRS-EDIT-001</t>
-  </si>
-  <si>
-    <t>033</t>
-  </si>
-  <si>
-    <t>SRS-EDIT-002</t>
-  </si>
-  <si>
     <t>CRS-5.1</t>
   </si>
   <si>
-    <t>034</t>
-  </si>
-  <si>
-    <t>SRS-EDIT-003</t>
-  </si>
-  <si>
-    <t>035</t>
-  </si>
-  <si>
-    <t>SRS-EDIT-004</t>
-  </si>
-  <si>
     <t>CRS-5.2</t>
   </si>
   <si>
-    <t>036</t>
-  </si>
-  <si>
-    <t>SRS-EDIT-005</t>
-  </si>
-  <si>
-    <t>037</t>
-  </si>
-  <si>
-    <t>SRS-EDIT-006</t>
-  </si>
-  <si>
-    <t>038</t>
-  </si>
-  <si>
-    <t>SRS-EDIT-007</t>
-  </si>
-  <si>
     <t>043</t>
   </si>
   <si>
@@ -812,18 +752,6 @@
     <t>SRS-NOTIFI-002</t>
   </si>
   <si>
-    <t>058</t>
-  </si>
-  <si>
-    <t>SRS-NOTIFI-003</t>
-  </si>
-  <si>
-    <t>059</t>
-  </si>
-  <si>
-    <t>SRS-NOTIFI-004</t>
-  </si>
-  <si>
     <t>060</t>
   </si>
   <si>
@@ -890,36 +818,6 @@
     <t>SRS-DELUSR-002</t>
   </si>
   <si>
-    <t>071</t>
-  </si>
-  <si>
-    <t>SRS-DELUSR-003</t>
-  </si>
-  <si>
-    <t>072</t>
-  </si>
-  <si>
-    <t>SRS-DELUSR-004</t>
-  </si>
-  <si>
-    <t>073</t>
-  </si>
-  <si>
-    <t>SRS-DELUSR-005</t>
-  </si>
-  <si>
-    <t>074</t>
-  </si>
-  <si>
-    <t>SRS-DELUSR-006</t>
-  </si>
-  <si>
-    <t>075</t>
-  </si>
-  <si>
-    <t>SRS-DELUSR-007</t>
-  </si>
-  <si>
     <t>076</t>
   </si>
   <si>
@@ -1226,18 +1124,12 @@
     <t>CRS-3.4</t>
   </si>
   <si>
-    <t>CRS-4.1,CRS-4.2</t>
-  </si>
-  <si>
     <t>CRS-4.3</t>
   </si>
   <si>
     <t>CRS-6.1</t>
   </si>
   <si>
-    <t>CRS-6.2</t>
-  </si>
-  <si>
     <t>CRS-7.1</t>
   </si>
   <si>
@@ -1256,9 +1148,6 @@
     <t>Sequence (3.0-3.5)</t>
   </si>
   <si>
-    <t>Sequence (4.0-4.6)</t>
-  </si>
-  <si>
     <t>Sequence (5.0-5.3)</t>
   </si>
   <si>
@@ -1277,45 +1166,84 @@
     <t>AdminSequence (1.0-1.7)</t>
   </si>
   <si>
-    <t>https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf
-https://github.com/AlaaOsama25/learning-hub/blob/Mazrouaa/Design/Diagrams/DDD/ERD/ERD%20of%20learning%20hub%20ver%204.pdf</t>
-  </si>
-  <si>
     <t>Wire Frame</t>
-  </si>
-  <si>
-    <t>Registeration page No.2</t>
-  </si>
-  <si>
-    <t>Login page No.1</t>
-  </si>
-  <si>
-    <t>All pages(No.1-No.17)</t>
-  </si>
-  <si>
-    <t>Pages(5-7-8-10)</t>
-  </si>
-  <si>
-    <t>Page 3</t>
-  </si>
-  <si>
-    <t>Page 4</t>
-  </si>
-  <si>
-    <t>Page 12</t>
-  </si>
-  <si>
-    <t>Page 15</t>
-  </si>
-  <si>
-    <t>Page 16</t>
-  </si>
-  <si>
-    <t>Page 17</t>
   </si>
   <si>
     <t xml:space="preserve">
 (Sequence diagram)</t>
+  </si>
+  <si>
+    <t>https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf
+https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ERD/ERD%20of%20learning%20hub%20version%206.pdf</t>
+  </si>
+  <si>
+    <t>CRS-3.3</t>
+  </si>
+  <si>
+    <t>CRS-4.2</t>
+  </si>
+  <si>
+    <t>CRS-4.4</t>
+  </si>
+  <si>
+    <t>CRS-4.5</t>
+  </si>
+  <si>
+    <t>SRS-DELETE -008</t>
+  </si>
+  <si>
+    <t>CRS-5.3</t>
+  </si>
+  <si>
+    <t>SRS-ADDUSR-010</t>
+  </si>
+  <si>
+    <t>CRS-7.2</t>
+  </si>
+  <si>
+    <t>CRS-8.2</t>
+  </si>
+  <si>
+    <t>SRS-FOLLOW-001</t>
+  </si>
+  <si>
+    <t>SRS-FOLLOW-002</t>
+  </si>
+  <si>
+    <t>SRS-FOLLOW-003</t>
+  </si>
+  <si>
+    <t>SRS-FOLLOW-004</t>
+  </si>
+  <si>
+    <t>CRS-9.2</t>
+  </si>
+  <si>
+    <t>CRS-9.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registeration page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login page </t>
+  </si>
+  <si>
+    <t>All pages</t>
+  </si>
+  <si>
+    <t>Home Page &amp; Categories Pages</t>
+  </si>
+  <si>
+    <t>Notification Page</t>
+  </si>
+  <si>
+    <t>Add User Page</t>
+  </si>
+  <si>
+    <t>Delete User Page</t>
+  </si>
+  <si>
+    <t>Categories Page</t>
   </si>
 </sst>
 </file>
@@ -1325,7 +1253,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1379,13 +1307,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="8"/>
-      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1918,7 +1839,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1988,7 +1909,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2016,10 +1937,10 @@
     <xf numFmtId="49" fontId="6" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2049,91 +1970,91 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2141,6 +2062,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="44"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2159,27 +2101,6 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor indexed="45"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="44"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2484,10 +2405,10 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="56"/>
+      <c r="B4" s="64"/>
     </row>
     <row r="5" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
@@ -2587,10 +2508,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L167"/>
+  <dimension ref="A1:L156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2631,15 +2552,15 @@
         <v>21</v>
       </c>
       <c r="B2" s="11"/>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
       <c r="J2" s="29"/>
       <c r="K2" s="29"/>
       <c r="L2" s="30"/>
@@ -2649,15 +2570,15 @@
         <v>23</v>
       </c>
       <c r="B3" s="12"/>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
       <c r="J3" s="29"/>
       <c r="K3" s="29"/>
       <c r="L3" s="30"/>
@@ -2667,15 +2588,15 @@
         <v>25</v>
       </c>
       <c r="B4" s="14"/>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
       <c r="J4" s="29"/>
       <c r="K4" s="29"/>
       <c r="L4" s="31"/>
@@ -2684,21 +2605,21 @@
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="63" t="s">
-        <v>300</v>
-      </c>
-      <c r="E5" s="64" t="s">
+      <c r="D5" s="56" t="s">
+        <v>252</v>
+      </c>
+      <c r="E5" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="70"/>
-      <c r="G5" s="71" t="s">
-        <v>289</v>
+      <c r="F5" s="69"/>
+      <c r="G5" s="60" t="s">
+        <v>251</v>
       </c>
       <c r="H5" s="54" t="s">
         <v>30</v>
@@ -2716,27 +2637,27 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="57" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>286</v>
-      </c>
-      <c r="E6" s="66" t="s">
+        <v>249</v>
+      </c>
+      <c r="E6" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G6" s="72" t="s">
-        <v>290</v>
+      <c r="F6" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G6" s="61" t="s">
+        <v>269</v>
       </c>
       <c r="H6" s="18"/>
       <c r="I6" s="19"/>
@@ -2744,27 +2665,27 @@
       <c r="K6" s="36"/>
       <c r="L6" s="37"/>
     </row>
-    <row r="7" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="57" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>37</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>286</v>
-      </c>
-      <c r="E7" s="66" t="s">
+        <v>249</v>
+      </c>
+      <c r="E7" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G7" s="72" t="s">
-        <v>290</v>
+      <c r="F7" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G7" s="61" t="s">
+        <v>269</v>
       </c>
       <c r="H7" s="20"/>
       <c r="I7" s="21"/>
@@ -2772,27 +2693,27 @@
       <c r="K7" s="39"/>
       <c r="L7" s="40"/>
     </row>
-    <row r="8" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="57" t="s">
         <v>42</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>37</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>286</v>
-      </c>
-      <c r="E8" s="66" t="s">
+        <v>249</v>
+      </c>
+      <c r="E8" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G8" s="72" t="s">
-        <v>290</v>
+      <c r="F8" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G8" s="61" t="s">
+        <v>269</v>
       </c>
       <c r="H8" s="20"/>
       <c r="I8" s="21"/>
@@ -2800,27 +2721,27 @@
       <c r="K8" s="39"/>
       <c r="L8" s="40"/>
     </row>
-    <row r="9" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="57" t="s">
         <v>44</v>
       </c>
       <c r="C9" s="24" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>286</v>
-      </c>
-      <c r="E9" s="66" t="s">
+        <v>249</v>
+      </c>
+      <c r="E9" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G9" s="72" t="s">
-        <v>290</v>
+      <c r="F9" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G9" s="61" t="s">
+        <v>269</v>
       </c>
       <c r="H9" s="20"/>
       <c r="I9" s="21"/>
@@ -2828,27 +2749,27 @@
       <c r="K9" s="39"/>
       <c r="L9" s="40"/>
     </row>
-    <row r="10" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="57" t="s">
         <v>47</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>286</v>
-      </c>
-      <c r="E10" s="66" t="s">
+        <v>249</v>
+      </c>
+      <c r="E10" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G10" s="72" t="s">
-        <v>290</v>
+      <c r="F10" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G10" s="61" t="s">
+        <v>269</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="21"/>
@@ -2856,27 +2777,27 @@
       <c r="K10" s="39"/>
       <c r="L10" s="40"/>
     </row>
-    <row r="11" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="57" t="s">
         <v>50</v>
       </c>
       <c r="C11" s="24" t="s">
         <v>48</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>286</v>
-      </c>
-      <c r="E11" s="66" t="s">
+        <v>249</v>
+      </c>
+      <c r="E11" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G11" s="72" t="s">
-        <v>290</v>
+      <c r="F11" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G11" s="61" t="s">
+        <v>269</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="21"/>
@@ -2884,27 +2805,27 @@
       <c r="K11" s="39"/>
       <c r="L11" s="40"/>
     </row>
-    <row r="12" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="57" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>48</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>286</v>
-      </c>
-      <c r="E12" s="66" t="s">
+        <v>249</v>
+      </c>
+      <c r="E12" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G12" s="72" t="s">
-        <v>290</v>
+      <c r="F12" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G12" s="61" t="s">
+        <v>269</v>
       </c>
       <c r="H12" s="20"/>
       <c r="I12" s="21"/>
@@ -2912,27 +2833,27 @@
       <c r="K12" s="39"/>
       <c r="L12" s="40"/>
     </row>
-    <row r="13" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="65" t="s">
+      <c r="B13" s="57" t="s">
         <v>54</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>48</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>286</v>
-      </c>
-      <c r="E13" s="66" t="s">
+        <v>249</v>
+      </c>
+      <c r="E13" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G13" s="72" t="s">
-        <v>290</v>
+      <c r="F13" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G13" s="61" t="s">
+        <v>269</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="21"/>
@@ -2940,27 +2861,27 @@
       <c r="K13" s="39"/>
       <c r="L13" s="40"/>
     </row>
-    <row r="14" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="68" t="s">
+      <c r="B14" s="59" t="s">
         <v>56</v>
       </c>
       <c r="C14" s="24" t="s">
         <v>57</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="E14" s="66" t="s">
+        <v>250</v>
+      </c>
+      <c r="E14" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G14" s="73" t="s">
-        <v>291</v>
+      <c r="F14" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G14" s="62" t="s">
+        <v>270</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="21"/>
@@ -2968,27 +2889,27 @@
       <c r="K14" s="39"/>
       <c r="L14" s="40"/>
     </row>
-    <row r="15" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="59" t="s">
         <v>59</v>
       </c>
       <c r="C15" s="24" t="s">
         <v>57</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="E15" s="66" t="s">
+        <v>250</v>
+      </c>
+      <c r="E15" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G15" s="73" t="s">
-        <v>291</v>
+      <c r="F15" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G15" s="62" t="s">
+        <v>270</v>
       </c>
       <c r="H15" s="20"/>
       <c r="I15" s="21"/>
@@ -2996,27 +2917,27 @@
       <c r="K15" s="39"/>
       <c r="L15" s="40"/>
     </row>
-    <row r="16" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="59" t="s">
         <v>61</v>
       </c>
       <c r="C16" s="24" t="s">
         <v>57</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="E16" s="66" t="s">
+        <v>250</v>
+      </c>
+      <c r="E16" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G16" s="73" t="s">
-        <v>291</v>
+      <c r="F16" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G16" s="62" t="s">
+        <v>270</v>
       </c>
       <c r="H16" s="20"/>
       <c r="I16" s="21"/>
@@ -3024,27 +2945,27 @@
       <c r="K16" s="39"/>
       <c r="L16" s="40"/>
     </row>
-    <row r="17" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="59" t="s">
         <v>63</v>
       </c>
       <c r="C17" s="24" t="s">
         <v>57</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="E17" s="66" t="s">
+        <v>250</v>
+      </c>
+      <c r="E17" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G17" s="73" t="s">
-        <v>291</v>
+      <c r="F17" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G17" s="62" t="s">
+        <v>270</v>
       </c>
       <c r="H17" s="20"/>
       <c r="I17" s="21"/>
@@ -3052,27 +2973,27 @@
       <c r="K17" s="39"/>
       <c r="L17" s="40"/>
     </row>
-    <row r="18" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="68" t="s">
+      <c r="B18" s="59" t="s">
         <v>65</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="E18" s="66" t="s">
+        <v>243</v>
+      </c>
+      <c r="E18" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G18" s="73" t="s">
-        <v>291</v>
+      <c r="F18" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G18" s="62" t="s">
+        <v>271</v>
       </c>
       <c r="H18" s="20"/>
       <c r="I18" s="21"/>
@@ -3080,27 +3001,27 @@
       <c r="K18" s="39"/>
       <c r="L18" s="40"/>
     </row>
-    <row r="19" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="68" t="s">
         <v>67</v>
       </c>
+      <c r="B19" s="59" t="s">
+        <v>68</v>
+      </c>
       <c r="C19" s="24" t="s">
-        <v>68</v>
+        <v>236</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="E19" s="66" t="s">
+        <v>243</v>
+      </c>
+      <c r="E19" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G19" s="73" t="s">
-        <v>292</v>
+      <c r="F19" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G19" s="62" t="s">
+        <v>271</v>
       </c>
       <c r="H19" s="20"/>
       <c r="I19" s="21"/>
@@ -3108,27 +3029,27 @@
       <c r="K19" s="39"/>
       <c r="L19" s="40"/>
     </row>
-    <row r="20" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="68" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>71</v>
-      </c>
       <c r="D20" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="E20" s="66" t="s">
+        <v>243</v>
+      </c>
+      <c r="E20" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G20" s="73" t="s">
-        <v>292</v>
+      <c r="F20" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G20" s="62" t="s">
+        <v>271</v>
       </c>
       <c r="H20" s="20"/>
       <c r="I20" s="21"/>
@@ -3136,27 +3057,27 @@
       <c r="K20" s="39"/>
       <c r="L20" s="40"/>
     </row>
-    <row r="21" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="59" t="s">
         <v>73</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="E21" s="66" t="s">
+        <v>243</v>
+      </c>
+      <c r="E21" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F21" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G21" s="73" t="s">
-        <v>292</v>
+      <c r="F21" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G21" s="62" t="s">
+        <v>271</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="21"/>
@@ -3164,27 +3085,27 @@
       <c r="K21" s="39"/>
       <c r="L21" s="40"/>
     </row>
-    <row r="22" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="68" t="s">
+      <c r="B22" s="59" t="s">
         <v>75</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="E22" s="66" t="s">
+        <v>244</v>
+      </c>
+      <c r="E22" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G22" s="73" t="s">
-        <v>292</v>
+      <c r="F22" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G22" s="62" t="s">
+        <v>272</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="21"/>
@@ -3192,27 +3113,27 @@
       <c r="K22" s="39"/>
       <c r="L22" s="40"/>
     </row>
-    <row r="23" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="68" t="s">
         <v>77</v>
       </c>
+      <c r="B23" s="59" t="s">
+        <v>78</v>
+      </c>
       <c r="C23" s="24" t="s">
-        <v>68</v>
+        <v>255</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="E23" s="66" t="s">
+        <v>244</v>
+      </c>
+      <c r="E23" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G23" s="73" t="s">
-        <v>292</v>
+      <c r="F23" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G23" s="62" t="s">
+        <v>272</v>
       </c>
       <c r="H23" s="20"/>
       <c r="I23" s="21"/>
@@ -3220,27 +3141,27 @@
       <c r="K23" s="39"/>
       <c r="L23" s="40"/>
     </row>
-    <row r="24" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="68" t="s">
         <v>79</v>
       </c>
+      <c r="B24" s="59" t="s">
+        <v>80</v>
+      </c>
       <c r="C24" s="24" t="s">
-        <v>271</v>
+        <v>76</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="E24" s="66" t="s">
+        <v>244</v>
+      </c>
+      <c r="E24" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G24" s="73" t="s">
-        <v>293</v>
+      <c r="F24" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G24" s="62" t="s">
+        <v>272</v>
       </c>
       <c r="H24" s="20"/>
       <c r="I24" s="21"/>
@@ -3248,27 +3169,27 @@
       <c r="K24" s="39"/>
       <c r="L24" s="40"/>
     </row>
-    <row r="25" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="68" t="s">
+      <c r="B25" s="59" t="s">
         <v>82</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>80</v>
+        <v>237</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="E25" s="66" t="s">
+        <v>244</v>
+      </c>
+      <c r="E25" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F25" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G25" s="73" t="s">
-        <v>293</v>
+      <c r="F25" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G25" s="62" t="s">
+        <v>272</v>
       </c>
       <c r="H25" s="20"/>
       <c r="I25" s="21"/>
@@ -3276,27 +3197,27 @@
       <c r="K25" s="39"/>
       <c r="L25" s="40"/>
     </row>
-    <row r="26" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="68" t="s">
+      <c r="B26" s="59" t="s">
         <v>84</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>80</v>
+        <v>256</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="E26" s="66" t="s">
+        <v>244</v>
+      </c>
+      <c r="E26" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F26" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G26" s="73" t="s">
-        <v>293</v>
+      <c r="F26" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G26" s="62" t="s">
+        <v>272</v>
       </c>
       <c r="H26" s="20"/>
       <c r="I26" s="21"/>
@@ -3304,27 +3225,27 @@
       <c r="K26" s="39"/>
       <c r="L26" s="40"/>
     </row>
-    <row r="27" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="68" t="s">
+      <c r="B27" s="59" t="s">
         <v>86</v>
       </c>
       <c r="C27" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="E27" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G27" s="62" t="s">
         <v>272</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="E27" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F27" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G27" s="73" t="s">
-        <v>293</v>
       </c>
       <c r="H27" s="20"/>
       <c r="I27" s="21"/>
@@ -3332,27 +3253,27 @@
       <c r="K27" s="39"/>
       <c r="L27" s="40"/>
     </row>
-    <row r="28" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="68" t="s">
+      <c r="B28" s="59" t="s">
         <v>88</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>80</v>
+        <v>237</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="E28" s="66" t="s">
+        <v>244</v>
+      </c>
+      <c r="E28" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G28" s="73" t="s">
-        <v>293</v>
+      <c r="F28" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G28" s="62" t="s">
+        <v>272</v>
       </c>
       <c r="H28" s="20"/>
       <c r="I28" s="21"/>
@@ -3360,27 +3281,27 @@
       <c r="K28" s="39"/>
       <c r="L28" s="40"/>
     </row>
-    <row r="29" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="68" t="s">
+      <c r="B29" s="59" t="s">
         <v>90</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>80</v>
+        <v>257</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="E29" s="66" t="s">
+        <v>244</v>
+      </c>
+      <c r="E29" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G29" s="73" t="s">
-        <v>293</v>
+      <c r="F29" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G29" s="62" t="s">
+        <v>272</v>
       </c>
       <c r="H29" s="20"/>
       <c r="I29" s="21"/>
@@ -3388,27 +3309,27 @@
       <c r="K29" s="39"/>
       <c r="L29" s="40"/>
     </row>
-    <row r="30" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A30" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="B30" s="68" t="s">
+      <c r="B30" s="59" t="s">
         <v>92</v>
       </c>
       <c r="C30" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="E30" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G30" s="62" t="s">
         <v>272</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="E30" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G30" s="73" t="s">
-        <v>293</v>
       </c>
       <c r="H30" s="20"/>
       <c r="I30" s="21"/>
@@ -3416,167 +3337,167 @@
       <c r="K30" s="39"/>
       <c r="L30" s="40"/>
     </row>
-    <row r="31" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="22" t="s">
+    <row r="31" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="59" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="B31" s="68" t="s">
+      <c r="D31" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="E31" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G31" s="62" t="s">
+        <v>272</v>
+      </c>
+      <c r="H31" s="26"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="41"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="43"/>
+    </row>
+    <row r="32" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="E32" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G32" s="62" t="s">
+        <v>272</v>
+      </c>
+      <c r="H32" s="26"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="43"/>
+    </row>
+    <row r="33" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="E33" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G33" s="62" t="s">
+        <v>272</v>
+      </c>
+      <c r="H33" s="26"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="41"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="43"/>
+    </row>
+    <row r="34" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="E31" s="66" t="s">
+      <c r="D34" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="E34" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F31" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G31" s="73" t="s">
-        <v>293</v>
-      </c>
-      <c r="H31" s="20"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="40"/>
-    </row>
-    <row r="32" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="B32" s="68" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="E32" s="66" t="s">
+      <c r="F34" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G34" s="62" t="s">
+        <v>272</v>
+      </c>
+      <c r="H34" s="26"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="43"/>
+    </row>
+    <row r="35" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="E35" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F32" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G32" s="73" t="s">
-        <v>293</v>
-      </c>
-      <c r="H32" s="20"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="38"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="40"/>
-    </row>
-    <row r="33" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="B33" s="68" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="E33" s="66" t="s">
+      <c r="F35" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G35" s="62" t="s">
+        <v>272</v>
+      </c>
+      <c r="H35" s="26"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="42"/>
+      <c r="L35" s="43"/>
+    </row>
+    <row r="36" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="E36" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F33" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G33" s="73" t="s">
-        <v>293</v>
-      </c>
-      <c r="H33" s="20"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="40"/>
-    </row>
-    <row r="34" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="B34" s="68" t="s">
-        <v>100</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="E34" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F34" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G34" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="H34" s="20"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="38"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="40"/>
-    </row>
-    <row r="35" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
-      <c r="A35" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="B35" s="68" t="s">
-        <v>102</v>
-      </c>
-      <c r="C35" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="E35" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F35" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G35" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="H35" s="20"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="38"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="40"/>
-    </row>
-    <row r="36" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="B36" s="68" t="s">
-        <v>105</v>
-      </c>
-      <c r="C36" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="E36" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F36" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G36" s="73" t="s">
-        <v>294</v>
+      <c r="F36" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G36" s="62" t="s">
+        <v>272</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="27"/>
@@ -3584,27 +3505,27 @@
       <c r="K36" s="42"/>
       <c r="L36" s="43"/>
     </row>
-    <row r="37" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="B37" s="68" t="s">
         <v>107</v>
       </c>
+      <c r="B37" s="59" t="s">
+        <v>108</v>
+      </c>
       <c r="C37" s="24" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="E37" s="66" t="s">
+        <v>245</v>
+      </c>
+      <c r="E37" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F37" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G37" s="73" t="s">
-        <v>294</v>
+      <c r="F37" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G37" s="62" t="s">
+        <v>272</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="27"/>
@@ -3612,27 +3533,27 @@
       <c r="K37" s="42"/>
       <c r="L37" s="43"/>
     </row>
-    <row r="38" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="B38" s="68" t="s">
-        <v>110</v>
+        <v>107</v>
+      </c>
+      <c r="B38" s="59" t="s">
+        <v>258</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>108</v>
+        <v>259</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="E38" s="66" t="s">
+        <v>245</v>
+      </c>
+      <c r="E38" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F38" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G38" s="73" t="s">
-        <v>294</v>
+      <c r="F38" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G38" s="62" t="s">
+        <v>272</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="27"/>
@@ -3640,27 +3561,25 @@
       <c r="K38" s="42"/>
       <c r="L38" s="43"/>
     </row>
-    <row r="39" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="B39" s="68" t="s">
-        <v>112</v>
+        <v>109</v>
+      </c>
+      <c r="B39" s="59" t="s">
+        <v>110</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="E39" s="66" t="s">
+        <v>238</v>
+      </c>
+      <c r="D39" s="20"/>
+      <c r="E39" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F39" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G39" s="73" t="s">
-        <v>294</v>
+      <c r="F39" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G39" s="62" t="s">
+        <v>273</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="27"/>
@@ -3668,27 +3587,25 @@
       <c r="K39" s="42"/>
       <c r="L39" s="43"/>
     </row>
-    <row r="40" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="B40" s="68" t="s">
-        <v>114</v>
+        <v>111</v>
+      </c>
+      <c r="B40" s="59" t="s">
+        <v>112</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="E40" s="66" t="s">
+        <v>238</v>
+      </c>
+      <c r="D40" s="20"/>
+      <c r="E40" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F40" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G40" s="73" t="s">
-        <v>294</v>
+      <c r="F40" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G40" s="62" t="s">
+        <v>273</v>
       </c>
       <c r="H40" s="26"/>
       <c r="I40" s="27"/>
@@ -3696,27 +3613,27 @@
       <c r="K40" s="42"/>
       <c r="L40" s="43"/>
     </row>
-    <row r="41" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="B41" s="68" t="s">
-        <v>116</v>
+        <v>113</v>
+      </c>
+      <c r="B41" s="59" t="s">
+        <v>114</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>273</v>
+        <v>37</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E41" s="66" t="s">
+        <v>246</v>
+      </c>
+      <c r="E41" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F41" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G41" s="73" t="s">
-        <v>295</v>
+      <c r="F41" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G41" s="62" t="s">
+        <v>274</v>
       </c>
       <c r="H41" s="26"/>
       <c r="I41" s="27"/>
@@ -3724,27 +3641,27 @@
       <c r="K41" s="42"/>
       <c r="L41" s="43"/>
     </row>
-    <row r="42" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="B42" s="68" t="s">
-        <v>118</v>
+        <v>115</v>
+      </c>
+      <c r="B42" s="59" t="s">
+        <v>116</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>273</v>
+        <v>37</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E42" s="66" t="s">
+        <v>246</v>
+      </c>
+      <c r="E42" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G42" s="73" t="s">
-        <v>295</v>
+      <c r="F42" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G42" s="62" t="s">
+        <v>274</v>
       </c>
       <c r="H42" s="26"/>
       <c r="I42" s="27"/>
@@ -3752,27 +3669,27 @@
       <c r="K42" s="42"/>
       <c r="L42" s="43"/>
     </row>
-    <row r="43" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="B43" s="68" t="s">
-        <v>120</v>
+        <v>117</v>
+      </c>
+      <c r="B43" s="59" t="s">
+        <v>118</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>273</v>
+        <v>37</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E43" s="66" t="s">
+        <v>246</v>
+      </c>
+      <c r="E43" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F43" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G43" s="73" t="s">
-        <v>295</v>
+      <c r="F43" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G43" s="62" t="s">
+        <v>274</v>
       </c>
       <c r="H43" s="26"/>
       <c r="I43" s="27"/>
@@ -3780,27 +3697,27 @@
       <c r="K43" s="42"/>
       <c r="L43" s="43"/>
     </row>
-    <row r="44" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="B44" s="68" t="s">
-        <v>122</v>
+        <v>119</v>
+      </c>
+      <c r="B44" s="59" t="s">
+        <v>120</v>
       </c>
       <c r="C44" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="E44" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G44" s="62" t="s">
         <v>274</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E44" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F44" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G44" s="73" t="s">
-        <v>295</v>
       </c>
       <c r="H44" s="26"/>
       <c r="I44" s="27"/>
@@ -3808,27 +3725,27 @@
       <c r="K44" s="42"/>
       <c r="L44" s="43"/>
     </row>
-    <row r="45" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="B45" s="68" t="s">
-        <v>124</v>
+        <v>121</v>
+      </c>
+      <c r="B45" s="59" t="s">
+        <v>122</v>
       </c>
       <c r="C45" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="E45" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F45" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G45" s="62" t="s">
         <v>274</v>
-      </c>
-      <c r="D45" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E45" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F45" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G45" s="73" t="s">
-        <v>295</v>
       </c>
       <c r="H45" s="26"/>
       <c r="I45" s="27"/>
@@ -3836,27 +3753,27 @@
       <c r="K45" s="42"/>
       <c r="L45" s="43"/>
     </row>
-    <row r="46" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="B46" s="68" t="s">
-        <v>126</v>
+        <v>123</v>
+      </c>
+      <c r="B46" s="59" t="s">
+        <v>124</v>
       </c>
       <c r="C46" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="E46" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F46" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G46" s="62" t="s">
         <v>274</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E46" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F46" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G46" s="73" t="s">
-        <v>295</v>
       </c>
       <c r="H46" s="26"/>
       <c r="I46" s="27"/>
@@ -3864,27 +3781,27 @@
       <c r="K46" s="42"/>
       <c r="L46" s="43"/>
     </row>
-    <row r="47" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="B47" s="68" t="s">
-        <v>128</v>
+        <v>125</v>
+      </c>
+      <c r="B47" s="59" t="s">
+        <v>126</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="E47" s="66" t="s">
+        <v>246</v>
+      </c>
+      <c r="E47" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F47" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G47" s="73" t="s">
-        <v>295</v>
+      <c r="F47" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G47" s="62" t="s">
+        <v>274</v>
       </c>
       <c r="H47" s="26"/>
       <c r="I47" s="27"/>
@@ -3892,25 +3809,27 @@
       <c r="K47" s="42"/>
       <c r="L47" s="43"/>
     </row>
-    <row r="48" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="B48" s="68" t="s">
-        <v>130</v>
+        <v>127</v>
+      </c>
+      <c r="B48" s="59" t="s">
+        <v>128</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>275</v>
-      </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="66" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="E48" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F48" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G48" s="73" t="s">
-        <v>296</v>
+      <c r="F48" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G48" s="62" t="s">
+        <v>274</v>
       </c>
       <c r="H48" s="26"/>
       <c r="I48" s="27"/>
@@ -3918,25 +3837,27 @@
       <c r="K48" s="42"/>
       <c r="L48" s="43"/>
     </row>
-    <row r="49" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="B49" s="68" t="s">
-        <v>132</v>
+        <v>129</v>
+      </c>
+      <c r="B49" s="59" t="s">
+        <v>130</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>275</v>
-      </c>
-      <c r="D49" s="20"/>
-      <c r="E49" s="66" t="s">
+        <v>239</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="E49" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F49" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G49" s="73" t="s">
-        <v>296</v>
+      <c r="F49" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G49" s="62" t="s">
+        <v>274</v>
       </c>
       <c r="H49" s="26"/>
       <c r="I49" s="27"/>
@@ -3944,25 +3865,27 @@
       <c r="K49" s="42"/>
       <c r="L49" s="43"/>
     </row>
-    <row r="50" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="B50" s="68" t="s">
-        <v>134</v>
+        <v>129</v>
+      </c>
+      <c r="B50" s="59" t="s">
+        <v>260</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>275</v>
-      </c>
-      <c r="D50" s="20"/>
-      <c r="E50" s="66" t="s">
+        <v>261</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="E50" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F50" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G50" s="73" t="s">
-        <v>296</v>
+      <c r="F50" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G50" s="62" t="s">
+        <v>274</v>
       </c>
       <c r="H50" s="26"/>
       <c r="I50" s="27"/>
@@ -3970,25 +3893,27 @@
       <c r="K50" s="42"/>
       <c r="L50" s="43"/>
     </row>
-    <row r="51" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="B51" s="68" t="s">
-        <v>136</v>
+        <v>131</v>
+      </c>
+      <c r="B51" s="59" t="s">
+        <v>132</v>
       </c>
       <c r="C51" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="E51" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F51" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G51" s="62" t="s">
         <v>275</v>
-      </c>
-      <c r="D51" s="20"/>
-      <c r="E51" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F51" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G51" s="73" t="s">
-        <v>296</v>
       </c>
       <c r="H51" s="26"/>
       <c r="I51" s="27"/>
@@ -3996,27 +3921,27 @@
       <c r="K51" s="42"/>
       <c r="L51" s="43"/>
     </row>
-    <row r="52" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="B52" s="68" t="s">
-        <v>138</v>
+        <v>133</v>
+      </c>
+      <c r="B52" s="59" t="s">
+        <v>134</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="E52" s="66" t="s">
+        <v>247</v>
+      </c>
+      <c r="E52" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F52" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G52" s="73" t="s">
-        <v>297</v>
+      <c r="F52" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G52" s="62" t="s">
+        <v>275</v>
       </c>
       <c r="H52" s="26"/>
       <c r="I52" s="27"/>
@@ -4024,27 +3949,25 @@
       <c r="K52" s="42"/>
       <c r="L52" s="43"/>
     </row>
-    <row r="53" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="B53" s="68" t="s">
-        <v>140</v>
+        <v>133</v>
+      </c>
+      <c r="B53" s="59" t="s">
+        <v>263</v>
       </c>
       <c r="C53" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="D53" s="20"/>
+      <c r="E53" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F53" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G53" s="62" t="s">
         <v>276</v>
-      </c>
-      <c r="D53" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="E53" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F53" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G53" s="73" t="s">
-        <v>297</v>
       </c>
       <c r="H53" s="26"/>
       <c r="I53" s="27"/>
@@ -4052,27 +3975,25 @@
       <c r="K53" s="42"/>
       <c r="L53" s="43"/>
     </row>
-    <row r="54" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="B54" s="68" t="s">
-        <v>142</v>
+        <v>133</v>
+      </c>
+      <c r="B54" s="59" t="s">
+        <v>264</v>
       </c>
       <c r="C54" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="D54" s="20"/>
+      <c r="E54" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F54" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G54" s="62" t="s">
         <v>276</v>
-      </c>
-      <c r="D54" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="E54" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F54" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G54" s="73" t="s">
-        <v>297</v>
       </c>
       <c r="H54" s="26"/>
       <c r="I54" s="27"/>
@@ -4080,27 +4001,25 @@
       <c r="K54" s="42"/>
       <c r="L54" s="43"/>
     </row>
-    <row r="55" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="B55" s="68" t="s">
-        <v>144</v>
+        <v>133</v>
+      </c>
+      <c r="B55" s="59" t="s">
+        <v>265</v>
       </c>
       <c r="C55" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="D55" s="20"/>
+      <c r="E55" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F55" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G55" s="62" t="s">
         <v>276</v>
-      </c>
-      <c r="D55" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="E55" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F55" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G55" s="73" t="s">
-        <v>297</v>
       </c>
       <c r="H55" s="26"/>
       <c r="I55" s="27"/>
@@ -4108,27 +4027,25 @@
       <c r="K55" s="42"/>
       <c r="L55" s="43"/>
     </row>
-    <row r="56" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="B56" s="68" t="s">
-        <v>146</v>
+        <v>133</v>
+      </c>
+      <c r="B56" s="59" t="s">
+        <v>266</v>
       </c>
       <c r="C56" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="D56" s="20"/>
+      <c r="E56" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F56" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G56" s="62" t="s">
         <v>276</v>
-      </c>
-      <c r="D56" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="E56" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F56" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G56" s="73" t="s">
-        <v>297</v>
       </c>
       <c r="H56" s="26"/>
       <c r="I56" s="27"/>
@@ -4136,27 +4053,27 @@
       <c r="K56" s="42"/>
       <c r="L56" s="43"/>
     </row>
-    <row r="57" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="B57" s="68" t="s">
-        <v>148</v>
+        <v>135</v>
+      </c>
+      <c r="B57" s="59" t="s">
+        <v>136</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="E57" s="66" t="s">
+        <v>248</v>
+      </c>
+      <c r="E57" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F57" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G57" s="73" t="s">
-        <v>297</v>
+      <c r="F57" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="G57" s="62" t="s">
+        <v>271</v>
       </c>
       <c r="H57" s="26"/>
       <c r="I57" s="27"/>
@@ -4164,445 +4081,313 @@
       <c r="K57" s="42"/>
       <c r="L57" s="43"/>
     </row>
-    <row r="58" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="B58" s="68" t="s">
-        <v>150</v>
-      </c>
-      <c r="C58" s="24" t="s">
-        <v>276</v>
-      </c>
-      <c r="D58" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="E58" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F58" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G58" s="73" t="s">
-        <v>297</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="B58" s="70"/>
+      <c r="C58" s="71"/>
+      <c r="D58" s="71"/>
+      <c r="E58" s="71"/>
+      <c r="F58" s="72"/>
+      <c r="G58" s="55"/>
       <c r="H58" s="26"/>
       <c r="I58" s="27"/>
       <c r="J58" s="41"/>
       <c r="K58" s="42"/>
       <c r="L58" s="43"/>
     </row>
-    <row r="59" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="B59" s="68" t="s">
-        <v>152</v>
-      </c>
-      <c r="C59" s="24" t="s">
-        <v>276</v>
-      </c>
-      <c r="D59" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="E59" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F59" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G59" s="73" t="s">
-        <v>297</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="B59" s="70"/>
+      <c r="C59" s="71"/>
+      <c r="D59" s="71"/>
+      <c r="E59" s="71"/>
+      <c r="F59" s="72"/>
+      <c r="G59" s="55"/>
       <c r="H59" s="26"/>
       <c r="I59" s="27"/>
       <c r="J59" s="41"/>
       <c r="K59" s="42"/>
       <c r="L59" s="43"/>
     </row>
-    <row r="60" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="B60" s="68" t="s">
-        <v>154</v>
-      </c>
-      <c r="C60" s="24" t="s">
-        <v>276</v>
-      </c>
-      <c r="D60" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="E60" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F60" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G60" s="73" t="s">
-        <v>297</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="B60" s="70"/>
+      <c r="C60" s="71"/>
+      <c r="D60" s="71"/>
+      <c r="E60" s="71"/>
+      <c r="F60" s="72"/>
+      <c r="G60" s="55"/>
       <c r="H60" s="26"/>
       <c r="I60" s="27"/>
       <c r="J60" s="41"/>
       <c r="K60" s="42"/>
       <c r="L60" s="43"/>
     </row>
-    <row r="61" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="B61" s="68" t="s">
-        <v>156</v>
-      </c>
-      <c r="C61" s="24" t="s">
-        <v>277</v>
-      </c>
-      <c r="D61" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="E61" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F61" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G61" s="73" t="s">
-        <v>298</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="B61" s="70"/>
+      <c r="C61" s="71"/>
+      <c r="D61" s="71"/>
+      <c r="E61" s="71"/>
+      <c r="F61" s="72"/>
+      <c r="G61" s="55"/>
       <c r="H61" s="26"/>
       <c r="I61" s="27"/>
       <c r="J61" s="41"/>
       <c r="K61" s="42"/>
       <c r="L61" s="43"/>
     </row>
-    <row r="62" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="B62" s="68" t="s">
-        <v>158</v>
-      </c>
-      <c r="C62" s="24" t="s">
-        <v>277</v>
-      </c>
-      <c r="D62" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="E62" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F62" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G62" s="73" t="s">
-        <v>298</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="B62" s="70"/>
+      <c r="C62" s="71"/>
+      <c r="D62" s="71"/>
+      <c r="E62" s="71"/>
+      <c r="F62" s="72"/>
+      <c r="G62" s="55"/>
       <c r="H62" s="26"/>
       <c r="I62" s="27"/>
       <c r="J62" s="41"/>
       <c r="K62" s="42"/>
       <c r="L62" s="43"/>
     </row>
-    <row r="63" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="B63" s="68" t="s">
-        <v>160</v>
-      </c>
-      <c r="C63" s="24" t="s">
-        <v>277</v>
-      </c>
-      <c r="D63" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="E63" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F63" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G63" s="73" t="s">
-        <v>298</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="B63" s="70"/>
+      <c r="C63" s="71"/>
+      <c r="D63" s="71"/>
+      <c r="E63" s="71"/>
+      <c r="F63" s="72"/>
+      <c r="G63" s="55"/>
       <c r="H63" s="26"/>
       <c r="I63" s="27"/>
       <c r="J63" s="41"/>
       <c r="K63" s="42"/>
       <c r="L63" s="43"/>
     </row>
-    <row r="64" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="B64" s="68" t="s">
-        <v>162</v>
-      </c>
-      <c r="C64" s="24" t="s">
-        <v>277</v>
-      </c>
-      <c r="D64" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="E64" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F64" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G64" s="73" t="s">
-        <v>298</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="B64" s="70"/>
+      <c r="C64" s="71"/>
+      <c r="D64" s="71"/>
+      <c r="E64" s="71"/>
+      <c r="F64" s="72"/>
+      <c r="G64" s="55"/>
       <c r="H64" s="26"/>
       <c r="I64" s="27"/>
       <c r="J64" s="41"/>
       <c r="K64" s="42"/>
       <c r="L64" s="43"/>
     </row>
-    <row r="65" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="B65" s="68" t="s">
-        <v>164</v>
-      </c>
-      <c r="C65" s="24" t="s">
-        <v>277</v>
-      </c>
-      <c r="D65" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="E65" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F65" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G65" s="73" t="s">
-        <v>298</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="B65" s="70"/>
+      <c r="C65" s="71"/>
+      <c r="D65" s="71"/>
+      <c r="E65" s="71"/>
+      <c r="F65" s="72"/>
+      <c r="G65" s="55"/>
       <c r="H65" s="26"/>
       <c r="I65" s="27"/>
       <c r="J65" s="41"/>
       <c r="K65" s="42"/>
       <c r="L65" s="43"/>
     </row>
-    <row r="66" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="B66" s="68" t="s">
-        <v>166</v>
-      </c>
-      <c r="C66" s="24" t="s">
-        <v>277</v>
-      </c>
-      <c r="D66" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="E66" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F66" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G66" s="73" t="s">
-        <v>298</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="B66" s="23"/>
+      <c r="C66" s="26"/>
+      <c r="D66" s="26"/>
+      <c r="E66" s="26"/>
+      <c r="F66" s="44"/>
+      <c r="G66" s="44"/>
       <c r="H66" s="26"/>
       <c r="I66" s="27"/>
       <c r="J66" s="41"/>
       <c r="K66" s="42"/>
       <c r="L66" s="43"/>
     </row>
-    <row r="67" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A67" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="B67" s="68" t="s">
-        <v>168</v>
-      </c>
-      <c r="C67" s="24" t="s">
-        <v>277</v>
-      </c>
-      <c r="D67" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="E67" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F67" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G67" s="73" t="s">
-        <v>298</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="B67" s="23"/>
+      <c r="C67" s="26"/>
+      <c r="D67" s="26"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="44"/>
+      <c r="G67" s="44"/>
       <c r="H67" s="26"/>
       <c r="I67" s="27"/>
       <c r="J67" s="41"/>
       <c r="K67" s="42"/>
       <c r="L67" s="43"/>
     </row>
-    <row r="68" spans="1:12" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A68" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="B68" s="68" t="s">
-        <v>170</v>
-      </c>
-      <c r="C68" s="24" t="s">
-        <v>278</v>
-      </c>
-      <c r="D68" s="20" t="s">
-        <v>285</v>
-      </c>
-      <c r="E68" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F68" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="G68" s="73" t="s">
-        <v>299</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="B68" s="23"/>
+      <c r="C68" s="26"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="44"/>
+      <c r="G68" s="44"/>
       <c r="H68" s="26"/>
       <c r="I68" s="27"/>
       <c r="J68" s="41"/>
       <c r="K68" s="42"/>
       <c r="L68" s="43"/>
     </row>
-    <row r="69" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A69" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="B69" s="60"/>
-      <c r="C69" s="61"/>
-      <c r="D69" s="61"/>
-      <c r="E69" s="61"/>
-      <c r="F69" s="62"/>
-      <c r="G69" s="69"/>
+        <v>148</v>
+      </c>
+      <c r="B69" s="23"/>
+      <c r="C69" s="26"/>
+      <c r="D69" s="26"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="44"/>
+      <c r="G69" s="44"/>
       <c r="H69" s="26"/>
       <c r="I69" s="27"/>
       <c r="J69" s="41"/>
       <c r="K69" s="42"/>
       <c r="L69" s="43"/>
     </row>
-    <row r="70" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A70" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="B70" s="60"/>
-      <c r="C70" s="61"/>
-      <c r="D70" s="61"/>
-      <c r="E70" s="61"/>
-      <c r="F70" s="62"/>
-      <c r="G70" s="69"/>
+        <v>149</v>
+      </c>
+      <c r="B70" s="23"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="26"/>
+      <c r="E70" s="26"/>
+      <c r="F70" s="44"/>
+      <c r="G70" s="44"/>
       <c r="H70" s="26"/>
       <c r="I70" s="27"/>
       <c r="J70" s="41"/>
       <c r="K70" s="42"/>
       <c r="L70" s="43"/>
     </row>
-    <row r="71" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A71" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="B71" s="60"/>
-      <c r="C71" s="61"/>
-      <c r="D71" s="61"/>
-      <c r="E71" s="61"/>
-      <c r="F71" s="62"/>
-      <c r="G71" s="69"/>
+        <v>150</v>
+      </c>
+      <c r="B71" s="23"/>
+      <c r="C71" s="26"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="44"/>
+      <c r="G71" s="44"/>
       <c r="H71" s="26"/>
       <c r="I71" s="27"/>
       <c r="J71" s="41"/>
       <c r="K71" s="42"/>
       <c r="L71" s="43"/>
     </row>
-    <row r="72" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A72" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="B72" s="60"/>
-      <c r="C72" s="61"/>
-      <c r="D72" s="61"/>
-      <c r="E72" s="61"/>
-      <c r="F72" s="62"/>
-      <c r="G72" s="69"/>
+        <v>151</v>
+      </c>
+      <c r="B72" s="23"/>
+      <c r="C72" s="26"/>
+      <c r="D72" s="26"/>
+      <c r="E72" s="26"/>
+      <c r="F72" s="44"/>
+      <c r="G72" s="44"/>
       <c r="H72" s="26"/>
       <c r="I72" s="27"/>
       <c r="J72" s="41"/>
       <c r="K72" s="42"/>
       <c r="L72" s="43"/>
     </row>
-    <row r="73" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A73" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="B73" s="60"/>
-      <c r="C73" s="61"/>
-      <c r="D73" s="61"/>
-      <c r="E73" s="61"/>
-      <c r="F73" s="62"/>
-      <c r="G73" s="69"/>
+        <v>152</v>
+      </c>
+      <c r="B73" s="23"/>
+      <c r="C73" s="26"/>
+      <c r="D73" s="26"/>
+      <c r="E73" s="26"/>
+      <c r="F73" s="44"/>
+      <c r="G73" s="44"/>
       <c r="H73" s="26"/>
       <c r="I73" s="27"/>
       <c r="J73" s="41"/>
       <c r="K73" s="42"/>
       <c r="L73" s="43"/>
     </row>
-    <row r="74" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A74" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="B74" s="60"/>
-      <c r="C74" s="61"/>
-      <c r="D74" s="61"/>
-      <c r="E74" s="61"/>
-      <c r="F74" s="62"/>
-      <c r="G74" s="69"/>
+        <v>153</v>
+      </c>
+      <c r="B74" s="23"/>
+      <c r="C74" s="26"/>
+      <c r="D74" s="26"/>
+      <c r="E74" s="26"/>
+      <c r="F74" s="44"/>
+      <c r="G74" s="44"/>
       <c r="H74" s="26"/>
       <c r="I74" s="27"/>
       <c r="J74" s="41"/>
       <c r="K74" s="42"/>
       <c r="L74" s="43"/>
     </row>
-    <row r="75" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A75" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="B75" s="60"/>
-      <c r="C75" s="61"/>
-      <c r="D75" s="61"/>
-      <c r="E75" s="61"/>
-      <c r="F75" s="62"/>
-      <c r="G75" s="69"/>
+        <v>154</v>
+      </c>
+      <c r="B75" s="23"/>
+      <c r="C75" s="26"/>
+      <c r="D75" s="26"/>
+      <c r="E75" s="26"/>
+      <c r="F75" s="44"/>
+      <c r="G75" s="44"/>
       <c r="H75" s="26"/>
       <c r="I75" s="27"/>
       <c r="J75" s="41"/>
       <c r="K75" s="42"/>
       <c r="L75" s="43"/>
     </row>
-    <row r="76" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A76" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="B76" s="60"/>
-      <c r="C76" s="61"/>
-      <c r="D76" s="61"/>
-      <c r="E76" s="61"/>
-      <c r="F76" s="62"/>
-      <c r="G76" s="69"/>
+        <v>155</v>
+      </c>
+      <c r="B76" s="23"/>
+      <c r="C76" s="26"/>
+      <c r="D76" s="26"/>
+      <c r="E76" s="26"/>
+      <c r="F76" s="44"/>
+      <c r="G76" s="44"/>
       <c r="H76" s="26"/>
       <c r="I76" s="27"/>
       <c r="J76" s="41"/>
       <c r="K76" s="42"/>
       <c r="L76" s="43"/>
     </row>
-    <row r="77" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A77" s="25" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="B77" s="23"/>
       <c r="C77" s="26"/>
@@ -4618,7 +4403,7 @@
     </row>
     <row r="78" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A78" s="25" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="B78" s="23"/>
       <c r="C78" s="26"/>
@@ -4634,7 +4419,7 @@
     </row>
     <row r="79" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A79" s="25" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="B79" s="23"/>
       <c r="C79" s="26"/>
@@ -4650,7 +4435,7 @@
     </row>
     <row r="80" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A80" s="25" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="B80" s="23"/>
       <c r="C80" s="26"/>
@@ -4666,7 +4451,7 @@
     </row>
     <row r="81" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A81" s="25" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
       <c r="B81" s="23"/>
       <c r="C81" s="26"/>
@@ -4682,7 +4467,7 @@
     </row>
     <row r="82" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A82" s="25" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
       <c r="B82" s="23"/>
       <c r="C82" s="26"/>
@@ -4698,7 +4483,7 @@
     </row>
     <row r="83" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A83" s="25" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
       <c r="B83" s="23"/>
       <c r="C83" s="26"/>
@@ -4714,7 +4499,7 @@
     </row>
     <row r="84" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A84" s="25" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="B84" s="23"/>
       <c r="C84" s="26"/>
@@ -4730,7 +4515,7 @@
     </row>
     <row r="85" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A85" s="25" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
       <c r="B85" s="23"/>
       <c r="C85" s="26"/>
@@ -4746,7 +4531,7 @@
     </row>
     <row r="86" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A86" s="25" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="B86" s="23"/>
       <c r="C86" s="26"/>
@@ -4762,7 +4547,7 @@
     </row>
     <row r="87" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A87" s="25" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
       <c r="B87" s="23"/>
       <c r="C87" s="26"/>
@@ -4778,7 +4563,7 @@
     </row>
     <row r="88" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A88" s="25" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="B88" s="23"/>
       <c r="C88" s="26"/>
@@ -4794,7 +4579,7 @@
     </row>
     <row r="89" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A89" s="25" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="B89" s="23"/>
       <c r="C89" s="26"/>
@@ -4810,7 +4595,7 @@
     </row>
     <row r="90" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A90" s="25" t="s">
-        <v>192</v>
+        <v>169</v>
       </c>
       <c r="B90" s="23"/>
       <c r="C90" s="26"/>
@@ -4826,7 +4611,7 @@
     </row>
     <row r="91" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A91" s="25" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="B91" s="23"/>
       <c r="C91" s="26"/>
@@ -4842,7 +4627,7 @@
     </row>
     <row r="92" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A92" s="25" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="B92" s="23"/>
       <c r="C92" s="26"/>
@@ -4858,7 +4643,7 @@
     </row>
     <row r="93" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A93" s="25" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="B93" s="23"/>
       <c r="C93" s="26"/>
@@ -4874,7 +4659,7 @@
     </row>
     <row r="94" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A94" s="25" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
       <c r="B94" s="23"/>
       <c r="C94" s="26"/>
@@ -4890,7 +4675,7 @@
     </row>
     <row r="95" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A95" s="25" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="B95" s="23"/>
       <c r="C95" s="26"/>
@@ -4906,7 +4691,7 @@
     </row>
     <row r="96" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A96" s="25" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
       <c r="B96" s="23"/>
       <c r="C96" s="26"/>
@@ -4922,7 +4707,7 @@
     </row>
     <row r="97" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A97" s="25" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
       <c r="B97" s="23"/>
       <c r="C97" s="26"/>
@@ -4938,7 +4723,7 @@
     </row>
     <row r="98" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A98" s="25" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="B98" s="23"/>
       <c r="C98" s="26"/>
@@ -4954,7 +4739,7 @@
     </row>
     <row r="99" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A99" s="25" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="B99" s="23"/>
       <c r="C99" s="26"/>
@@ -4970,7 +4755,7 @@
     </row>
     <row r="100" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A100" s="25" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
       <c r="B100" s="23"/>
       <c r="C100" s="26"/>
@@ -4986,7 +4771,7 @@
     </row>
     <row r="101" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A101" s="25" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
       <c r="B101" s="23"/>
       <c r="C101" s="26"/>
@@ -5002,7 +4787,7 @@
     </row>
     <row r="102" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A102" s="25" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="B102" s="23"/>
       <c r="C102" s="26"/>
@@ -5018,7 +4803,7 @@
     </row>
     <row r="103" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A103" s="25" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="B103" s="23"/>
       <c r="C103" s="26"/>
@@ -5034,7 +4819,7 @@
     </row>
     <row r="104" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A104" s="25" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="B104" s="23"/>
       <c r="C104" s="26"/>
@@ -5050,7 +4835,7 @@
     </row>
     <row r="105" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A105" s="25" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="B105" s="23"/>
       <c r="C105" s="26"/>
@@ -5066,7 +4851,7 @@
     </row>
     <row r="106" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A106" s="25" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="B106" s="23"/>
       <c r="C106" s="26"/>
@@ -5082,7 +4867,7 @@
     </row>
     <row r="107" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A107" s="25" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="B107" s="23"/>
       <c r="C107" s="26"/>
@@ -5098,7 +4883,7 @@
     </row>
     <row r="108" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A108" s="25" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="B108" s="23"/>
       <c r="C108" s="26"/>
@@ -5114,7 +4899,7 @@
     </row>
     <row r="109" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A109" s="25" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="B109" s="23"/>
       <c r="C109" s="26"/>
@@ -5130,7 +4915,7 @@
     </row>
     <row r="110" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A110" s="25" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="B110" s="23"/>
       <c r="C110" s="26"/>
@@ -5146,7 +4931,7 @@
     </row>
     <row r="111" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A111" s="25" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="B111" s="23"/>
       <c r="C111" s="26"/>
@@ -5162,7 +4947,7 @@
     </row>
     <row r="112" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A112" s="25" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="B112" s="23"/>
       <c r="C112" s="26"/>
@@ -5178,7 +4963,7 @@
     </row>
     <row r="113" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A113" s="25" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="B113" s="23"/>
       <c r="C113" s="26"/>
@@ -5194,7 +4979,7 @@
     </row>
     <row r="114" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A114" s="25" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
       <c r="B114" s="23"/>
       <c r="C114" s="26"/>
@@ -5210,7 +4995,7 @@
     </row>
     <row r="115" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A115" s="25" t="s">
-        <v>217</v>
+        <v>194</v>
       </c>
       <c r="B115" s="23"/>
       <c r="C115" s="26"/>
@@ -5226,7 +5011,7 @@
     </row>
     <row r="116" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A116" s="25" t="s">
-        <v>218</v>
+        <v>195</v>
       </c>
       <c r="B116" s="23"/>
       <c r="C116" s="26"/>
@@ -5242,7 +5027,7 @@
     </row>
     <row r="117" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A117" s="25" t="s">
-        <v>219</v>
+        <v>196</v>
       </c>
       <c r="B117" s="23"/>
       <c r="C117" s="26"/>
@@ -5258,7 +5043,7 @@
     </row>
     <row r="118" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A118" s="25" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="B118" s="23"/>
       <c r="C118" s="26"/>
@@ -5274,7 +5059,7 @@
     </row>
     <row r="119" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A119" s="25" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="B119" s="23"/>
       <c r="C119" s="26"/>
@@ -5290,7 +5075,7 @@
     </row>
     <row r="120" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A120" s="25" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="B120" s="23"/>
       <c r="C120" s="26"/>
@@ -5306,7 +5091,7 @@
     </row>
     <row r="121" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A121" s="25" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="B121" s="23"/>
       <c r="C121" s="26"/>
@@ -5322,7 +5107,7 @@
     </row>
     <row r="122" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A122" s="25" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="B122" s="23"/>
       <c r="C122" s="26"/>
@@ -5338,7 +5123,7 @@
     </row>
     <row r="123" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A123" s="25" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
       <c r="B123" s="23"/>
       <c r="C123" s="26"/>
@@ -5354,7 +5139,7 @@
     </row>
     <row r="124" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A124" s="25" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
       <c r="B124" s="23"/>
       <c r="C124" s="26"/>
@@ -5370,7 +5155,7 @@
     </row>
     <row r="125" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A125" s="25" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="B125" s="23"/>
       <c r="C125" s="26"/>
@@ -5386,7 +5171,7 @@
     </row>
     <row r="126" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A126" s="25" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
       <c r="B126" s="23"/>
       <c r="C126" s="26"/>
@@ -5402,7 +5187,7 @@
     </row>
     <row r="127" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A127" s="25" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="B127" s="23"/>
       <c r="C127" s="26"/>
@@ -5418,7 +5203,7 @@
     </row>
     <row r="128" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A128" s="25" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="B128" s="23"/>
       <c r="C128" s="26"/>
@@ -5434,7 +5219,7 @@
     </row>
     <row r="129" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A129" s="25" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="B129" s="23"/>
       <c r="C129" s="26"/>
@@ -5450,7 +5235,7 @@
     </row>
     <row r="130" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A130" s="25" t="s">
-        <v>232</v>
+        <v>209</v>
       </c>
       <c r="B130" s="23"/>
       <c r="C130" s="26"/>
@@ -5466,7 +5251,7 @@
     </row>
     <row r="131" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A131" s="25" t="s">
-        <v>233</v>
+        <v>210</v>
       </c>
       <c r="B131" s="23"/>
       <c r="C131" s="26"/>
@@ -5482,7 +5267,7 @@
     </row>
     <row r="132" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A132" s="25" t="s">
-        <v>234</v>
+        <v>211</v>
       </c>
       <c r="B132" s="23"/>
       <c r="C132" s="26"/>
@@ -5498,7 +5283,7 @@
     </row>
     <row r="133" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A133" s="25" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
       <c r="B133" s="23"/>
       <c r="C133" s="26"/>
@@ -5514,7 +5299,7 @@
     </row>
     <row r="134" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A134" s="25" t="s">
-        <v>236</v>
+        <v>213</v>
       </c>
       <c r="B134" s="23"/>
       <c r="C134" s="26"/>
@@ -5530,7 +5315,7 @@
     </row>
     <row r="135" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A135" s="25" t="s">
-        <v>237</v>
+        <v>214</v>
       </c>
       <c r="B135" s="23"/>
       <c r="C135" s="26"/>
@@ -5546,7 +5331,7 @@
     </row>
     <row r="136" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A136" s="25" t="s">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="B136" s="23"/>
       <c r="C136" s="26"/>
@@ -5562,7 +5347,7 @@
     </row>
     <row r="137" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A137" s="25" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="B137" s="23"/>
       <c r="C137" s="26"/>
@@ -5578,7 +5363,7 @@
     </row>
     <row r="138" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A138" s="25" t="s">
-        <v>240</v>
+        <v>217</v>
       </c>
       <c r="B138" s="23"/>
       <c r="C138" s="26"/>
@@ -5594,7 +5379,7 @@
     </row>
     <row r="139" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A139" s="25" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="B139" s="23"/>
       <c r="C139" s="26"/>
@@ -5610,7 +5395,7 @@
     </row>
     <row r="140" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A140" s="25" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="B140" s="23"/>
       <c r="C140" s="26"/>
@@ -5626,7 +5411,7 @@
     </row>
     <row r="141" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A141" s="25" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="B141" s="23"/>
       <c r="C141" s="26"/>
@@ -5642,7 +5427,7 @@
     </row>
     <row r="142" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A142" s="25" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="B142" s="23"/>
       <c r="C142" s="26"/>
@@ -5658,7 +5443,7 @@
     </row>
     <row r="143" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A143" s="25" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
       <c r="B143" s="23"/>
       <c r="C143" s="26"/>
@@ -5674,7 +5459,7 @@
     </row>
     <row r="144" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A144" s="25" t="s">
-        <v>246</v>
+        <v>223</v>
       </c>
       <c r="B144" s="23"/>
       <c r="C144" s="26"/>
@@ -5690,7 +5475,7 @@
     </row>
     <row r="145" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A145" s="25" t="s">
-        <v>247</v>
+        <v>224</v>
       </c>
       <c r="B145" s="23"/>
       <c r="C145" s="26"/>
@@ -5706,7 +5491,7 @@
     </row>
     <row r="146" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A146" s="25" t="s">
-        <v>248</v>
+        <v>225</v>
       </c>
       <c r="B146" s="23"/>
       <c r="C146" s="26"/>
@@ -5722,7 +5507,7 @@
     </row>
     <row r="147" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A147" s="25" t="s">
-        <v>249</v>
+        <v>226</v>
       </c>
       <c r="B147" s="23"/>
       <c r="C147" s="26"/>
@@ -5738,7 +5523,7 @@
     </row>
     <row r="148" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A148" s="25" t="s">
-        <v>250</v>
+        <v>227</v>
       </c>
       <c r="B148" s="23"/>
       <c r="C148" s="26"/>
@@ -5754,7 +5539,7 @@
     </row>
     <row r="149" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A149" s="25" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
       <c r="B149" s="23"/>
       <c r="C149" s="26"/>
@@ -5770,7 +5555,7 @@
     </row>
     <row r="150" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A150" s="25" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
       <c r="B150" s="23"/>
       <c r="C150" s="26"/>
@@ -5786,7 +5571,7 @@
     </row>
     <row r="151" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A151" s="25" t="s">
-        <v>253</v>
+        <v>230</v>
       </c>
       <c r="B151" s="23"/>
       <c r="C151" s="26"/>
@@ -5802,7 +5587,7 @@
     </row>
     <row r="152" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A152" s="25" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="B152" s="23"/>
       <c r="C152" s="26"/>
@@ -5818,7 +5603,7 @@
     </row>
     <row r="153" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A153" s="25" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
       <c r="B153" s="23"/>
       <c r="C153" s="26"/>
@@ -5834,7 +5619,7 @@
     </row>
     <row r="154" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A154" s="25" t="s">
-        <v>256</v>
+        <v>233</v>
       </c>
       <c r="B154" s="23"/>
       <c r="C154" s="26"/>
@@ -5850,7 +5635,7 @@
     </row>
     <row r="155" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A155" s="25" t="s">
-        <v>257</v>
+        <v>234</v>
       </c>
       <c r="B155" s="23"/>
       <c r="C155" s="26"/>
@@ -5866,7 +5651,7 @@
     </row>
     <row r="156" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A156" s="25" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
       <c r="B156" s="23"/>
       <c r="C156" s="26"/>
@@ -5880,228 +5665,83 @@
       <c r="K156" s="42"/>
       <c r="L156" s="43"/>
     </row>
-    <row r="157" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A157" s="25" t="s">
-        <v>259</v>
-      </c>
-      <c r="B157" s="23"/>
-      <c r="C157" s="26"/>
-      <c r="D157" s="26"/>
-      <c r="E157" s="26"/>
-      <c r="F157" s="44"/>
-      <c r="G157" s="44"/>
-      <c r="H157" s="26"/>
-      <c r="I157" s="27"/>
-      <c r="J157" s="41"/>
-      <c r="K157" s="42"/>
-      <c r="L157" s="43"/>
-    </row>
-    <row r="158" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A158" s="25" t="s">
-        <v>260</v>
-      </c>
-      <c r="B158" s="23"/>
-      <c r="C158" s="26"/>
-      <c r="D158" s="26"/>
-      <c r="E158" s="26"/>
-      <c r="F158" s="44"/>
-      <c r="G158" s="44"/>
-      <c r="H158" s="26"/>
-      <c r="I158" s="27"/>
-      <c r="J158" s="41"/>
-      <c r="K158" s="42"/>
-      <c r="L158" s="43"/>
-    </row>
-    <row r="159" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A159" s="25" t="s">
-        <v>261</v>
-      </c>
-      <c r="B159" s="23"/>
-      <c r="C159" s="26"/>
-      <c r="D159" s="26"/>
-      <c r="E159" s="26"/>
-      <c r="F159" s="44"/>
-      <c r="G159" s="44"/>
-      <c r="H159" s="26"/>
-      <c r="I159" s="27"/>
-      <c r="J159" s="41"/>
-      <c r="K159" s="42"/>
-      <c r="L159" s="43"/>
-    </row>
-    <row r="160" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A160" s="25" t="s">
-        <v>262</v>
-      </c>
-      <c r="B160" s="23"/>
-      <c r="C160" s="26"/>
-      <c r="D160" s="26"/>
-      <c r="E160" s="26"/>
-      <c r="F160" s="44"/>
-      <c r="G160" s="44"/>
-      <c r="H160" s="26"/>
-      <c r="I160" s="27"/>
-      <c r="J160" s="41"/>
-      <c r="K160" s="42"/>
-      <c r="L160" s="43"/>
-    </row>
-    <row r="161" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A161" s="25" t="s">
-        <v>263</v>
-      </c>
-      <c r="B161" s="23"/>
-      <c r="C161" s="26"/>
-      <c r="D161" s="26"/>
-      <c r="E161" s="26"/>
-      <c r="F161" s="44"/>
-      <c r="G161" s="44"/>
-      <c r="H161" s="26"/>
-      <c r="I161" s="27"/>
-      <c r="J161" s="41"/>
-      <c r="K161" s="42"/>
-      <c r="L161" s="43"/>
-    </row>
-    <row r="162" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A162" s="25" t="s">
-        <v>264</v>
-      </c>
-      <c r="B162" s="23"/>
-      <c r="C162" s="26"/>
-      <c r="D162" s="26"/>
-      <c r="E162" s="26"/>
-      <c r="F162" s="44"/>
-      <c r="G162" s="44"/>
-      <c r="H162" s="26"/>
-      <c r="I162" s="27"/>
-      <c r="J162" s="41"/>
-      <c r="K162" s="42"/>
-      <c r="L162" s="43"/>
-    </row>
-    <row r="163" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A163" s="25" t="s">
-        <v>265</v>
-      </c>
-      <c r="B163" s="23"/>
-      <c r="C163" s="26"/>
-      <c r="D163" s="26"/>
-      <c r="E163" s="26"/>
-      <c r="F163" s="44"/>
-      <c r="G163" s="44"/>
-      <c r="H163" s="26"/>
-      <c r="I163" s="27"/>
-      <c r="J163" s="41"/>
-      <c r="K163" s="42"/>
-      <c r="L163" s="43"/>
-    </row>
-    <row r="164" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A164" s="25" t="s">
-        <v>266</v>
-      </c>
-      <c r="B164" s="23"/>
-      <c r="C164" s="26"/>
-      <c r="D164" s="26"/>
-      <c r="E164" s="26"/>
-      <c r="F164" s="44"/>
-      <c r="G164" s="44"/>
-      <c r="H164" s="26"/>
-      <c r="I164" s="27"/>
-      <c r="J164" s="41"/>
-      <c r="K164" s="42"/>
-      <c r="L164" s="43"/>
-    </row>
-    <row r="165" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A165" s="25" t="s">
-        <v>267</v>
-      </c>
-      <c r="B165" s="23"/>
-      <c r="C165" s="26"/>
-      <c r="D165" s="26"/>
-      <c r="E165" s="26"/>
-      <c r="F165" s="44"/>
-      <c r="G165" s="44"/>
-      <c r="H165" s="26"/>
-      <c r="I165" s="27"/>
-      <c r="J165" s="41"/>
-      <c r="K165" s="42"/>
-      <c r="L165" s="43"/>
-    </row>
-    <row r="166" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A166" s="25" t="s">
-        <v>268</v>
-      </c>
-      <c r="B166" s="23"/>
-      <c r="C166" s="26"/>
-      <c r="D166" s="26"/>
-      <c r="E166" s="26"/>
-      <c r="F166" s="44"/>
-      <c r="G166" s="44"/>
-      <c r="H166" s="26"/>
-      <c r="I166" s="27"/>
-      <c r="J166" s="41"/>
-      <c r="K166" s="42"/>
-      <c r="L166" s="43"/>
-    </row>
-    <row r="167" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A167" s="25" t="s">
-        <v>269</v>
-      </c>
-      <c r="B167" s="23"/>
-      <c r="C167" s="26"/>
-      <c r="D167" s="26"/>
-      <c r="E167" s="26"/>
-      <c r="F167" s="44"/>
-      <c r="G167" s="44"/>
-      <c r="H167" s="26"/>
-      <c r="I167" s="27"/>
-      <c r="J167" s="41"/>
-      <c r="K167" s="42"/>
-      <c r="L167" s="43"/>
-    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="C3:I3"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B69:F76"/>
+    <mergeCell ref="B58:F65"/>
   </mergeCells>
-  <phoneticPr fontId="13" type="noConversion"/>
-  <conditionalFormatting sqref="F77:G167">
-    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
+  <phoneticPr fontId="12" type="noConversion"/>
+  <conditionalFormatting sqref="C1:I1 L1 K5:L5 C157:I65512">
+    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Critical"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F66:G156">
+    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Testing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:I1 C168:I65523 K5:L5 L1">
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
-      <formula>"Critical"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Medium"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F77:G167" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F66:G156" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"In Progress, Testing, Completed"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F6" r:id="rId1" display="learning-hub/ClassDiagram LearningHub.vpd.pdf at main · AlaaOsama25/learning-hub (github.com)_x000a__x000a_https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ERD/ERD%20of%20learning%20hub.pdf" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="F7:F68" r:id="rId2" display="learning-hub/ClassDiagram LearningHub.vpd.pdf at main · AlaaOsama25/learning-hub (github.com)_x000a__x000a_https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ERD/ERD%20of%20learning%20hub.pdf" xr:uid="{2B9313EA-C154-41C7-BAEB-9E130565F243}"/>
+    <hyperlink ref="F6" r:id="rId1" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{ED9B5678-481C-4C26-90B0-81BF0D2A14A2}"/>
+    <hyperlink ref="F8" r:id="rId2" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{68AEA8D1-BA06-4753-A112-C8CDC3C9B858}"/>
+    <hyperlink ref="F9" r:id="rId3" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{E9AB3FEA-0B92-4378-B58E-ACDD396775B8}"/>
+    <hyperlink ref="F7" r:id="rId4" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{804B6DAF-F01F-47A6-B347-EBD9F82996A3}"/>
+    <hyperlink ref="F10" r:id="rId5" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{33A5D95D-A613-4E33-91D0-F91836E3F1AE}"/>
+    <hyperlink ref="F11" r:id="rId6" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{C3759B12-8922-4CB0-82CE-159B2E9BAD5C}"/>
+    <hyperlink ref="F12" r:id="rId7" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{694625FA-5480-401A-B718-0589C8C7FCB1}"/>
+    <hyperlink ref="F13" r:id="rId8" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{0EFC58B7-09DF-45D7-9F0D-8454B41A91CD}"/>
+    <hyperlink ref="F14" r:id="rId9" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{61D9B4E2-2553-4CD5-9EAA-D95C845D5E64}"/>
+    <hyperlink ref="F15" r:id="rId10" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{015101B7-3E02-4376-9F93-EFD46BAFC1D8}"/>
+    <hyperlink ref="F16" r:id="rId11" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{4224CAE8-D477-4CC7-BBE2-9EC01B45D9FA}"/>
+    <hyperlink ref="F17" r:id="rId12" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{1641E57A-493F-4C05-834C-BDA7EFE326BC}"/>
+    <hyperlink ref="F18" r:id="rId13" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{E3AC5E34-DCAB-4B2D-91B7-DB7578DA7DA7}"/>
+    <hyperlink ref="F19" r:id="rId14" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{450A100B-9C54-462D-A844-DDBA03CEF330}"/>
+    <hyperlink ref="F20" r:id="rId15" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{0889437B-D418-49FA-A794-93D1B2A8DA5E}"/>
+    <hyperlink ref="F21" r:id="rId16" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{BEED0499-EB3F-4BC0-9EDD-B86CB5E04A15}"/>
+    <hyperlink ref="F22" r:id="rId17" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{D6FAD608-8B7D-40E7-8782-630B06F5438D}"/>
+    <hyperlink ref="F23" r:id="rId18" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A8B04DA8-15DA-424E-A339-EBF3D5430B4F}"/>
+    <hyperlink ref="F24" r:id="rId19" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{4055ADBA-18D1-49A8-AF10-C2B900AF0C71}"/>
+    <hyperlink ref="F25" r:id="rId20" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{DD5F08E8-4172-45BF-99C6-6877BD8883EF}"/>
+    <hyperlink ref="F26" r:id="rId21" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A6ED9626-4857-447E-8005-4923CC397323}"/>
+    <hyperlink ref="F27" r:id="rId22" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{060B7E8F-B19A-41D8-9F65-568E32450C69}"/>
+    <hyperlink ref="F28" r:id="rId23" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{AA2E7730-A407-494B-B217-60F04820FCD4}"/>
+    <hyperlink ref="F29" r:id="rId24" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{74162190-91F8-476D-8EED-5D782DF17E48}"/>
+    <hyperlink ref="F30" r:id="rId25" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{7498F791-7384-42D1-9284-7F13767D742A}"/>
+    <hyperlink ref="F31:F32" r:id="rId26" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{050B8A83-DABB-488A-A85F-114F7A41BF73}"/>
+    <hyperlink ref="F33:F57" r:id="rId27" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{94B9B623-DFA0-4247-B85F-18BC495D0A60}"/>
+    <hyperlink ref="F38" r:id="rId28" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{BA549CD2-BF8E-4F33-BAA0-710A9A6DB67D}"/>
+    <hyperlink ref="F50" r:id="rId29" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A15E1050-2C34-46FF-9F75-47F3E14BE3D5}"/>
+    <hyperlink ref="F53" r:id="rId30" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{516C8DDD-DD0B-4386-9826-11FC217EBBD0}"/>
+    <hyperlink ref="F54" r:id="rId31" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{78B541DE-49EF-4FCE-8337-1A697E954BB1}"/>
+    <hyperlink ref="F55" r:id="rId32" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{EEDB3697-71C1-43EC-91D5-4BBDAD2C1152}"/>
+    <hyperlink ref="F56" r:id="rId33" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{8564B7C9-3C2D-425E-9C41-C12DEFF1388B}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" r:id="rId3"/>
+  <pageSetup orientation="landscape" r:id="rId34"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;"Arial,Bold"&amp;8UP Template Version&amp;"Arial,Regular": 11/30/06&amp;R&amp;8Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId4"/>
+  <legacyDrawing r:id="rId35"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update Traceability_Matrix learning hub ver 2.xlsx
update sequence diagram linkage in rtm
</commit_message>
<xml_diff>
--- a/RTM/Traceability_Matrix learning hub ver 2.xlsx
+++ b/RTM/Traceability_Matrix learning hub ver 2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alaa Osama\Documents\GitHub\learning-hub\RTM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed Mazrouaa\Documents\GitHub\learning-hub\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028132BE-D214-47CB-A306-A8C3C26551D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DD28E5-CF29-487E-8852-12379FFFF430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" state="hidden" r:id="rId1"/>
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="278">
   <si>
     <t>For detail regarding the practice of Requirements Management, please refer to the Requirements Management Practices Guide</t>
   </si>
@@ -1142,28 +1142,7 @@
     <t>CRS-10.1</t>
   </si>
   <si>
-    <t>Sequence (2.0-2.5)</t>
-  </si>
-  <si>
-    <t>Sequence (3.0-3.5)</t>
-  </si>
-  <si>
-    <t>Sequence (5.0-5.3)</t>
-  </si>
-  <si>
-    <t>Sequence (6.0-6.5)</t>
-  </si>
-  <si>
-    <t>Sequence (7.0-7.5)</t>
-  </si>
-  <si>
-    <t>Sequence (8.0-8.2)</t>
-  </si>
-  <si>
     <t>UserSequence (1.0-1.8)</t>
-  </si>
-  <si>
-    <t>AdminSequence (1.0-1.7)</t>
   </si>
   <si>
     <t>Wire Frame</t>
@@ -1244,6 +1223,36 @@
   </si>
   <si>
     <t>Categories Page</t>
+  </si>
+  <si>
+    <t>AdminSequence (1.0-1.7)
+UserSequence (2.0-2.7)</t>
+  </si>
+  <si>
+    <t>AdminSequence (2.0-2.5)
+UserSequence (3.0-3.5)</t>
+  </si>
+  <si>
+    <t>AdminSequence (3.0-3.8)
+UserSequence (4.0-4.8)</t>
+  </si>
+  <si>
+    <t>AdminSequence (4.0-4.3)
+UserSequence (7.0-7.4)</t>
+  </si>
+  <si>
+    <t>AdminSequence (7.0-8.3)
+UserSequence (5.0-6.5)</t>
+  </si>
+  <si>
+    <t>AdminSequence (5.0-5.5)</t>
+  </si>
+  <si>
+    <t>AdminSequence (6.0-6.5)</t>
+  </si>
+  <si>
+    <t>AdminSequence (9.0-9.2)
+UserSequence (8.0-8.2)</t>
   </si>
 </sst>
 </file>
@@ -2023,6 +2032,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2052,9 +2064,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2405,10 +2414,10 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="64"/>
+      <c r="B4" s="65"/>
     </row>
     <row r="5" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
@@ -2510,8 +2519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2552,15 +2561,15 @@
         <v>21</v>
       </c>
       <c r="B2" s="11"/>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
       <c r="J2" s="29"/>
       <c r="K2" s="29"/>
       <c r="L2" s="30"/>
@@ -2570,15 +2579,15 @@
         <v>23</v>
       </c>
       <c r="B3" s="12"/>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
       <c r="J3" s="29"/>
       <c r="K3" s="29"/>
       <c r="L3" s="30"/>
@@ -2588,15 +2597,15 @@
         <v>25</v>
       </c>
       <c r="B4" s="14"/>
-      <c r="C4" s="66" t="s">
+      <c r="C4" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
       <c r="J4" s="29"/>
       <c r="K4" s="29"/>
       <c r="L4" s="31"/>
@@ -2612,14 +2621,14 @@
         <v>29</v>
       </c>
       <c r="D5" s="56" t="s">
-        <v>252</v>
-      </c>
-      <c r="E5" s="68" t="s">
+        <v>245</v>
+      </c>
+      <c r="E5" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="69"/>
+      <c r="F5" s="70"/>
       <c r="G5" s="60" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="H5" s="54" t="s">
         <v>30</v>
@@ -2648,16 +2657,16 @@
         <v>37</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E6" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="73" t="s">
-        <v>253</v>
+      <c r="F6" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G6" s="61" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="H6" s="18"/>
       <c r="I6" s="19"/>
@@ -2676,16 +2685,16 @@
         <v>37</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E7" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="73" t="s">
-        <v>253</v>
+      <c r="F7" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G7" s="61" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="H7" s="20"/>
       <c r="I7" s="21"/>
@@ -2704,16 +2713,16 @@
         <v>37</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E8" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="73" t="s">
-        <v>253</v>
+      <c r="F8" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G8" s="61" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="H8" s="20"/>
       <c r="I8" s="21"/>
@@ -2732,16 +2741,16 @@
         <v>45</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E9" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="73" t="s">
-        <v>253</v>
+      <c r="F9" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G9" s="61" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="H9" s="20"/>
       <c r="I9" s="21"/>
@@ -2760,16 +2769,16 @@
         <v>48</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E10" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="73" t="s">
-        <v>253</v>
+      <c r="F10" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G10" s="61" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="21"/>
@@ -2788,16 +2797,16 @@
         <v>48</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E11" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="73" t="s">
-        <v>253</v>
+      <c r="F11" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G11" s="61" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="21"/>
@@ -2816,16 +2825,16 @@
         <v>48</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E12" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="73" t="s">
-        <v>253</v>
+      <c r="F12" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G12" s="61" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="H12" s="20"/>
       <c r="I12" s="21"/>
@@ -2844,16 +2853,16 @@
         <v>48</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E13" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="73" t="s">
-        <v>253</v>
+      <c r="F13" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G13" s="61" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="21"/>
@@ -2872,16 +2881,16 @@
         <v>57</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="E14" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="73" t="s">
-        <v>253</v>
+      <c r="F14" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G14" s="62" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="21"/>
@@ -2900,16 +2909,16 @@
         <v>57</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="E15" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="73" t="s">
-        <v>253</v>
+      <c r="F15" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G15" s="62" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="H15" s="20"/>
       <c r="I15" s="21"/>
@@ -2928,16 +2937,16 @@
         <v>57</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="E16" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="73" t="s">
-        <v>253</v>
+      <c r="F16" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G16" s="62" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="H16" s="20"/>
       <c r="I16" s="21"/>
@@ -2956,16 +2965,16 @@
         <v>57</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="E17" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="73" t="s">
-        <v>253</v>
+      <c r="F17" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G17" s="62" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="H17" s="20"/>
       <c r="I17" s="21"/>
@@ -2984,16 +2993,16 @@
         <v>66</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
       <c r="E18" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="73" t="s">
-        <v>253</v>
+      <c r="F18" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G18" s="62" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="H18" s="20"/>
       <c r="I18" s="21"/>
@@ -3012,16 +3021,16 @@
         <v>236</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
       <c r="E19" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="73" t="s">
-        <v>253</v>
+      <c r="F19" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G19" s="62" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="H19" s="20"/>
       <c r="I19" s="21"/>
@@ -3040,16 +3049,16 @@
         <v>69</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
       <c r="E20" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="73" t="s">
-        <v>253</v>
+      <c r="F20" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G20" s="62" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="H20" s="20"/>
       <c r="I20" s="21"/>
@@ -3065,19 +3074,19 @@
         <v>73</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
       <c r="E21" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F21" s="73" t="s">
-        <v>253</v>
+      <c r="F21" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G21" s="62" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="21"/>
@@ -3096,16 +3105,16 @@
         <v>76</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
       <c r="E22" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="73" t="s">
-        <v>253</v>
+      <c r="F22" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G22" s="62" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="21"/>
@@ -3121,19 +3130,19 @@
         <v>78</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
       <c r="E23" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="73" t="s">
-        <v>253</v>
+      <c r="F23" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G23" s="62" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H23" s="20"/>
       <c r="I23" s="21"/>
@@ -3152,16 +3161,16 @@
         <v>76</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
       <c r="E24" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="73" t="s">
-        <v>253</v>
+      <c r="F24" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G24" s="62" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H24" s="20"/>
       <c r="I24" s="21"/>
@@ -3180,16 +3189,16 @@
         <v>237</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
       <c r="E25" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F25" s="73" t="s">
-        <v>253</v>
+      <c r="F25" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G25" s="62" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H25" s="20"/>
       <c r="I25" s="21"/>
@@ -3205,19 +3214,19 @@
         <v>84</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
       <c r="E26" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F26" s="73" t="s">
-        <v>253</v>
+      <c r="F26" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G26" s="62" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H26" s="20"/>
       <c r="I26" s="21"/>
@@ -3236,16 +3245,16 @@
         <v>76</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
       <c r="E27" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="73" t="s">
-        <v>253</v>
+      <c r="F27" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G27" s="62" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H27" s="20"/>
       <c r="I27" s="21"/>
@@ -3264,16 +3273,16 @@
         <v>237</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
       <c r="E28" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="73" t="s">
-        <v>253</v>
+      <c r="F28" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G28" s="62" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H28" s="20"/>
       <c r="I28" s="21"/>
@@ -3289,19 +3298,19 @@
         <v>90</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
       <c r="E29" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="73" t="s">
-        <v>253</v>
+      <c r="F29" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G29" s="62" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H29" s="20"/>
       <c r="I29" s="21"/>
@@ -3320,16 +3329,16 @@
         <v>76</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
       <c r="E30" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F30" s="73" t="s">
-        <v>253</v>
+      <c r="F30" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G30" s="62" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H30" s="20"/>
       <c r="I30" s="21"/>
@@ -3348,16 +3357,16 @@
         <v>93</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>245</v>
+        <v>273</v>
       </c>
       <c r="E31" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F31" s="73" t="s">
-        <v>253</v>
+      <c r="F31" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G31" s="62" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H31" s="26"/>
       <c r="I31" s="27"/>
@@ -3376,16 +3385,16 @@
         <v>93</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>245</v>
+        <v>273</v>
       </c>
       <c r="E32" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F32" s="73" t="s">
-        <v>253</v>
+      <c r="F32" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G32" s="62" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H32" s="26"/>
       <c r="I32" s="27"/>
@@ -3404,16 +3413,16 @@
         <v>93</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>245</v>
+        <v>273</v>
       </c>
       <c r="E33" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F33" s="73" t="s">
-        <v>253</v>
+      <c r="F33" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G33" s="62" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="27"/>
@@ -3432,16 +3441,16 @@
         <v>94</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>245</v>
+        <v>273</v>
       </c>
       <c r="E34" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F34" s="73" t="s">
-        <v>253</v>
+      <c r="F34" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G34" s="62" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="27"/>
@@ -3460,16 +3469,16 @@
         <v>94</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>245</v>
+        <v>273</v>
       </c>
       <c r="E35" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F35" s="73" t="s">
-        <v>253</v>
+      <c r="F35" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G35" s="62" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="27"/>
@@ -3488,16 +3497,16 @@
         <v>94</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>245</v>
+        <v>273</v>
       </c>
       <c r="E36" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F36" s="73" t="s">
-        <v>253</v>
+      <c r="F36" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G36" s="62" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="27"/>
@@ -3516,16 +3525,16 @@
         <v>93</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>245</v>
+        <v>273</v>
       </c>
       <c r="E37" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F37" s="73" t="s">
-        <v>253</v>
+      <c r="F37" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G37" s="62" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="27"/>
@@ -3538,22 +3547,22 @@
         <v>107</v>
       </c>
       <c r="B38" s="59" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>245</v>
+        <v>273</v>
       </c>
       <c r="E38" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F38" s="73" t="s">
-        <v>253</v>
+      <c r="F38" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G38" s="62" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="27"/>
@@ -3571,15 +3580,17 @@
       <c r="C39" s="24" t="s">
         <v>238</v>
       </c>
-      <c r="D39" s="20"/>
+      <c r="D39" s="20" t="s">
+        <v>274</v>
+      </c>
       <c r="E39" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F39" s="73" t="s">
-        <v>253</v>
+      <c r="F39" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G39" s="62" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="27"/>
@@ -3597,15 +3608,17 @@
       <c r="C40" s="24" t="s">
         <v>238</v>
       </c>
-      <c r="D40" s="20"/>
+      <c r="D40" s="20" t="s">
+        <v>274</v>
+      </c>
       <c r="E40" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F40" s="73" t="s">
-        <v>253</v>
+      <c r="F40" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G40" s="62" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="H40" s="26"/>
       <c r="I40" s="27"/>
@@ -3624,16 +3637,16 @@
         <v>37</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>246</v>
+        <v>275</v>
       </c>
       <c r="E41" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F41" s="73" t="s">
-        <v>253</v>
+      <c r="F41" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G41" s="62" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H41" s="26"/>
       <c r="I41" s="27"/>
@@ -3652,16 +3665,16 @@
         <v>37</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>246</v>
+        <v>275</v>
       </c>
       <c r="E42" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="73" t="s">
-        <v>253</v>
+      <c r="F42" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G42" s="62" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H42" s="26"/>
       <c r="I42" s="27"/>
@@ -3680,16 +3693,16 @@
         <v>37</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>246</v>
+        <v>275</v>
       </c>
       <c r="E43" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F43" s="73" t="s">
-        <v>253</v>
+      <c r="F43" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G43" s="62" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H43" s="26"/>
       <c r="I43" s="27"/>
@@ -3708,16 +3721,16 @@
         <v>45</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>246</v>
+        <v>275</v>
       </c>
       <c r="E44" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F44" s="73" t="s">
-        <v>253</v>
+      <c r="F44" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G44" s="62" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H44" s="26"/>
       <c r="I44" s="27"/>
@@ -3736,16 +3749,16 @@
         <v>48</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>246</v>
+        <v>275</v>
       </c>
       <c r="E45" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F45" s="73" t="s">
-        <v>253</v>
+      <c r="F45" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G45" s="62" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H45" s="26"/>
       <c r="I45" s="27"/>
@@ -3764,16 +3777,16 @@
         <v>48</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>246</v>
+        <v>275</v>
       </c>
       <c r="E46" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F46" s="73" t="s">
-        <v>253</v>
+      <c r="F46" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G46" s="62" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H46" s="26"/>
       <c r="I46" s="27"/>
@@ -3792,16 +3805,16 @@
         <v>48</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>246</v>
+        <v>275</v>
       </c>
       <c r="E47" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F47" s="73" t="s">
-        <v>253</v>
+      <c r="F47" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G47" s="62" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H47" s="26"/>
       <c r="I47" s="27"/>
@@ -3820,16 +3833,16 @@
         <v>48</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>246</v>
+        <v>275</v>
       </c>
       <c r="E48" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F48" s="73" t="s">
-        <v>253</v>
+      <c r="F48" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G48" s="62" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H48" s="26"/>
       <c r="I48" s="27"/>
@@ -3848,16 +3861,16 @@
         <v>239</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>246</v>
+        <v>275</v>
       </c>
       <c r="E49" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F49" s="73" t="s">
-        <v>253</v>
+      <c r="F49" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G49" s="62" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H49" s="26"/>
       <c r="I49" s="27"/>
@@ -3870,22 +3883,22 @@
         <v>129</v>
       </c>
       <c r="B50" s="59" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>246</v>
+        <v>275</v>
       </c>
       <c r="E50" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F50" s="73" t="s">
-        <v>253</v>
+      <c r="F50" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G50" s="62" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H50" s="26"/>
       <c r="I50" s="27"/>
@@ -3904,16 +3917,16 @@
         <v>240</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>247</v>
+        <v>276</v>
       </c>
       <c r="E51" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F51" s="73" t="s">
-        <v>253</v>
+      <c r="F51" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G51" s="62" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="H51" s="26"/>
       <c r="I51" s="27"/>
@@ -3929,19 +3942,19 @@
         <v>134</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>247</v>
+        <v>276</v>
       </c>
       <c r="E52" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F52" s="73" t="s">
-        <v>253</v>
+      <c r="F52" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G52" s="62" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="H52" s="26"/>
       <c r="I52" s="27"/>
@@ -3954,20 +3967,22 @@
         <v>133</v>
       </c>
       <c r="B53" s="59" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C53" s="24" t="s">
         <v>241</v>
       </c>
-      <c r="D53" s="20"/>
+      <c r="D53" s="20" t="s">
+        <v>274</v>
+      </c>
       <c r="E53" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F53" s="73" t="s">
-        <v>253</v>
+      <c r="F53" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G53" s="62" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="H53" s="26"/>
       <c r="I53" s="27"/>
@@ -3980,20 +3995,22 @@
         <v>133</v>
       </c>
       <c r="B54" s="59" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>267</v>
-      </c>
-      <c r="D54" s="20"/>
+        <v>260</v>
+      </c>
+      <c r="D54" s="20" t="s">
+        <v>274</v>
+      </c>
       <c r="E54" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F54" s="73" t="s">
-        <v>253</v>
+      <c r="F54" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G54" s="62" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="H54" s="26"/>
       <c r="I54" s="27"/>
@@ -4006,20 +4023,22 @@
         <v>133</v>
       </c>
       <c r="B55" s="59" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="C55" s="24" t="s">
         <v>241</v>
       </c>
-      <c r="D55" s="20"/>
+      <c r="D55" s="20" t="s">
+        <v>274</v>
+      </c>
       <c r="E55" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F55" s="73" t="s">
-        <v>253</v>
+      <c r="F55" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G55" s="62" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="H55" s="26"/>
       <c r="I55" s="27"/>
@@ -4032,20 +4051,22 @@
         <v>133</v>
       </c>
       <c r="B56" s="59" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>268</v>
-      </c>
-      <c r="D56" s="20"/>
+        <v>261</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>274</v>
+      </c>
       <c r="E56" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F56" s="73" t="s">
-        <v>253</v>
+      <c r="F56" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G56" s="62" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="H56" s="26"/>
       <c r="I56" s="27"/>
@@ -4064,16 +4085,16 @@
         <v>242</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>248</v>
+        <v>277</v>
       </c>
       <c r="E57" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F57" s="73" t="s">
-        <v>253</v>
+      <c r="F57" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="G57" s="62" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="H57" s="26"/>
       <c r="I57" s="27"/>
@@ -4085,11 +4106,11 @@
       <c r="A58" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="B58" s="70"/>
-      <c r="C58" s="71"/>
-      <c r="D58" s="71"/>
-      <c r="E58" s="71"/>
-      <c r="F58" s="72"/>
+      <c r="B58" s="71"/>
+      <c r="C58" s="72"/>
+      <c r="D58" s="72"/>
+      <c r="E58" s="72"/>
+      <c r="F58" s="73"/>
       <c r="G58" s="55"/>
       <c r="H58" s="26"/>
       <c r="I58" s="27"/>
@@ -4101,11 +4122,11 @@
       <c r="A59" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="B59" s="70"/>
-      <c r="C59" s="71"/>
-      <c r="D59" s="71"/>
-      <c r="E59" s="71"/>
-      <c r="F59" s="72"/>
+      <c r="B59" s="71"/>
+      <c r="C59" s="72"/>
+      <c r="D59" s="72"/>
+      <c r="E59" s="72"/>
+      <c r="F59" s="73"/>
       <c r="G59" s="55"/>
       <c r="H59" s="26"/>
       <c r="I59" s="27"/>
@@ -4117,11 +4138,11 @@
       <c r="A60" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="B60" s="70"/>
-      <c r="C60" s="71"/>
-      <c r="D60" s="71"/>
-      <c r="E60" s="71"/>
-      <c r="F60" s="72"/>
+      <c r="B60" s="71"/>
+      <c r="C60" s="72"/>
+      <c r="D60" s="72"/>
+      <c r="E60" s="72"/>
+      <c r="F60" s="73"/>
       <c r="G60" s="55"/>
       <c r="H60" s="26"/>
       <c r="I60" s="27"/>
@@ -4133,11 +4154,11 @@
       <c r="A61" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="B61" s="70"/>
-      <c r="C61" s="71"/>
-      <c r="D61" s="71"/>
-      <c r="E61" s="71"/>
-      <c r="F61" s="72"/>
+      <c r="B61" s="71"/>
+      <c r="C61" s="72"/>
+      <c r="D61" s="72"/>
+      <c r="E61" s="72"/>
+      <c r="F61" s="73"/>
       <c r="G61" s="55"/>
       <c r="H61" s="26"/>
       <c r="I61" s="27"/>
@@ -4149,11 +4170,11 @@
       <c r="A62" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="B62" s="70"/>
-      <c r="C62" s="71"/>
-      <c r="D62" s="71"/>
-      <c r="E62" s="71"/>
-      <c r="F62" s="72"/>
+      <c r="B62" s="71"/>
+      <c r="C62" s="72"/>
+      <c r="D62" s="72"/>
+      <c r="E62" s="72"/>
+      <c r="F62" s="73"/>
       <c r="G62" s="55"/>
       <c r="H62" s="26"/>
       <c r="I62" s="27"/>
@@ -4165,11 +4186,11 @@
       <c r="A63" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="B63" s="70"/>
-      <c r="C63" s="71"/>
-      <c r="D63" s="71"/>
-      <c r="E63" s="71"/>
-      <c r="F63" s="72"/>
+      <c r="B63" s="71"/>
+      <c r="C63" s="72"/>
+      <c r="D63" s="72"/>
+      <c r="E63" s="72"/>
+      <c r="F63" s="73"/>
       <c r="G63" s="55"/>
       <c r="H63" s="26"/>
       <c r="I63" s="27"/>
@@ -4181,11 +4202,11 @@
       <c r="A64" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="B64" s="70"/>
-      <c r="C64" s="71"/>
-      <c r="D64" s="71"/>
-      <c r="E64" s="71"/>
-      <c r="F64" s="72"/>
+      <c r="B64" s="71"/>
+      <c r="C64" s="72"/>
+      <c r="D64" s="72"/>
+      <c r="E64" s="72"/>
+      <c r="F64" s="73"/>
       <c r="G64" s="55"/>
       <c r="H64" s="26"/>
       <c r="I64" s="27"/>
@@ -4197,11 +4218,11 @@
       <c r="A65" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="B65" s="70"/>
-      <c r="C65" s="71"/>
-      <c r="D65" s="71"/>
-      <c r="E65" s="71"/>
-      <c r="F65" s="72"/>
+      <c r="B65" s="71"/>
+      <c r="C65" s="72"/>
+      <c r="D65" s="72"/>
+      <c r="E65" s="72"/>
+      <c r="F65" s="73"/>
       <c r="G65" s="55"/>
       <c r="H65" s="26"/>
       <c r="I65" s="27"/>

</xml_diff>

<commit_message>
remover login requirment no2
remover login requirment no2
</commit_message>
<xml_diff>
--- a/RTM/Traceability_Matrix learning hub ver 2.xlsx
+++ b/RTM/Traceability_Matrix learning hub ver 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed Mazrouaa\Documents\GitHub\learning-hub\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DD28E5-CF29-487E-8852-12379FFFF430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CB2172-9C88-4F16-B393-60DD12051094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Requirement_Traceability_Matrix!$A$5:$L$8</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Requirement_Traceability_Matrix!$A$1:$L$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Requirement_Traceability_Matrix!$A$1:$L$29</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Requirement_Traceability_Matrix!$1:$5</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="276">
   <si>
     <t>For detail regarding the practice of Requirements Management, please refer to the Requirements Management Practices Guide</t>
   </si>
@@ -587,9 +587,6 @@
     <t>CRS-2.1,2.2</t>
   </si>
   <si>
-    <t>011</t>
-  </si>
-  <si>
     <t>SRS_LOGIN_002</t>
   </si>
   <si>
@@ -600,9 +597,6 @@
   </si>
   <si>
     <t>013</t>
-  </si>
-  <si>
-    <t>SRS_LOGIN_004</t>
   </si>
   <si>
     <t>015</t>
@@ -2517,10 +2511,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L156"/>
+  <dimension ref="A1:L155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2621,14 +2615,14 @@
         <v>29</v>
       </c>
       <c r="D5" s="56" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E5" s="69" t="s">
         <v>38</v>
       </c>
       <c r="F5" s="70"/>
       <c r="G5" s="60" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H5" s="54" t="s">
         <v>30</v>
@@ -2657,16 +2651,16 @@
         <v>37</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E6" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F6" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G6" s="61" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H6" s="18"/>
       <c r="I6" s="19"/>
@@ -2685,16 +2679,16 @@
         <v>37</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E7" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F7" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G7" s="61" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H7" s="20"/>
       <c r="I7" s="21"/>
@@ -2713,16 +2707,16 @@
         <v>37</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E8" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F8" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G8" s="61" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H8" s="20"/>
       <c r="I8" s="21"/>
@@ -2741,16 +2735,16 @@
         <v>45</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E9" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F9" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G9" s="61" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H9" s="20"/>
       <c r="I9" s="21"/>
@@ -2769,16 +2763,16 @@
         <v>48</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E10" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F10" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G10" s="61" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="21"/>
@@ -2797,16 +2791,16 @@
         <v>48</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E11" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F11" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G11" s="61" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="21"/>
@@ -2825,16 +2819,16 @@
         <v>48</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E12" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F12" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G12" s="61" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H12" s="20"/>
       <c r="I12" s="21"/>
@@ -2853,16 +2847,16 @@
         <v>48</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E13" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F13" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G13" s="61" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="21"/>
@@ -2881,16 +2875,16 @@
         <v>57</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E14" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F14" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G14" s="62" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="21"/>
@@ -2900,25 +2894,25 @@
     </row>
     <row r="15" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="59" t="s">
         <v>58</v>
-      </c>
-      <c r="B15" s="59" t="s">
-        <v>59</v>
       </c>
       <c r="C15" s="24" t="s">
         <v>57</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E15" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F15" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G15" s="62" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H15" s="20"/>
       <c r="I15" s="21"/>
@@ -2928,25 +2922,25 @@
     </row>
     <row r="16" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="59" t="s">
         <v>60</v>
-      </c>
-      <c r="B16" s="59" t="s">
-        <v>61</v>
       </c>
       <c r="C16" s="24" t="s">
         <v>57</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E16" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F16" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G16" s="62" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H16" s="20"/>
       <c r="I16" s="21"/>
@@ -2962,19 +2956,19 @@
         <v>63</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E17" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F17" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G17" s="62" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H17" s="20"/>
       <c r="I17" s="21"/>
@@ -2984,25 +2978,25 @@
     </row>
     <row r="18" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B18" s="59" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>66</v>
+        <v>234</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E18" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F18" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G18" s="62" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H18" s="20"/>
       <c r="I18" s="21"/>
@@ -3012,25 +3006,25 @@
     </row>
     <row r="19" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="59" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>236</v>
-      </c>
       <c r="D19" s="20" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E19" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F19" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G19" s="62" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H19" s="20"/>
       <c r="I19" s="21"/>
@@ -3046,19 +3040,19 @@
         <v>71</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>69</v>
+        <v>245</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E20" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F20" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G20" s="62" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H20" s="20"/>
       <c r="I20" s="21"/>
@@ -3074,19 +3068,19 @@
         <v>73</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>247</v>
+        <v>74</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E21" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F21" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G21" s="62" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="21"/>
@@ -3096,25 +3090,25 @@
     </row>
     <row r="22" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B22" s="59" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>76</v>
+        <v>246</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E22" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F22" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G22" s="62" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="21"/>
@@ -3130,19 +3124,19 @@
         <v>78</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>248</v>
+        <v>74</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E23" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F23" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G23" s="62" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H23" s="20"/>
       <c r="I23" s="21"/>
@@ -3158,19 +3152,19 @@
         <v>80</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>76</v>
+        <v>235</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E24" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F24" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G24" s="62" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H24" s="20"/>
       <c r="I24" s="21"/>
@@ -3186,19 +3180,19 @@
         <v>82</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E25" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F25" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G25" s="62" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H25" s="20"/>
       <c r="I25" s="21"/>
@@ -3214,19 +3208,19 @@
         <v>84</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>249</v>
+        <v>74</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E26" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F26" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G26" s="62" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H26" s="20"/>
       <c r="I26" s="21"/>
@@ -3242,19 +3236,19 @@
         <v>86</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>76</v>
+        <v>235</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E27" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F27" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G27" s="62" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H27" s="20"/>
       <c r="I27" s="21"/>
@@ -3270,19 +3264,19 @@
         <v>88</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E28" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F28" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G28" s="62" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H28" s="20"/>
       <c r="I28" s="21"/>
@@ -3298,19 +3292,19 @@
         <v>90</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>250</v>
+        <v>74</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E29" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F29" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G29" s="62" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H29" s="20"/>
       <c r="I29" s="21"/>
@@ -3318,33 +3312,33 @@
       <c r="K29" s="39"/>
       <c r="L29" s="40"/>
     </row>
-    <row r="30" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A30" s="22" t="s">
+    <row r="30" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="59" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="B30" s="59" t="s">
-        <v>92</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>76</v>
-      </c>
       <c r="D30" s="20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E30" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F30" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G30" s="62" t="s">
-        <v>265</v>
-      </c>
-      <c r="H30" s="20"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="40"/>
+        <v>263</v>
+      </c>
+      <c r="H30" s="26"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="43"/>
     </row>
     <row r="31" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
@@ -3354,19 +3348,19 @@
         <v>96</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E31" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F31" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G31" s="62" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H31" s="26"/>
       <c r="I31" s="27"/>
@@ -3382,19 +3376,19 @@
         <v>98</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E32" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F32" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G32" s="62" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H32" s="26"/>
       <c r="I32" s="27"/>
@@ -3410,19 +3404,19 @@
         <v>100</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E33" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F33" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G33" s="62" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="27"/>
@@ -3438,19 +3432,19 @@
         <v>102</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E34" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F34" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G34" s="62" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="27"/>
@@ -3466,19 +3460,19 @@
         <v>104</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E35" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F35" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G35" s="62" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="27"/>
@@ -3494,19 +3488,19 @@
         <v>106</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E36" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F36" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G36" s="62" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="27"/>
@@ -3516,25 +3510,25 @@
     </row>
     <row r="37" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B37" s="59" t="s">
-        <v>108</v>
+        <v>249</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>93</v>
+        <v>250</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E37" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F37" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G37" s="62" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="27"/>
@@ -3547,22 +3541,22 @@
         <v>107</v>
       </c>
       <c r="B38" s="59" t="s">
-        <v>251</v>
+        <v>108</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E38" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F38" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G38" s="62" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="27"/>
@@ -3578,19 +3572,19 @@
         <v>110</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E39" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F39" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G39" s="62" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="27"/>
@@ -3606,19 +3600,19 @@
         <v>112</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>238</v>
+        <v>37</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E40" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F40" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G40" s="62" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H40" s="26"/>
       <c r="I40" s="27"/>
@@ -3637,16 +3631,16 @@
         <v>37</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E41" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G41" s="62" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H41" s="26"/>
       <c r="I41" s="27"/>
@@ -3665,16 +3659,16 @@
         <v>37</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E42" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F42" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G42" s="62" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H42" s="26"/>
       <c r="I42" s="27"/>
@@ -3690,19 +3684,19 @@
         <v>118</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E43" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F43" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G43" s="62" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H43" s="26"/>
       <c r="I43" s="27"/>
@@ -3718,19 +3712,19 @@
         <v>120</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E44" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F44" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G44" s="62" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H44" s="26"/>
       <c r="I44" s="27"/>
@@ -3749,16 +3743,16 @@
         <v>48</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E45" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F45" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G45" s="62" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H45" s="26"/>
       <c r="I45" s="27"/>
@@ -3777,16 +3771,16 @@
         <v>48</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E46" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F46" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G46" s="62" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H46" s="26"/>
       <c r="I46" s="27"/>
@@ -3805,16 +3799,16 @@
         <v>48</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E47" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F47" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G47" s="62" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H47" s="26"/>
       <c r="I47" s="27"/>
@@ -3830,19 +3824,19 @@
         <v>128</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>48</v>
+        <v>237</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E48" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F48" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G48" s="62" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H48" s="26"/>
       <c r="I48" s="27"/>
@@ -3852,25 +3846,25 @@
     </row>
     <row r="49" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B49" s="59" t="s">
-        <v>130</v>
+        <v>251</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E49" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F49" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G49" s="62" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H49" s="26"/>
       <c r="I49" s="27"/>
@@ -3883,22 +3877,22 @@
         <v>129</v>
       </c>
       <c r="B50" s="59" t="s">
-        <v>253</v>
+        <v>130</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E50" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F50" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G50" s="62" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H50" s="26"/>
       <c r="I50" s="27"/>
@@ -3914,19 +3908,19 @@
         <v>132</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E51" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F51" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G51" s="62" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H51" s="26"/>
       <c r="I51" s="27"/>
@@ -3936,25 +3930,25 @@
     </row>
     <row r="52" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B52" s="59" t="s">
-        <v>134</v>
+        <v>254</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E52" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F52" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G52" s="62" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H52" s="26"/>
       <c r="I52" s="27"/>
@@ -3964,25 +3958,25 @@
     </row>
     <row r="53" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B53" s="59" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>241</v>
+        <v>258</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E53" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F53" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G53" s="62" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H53" s="26"/>
       <c r="I53" s="27"/>
@@ -3992,25 +3986,25 @@
     </row>
     <row r="54" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B54" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E54" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F54" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G54" s="62" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H54" s="26"/>
       <c r="I54" s="27"/>
@@ -4020,25 +4014,25 @@
     </row>
     <row r="55" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B55" s="59" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E55" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F55" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G55" s="62" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H55" s="26"/>
       <c r="I55" s="27"/>
@@ -4051,22 +4045,22 @@
         <v>133</v>
       </c>
       <c r="B56" s="59" t="s">
-        <v>259</v>
+        <v>134</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E56" s="58" t="s">
         <v>38</v>
       </c>
       <c r="F56" s="63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G56" s="62" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="H56" s="26"/>
       <c r="I56" s="27"/>
@@ -4074,37 +4068,25 @@
       <c r="K56" s="42"/>
       <c r="L56" s="43"/>
     </row>
-    <row r="57" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="B57" s="59" t="s">
-        <v>136</v>
-      </c>
-      <c r="C57" s="24" t="s">
-        <v>242</v>
-      </c>
-      <c r="D57" s="20" t="s">
-        <v>277</v>
-      </c>
-      <c r="E57" s="58" t="s">
-        <v>38</v>
-      </c>
-      <c r="F57" s="63" t="s">
-        <v>246</v>
-      </c>
-      <c r="G57" s="62" t="s">
-        <v>264</v>
-      </c>
+      <c r="B57" s="71"/>
+      <c r="C57" s="72"/>
+      <c r="D57" s="72"/>
+      <c r="E57" s="72"/>
+      <c r="F57" s="73"/>
+      <c r="G57" s="55"/>
       <c r="H57" s="26"/>
       <c r="I57" s="27"/>
       <c r="J57" s="41"/>
       <c r="K57" s="42"/>
       <c r="L57" s="43"/>
     </row>
-    <row r="58" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B58" s="71"/>
       <c r="C58" s="72"/>
@@ -4120,7 +4102,7 @@
     </row>
     <row r="59" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B59" s="71"/>
       <c r="C59" s="72"/>
@@ -4136,7 +4118,7 @@
     </row>
     <row r="60" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B60" s="71"/>
       <c r="C60" s="72"/>
@@ -4152,7 +4134,7 @@
     </row>
     <row r="61" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B61" s="71"/>
       <c r="C61" s="72"/>
@@ -4168,7 +4150,7 @@
     </row>
     <row r="62" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B62" s="71"/>
       <c r="C62" s="72"/>
@@ -4184,7 +4166,7 @@
     </row>
     <row r="63" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B63" s="71"/>
       <c r="C63" s="72"/>
@@ -4200,7 +4182,7 @@
     </row>
     <row r="64" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B64" s="71"/>
       <c r="C64" s="72"/>
@@ -4216,23 +4198,23 @@
     </row>
     <row r="65" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="B65" s="71"/>
-      <c r="C65" s="72"/>
-      <c r="D65" s="72"/>
-      <c r="E65" s="72"/>
-      <c r="F65" s="73"/>
-      <c r="G65" s="55"/>
+        <v>143</v>
+      </c>
+      <c r="B65" s="23"/>
+      <c r="C65" s="26"/>
+      <c r="D65" s="26"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="44"/>
+      <c r="G65" s="44"/>
       <c r="H65" s="26"/>
       <c r="I65" s="27"/>
       <c r="J65" s="41"/>
       <c r="K65" s="42"/>
       <c r="L65" s="43"/>
     </row>
-    <row r="66" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A66" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B66" s="23"/>
       <c r="C66" s="26"/>
@@ -4248,7 +4230,7 @@
     </row>
     <row r="67" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A67" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B67" s="23"/>
       <c r="C67" s="26"/>
@@ -4264,7 +4246,7 @@
     </row>
     <row r="68" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A68" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B68" s="23"/>
       <c r="C68" s="26"/>
@@ -4280,7 +4262,7 @@
     </row>
     <row r="69" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A69" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B69" s="23"/>
       <c r="C69" s="26"/>
@@ -4296,7 +4278,7 @@
     </row>
     <row r="70" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A70" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B70" s="23"/>
       <c r="C70" s="26"/>
@@ -4312,7 +4294,7 @@
     </row>
     <row r="71" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A71" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B71" s="23"/>
       <c r="C71" s="26"/>
@@ -4328,7 +4310,7 @@
     </row>
     <row r="72" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A72" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B72" s="23"/>
       <c r="C72" s="26"/>
@@ -4344,7 +4326,7 @@
     </row>
     <row r="73" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A73" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B73" s="23"/>
       <c r="C73" s="26"/>
@@ -4360,7 +4342,7 @@
     </row>
     <row r="74" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A74" s="25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B74" s="23"/>
       <c r="C74" s="26"/>
@@ -4376,7 +4358,7 @@
     </row>
     <row r="75" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A75" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B75" s="23"/>
       <c r="C75" s="26"/>
@@ -4392,7 +4374,7 @@
     </row>
     <row r="76" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A76" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B76" s="23"/>
       <c r="C76" s="26"/>
@@ -4408,7 +4390,7 @@
     </row>
     <row r="77" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A77" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B77" s="23"/>
       <c r="C77" s="26"/>
@@ -4424,7 +4406,7 @@
     </row>
     <row r="78" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A78" s="25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B78" s="23"/>
       <c r="C78" s="26"/>
@@ -4440,7 +4422,7 @@
     </row>
     <row r="79" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A79" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B79" s="23"/>
       <c r="C79" s="26"/>
@@ -4456,7 +4438,7 @@
     </row>
     <row r="80" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A80" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B80" s="23"/>
       <c r="C80" s="26"/>
@@ -4472,7 +4454,7 @@
     </row>
     <row r="81" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A81" s="25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B81" s="23"/>
       <c r="C81" s="26"/>
@@ -4488,7 +4470,7 @@
     </row>
     <row r="82" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A82" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B82" s="23"/>
       <c r="C82" s="26"/>
@@ -4504,7 +4486,7 @@
     </row>
     <row r="83" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A83" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B83" s="23"/>
       <c r="C83" s="26"/>
@@ -4520,7 +4502,7 @@
     </row>
     <row r="84" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A84" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B84" s="23"/>
       <c r="C84" s="26"/>
@@ -4536,7 +4518,7 @@
     </row>
     <row r="85" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A85" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B85" s="23"/>
       <c r="C85" s="26"/>
@@ -4552,7 +4534,7 @@
     </row>
     <row r="86" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A86" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B86" s="23"/>
       <c r="C86" s="26"/>
@@ -4568,7 +4550,7 @@
     </row>
     <row r="87" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A87" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B87" s="23"/>
       <c r="C87" s="26"/>
@@ -4584,7 +4566,7 @@
     </row>
     <row r="88" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A88" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B88" s="23"/>
       <c r="C88" s="26"/>
@@ -4600,7 +4582,7 @@
     </row>
     <row r="89" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A89" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B89" s="23"/>
       <c r="C89" s="26"/>
@@ -4616,7 +4598,7 @@
     </row>
     <row r="90" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A90" s="25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B90" s="23"/>
       <c r="C90" s="26"/>
@@ -4632,7 +4614,7 @@
     </row>
     <row r="91" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A91" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B91" s="23"/>
       <c r="C91" s="26"/>
@@ -4648,7 +4630,7 @@
     </row>
     <row r="92" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A92" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B92" s="23"/>
       <c r="C92" s="26"/>
@@ -4664,7 +4646,7 @@
     </row>
     <row r="93" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A93" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B93" s="23"/>
       <c r="C93" s="26"/>
@@ -4680,7 +4662,7 @@
     </row>
     <row r="94" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A94" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B94" s="23"/>
       <c r="C94" s="26"/>
@@ -4696,7 +4678,7 @@
     </row>
     <row r="95" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A95" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B95" s="23"/>
       <c r="C95" s="26"/>
@@ -4712,7 +4694,7 @@
     </row>
     <row r="96" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A96" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B96" s="23"/>
       <c r="C96" s="26"/>
@@ -4728,7 +4710,7 @@
     </row>
     <row r="97" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A97" s="25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B97" s="23"/>
       <c r="C97" s="26"/>
@@ -4744,7 +4726,7 @@
     </row>
     <row r="98" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A98" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B98" s="23"/>
       <c r="C98" s="26"/>
@@ -4760,7 +4742,7 @@
     </row>
     <row r="99" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A99" s="25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B99" s="23"/>
       <c r="C99" s="26"/>
@@ -4776,7 +4758,7 @@
     </row>
     <row r="100" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A100" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B100" s="23"/>
       <c r="C100" s="26"/>
@@ -4792,7 +4774,7 @@
     </row>
     <row r="101" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A101" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B101" s="23"/>
       <c r="C101" s="26"/>
@@ -4808,7 +4790,7 @@
     </row>
     <row r="102" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A102" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B102" s="23"/>
       <c r="C102" s="26"/>
@@ -4824,7 +4806,7 @@
     </row>
     <row r="103" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A103" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B103" s="23"/>
       <c r="C103" s="26"/>
@@ -4840,7 +4822,7 @@
     </row>
     <row r="104" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A104" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B104" s="23"/>
       <c r="C104" s="26"/>
@@ -4856,7 +4838,7 @@
     </row>
     <row r="105" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A105" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B105" s="23"/>
       <c r="C105" s="26"/>
@@ -4872,7 +4854,7 @@
     </row>
     <row r="106" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A106" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B106" s="23"/>
       <c r="C106" s="26"/>
@@ -4888,7 +4870,7 @@
     </row>
     <row r="107" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A107" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B107" s="23"/>
       <c r="C107" s="26"/>
@@ -4904,7 +4886,7 @@
     </row>
     <row r="108" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A108" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B108" s="23"/>
       <c r="C108" s="26"/>
@@ -4920,7 +4902,7 @@
     </row>
     <row r="109" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A109" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B109" s="23"/>
       <c r="C109" s="26"/>
@@ -4936,7 +4918,7 @@
     </row>
     <row r="110" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A110" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B110" s="23"/>
       <c r="C110" s="26"/>
@@ -4952,7 +4934,7 @@
     </row>
     <row r="111" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A111" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B111" s="23"/>
       <c r="C111" s="26"/>
@@ -4968,7 +4950,7 @@
     </row>
     <row r="112" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A112" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B112" s="23"/>
       <c r="C112" s="26"/>
@@ -4984,7 +4966,7 @@
     </row>
     <row r="113" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A113" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B113" s="23"/>
       <c r="C113" s="26"/>
@@ -5000,7 +4982,7 @@
     </row>
     <row r="114" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A114" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B114" s="23"/>
       <c r="C114" s="26"/>
@@ -5016,7 +4998,7 @@
     </row>
     <row r="115" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A115" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B115" s="23"/>
       <c r="C115" s="26"/>
@@ -5032,7 +5014,7 @@
     </row>
     <row r="116" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A116" s="25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B116" s="23"/>
       <c r="C116" s="26"/>
@@ -5048,7 +5030,7 @@
     </row>
     <row r="117" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A117" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B117" s="23"/>
       <c r="C117" s="26"/>
@@ -5064,7 +5046,7 @@
     </row>
     <row r="118" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A118" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B118" s="23"/>
       <c r="C118" s="26"/>
@@ -5080,7 +5062,7 @@
     </row>
     <row r="119" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A119" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B119" s="23"/>
       <c r="C119" s="26"/>
@@ -5096,7 +5078,7 @@
     </row>
     <row r="120" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A120" s="25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B120" s="23"/>
       <c r="C120" s="26"/>
@@ -5112,7 +5094,7 @@
     </row>
     <row r="121" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A121" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B121" s="23"/>
       <c r="C121" s="26"/>
@@ -5128,7 +5110,7 @@
     </row>
     <row r="122" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A122" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B122" s="23"/>
       <c r="C122" s="26"/>
@@ -5144,7 +5126,7 @@
     </row>
     <row r="123" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A123" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B123" s="23"/>
       <c r="C123" s="26"/>
@@ -5160,7 +5142,7 @@
     </row>
     <row r="124" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A124" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B124" s="23"/>
       <c r="C124" s="26"/>
@@ -5176,7 +5158,7 @@
     </row>
     <row r="125" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A125" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B125" s="23"/>
       <c r="C125" s="26"/>
@@ -5192,7 +5174,7 @@
     </row>
     <row r="126" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A126" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B126" s="23"/>
       <c r="C126" s="26"/>
@@ -5208,7 +5190,7 @@
     </row>
     <row r="127" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A127" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B127" s="23"/>
       <c r="C127" s="26"/>
@@ -5224,7 +5206,7 @@
     </row>
     <row r="128" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A128" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B128" s="23"/>
       <c r="C128" s="26"/>
@@ -5240,7 +5222,7 @@
     </row>
     <row r="129" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A129" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B129" s="23"/>
       <c r="C129" s="26"/>
@@ -5256,7 +5238,7 @@
     </row>
     <row r="130" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A130" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B130" s="23"/>
       <c r="C130" s="26"/>
@@ -5272,7 +5254,7 @@
     </row>
     <row r="131" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A131" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B131" s="23"/>
       <c r="C131" s="26"/>
@@ -5288,7 +5270,7 @@
     </row>
     <row r="132" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A132" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B132" s="23"/>
       <c r="C132" s="26"/>
@@ -5304,7 +5286,7 @@
     </row>
     <row r="133" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A133" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B133" s="23"/>
       <c r="C133" s="26"/>
@@ -5320,7 +5302,7 @@
     </row>
     <row r="134" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A134" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B134" s="23"/>
       <c r="C134" s="26"/>
@@ -5336,7 +5318,7 @@
     </row>
     <row r="135" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A135" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B135" s="23"/>
       <c r="C135" s="26"/>
@@ -5352,7 +5334,7 @@
     </row>
     <row r="136" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A136" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B136" s="23"/>
       <c r="C136" s="26"/>
@@ -5368,7 +5350,7 @@
     </row>
     <row r="137" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A137" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B137" s="23"/>
       <c r="C137" s="26"/>
@@ -5384,7 +5366,7 @@
     </row>
     <row r="138" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A138" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B138" s="23"/>
       <c r="C138" s="26"/>
@@ -5400,7 +5382,7 @@
     </row>
     <row r="139" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A139" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B139" s="23"/>
       <c r="C139" s="26"/>
@@ -5416,7 +5398,7 @@
     </row>
     <row r="140" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A140" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B140" s="23"/>
       <c r="C140" s="26"/>
@@ -5432,7 +5414,7 @@
     </row>
     <row r="141" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A141" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B141" s="23"/>
       <c r="C141" s="26"/>
@@ -5448,7 +5430,7 @@
     </row>
     <row r="142" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A142" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B142" s="23"/>
       <c r="C142" s="26"/>
@@ -5464,7 +5446,7 @@
     </row>
     <row r="143" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A143" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B143" s="23"/>
       <c r="C143" s="26"/>
@@ -5480,7 +5462,7 @@
     </row>
     <row r="144" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A144" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B144" s="23"/>
       <c r="C144" s="26"/>
@@ -5496,7 +5478,7 @@
     </row>
     <row r="145" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A145" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B145" s="23"/>
       <c r="C145" s="26"/>
@@ -5512,7 +5494,7 @@
     </row>
     <row r="146" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A146" s="25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B146" s="23"/>
       <c r="C146" s="26"/>
@@ -5528,7 +5510,7 @@
     </row>
     <row r="147" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A147" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B147" s="23"/>
       <c r="C147" s="26"/>
@@ -5544,7 +5526,7 @@
     </row>
     <row r="148" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A148" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B148" s="23"/>
       <c r="C148" s="26"/>
@@ -5560,7 +5542,7 @@
     </row>
     <row r="149" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A149" s="25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B149" s="23"/>
       <c r="C149" s="26"/>
@@ -5576,7 +5558,7 @@
     </row>
     <row r="150" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A150" s="25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B150" s="23"/>
       <c r="C150" s="26"/>
@@ -5592,7 +5574,7 @@
     </row>
     <row r="151" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A151" s="25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B151" s="23"/>
       <c r="C151" s="26"/>
@@ -5608,7 +5590,7 @@
     </row>
     <row r="152" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A152" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B152" s="23"/>
       <c r="C152" s="26"/>
@@ -5624,7 +5606,7 @@
     </row>
     <row r="153" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A153" s="25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B153" s="23"/>
       <c r="C153" s="26"/>
@@ -5640,7 +5622,7 @@
     </row>
     <row r="154" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A154" s="25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B154" s="23"/>
       <c r="C154" s="26"/>
@@ -5656,7 +5638,7 @@
     </row>
     <row r="155" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A155" s="25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B155" s="23"/>
       <c r="C155" s="26"/>
@@ -5670,32 +5652,16 @@
       <c r="K155" s="42"/>
       <c r="L155" s="43"/>
     </row>
-    <row r="156" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A156" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="B156" s="23"/>
-      <c r="C156" s="26"/>
-      <c r="D156" s="26"/>
-      <c r="E156" s="26"/>
-      <c r="F156" s="44"/>
-      <c r="G156" s="44"/>
-      <c r="H156" s="26"/>
-      <c r="I156" s="27"/>
-      <c r="J156" s="41"/>
-      <c r="K156" s="42"/>
-      <c r="L156" s="43"/>
-    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="C3:I3"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B58:F65"/>
+    <mergeCell ref="B57:F64"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
-  <conditionalFormatting sqref="C1:I1 L1 K5:L5 C157:I65512">
+  <conditionalFormatting sqref="C1:I1 L1 K5:L5 C156:I65511">
     <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
@@ -5706,7 +5672,7 @@
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F66:G156">
+  <conditionalFormatting sqref="F65:G155">
     <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
@@ -5718,7 +5684,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F66:G156" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F65:G155" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"In Progress, Testing, Completed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5732,37 +5698,36 @@
     <hyperlink ref="F12" r:id="rId7" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{694625FA-5480-401A-B718-0589C8C7FCB1}"/>
     <hyperlink ref="F13" r:id="rId8" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{0EFC58B7-09DF-45D7-9F0D-8454B41A91CD}"/>
     <hyperlink ref="F14" r:id="rId9" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{61D9B4E2-2553-4CD5-9EAA-D95C845D5E64}"/>
-    <hyperlink ref="F15" r:id="rId10" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{015101B7-3E02-4376-9F93-EFD46BAFC1D8}"/>
-    <hyperlink ref="F16" r:id="rId11" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{4224CAE8-D477-4CC7-BBE2-9EC01B45D9FA}"/>
-    <hyperlink ref="F17" r:id="rId12" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{1641E57A-493F-4C05-834C-BDA7EFE326BC}"/>
-    <hyperlink ref="F18" r:id="rId13" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{E3AC5E34-DCAB-4B2D-91B7-DB7578DA7DA7}"/>
-    <hyperlink ref="F19" r:id="rId14" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{450A100B-9C54-462D-A844-DDBA03CEF330}"/>
-    <hyperlink ref="F20" r:id="rId15" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{0889437B-D418-49FA-A794-93D1B2A8DA5E}"/>
-    <hyperlink ref="F21" r:id="rId16" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{BEED0499-EB3F-4BC0-9EDD-B86CB5E04A15}"/>
-    <hyperlink ref="F22" r:id="rId17" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{D6FAD608-8B7D-40E7-8782-630B06F5438D}"/>
-    <hyperlink ref="F23" r:id="rId18" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A8B04DA8-15DA-424E-A339-EBF3D5430B4F}"/>
-    <hyperlink ref="F24" r:id="rId19" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{4055ADBA-18D1-49A8-AF10-C2B900AF0C71}"/>
-    <hyperlink ref="F25" r:id="rId20" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{DD5F08E8-4172-45BF-99C6-6877BD8883EF}"/>
-    <hyperlink ref="F26" r:id="rId21" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A6ED9626-4857-447E-8005-4923CC397323}"/>
-    <hyperlink ref="F27" r:id="rId22" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{060B7E8F-B19A-41D8-9F65-568E32450C69}"/>
-    <hyperlink ref="F28" r:id="rId23" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{AA2E7730-A407-494B-B217-60F04820FCD4}"/>
-    <hyperlink ref="F29" r:id="rId24" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{74162190-91F8-476D-8EED-5D782DF17E48}"/>
-    <hyperlink ref="F30" r:id="rId25" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{7498F791-7384-42D1-9284-7F13767D742A}"/>
-    <hyperlink ref="F31:F32" r:id="rId26" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{050B8A83-DABB-488A-A85F-114F7A41BF73}"/>
-    <hyperlink ref="F33:F57" r:id="rId27" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{94B9B623-DFA0-4247-B85F-18BC495D0A60}"/>
-    <hyperlink ref="F38" r:id="rId28" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{BA549CD2-BF8E-4F33-BAA0-710A9A6DB67D}"/>
-    <hyperlink ref="F50" r:id="rId29" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A15E1050-2C34-46FF-9F75-47F3E14BE3D5}"/>
-    <hyperlink ref="F53" r:id="rId30" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{516C8DDD-DD0B-4386-9826-11FC217EBBD0}"/>
-    <hyperlink ref="F54" r:id="rId31" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{78B541DE-49EF-4FCE-8337-1A697E954BB1}"/>
-    <hyperlink ref="F55" r:id="rId32" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{EEDB3697-71C1-43EC-91D5-4BBDAD2C1152}"/>
-    <hyperlink ref="F56" r:id="rId33" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{8564B7C9-3C2D-425E-9C41-C12DEFF1388B}"/>
+    <hyperlink ref="F15" r:id="rId10" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{4224CAE8-D477-4CC7-BBE2-9EC01B45D9FA}"/>
+    <hyperlink ref="F16" r:id="rId11" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{1641E57A-493F-4C05-834C-BDA7EFE326BC}"/>
+    <hyperlink ref="F17" r:id="rId12" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{E3AC5E34-DCAB-4B2D-91B7-DB7578DA7DA7}"/>
+    <hyperlink ref="F18" r:id="rId13" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{450A100B-9C54-462D-A844-DDBA03CEF330}"/>
+    <hyperlink ref="F19" r:id="rId14" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{0889437B-D418-49FA-A794-93D1B2A8DA5E}"/>
+    <hyperlink ref="F20" r:id="rId15" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{BEED0499-EB3F-4BC0-9EDD-B86CB5E04A15}"/>
+    <hyperlink ref="F21" r:id="rId16" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{D6FAD608-8B7D-40E7-8782-630B06F5438D}"/>
+    <hyperlink ref="F22" r:id="rId17" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A8B04DA8-15DA-424E-A339-EBF3D5430B4F}"/>
+    <hyperlink ref="F23" r:id="rId18" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{4055ADBA-18D1-49A8-AF10-C2B900AF0C71}"/>
+    <hyperlink ref="F24" r:id="rId19" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{DD5F08E8-4172-45BF-99C6-6877BD8883EF}"/>
+    <hyperlink ref="F25" r:id="rId20" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A6ED9626-4857-447E-8005-4923CC397323}"/>
+    <hyperlink ref="F26" r:id="rId21" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{060B7E8F-B19A-41D8-9F65-568E32450C69}"/>
+    <hyperlink ref="F27" r:id="rId22" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{AA2E7730-A407-494B-B217-60F04820FCD4}"/>
+    <hyperlink ref="F28" r:id="rId23" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{74162190-91F8-476D-8EED-5D782DF17E48}"/>
+    <hyperlink ref="F29" r:id="rId24" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{7498F791-7384-42D1-9284-7F13767D742A}"/>
+    <hyperlink ref="F30:F31" r:id="rId25" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{050B8A83-DABB-488A-A85F-114F7A41BF73}"/>
+    <hyperlink ref="F32:F56" r:id="rId26" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{94B9B623-DFA0-4247-B85F-18BC495D0A60}"/>
+    <hyperlink ref="F37" r:id="rId27" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{BA549CD2-BF8E-4F33-BAA0-710A9A6DB67D}"/>
+    <hyperlink ref="F49" r:id="rId28" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A15E1050-2C34-46FF-9F75-47F3E14BE3D5}"/>
+    <hyperlink ref="F52" r:id="rId29" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{516C8DDD-DD0B-4386-9826-11FC217EBBD0}"/>
+    <hyperlink ref="F53" r:id="rId30" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{78B541DE-49EF-4FCE-8337-1A697E954BB1}"/>
+    <hyperlink ref="F54" r:id="rId31" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{EEDB3697-71C1-43EC-91D5-4BBDAD2C1152}"/>
+    <hyperlink ref="F55" r:id="rId32" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{8564B7C9-3C2D-425E-9C41-C12DEFF1388B}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" r:id="rId34"/>
+  <pageSetup orientation="landscape" r:id="rId33"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;"Arial,Bold"&amp;8UP Template Version&amp;"Arial,Regular": 11/30/06&amp;R&amp;8Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId35"/>
+  <legacyDrawing r:id="rId34"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add 3 sequence diagrams
addarticle()
upload video()
Registeruser()
</commit_message>
<xml_diff>
--- a/RTM/Traceability_Matrix learning hub ver 2.xlsx
+++ b/RTM/Traceability_Matrix learning hub ver 2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed Mazrouaa\Documents\GitHub\learning-hub\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CB2172-9C88-4F16-B393-60DD12051094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5C72B2-C95A-45DC-81D9-64A41BD77D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Requirement_Traceability_Matrix!$A$5:$L$8</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Requirement_Traceability_Matrix!$A$1:$L$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Requirement_Traceability_Matrix!$A$1:$L$30</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Requirement_Traceability_Matrix!$1:$5</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="277">
   <si>
     <t>For detail regarding the practice of Requirements Management, please refer to the Requirements Management Practices Guide</t>
   </si>
@@ -1247,6 +1247,20 @@
   <si>
     <t>AdminSequence (9.0-9.2)
 UserSequence (8.0-8.2)</t>
+  </si>
+  <si>
+    <r>
+      <t>SRS-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> REGS -009</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2511,10 +2525,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L155"/>
+  <dimension ref="A1:L156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2866,16 +2880,16 @@
     </row>
     <row r="14" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="59" t="s">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="B14" s="57" t="s">
+        <v>276</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="E14" s="58" t="s">
         <v>38</v>
@@ -2883,8 +2897,8 @@
       <c r="F14" s="63" t="s">
         <v>244</v>
       </c>
-      <c r="G14" s="62" t="s">
-        <v>261</v>
+      <c r="G14" s="61" t="s">
+        <v>260</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="21"/>
@@ -2894,10 +2908,10 @@
     </row>
     <row r="15" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B15" s="59" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C15" s="24" t="s">
         <v>57</v>
@@ -2922,10 +2936,10 @@
     </row>
     <row r="16" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" s="59" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C16" s="24" t="s">
         <v>57</v>
@@ -2950,16 +2964,16 @@
     </row>
     <row r="17" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="59" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E17" s="58" t="s">
         <v>38</v>
@@ -2968,7 +2982,7 @@
         <v>244</v>
       </c>
       <c r="G17" s="62" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H17" s="20"/>
       <c r="I17" s="21"/>
@@ -2978,13 +2992,13 @@
     </row>
     <row r="18" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B18" s="59" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>234</v>
+        <v>64</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>269</v>
@@ -3006,13 +3020,13 @@
     </row>
     <row r="19" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B19" s="59" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>67</v>
+        <v>234</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>269</v>
@@ -3034,13 +3048,13 @@
     </row>
     <row r="20" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B20" s="59" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>245</v>
+        <v>67</v>
       </c>
       <c r="D20" s="20" t="s">
         <v>269</v>
@@ -3062,16 +3076,16 @@
     </row>
     <row r="21" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B21" s="59" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>74</v>
+        <v>245</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E21" s="58" t="s">
         <v>38</v>
@@ -3080,7 +3094,7 @@
         <v>244</v>
       </c>
       <c r="G21" s="62" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="21"/>
@@ -3090,13 +3104,13 @@
     </row>
     <row r="22" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B22" s="59" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>246</v>
+        <v>74</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>270</v>
@@ -3118,13 +3132,13 @@
     </row>
     <row r="23" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B23" s="59" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>74</v>
+        <v>246</v>
       </c>
       <c r="D23" s="20" t="s">
         <v>270</v>
@@ -3146,13 +3160,13 @@
     </row>
     <row r="24" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B24" s="59" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>235</v>
+        <v>74</v>
       </c>
       <c r="D24" s="20" t="s">
         <v>270</v>
@@ -3174,13 +3188,13 @@
     </row>
     <row r="25" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B25" s="59" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="D25" s="20" t="s">
         <v>270</v>
@@ -3202,13 +3216,13 @@
     </row>
     <row r="26" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B26" s="59" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>74</v>
+        <v>247</v>
       </c>
       <c r="D26" s="20" t="s">
         <v>270</v>
@@ -3230,13 +3244,13 @@
     </row>
     <row r="27" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B27" s="59" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>235</v>
+        <v>74</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>270</v>
@@ -3258,13 +3272,13 @@
     </row>
     <row r="28" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B28" s="59" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="D28" s="20" t="s">
         <v>270</v>
@@ -3286,13 +3300,13 @@
     </row>
     <row r="29" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B29" s="59" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>74</v>
+        <v>248</v>
       </c>
       <c r="D29" s="20" t="s">
         <v>270</v>
@@ -3312,18 +3326,18 @@
       <c r="K29" s="39"/>
       <c r="L29" s="40"/>
     </row>
-    <row r="30" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="25" t="s">
-        <v>93</v>
+    <row r="30" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A30" s="22" t="s">
+        <v>89</v>
       </c>
       <c r="B30" s="59" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E30" s="58" t="s">
         <v>38</v>
@@ -3334,18 +3348,18 @@
       <c r="G30" s="62" t="s">
         <v>263</v>
       </c>
-      <c r="H30" s="26"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="43"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="40"/>
     </row>
     <row r="31" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B31" s="59" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C31" s="24" t="s">
         <v>91</v>
@@ -3370,10 +3384,10 @@
     </row>
     <row r="32" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B32" s="59" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C32" s="24" t="s">
         <v>91</v>
@@ -3398,13 +3412,13 @@
     </row>
     <row r="33" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B33" s="59" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D33" s="20" t="s">
         <v>271</v>
@@ -3426,10 +3440,10 @@
     </row>
     <row r="34" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B34" s="59" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C34" s="24" t="s">
         <v>92</v>
@@ -3454,10 +3468,10 @@
     </row>
     <row r="35" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B35" s="59" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C35" s="24" t="s">
         <v>92</v>
@@ -3482,13 +3496,13 @@
     </row>
     <row r="36" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="25" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B36" s="59" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D36" s="20" t="s">
         <v>271</v>
@@ -3513,10 +3527,10 @@
         <v>105</v>
       </c>
       <c r="B37" s="59" t="s">
-        <v>249</v>
+        <v>106</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>250</v>
+        <v>91</v>
       </c>
       <c r="D37" s="20" t="s">
         <v>271</v>
@@ -3538,16 +3552,16 @@
     </row>
     <row r="38" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B38" s="59" t="s">
-        <v>108</v>
+        <v>249</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E38" s="58" t="s">
         <v>38</v>
@@ -3556,7 +3570,7 @@
         <v>244</v>
       </c>
       <c r="G38" s="62" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="27"/>
@@ -3566,10 +3580,10 @@
     </row>
     <row r="39" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B39" s="59" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C39" s="24" t="s">
         <v>236</v>
@@ -3594,16 +3608,16 @@
     </row>
     <row r="40" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B40" s="59" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>37</v>
+        <v>236</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E40" s="58" t="s">
         <v>38</v>
@@ -3612,7 +3626,7 @@
         <v>244</v>
       </c>
       <c r="G40" s="62" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H40" s="26"/>
       <c r="I40" s="27"/>
@@ -3622,10 +3636,10 @@
     </row>
     <row r="41" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B41" s="59" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C41" s="24" t="s">
         <v>37</v>
@@ -3650,10 +3664,10 @@
     </row>
     <row r="42" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B42" s="59" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C42" s="24" t="s">
         <v>37</v>
@@ -3678,13 +3692,13 @@
     </row>
     <row r="43" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="25" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B43" s="59" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D43" s="20" t="s">
         <v>273</v>
@@ -3706,13 +3720,13 @@
     </row>
     <row r="44" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B44" s="59" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D44" s="20" t="s">
         <v>273</v>
@@ -3734,10 +3748,10 @@
     </row>
     <row r="45" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B45" s="59" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C45" s="24" t="s">
         <v>48</v>
@@ -3762,10 +3776,10 @@
     </row>
     <row r="46" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B46" s="59" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C46" s="24" t="s">
         <v>48</v>
@@ -3790,10 +3804,10 @@
     </row>
     <row r="47" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="25" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B47" s="59" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C47" s="24" t="s">
         <v>48</v>
@@ -3818,13 +3832,13 @@
     </row>
     <row r="48" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B48" s="59" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>237</v>
+        <v>48</v>
       </c>
       <c r="D48" s="20" t="s">
         <v>273</v>
@@ -3849,10 +3863,10 @@
         <v>127</v>
       </c>
       <c r="B49" s="59" t="s">
-        <v>251</v>
+        <v>128</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="D49" s="20" t="s">
         <v>273</v>
@@ -3874,16 +3888,16 @@
     </row>
     <row r="50" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B50" s="59" t="s">
-        <v>130</v>
+        <v>251</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E50" s="58" t="s">
         <v>38</v>
@@ -3892,7 +3906,7 @@
         <v>244</v>
       </c>
       <c r="G50" s="62" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H50" s="26"/>
       <c r="I50" s="27"/>
@@ -3902,13 +3916,13 @@
     </row>
     <row r="51" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B51" s="59" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="D51" s="20" t="s">
         <v>274</v>
@@ -3933,13 +3947,13 @@
         <v>131</v>
       </c>
       <c r="B52" s="59" t="s">
-        <v>254</v>
+        <v>132</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E52" s="58" t="s">
         <v>38</v>
@@ -3948,7 +3962,7 @@
         <v>244</v>
       </c>
       <c r="G52" s="62" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H52" s="26"/>
       <c r="I52" s="27"/>
@@ -3961,10 +3975,10 @@
         <v>131</v>
       </c>
       <c r="B53" s="59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="D53" s="20" t="s">
         <v>272</v>
@@ -3989,10 +4003,10 @@
         <v>131</v>
       </c>
       <c r="B54" s="59" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>239</v>
+        <v>258</v>
       </c>
       <c r="D54" s="20" t="s">
         <v>272</v>
@@ -4017,10 +4031,10 @@
         <v>131</v>
       </c>
       <c r="B55" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="D55" s="20" t="s">
         <v>272</v>
@@ -4042,16 +4056,16 @@
     </row>
     <row r="56" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B56" s="59" t="s">
-        <v>134</v>
+        <v>257</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>240</v>
+        <v>259</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E56" s="58" t="s">
         <v>38</v>
@@ -4060,7 +4074,7 @@
         <v>244</v>
       </c>
       <c r="G56" s="62" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="H56" s="26"/>
       <c r="I56" s="27"/>
@@ -4068,25 +4082,37 @@
       <c r="K56" s="42"/>
       <c r="L56" s="43"/>
     </row>
-    <row r="57" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="B57" s="71"/>
-      <c r="C57" s="72"/>
-      <c r="D57" s="72"/>
-      <c r="E57" s="72"/>
-      <c r="F57" s="73"/>
-      <c r="G57" s="55"/>
+        <v>133</v>
+      </c>
+      <c r="B57" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="C57" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="E57" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F57" s="63" t="s">
+        <v>244</v>
+      </c>
+      <c r="G57" s="62" t="s">
+        <v>262</v>
+      </c>
       <c r="H57" s="26"/>
       <c r="I57" s="27"/>
       <c r="J57" s="41"/>
       <c r="K57" s="42"/>
       <c r="L57" s="43"/>
     </row>
-    <row r="58" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B58" s="71"/>
       <c r="C58" s="72"/>
@@ -4102,7 +4128,7 @@
     </row>
     <row r="59" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B59" s="71"/>
       <c r="C59" s="72"/>
@@ -4118,7 +4144,7 @@
     </row>
     <row r="60" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B60" s="71"/>
       <c r="C60" s="72"/>
@@ -4134,7 +4160,7 @@
     </row>
     <row r="61" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B61" s="71"/>
       <c r="C61" s="72"/>
@@ -4150,7 +4176,7 @@
     </row>
     <row r="62" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B62" s="71"/>
       <c r="C62" s="72"/>
@@ -4166,7 +4192,7 @@
     </row>
     <row r="63" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B63" s="71"/>
       <c r="C63" s="72"/>
@@ -4182,7 +4208,7 @@
     </row>
     <row r="64" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B64" s="71"/>
       <c r="C64" s="72"/>
@@ -4198,23 +4224,23 @@
     </row>
     <row r="65" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="B65" s="23"/>
-      <c r="C65" s="26"/>
-      <c r="D65" s="26"/>
-      <c r="E65" s="26"/>
-      <c r="F65" s="44"/>
-      <c r="G65" s="44"/>
+        <v>142</v>
+      </c>
+      <c r="B65" s="71"/>
+      <c r="C65" s="72"/>
+      <c r="D65" s="72"/>
+      <c r="E65" s="72"/>
+      <c r="F65" s="73"/>
+      <c r="G65" s="55"/>
       <c r="H65" s="26"/>
       <c r="I65" s="27"/>
       <c r="J65" s="41"/>
       <c r="K65" s="42"/>
       <c r="L65" s="43"/>
     </row>
-    <row r="66" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B66" s="23"/>
       <c r="C66" s="26"/>
@@ -4230,7 +4256,7 @@
     </row>
     <row r="67" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A67" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B67" s="23"/>
       <c r="C67" s="26"/>
@@ -4246,7 +4272,7 @@
     </row>
     <row r="68" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A68" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B68" s="23"/>
       <c r="C68" s="26"/>
@@ -4262,7 +4288,7 @@
     </row>
     <row r="69" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A69" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B69" s="23"/>
       <c r="C69" s="26"/>
@@ -4278,7 +4304,7 @@
     </row>
     <row r="70" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A70" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B70" s="23"/>
       <c r="C70" s="26"/>
@@ -4294,7 +4320,7 @@
     </row>
     <row r="71" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A71" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B71" s="23"/>
       <c r="C71" s="26"/>
@@ -4310,7 +4336,7 @@
     </row>
     <row r="72" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A72" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B72" s="23"/>
       <c r="C72" s="26"/>
@@ -4326,7 +4352,7 @@
     </row>
     <row r="73" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A73" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B73" s="23"/>
       <c r="C73" s="26"/>
@@ -4342,7 +4368,7 @@
     </row>
     <row r="74" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A74" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B74" s="23"/>
       <c r="C74" s="26"/>
@@ -4358,7 +4384,7 @@
     </row>
     <row r="75" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A75" s="25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B75" s="23"/>
       <c r="C75" s="26"/>
@@ -4374,7 +4400,7 @@
     </row>
     <row r="76" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A76" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B76" s="23"/>
       <c r="C76" s="26"/>
@@ -4390,7 +4416,7 @@
     </row>
     <row r="77" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A77" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B77" s="23"/>
       <c r="C77" s="26"/>
@@ -4406,7 +4432,7 @@
     </row>
     <row r="78" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A78" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B78" s="23"/>
       <c r="C78" s="26"/>
@@ -4422,7 +4448,7 @@
     </row>
     <row r="79" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A79" s="25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B79" s="23"/>
       <c r="C79" s="26"/>
@@ -4438,7 +4464,7 @@
     </row>
     <row r="80" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A80" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B80" s="23"/>
       <c r="C80" s="26"/>
@@ -4454,7 +4480,7 @@
     </row>
     <row r="81" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A81" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B81" s="23"/>
       <c r="C81" s="26"/>
@@ -4470,7 +4496,7 @@
     </row>
     <row r="82" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A82" s="25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B82" s="23"/>
       <c r="C82" s="26"/>
@@ -4486,7 +4512,7 @@
     </row>
     <row r="83" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A83" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B83" s="23"/>
       <c r="C83" s="26"/>
@@ -4502,7 +4528,7 @@
     </row>
     <row r="84" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A84" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B84" s="23"/>
       <c r="C84" s="26"/>
@@ -4518,7 +4544,7 @@
     </row>
     <row r="85" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A85" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B85" s="23"/>
       <c r="C85" s="26"/>
@@ -4534,7 +4560,7 @@
     </row>
     <row r="86" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A86" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B86" s="23"/>
       <c r="C86" s="26"/>
@@ -4550,7 +4576,7 @@
     </row>
     <row r="87" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A87" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B87" s="23"/>
       <c r="C87" s="26"/>
@@ -4566,7 +4592,7 @@
     </row>
     <row r="88" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A88" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B88" s="23"/>
       <c r="C88" s="26"/>
@@ -4582,7 +4608,7 @@
     </row>
     <row r="89" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A89" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B89" s="23"/>
       <c r="C89" s="26"/>
@@ -4598,7 +4624,7 @@
     </row>
     <row r="90" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A90" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B90" s="23"/>
       <c r="C90" s="26"/>
@@ -4614,7 +4640,7 @@
     </row>
     <row r="91" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A91" s="25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B91" s="23"/>
       <c r="C91" s="26"/>
@@ -4630,7 +4656,7 @@
     </row>
     <row r="92" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A92" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B92" s="23"/>
       <c r="C92" s="26"/>
@@ -4646,7 +4672,7 @@
     </row>
     <row r="93" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A93" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B93" s="23"/>
       <c r="C93" s="26"/>
@@ -4662,7 +4688,7 @@
     </row>
     <row r="94" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A94" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B94" s="23"/>
       <c r="C94" s="26"/>
@@ -4678,7 +4704,7 @@
     </row>
     <row r="95" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A95" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B95" s="23"/>
       <c r="C95" s="26"/>
@@ -4694,7 +4720,7 @@
     </row>
     <row r="96" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A96" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B96" s="23"/>
       <c r="C96" s="26"/>
@@ -4710,7 +4736,7 @@
     </row>
     <row r="97" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A97" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B97" s="23"/>
       <c r="C97" s="26"/>
@@ -4726,7 +4752,7 @@
     </row>
     <row r="98" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A98" s="25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B98" s="23"/>
       <c r="C98" s="26"/>
@@ -4742,7 +4768,7 @@
     </row>
     <row r="99" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A99" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B99" s="23"/>
       <c r="C99" s="26"/>
@@ -4758,7 +4784,7 @@
     </row>
     <row r="100" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A100" s="25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B100" s="23"/>
       <c r="C100" s="26"/>
@@ -4774,7 +4800,7 @@
     </row>
     <row r="101" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A101" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B101" s="23"/>
       <c r="C101" s="26"/>
@@ -4790,7 +4816,7 @@
     </row>
     <row r="102" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A102" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B102" s="23"/>
       <c r="C102" s="26"/>
@@ -4806,7 +4832,7 @@
     </row>
     <row r="103" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A103" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B103" s="23"/>
       <c r="C103" s="26"/>
@@ -4822,7 +4848,7 @@
     </row>
     <row r="104" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A104" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B104" s="23"/>
       <c r="C104" s="26"/>
@@ -4838,7 +4864,7 @@
     </row>
     <row r="105" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A105" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B105" s="23"/>
       <c r="C105" s="26"/>
@@ -4854,7 +4880,7 @@
     </row>
     <row r="106" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A106" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B106" s="23"/>
       <c r="C106" s="26"/>
@@ -4870,7 +4896,7 @@
     </row>
     <row r="107" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A107" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B107" s="23"/>
       <c r="C107" s="26"/>
@@ -4886,7 +4912,7 @@
     </row>
     <row r="108" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A108" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B108" s="23"/>
       <c r="C108" s="26"/>
@@ -4902,7 +4928,7 @@
     </row>
     <row r="109" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A109" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B109" s="23"/>
       <c r="C109" s="26"/>
@@ -4918,7 +4944,7 @@
     </row>
     <row r="110" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A110" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B110" s="23"/>
       <c r="C110" s="26"/>
@@ -4934,7 +4960,7 @@
     </row>
     <row r="111" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A111" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B111" s="23"/>
       <c r="C111" s="26"/>
@@ -4950,7 +4976,7 @@
     </row>
     <row r="112" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A112" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B112" s="23"/>
       <c r="C112" s="26"/>
@@ -4966,7 +4992,7 @@
     </row>
     <row r="113" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A113" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B113" s="23"/>
       <c r="C113" s="26"/>
@@ -4982,7 +5008,7 @@
     </row>
     <row r="114" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A114" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B114" s="23"/>
       <c r="C114" s="26"/>
@@ -4998,7 +5024,7 @@
     </row>
     <row r="115" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A115" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B115" s="23"/>
       <c r="C115" s="26"/>
@@ -5014,7 +5040,7 @@
     </row>
     <row r="116" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A116" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B116" s="23"/>
       <c r="C116" s="26"/>
@@ -5030,7 +5056,7 @@
     </row>
     <row r="117" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A117" s="25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B117" s="23"/>
       <c r="C117" s="26"/>
@@ -5046,7 +5072,7 @@
     </row>
     <row r="118" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A118" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B118" s="23"/>
       <c r="C118" s="26"/>
@@ -5062,7 +5088,7 @@
     </row>
     <row r="119" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A119" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B119" s="23"/>
       <c r="C119" s="26"/>
@@ -5078,7 +5104,7 @@
     </row>
     <row r="120" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A120" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B120" s="23"/>
       <c r="C120" s="26"/>
@@ -5094,7 +5120,7 @@
     </row>
     <row r="121" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A121" s="25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B121" s="23"/>
       <c r="C121" s="26"/>
@@ -5110,7 +5136,7 @@
     </row>
     <row r="122" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A122" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B122" s="23"/>
       <c r="C122" s="26"/>
@@ -5126,7 +5152,7 @@
     </row>
     <row r="123" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A123" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B123" s="23"/>
       <c r="C123" s="26"/>
@@ -5142,7 +5168,7 @@
     </row>
     <row r="124" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A124" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B124" s="23"/>
       <c r="C124" s="26"/>
@@ -5158,7 +5184,7 @@
     </row>
     <row r="125" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A125" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B125" s="23"/>
       <c r="C125" s="26"/>
@@ -5174,7 +5200,7 @@
     </row>
     <row r="126" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A126" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B126" s="23"/>
       <c r="C126" s="26"/>
@@ -5190,7 +5216,7 @@
     </row>
     <row r="127" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A127" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B127" s="23"/>
       <c r="C127" s="26"/>
@@ -5206,7 +5232,7 @@
     </row>
     <row r="128" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A128" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B128" s="23"/>
       <c r="C128" s="26"/>
@@ -5222,7 +5248,7 @@
     </row>
     <row r="129" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A129" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B129" s="23"/>
       <c r="C129" s="26"/>
@@ -5238,7 +5264,7 @@
     </row>
     <row r="130" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A130" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B130" s="23"/>
       <c r="C130" s="26"/>
@@ -5254,7 +5280,7 @@
     </row>
     <row r="131" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A131" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B131" s="23"/>
       <c r="C131" s="26"/>
@@ -5270,7 +5296,7 @@
     </row>
     <row r="132" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A132" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B132" s="23"/>
       <c r="C132" s="26"/>
@@ -5286,7 +5312,7 @@
     </row>
     <row r="133" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A133" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B133" s="23"/>
       <c r="C133" s="26"/>
@@ -5302,7 +5328,7 @@
     </row>
     <row r="134" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A134" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B134" s="23"/>
       <c r="C134" s="26"/>
@@ -5318,7 +5344,7 @@
     </row>
     <row r="135" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A135" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B135" s="23"/>
       <c r="C135" s="26"/>
@@ -5334,7 +5360,7 @@
     </row>
     <row r="136" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A136" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B136" s="23"/>
       <c r="C136" s="26"/>
@@ -5350,7 +5376,7 @@
     </row>
     <row r="137" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A137" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B137" s="23"/>
       <c r="C137" s="26"/>
@@ -5366,7 +5392,7 @@
     </row>
     <row r="138" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A138" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B138" s="23"/>
       <c r="C138" s="26"/>
@@ -5382,7 +5408,7 @@
     </row>
     <row r="139" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A139" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B139" s="23"/>
       <c r="C139" s="26"/>
@@ -5398,7 +5424,7 @@
     </row>
     <row r="140" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A140" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B140" s="23"/>
       <c r="C140" s="26"/>
@@ -5414,7 +5440,7 @@
     </row>
     <row r="141" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A141" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B141" s="23"/>
       <c r="C141" s="26"/>
@@ -5430,7 +5456,7 @@
     </row>
     <row r="142" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A142" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B142" s="23"/>
       <c r="C142" s="26"/>
@@ -5446,7 +5472,7 @@
     </row>
     <row r="143" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A143" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B143" s="23"/>
       <c r="C143" s="26"/>
@@ -5462,7 +5488,7 @@
     </row>
     <row r="144" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A144" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B144" s="23"/>
       <c r="C144" s="26"/>
@@ -5478,7 +5504,7 @@
     </row>
     <row r="145" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A145" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B145" s="23"/>
       <c r="C145" s="26"/>
@@ -5494,7 +5520,7 @@
     </row>
     <row r="146" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A146" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B146" s="23"/>
       <c r="C146" s="26"/>
@@ -5510,7 +5536,7 @@
     </row>
     <row r="147" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A147" s="25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B147" s="23"/>
       <c r="C147" s="26"/>
@@ -5526,7 +5552,7 @@
     </row>
     <row r="148" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A148" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B148" s="23"/>
       <c r="C148" s="26"/>
@@ -5542,7 +5568,7 @@
     </row>
     <row r="149" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A149" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B149" s="23"/>
       <c r="C149" s="26"/>
@@ -5558,7 +5584,7 @@
     </row>
     <row r="150" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A150" s="25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B150" s="23"/>
       <c r="C150" s="26"/>
@@ -5574,7 +5600,7 @@
     </row>
     <row r="151" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A151" s="25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B151" s="23"/>
       <c r="C151" s="26"/>
@@ -5590,7 +5616,7 @@
     </row>
     <row r="152" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A152" s="25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B152" s="23"/>
       <c r="C152" s="26"/>
@@ -5606,7 +5632,7 @@
     </row>
     <row r="153" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A153" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B153" s="23"/>
       <c r="C153" s="26"/>
@@ -5622,7 +5648,7 @@
     </row>
     <row r="154" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A154" s="25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B154" s="23"/>
       <c r="C154" s="26"/>
@@ -5638,7 +5664,7 @@
     </row>
     <row r="155" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A155" s="25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B155" s="23"/>
       <c r="C155" s="26"/>
@@ -5652,16 +5678,32 @@
       <c r="K155" s="42"/>
       <c r="L155" s="43"/>
     </row>
+    <row r="156" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A156" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="B156" s="23"/>
+      <c r="C156" s="26"/>
+      <c r="D156" s="26"/>
+      <c r="E156" s="26"/>
+      <c r="F156" s="44"/>
+      <c r="G156" s="44"/>
+      <c r="H156" s="26"/>
+      <c r="I156" s="27"/>
+      <c r="J156" s="41"/>
+      <c r="K156" s="42"/>
+      <c r="L156" s="43"/>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="C3:I3"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B57:F64"/>
+    <mergeCell ref="B58:F65"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
-  <conditionalFormatting sqref="C1:I1 L1 K5:L5 C156:I65511">
+  <conditionalFormatting sqref="C1:I1 L1 K5:L5 C157:I65512">
     <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
@@ -5672,7 +5714,7 @@
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F65:G155">
+  <conditionalFormatting sqref="F66:G156">
     <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
@@ -5684,7 +5726,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F65:G155" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F66:G156" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"In Progress, Testing, Completed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5697,37 +5739,38 @@
     <hyperlink ref="F11" r:id="rId6" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{C3759B12-8922-4CB0-82CE-159B2E9BAD5C}"/>
     <hyperlink ref="F12" r:id="rId7" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{694625FA-5480-401A-B718-0589C8C7FCB1}"/>
     <hyperlink ref="F13" r:id="rId8" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{0EFC58B7-09DF-45D7-9F0D-8454B41A91CD}"/>
-    <hyperlink ref="F14" r:id="rId9" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{61D9B4E2-2553-4CD5-9EAA-D95C845D5E64}"/>
-    <hyperlink ref="F15" r:id="rId10" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{4224CAE8-D477-4CC7-BBE2-9EC01B45D9FA}"/>
-    <hyperlink ref="F16" r:id="rId11" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{1641E57A-493F-4C05-834C-BDA7EFE326BC}"/>
-    <hyperlink ref="F17" r:id="rId12" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{E3AC5E34-DCAB-4B2D-91B7-DB7578DA7DA7}"/>
-    <hyperlink ref="F18" r:id="rId13" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{450A100B-9C54-462D-A844-DDBA03CEF330}"/>
-    <hyperlink ref="F19" r:id="rId14" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{0889437B-D418-49FA-A794-93D1B2A8DA5E}"/>
-    <hyperlink ref="F20" r:id="rId15" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{BEED0499-EB3F-4BC0-9EDD-B86CB5E04A15}"/>
-    <hyperlink ref="F21" r:id="rId16" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{D6FAD608-8B7D-40E7-8782-630B06F5438D}"/>
-    <hyperlink ref="F22" r:id="rId17" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A8B04DA8-15DA-424E-A339-EBF3D5430B4F}"/>
-    <hyperlink ref="F23" r:id="rId18" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{4055ADBA-18D1-49A8-AF10-C2B900AF0C71}"/>
-    <hyperlink ref="F24" r:id="rId19" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{DD5F08E8-4172-45BF-99C6-6877BD8883EF}"/>
-    <hyperlink ref="F25" r:id="rId20" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A6ED9626-4857-447E-8005-4923CC397323}"/>
-    <hyperlink ref="F26" r:id="rId21" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{060B7E8F-B19A-41D8-9F65-568E32450C69}"/>
-    <hyperlink ref="F27" r:id="rId22" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{AA2E7730-A407-494B-B217-60F04820FCD4}"/>
-    <hyperlink ref="F28" r:id="rId23" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{74162190-91F8-476D-8EED-5D782DF17E48}"/>
-    <hyperlink ref="F29" r:id="rId24" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{7498F791-7384-42D1-9284-7F13767D742A}"/>
-    <hyperlink ref="F30:F31" r:id="rId25" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{050B8A83-DABB-488A-A85F-114F7A41BF73}"/>
-    <hyperlink ref="F32:F56" r:id="rId26" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{94B9B623-DFA0-4247-B85F-18BC495D0A60}"/>
-    <hyperlink ref="F37" r:id="rId27" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{BA549CD2-BF8E-4F33-BAA0-710A9A6DB67D}"/>
-    <hyperlink ref="F49" r:id="rId28" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A15E1050-2C34-46FF-9F75-47F3E14BE3D5}"/>
-    <hyperlink ref="F52" r:id="rId29" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{516C8DDD-DD0B-4386-9826-11FC217EBBD0}"/>
-    <hyperlink ref="F53" r:id="rId30" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{78B541DE-49EF-4FCE-8337-1A697E954BB1}"/>
-    <hyperlink ref="F54" r:id="rId31" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{EEDB3697-71C1-43EC-91D5-4BBDAD2C1152}"/>
-    <hyperlink ref="F55" r:id="rId32" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{8564B7C9-3C2D-425E-9C41-C12DEFF1388B}"/>
+    <hyperlink ref="F15" r:id="rId9" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{61D9B4E2-2553-4CD5-9EAA-D95C845D5E64}"/>
+    <hyperlink ref="F16" r:id="rId10" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{4224CAE8-D477-4CC7-BBE2-9EC01B45D9FA}"/>
+    <hyperlink ref="F17" r:id="rId11" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{1641E57A-493F-4C05-834C-BDA7EFE326BC}"/>
+    <hyperlink ref="F18" r:id="rId12" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{E3AC5E34-DCAB-4B2D-91B7-DB7578DA7DA7}"/>
+    <hyperlink ref="F19" r:id="rId13" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{450A100B-9C54-462D-A844-DDBA03CEF330}"/>
+    <hyperlink ref="F20" r:id="rId14" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{0889437B-D418-49FA-A794-93D1B2A8DA5E}"/>
+    <hyperlink ref="F21" r:id="rId15" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{BEED0499-EB3F-4BC0-9EDD-B86CB5E04A15}"/>
+    <hyperlink ref="F22" r:id="rId16" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{D6FAD608-8B7D-40E7-8782-630B06F5438D}"/>
+    <hyperlink ref="F23" r:id="rId17" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A8B04DA8-15DA-424E-A339-EBF3D5430B4F}"/>
+    <hyperlink ref="F24" r:id="rId18" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{4055ADBA-18D1-49A8-AF10-C2B900AF0C71}"/>
+    <hyperlink ref="F25" r:id="rId19" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{DD5F08E8-4172-45BF-99C6-6877BD8883EF}"/>
+    <hyperlink ref="F26" r:id="rId20" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A6ED9626-4857-447E-8005-4923CC397323}"/>
+    <hyperlink ref="F27" r:id="rId21" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{060B7E8F-B19A-41D8-9F65-568E32450C69}"/>
+    <hyperlink ref="F28" r:id="rId22" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{AA2E7730-A407-494B-B217-60F04820FCD4}"/>
+    <hyperlink ref="F29" r:id="rId23" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{74162190-91F8-476D-8EED-5D782DF17E48}"/>
+    <hyperlink ref="F30" r:id="rId24" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{7498F791-7384-42D1-9284-7F13767D742A}"/>
+    <hyperlink ref="F31:F32" r:id="rId25" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{050B8A83-DABB-488A-A85F-114F7A41BF73}"/>
+    <hyperlink ref="F33:F57" r:id="rId26" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{94B9B623-DFA0-4247-B85F-18BC495D0A60}"/>
+    <hyperlink ref="F38" r:id="rId27" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{BA549CD2-BF8E-4F33-BAA0-710A9A6DB67D}"/>
+    <hyperlink ref="F50" r:id="rId28" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A15E1050-2C34-46FF-9F75-47F3E14BE3D5}"/>
+    <hyperlink ref="F53" r:id="rId29" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{516C8DDD-DD0B-4386-9826-11FC217EBBD0}"/>
+    <hyperlink ref="F54" r:id="rId30" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{78B541DE-49EF-4FCE-8337-1A697E954BB1}"/>
+    <hyperlink ref="F55" r:id="rId31" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{EEDB3697-71C1-43EC-91D5-4BBDAD2C1152}"/>
+    <hyperlink ref="F56" r:id="rId32" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{8564B7C9-3C2D-425E-9C41-C12DEFF1388B}"/>
+    <hyperlink ref="F14" r:id="rId33" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{9F0F1621-D6C1-457F-83C4-4E56356D2DC4}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" r:id="rId33"/>
+  <pageSetup orientation="landscape" r:id="rId34"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;"Arial,Bold"&amp;8UP Template Version&amp;"Arial,Regular": 11/30/06&amp;R&amp;8Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId34"/>
+  <legacyDrawing r:id="rId35"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
test cases of add (not completed)
</commit_message>
<xml_diff>
--- a/RTM/Traceability_Matrix learning hub ver 2.xlsx
+++ b/RTM/Traceability_Matrix learning hub ver 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed Mazrouaa\Documents\GitHub\learning-hub\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5C72B2-C95A-45DC-81D9-64A41BD77D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED75669F-AD11-442B-B206-835AD491427B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Requirement_Traceability_Matrix!$A$5:$L$8</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Requirement_Traceability_Matrix!$A$1:$L$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Requirement_Traceability_Matrix!$A$1:$L$31</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Requirement_Traceability_Matrix!$1:$5</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="279">
   <si>
     <t>For detail regarding the practice of Requirements Management, please refer to the Requirements Management Practices Guide</t>
   </si>
@@ -1262,6 +1262,33 @@
       <t xml:space="preserve"> REGS -009</t>
     </r>
   </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <r>
+      <t>SRS-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> REGS -010</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1270,10 +1297,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1856,59 +1890,59 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1923,14 +1957,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1939,25 +1973,25 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1987,90 +2021,90 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2525,10 +2559,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L156"/>
+  <dimension ref="A1:L157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2878,7 +2912,7 @@
       <c r="K13" s="39"/>
       <c r="L13" s="40"/>
     </row>
-    <row r="14" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>53</v>
       </c>
@@ -2906,18 +2940,18 @@
       <c r="K14" s="39"/>
       <c r="L14" s="40"/>
     </row>
-    <row r="15" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="59" t="s">
-        <v>56</v>
+        <v>277</v>
+      </c>
+      <c r="B15" s="57" t="s">
+        <v>278</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="E15" s="58" t="s">
         <v>38</v>
@@ -2925,8 +2959,8 @@
       <c r="F15" s="63" t="s">
         <v>244</v>
       </c>
-      <c r="G15" s="62" t="s">
-        <v>261</v>
+      <c r="G15" s="61" t="s">
+        <v>260</v>
       </c>
       <c r="H15" s="20"/>
       <c r="I15" s="21"/>
@@ -2936,10 +2970,10 @@
     </row>
     <row r="16" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B16" s="59" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C16" s="24" t="s">
         <v>57</v>
@@ -2964,10 +2998,10 @@
     </row>
     <row r="17" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B17" s="59" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C17" s="24" t="s">
         <v>57</v>
@@ -2992,16 +3026,16 @@
     </row>
     <row r="18" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="59" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E18" s="58" t="s">
         <v>38</v>
@@ -3010,7 +3044,7 @@
         <v>244</v>
       </c>
       <c r="G18" s="62" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H18" s="20"/>
       <c r="I18" s="21"/>
@@ -3020,13 +3054,13 @@
     </row>
     <row r="19" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B19" s="59" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>234</v>
+        <v>64</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>269</v>
@@ -3048,13 +3082,13 @@
     </row>
     <row r="20" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B20" s="59" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>67</v>
+        <v>234</v>
       </c>
       <c r="D20" s="20" t="s">
         <v>269</v>
@@ -3076,13 +3110,13 @@
     </row>
     <row r="21" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B21" s="59" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>245</v>
+        <v>67</v>
       </c>
       <c r="D21" s="20" t="s">
         <v>269</v>
@@ -3104,16 +3138,16 @@
     </row>
     <row r="22" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B22" s="59" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>74</v>
+        <v>245</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E22" s="58" t="s">
         <v>38</v>
@@ -3122,7 +3156,7 @@
         <v>244</v>
       </c>
       <c r="G22" s="62" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="21"/>
@@ -3132,13 +3166,13 @@
     </row>
     <row r="23" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B23" s="59" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>246</v>
+        <v>74</v>
       </c>
       <c r="D23" s="20" t="s">
         <v>270</v>
@@ -3160,13 +3194,13 @@
     </row>
     <row r="24" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B24" s="59" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>74</v>
+        <v>246</v>
       </c>
       <c r="D24" s="20" t="s">
         <v>270</v>
@@ -3188,13 +3222,13 @@
     </row>
     <row r="25" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B25" s="59" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>235</v>
+        <v>74</v>
       </c>
       <c r="D25" s="20" t="s">
         <v>270</v>
@@ -3216,13 +3250,13 @@
     </row>
     <row r="26" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B26" s="59" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="D26" s="20" t="s">
         <v>270</v>
@@ -3244,13 +3278,13 @@
     </row>
     <row r="27" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B27" s="59" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>74</v>
+        <v>247</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>270</v>
@@ -3272,13 +3306,13 @@
     </row>
     <row r="28" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B28" s="59" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>235</v>
+        <v>74</v>
       </c>
       <c r="D28" s="20" t="s">
         <v>270</v>
@@ -3300,13 +3334,13 @@
     </row>
     <row r="29" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B29" s="59" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="D29" s="20" t="s">
         <v>270</v>
@@ -3328,13 +3362,13 @@
     </row>
     <row r="30" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A30" s="22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B30" s="59" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>74</v>
+        <v>248</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>270</v>
@@ -3354,18 +3388,18 @@
       <c r="K30" s="39"/>
       <c r="L30" s="40"/>
     </row>
-    <row r="31" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="25" t="s">
-        <v>93</v>
+    <row r="31" spans="1:12" ht="66.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A31" s="22" t="s">
+        <v>89</v>
       </c>
       <c r="B31" s="59" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E31" s="58" t="s">
         <v>38</v>
@@ -3376,18 +3410,18 @@
       <c r="G31" s="62" t="s">
         <v>263</v>
       </c>
-      <c r="H31" s="26"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="42"/>
-      <c r="L31" s="43"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="40"/>
     </row>
     <row r="32" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B32" s="59" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C32" s="24" t="s">
         <v>91</v>
@@ -3412,10 +3446,10 @@
     </row>
     <row r="33" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="25" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B33" s="59" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C33" s="24" t="s">
         <v>91</v>
@@ -3440,13 +3474,13 @@
     </row>
     <row r="34" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B34" s="59" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D34" s="20" t="s">
         <v>271</v>
@@ -3468,10 +3502,10 @@
     </row>
     <row r="35" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B35" s="59" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C35" s="24" t="s">
         <v>92</v>
@@ -3496,10 +3530,10 @@
     </row>
     <row r="36" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B36" s="59" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C36" s="24" t="s">
         <v>92</v>
@@ -3524,13 +3558,13 @@
     </row>
     <row r="37" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="25" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B37" s="59" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D37" s="20" t="s">
         <v>271</v>
@@ -3555,10 +3589,10 @@
         <v>105</v>
       </c>
       <c r="B38" s="59" t="s">
-        <v>249</v>
+        <v>106</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>250</v>
+        <v>91</v>
       </c>
       <c r="D38" s="20" t="s">
         <v>271</v>
@@ -3580,16 +3614,16 @@
     </row>
     <row r="39" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B39" s="59" t="s">
-        <v>108</v>
+        <v>249</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E39" s="58" t="s">
         <v>38</v>
@@ -3598,7 +3632,7 @@
         <v>244</v>
       </c>
       <c r="G39" s="62" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="27"/>
@@ -3608,10 +3642,10 @@
     </row>
     <row r="40" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B40" s="59" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C40" s="24" t="s">
         <v>236</v>
@@ -3636,16 +3670,16 @@
     </row>
     <row r="41" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B41" s="59" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>37</v>
+        <v>236</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E41" s="58" t="s">
         <v>38</v>
@@ -3654,7 +3688,7 @@
         <v>244</v>
       </c>
       <c r="G41" s="62" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H41" s="26"/>
       <c r="I41" s="27"/>
@@ -3664,10 +3698,10 @@
     </row>
     <row r="42" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B42" s="59" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C42" s="24" t="s">
         <v>37</v>
@@ -3692,10 +3726,10 @@
     </row>
     <row r="43" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B43" s="59" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C43" s="24" t="s">
         <v>37</v>
@@ -3720,13 +3754,13 @@
     </row>
     <row r="44" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="25" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B44" s="59" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D44" s="20" t="s">
         <v>273</v>
@@ -3748,13 +3782,13 @@
     </row>
     <row r="45" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B45" s="59" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D45" s="20" t="s">
         <v>273</v>
@@ -3776,10 +3810,10 @@
     </row>
     <row r="46" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B46" s="59" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C46" s="24" t="s">
         <v>48</v>
@@ -3804,10 +3838,10 @@
     </row>
     <row r="47" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B47" s="59" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C47" s="24" t="s">
         <v>48</v>
@@ -3832,10 +3866,10 @@
     </row>
     <row r="48" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="25" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B48" s="59" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C48" s="24" t="s">
         <v>48</v>
@@ -3860,13 +3894,13 @@
     </row>
     <row r="49" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B49" s="59" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>237</v>
+        <v>48</v>
       </c>
       <c r="D49" s="20" t="s">
         <v>273</v>
@@ -3891,10 +3925,10 @@
         <v>127</v>
       </c>
       <c r="B50" s="59" t="s">
-        <v>251</v>
+        <v>128</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="D50" s="20" t="s">
         <v>273</v>
@@ -3916,16 +3950,16 @@
     </row>
     <row r="51" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B51" s="59" t="s">
-        <v>130</v>
+        <v>251</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E51" s="58" t="s">
         <v>38</v>
@@ -3934,7 +3968,7 @@
         <v>244</v>
       </c>
       <c r="G51" s="62" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H51" s="26"/>
       <c r="I51" s="27"/>
@@ -3944,13 +3978,13 @@
     </row>
     <row r="52" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B52" s="59" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="D52" s="20" t="s">
         <v>274</v>
@@ -3975,13 +4009,13 @@
         <v>131</v>
       </c>
       <c r="B53" s="59" t="s">
-        <v>254</v>
+        <v>132</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E53" s="58" t="s">
         <v>38</v>
@@ -3990,7 +4024,7 @@
         <v>244</v>
       </c>
       <c r="G53" s="62" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H53" s="26"/>
       <c r="I53" s="27"/>
@@ -4003,10 +4037,10 @@
         <v>131</v>
       </c>
       <c r="B54" s="59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="D54" s="20" t="s">
         <v>272</v>
@@ -4031,10 +4065,10 @@
         <v>131</v>
       </c>
       <c r="B55" s="59" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>239</v>
+        <v>258</v>
       </c>
       <c r="D55" s="20" t="s">
         <v>272</v>
@@ -4059,10 +4093,10 @@
         <v>131</v>
       </c>
       <c r="B56" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="D56" s="20" t="s">
         <v>272</v>
@@ -4084,16 +4118,16 @@
     </row>
     <row r="57" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B57" s="59" t="s">
-        <v>134</v>
+        <v>257</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>240</v>
+        <v>259</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E57" s="58" t="s">
         <v>38</v>
@@ -4102,7 +4136,7 @@
         <v>244</v>
       </c>
       <c r="G57" s="62" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="H57" s="26"/>
       <c r="I57" s="27"/>
@@ -4110,25 +4144,37 @@
       <c r="K57" s="42"/>
       <c r="L57" s="43"/>
     </row>
-    <row r="58" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="B58" s="71"/>
-      <c r="C58" s="72"/>
-      <c r="D58" s="72"/>
-      <c r="E58" s="72"/>
-      <c r="F58" s="73"/>
-      <c r="G58" s="55"/>
+        <v>133</v>
+      </c>
+      <c r="B58" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="C58" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="E58" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F58" s="63" t="s">
+        <v>244</v>
+      </c>
+      <c r="G58" s="62" t="s">
+        <v>262</v>
+      </c>
       <c r="H58" s="26"/>
       <c r="I58" s="27"/>
       <c r="J58" s="41"/>
       <c r="K58" s="42"/>
       <c r="L58" s="43"/>
     </row>
-    <row r="59" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B59" s="71"/>
       <c r="C59" s="72"/>
@@ -4144,7 +4190,7 @@
     </row>
     <row r="60" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B60" s="71"/>
       <c r="C60" s="72"/>
@@ -4160,7 +4206,7 @@
     </row>
     <row r="61" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B61" s="71"/>
       <c r="C61" s="72"/>
@@ -4176,7 +4222,7 @@
     </row>
     <row r="62" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B62" s="71"/>
       <c r="C62" s="72"/>
@@ -4192,7 +4238,7 @@
     </row>
     <row r="63" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B63" s="71"/>
       <c r="C63" s="72"/>
@@ -4208,7 +4254,7 @@
     </row>
     <row r="64" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B64" s="71"/>
       <c r="C64" s="72"/>
@@ -4224,7 +4270,7 @@
     </row>
     <row r="65" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B65" s="71"/>
       <c r="C65" s="72"/>
@@ -4240,23 +4286,23 @@
     </row>
     <row r="66" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="B66" s="23"/>
-      <c r="C66" s="26"/>
-      <c r="D66" s="26"/>
-      <c r="E66" s="26"/>
-      <c r="F66" s="44"/>
-      <c r="G66" s="44"/>
+        <v>142</v>
+      </c>
+      <c r="B66" s="71"/>
+      <c r="C66" s="72"/>
+      <c r="D66" s="72"/>
+      <c r="E66" s="72"/>
+      <c r="F66" s="73"/>
+      <c r="G66" s="55"/>
       <c r="H66" s="26"/>
       <c r="I66" s="27"/>
       <c r="J66" s="41"/>
       <c r="K66" s="42"/>
       <c r="L66" s="43"/>
     </row>
-    <row r="67" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B67" s="23"/>
       <c r="C67" s="26"/>
@@ -4272,7 +4318,7 @@
     </row>
     <row r="68" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A68" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B68" s="23"/>
       <c r="C68" s="26"/>
@@ -4288,7 +4334,7 @@
     </row>
     <row r="69" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A69" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B69" s="23"/>
       <c r="C69" s="26"/>
@@ -4304,7 +4350,7 @@
     </row>
     <row r="70" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A70" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B70" s="23"/>
       <c r="C70" s="26"/>
@@ -4320,7 +4366,7 @@
     </row>
     <row r="71" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A71" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B71" s="23"/>
       <c r="C71" s="26"/>
@@ -4336,7 +4382,7 @@
     </row>
     <row r="72" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A72" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B72" s="23"/>
       <c r="C72" s="26"/>
@@ -4352,7 +4398,7 @@
     </row>
     <row r="73" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A73" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B73" s="23"/>
       <c r="C73" s="26"/>
@@ -4368,7 +4414,7 @@
     </row>
     <row r="74" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A74" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B74" s="23"/>
       <c r="C74" s="26"/>
@@ -4384,7 +4430,7 @@
     </row>
     <row r="75" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A75" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B75" s="23"/>
       <c r="C75" s="26"/>
@@ -4400,7 +4446,7 @@
     </row>
     <row r="76" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A76" s="25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B76" s="23"/>
       <c r="C76" s="26"/>
@@ -4416,7 +4462,7 @@
     </row>
     <row r="77" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A77" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B77" s="23"/>
       <c r="C77" s="26"/>
@@ -4432,7 +4478,7 @@
     </row>
     <row r="78" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A78" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B78" s="23"/>
       <c r="C78" s="26"/>
@@ -4448,7 +4494,7 @@
     </row>
     <row r="79" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A79" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B79" s="23"/>
       <c r="C79" s="26"/>
@@ -4464,7 +4510,7 @@
     </row>
     <row r="80" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A80" s="25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B80" s="23"/>
       <c r="C80" s="26"/>
@@ -4480,7 +4526,7 @@
     </row>
     <row r="81" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A81" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B81" s="23"/>
       <c r="C81" s="26"/>
@@ -4496,7 +4542,7 @@
     </row>
     <row r="82" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A82" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B82" s="23"/>
       <c r="C82" s="26"/>
@@ -4512,7 +4558,7 @@
     </row>
     <row r="83" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A83" s="25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B83" s="23"/>
       <c r="C83" s="26"/>
@@ -4528,7 +4574,7 @@
     </row>
     <row r="84" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A84" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B84" s="23"/>
       <c r="C84" s="26"/>
@@ -4544,7 +4590,7 @@
     </row>
     <row r="85" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A85" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B85" s="23"/>
       <c r="C85" s="26"/>
@@ -4560,7 +4606,7 @@
     </row>
     <row r="86" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A86" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B86" s="23"/>
       <c r="C86" s="26"/>
@@ -4576,7 +4622,7 @@
     </row>
     <row r="87" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A87" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B87" s="23"/>
       <c r="C87" s="26"/>
@@ -4592,7 +4638,7 @@
     </row>
     <row r="88" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A88" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B88" s="23"/>
       <c r="C88" s="26"/>
@@ -4608,7 +4654,7 @@
     </row>
     <row r="89" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A89" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B89" s="23"/>
       <c r="C89" s="26"/>
@@ -4624,7 +4670,7 @@
     </row>
     <row r="90" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A90" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B90" s="23"/>
       <c r="C90" s="26"/>
@@ -4640,7 +4686,7 @@
     </row>
     <row r="91" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A91" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B91" s="23"/>
       <c r="C91" s="26"/>
@@ -4656,7 +4702,7 @@
     </row>
     <row r="92" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A92" s="25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B92" s="23"/>
       <c r="C92" s="26"/>
@@ -4672,7 +4718,7 @@
     </row>
     <row r="93" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A93" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B93" s="23"/>
       <c r="C93" s="26"/>
@@ -4688,7 +4734,7 @@
     </row>
     <row r="94" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A94" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B94" s="23"/>
       <c r="C94" s="26"/>
@@ -4704,7 +4750,7 @@
     </row>
     <row r="95" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A95" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B95" s="23"/>
       <c r="C95" s="26"/>
@@ -4720,7 +4766,7 @@
     </row>
     <row r="96" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A96" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B96" s="23"/>
       <c r="C96" s="26"/>
@@ -4736,7 +4782,7 @@
     </row>
     <row r="97" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A97" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B97" s="23"/>
       <c r="C97" s="26"/>
@@ -4752,7 +4798,7 @@
     </row>
     <row r="98" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A98" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B98" s="23"/>
       <c r="C98" s="26"/>
@@ -4768,7 +4814,7 @@
     </row>
     <row r="99" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A99" s="25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B99" s="23"/>
       <c r="C99" s="26"/>
@@ -4784,7 +4830,7 @@
     </row>
     <row r="100" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A100" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B100" s="23"/>
       <c r="C100" s="26"/>
@@ -4800,7 +4846,7 @@
     </row>
     <row r="101" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A101" s="25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B101" s="23"/>
       <c r="C101" s="26"/>
@@ -4816,7 +4862,7 @@
     </row>
     <row r="102" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A102" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B102" s="23"/>
       <c r="C102" s="26"/>
@@ -4832,7 +4878,7 @@
     </row>
     <row r="103" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A103" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B103" s="23"/>
       <c r="C103" s="26"/>
@@ -4848,7 +4894,7 @@
     </row>
     <row r="104" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A104" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B104" s="23"/>
       <c r="C104" s="26"/>
@@ -4864,7 +4910,7 @@
     </row>
     <row r="105" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A105" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B105" s="23"/>
       <c r="C105" s="26"/>
@@ -4880,7 +4926,7 @@
     </row>
     <row r="106" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A106" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B106" s="23"/>
       <c r="C106" s="26"/>
@@ -4896,7 +4942,7 @@
     </row>
     <row r="107" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A107" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B107" s="23"/>
       <c r="C107" s="26"/>
@@ -4912,7 +4958,7 @@
     </row>
     <row r="108" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A108" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B108" s="23"/>
       <c r="C108" s="26"/>
@@ -4928,7 +4974,7 @@
     </row>
     <row r="109" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A109" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B109" s="23"/>
       <c r="C109" s="26"/>
@@ -4944,7 +4990,7 @@
     </row>
     <row r="110" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A110" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B110" s="23"/>
       <c r="C110" s="26"/>
@@ -4960,7 +5006,7 @@
     </row>
     <row r="111" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A111" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B111" s="23"/>
       <c r="C111" s="26"/>
@@ -4976,7 +5022,7 @@
     </row>
     <row r="112" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A112" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B112" s="23"/>
       <c r="C112" s="26"/>
@@ -4992,7 +5038,7 @@
     </row>
     <row r="113" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A113" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B113" s="23"/>
       <c r="C113" s="26"/>
@@ -5008,7 +5054,7 @@
     </row>
     <row r="114" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A114" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B114" s="23"/>
       <c r="C114" s="26"/>
@@ -5024,7 +5070,7 @@
     </row>
     <row r="115" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A115" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B115" s="23"/>
       <c r="C115" s="26"/>
@@ -5040,7 +5086,7 @@
     </row>
     <row r="116" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A116" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B116" s="23"/>
       <c r="C116" s="26"/>
@@ -5056,7 +5102,7 @@
     </row>
     <row r="117" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A117" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B117" s="23"/>
       <c r="C117" s="26"/>
@@ -5072,7 +5118,7 @@
     </row>
     <row r="118" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A118" s="25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B118" s="23"/>
       <c r="C118" s="26"/>
@@ -5088,7 +5134,7 @@
     </row>
     <row r="119" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A119" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B119" s="23"/>
       <c r="C119" s="26"/>
@@ -5104,7 +5150,7 @@
     </row>
     <row r="120" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A120" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B120" s="23"/>
       <c r="C120" s="26"/>
@@ -5120,7 +5166,7 @@
     </row>
     <row r="121" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A121" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B121" s="23"/>
       <c r="C121" s="26"/>
@@ -5136,7 +5182,7 @@
     </row>
     <row r="122" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A122" s="25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B122" s="23"/>
       <c r="C122" s="26"/>
@@ -5152,7 +5198,7 @@
     </row>
     <row r="123" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A123" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B123" s="23"/>
       <c r="C123" s="26"/>
@@ -5168,7 +5214,7 @@
     </row>
     <row r="124" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A124" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B124" s="23"/>
       <c r="C124" s="26"/>
@@ -5184,7 +5230,7 @@
     </row>
     <row r="125" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A125" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B125" s="23"/>
       <c r="C125" s="26"/>
@@ -5200,7 +5246,7 @@
     </row>
     <row r="126" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A126" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B126" s="23"/>
       <c r="C126" s="26"/>
@@ -5216,7 +5262,7 @@
     </row>
     <row r="127" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A127" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B127" s="23"/>
       <c r="C127" s="26"/>
@@ -5232,7 +5278,7 @@
     </row>
     <row r="128" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A128" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B128" s="23"/>
       <c r="C128" s="26"/>
@@ -5248,7 +5294,7 @@
     </row>
     <row r="129" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A129" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B129" s="23"/>
       <c r="C129" s="26"/>
@@ -5264,7 +5310,7 @@
     </row>
     <row r="130" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A130" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B130" s="23"/>
       <c r="C130" s="26"/>
@@ -5280,7 +5326,7 @@
     </row>
     <row r="131" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A131" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B131" s="23"/>
       <c r="C131" s="26"/>
@@ -5296,7 +5342,7 @@
     </row>
     <row r="132" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A132" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B132" s="23"/>
       <c r="C132" s="26"/>
@@ -5312,7 +5358,7 @@
     </row>
     <row r="133" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A133" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B133" s="23"/>
       <c r="C133" s="26"/>
@@ -5328,7 +5374,7 @@
     </row>
     <row r="134" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A134" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B134" s="23"/>
       <c r="C134" s="26"/>
@@ -5344,7 +5390,7 @@
     </row>
     <row r="135" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A135" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B135" s="23"/>
       <c r="C135" s="26"/>
@@ -5360,7 +5406,7 @@
     </row>
     <row r="136" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A136" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B136" s="23"/>
       <c r="C136" s="26"/>
@@ -5376,7 +5422,7 @@
     </row>
     <row r="137" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A137" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B137" s="23"/>
       <c r="C137" s="26"/>
@@ -5392,7 +5438,7 @@
     </row>
     <row r="138" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A138" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B138" s="23"/>
       <c r="C138" s="26"/>
@@ -5408,7 +5454,7 @@
     </row>
     <row r="139" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A139" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B139" s="23"/>
       <c r="C139" s="26"/>
@@ -5424,7 +5470,7 @@
     </row>
     <row r="140" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A140" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B140" s="23"/>
       <c r="C140" s="26"/>
@@ -5440,7 +5486,7 @@
     </row>
     <row r="141" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A141" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B141" s="23"/>
       <c r="C141" s="26"/>
@@ -5456,7 +5502,7 @@
     </row>
     <row r="142" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A142" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B142" s="23"/>
       <c r="C142" s="26"/>
@@ -5472,7 +5518,7 @@
     </row>
     <row r="143" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A143" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B143" s="23"/>
       <c r="C143" s="26"/>
@@ -5488,7 +5534,7 @@
     </row>
     <row r="144" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A144" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B144" s="23"/>
       <c r="C144" s="26"/>
@@ -5504,7 +5550,7 @@
     </row>
     <row r="145" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A145" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B145" s="23"/>
       <c r="C145" s="26"/>
@@ -5520,7 +5566,7 @@
     </row>
     <row r="146" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A146" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B146" s="23"/>
       <c r="C146" s="26"/>
@@ -5536,7 +5582,7 @@
     </row>
     <row r="147" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A147" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B147" s="23"/>
       <c r="C147" s="26"/>
@@ -5552,7 +5598,7 @@
     </row>
     <row r="148" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A148" s="25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B148" s="23"/>
       <c r="C148" s="26"/>
@@ -5568,7 +5614,7 @@
     </row>
     <row r="149" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A149" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B149" s="23"/>
       <c r="C149" s="26"/>
@@ -5584,7 +5630,7 @@
     </row>
     <row r="150" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A150" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B150" s="23"/>
       <c r="C150" s="26"/>
@@ -5600,7 +5646,7 @@
     </row>
     <row r="151" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A151" s="25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B151" s="23"/>
       <c r="C151" s="26"/>
@@ -5616,7 +5662,7 @@
     </row>
     <row r="152" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A152" s="25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B152" s="23"/>
       <c r="C152" s="26"/>
@@ -5632,7 +5678,7 @@
     </row>
     <row r="153" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A153" s="25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B153" s="23"/>
       <c r="C153" s="26"/>
@@ -5648,7 +5694,7 @@
     </row>
     <row r="154" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A154" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B154" s="23"/>
       <c r="C154" s="26"/>
@@ -5664,7 +5710,7 @@
     </row>
     <row r="155" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A155" s="25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B155" s="23"/>
       <c r="C155" s="26"/>
@@ -5680,7 +5726,7 @@
     </row>
     <row r="156" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A156" s="25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B156" s="23"/>
       <c r="C156" s="26"/>
@@ -5694,16 +5740,32 @@
       <c r="K156" s="42"/>
       <c r="L156" s="43"/>
     </row>
+    <row r="157" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A157" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="B157" s="23"/>
+      <c r="C157" s="26"/>
+      <c r="D157" s="26"/>
+      <c r="E157" s="26"/>
+      <c r="F157" s="44"/>
+      <c r="G157" s="44"/>
+      <c r="H157" s="26"/>
+      <c r="I157" s="27"/>
+      <c r="J157" s="41"/>
+      <c r="K157" s="42"/>
+      <c r="L157" s="43"/>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="C3:I3"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B58:F65"/>
+    <mergeCell ref="B59:F66"/>
   </mergeCells>
-  <phoneticPr fontId="12" type="noConversion"/>
-  <conditionalFormatting sqref="C1:I1 L1 K5:L5 C157:I65512">
+  <phoneticPr fontId="13" type="noConversion"/>
+  <conditionalFormatting sqref="C1:I1 L1 K5:L5 C158:I65513">
     <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
@@ -5714,7 +5776,7 @@
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F66:G156">
+  <conditionalFormatting sqref="F67:G157">
     <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
@@ -5726,7 +5788,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F66:G156" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F67:G157" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"In Progress, Testing, Completed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5739,38 +5801,39 @@
     <hyperlink ref="F11" r:id="rId6" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{C3759B12-8922-4CB0-82CE-159B2E9BAD5C}"/>
     <hyperlink ref="F12" r:id="rId7" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{694625FA-5480-401A-B718-0589C8C7FCB1}"/>
     <hyperlink ref="F13" r:id="rId8" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{0EFC58B7-09DF-45D7-9F0D-8454B41A91CD}"/>
-    <hyperlink ref="F15" r:id="rId9" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{61D9B4E2-2553-4CD5-9EAA-D95C845D5E64}"/>
-    <hyperlink ref="F16" r:id="rId10" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{4224CAE8-D477-4CC7-BBE2-9EC01B45D9FA}"/>
-    <hyperlink ref="F17" r:id="rId11" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{1641E57A-493F-4C05-834C-BDA7EFE326BC}"/>
-    <hyperlink ref="F18" r:id="rId12" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{E3AC5E34-DCAB-4B2D-91B7-DB7578DA7DA7}"/>
-    <hyperlink ref="F19" r:id="rId13" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{450A100B-9C54-462D-A844-DDBA03CEF330}"/>
-    <hyperlink ref="F20" r:id="rId14" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{0889437B-D418-49FA-A794-93D1B2A8DA5E}"/>
-    <hyperlink ref="F21" r:id="rId15" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{BEED0499-EB3F-4BC0-9EDD-B86CB5E04A15}"/>
-    <hyperlink ref="F22" r:id="rId16" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{D6FAD608-8B7D-40E7-8782-630B06F5438D}"/>
-    <hyperlink ref="F23" r:id="rId17" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A8B04DA8-15DA-424E-A339-EBF3D5430B4F}"/>
-    <hyperlink ref="F24" r:id="rId18" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{4055ADBA-18D1-49A8-AF10-C2B900AF0C71}"/>
-    <hyperlink ref="F25" r:id="rId19" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{DD5F08E8-4172-45BF-99C6-6877BD8883EF}"/>
-    <hyperlink ref="F26" r:id="rId20" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A6ED9626-4857-447E-8005-4923CC397323}"/>
-    <hyperlink ref="F27" r:id="rId21" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{060B7E8F-B19A-41D8-9F65-568E32450C69}"/>
-    <hyperlink ref="F28" r:id="rId22" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{AA2E7730-A407-494B-B217-60F04820FCD4}"/>
-    <hyperlink ref="F29" r:id="rId23" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{74162190-91F8-476D-8EED-5D782DF17E48}"/>
-    <hyperlink ref="F30" r:id="rId24" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{7498F791-7384-42D1-9284-7F13767D742A}"/>
-    <hyperlink ref="F31:F32" r:id="rId25" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{050B8A83-DABB-488A-A85F-114F7A41BF73}"/>
-    <hyperlink ref="F33:F57" r:id="rId26" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{94B9B623-DFA0-4247-B85F-18BC495D0A60}"/>
-    <hyperlink ref="F38" r:id="rId27" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{BA549CD2-BF8E-4F33-BAA0-710A9A6DB67D}"/>
-    <hyperlink ref="F50" r:id="rId28" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A15E1050-2C34-46FF-9F75-47F3E14BE3D5}"/>
-    <hyperlink ref="F53" r:id="rId29" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{516C8DDD-DD0B-4386-9826-11FC217EBBD0}"/>
-    <hyperlink ref="F54" r:id="rId30" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{78B541DE-49EF-4FCE-8337-1A697E954BB1}"/>
-    <hyperlink ref="F55" r:id="rId31" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{EEDB3697-71C1-43EC-91D5-4BBDAD2C1152}"/>
-    <hyperlink ref="F56" r:id="rId32" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{8564B7C9-3C2D-425E-9C41-C12DEFF1388B}"/>
+    <hyperlink ref="F16" r:id="rId9" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{61D9B4E2-2553-4CD5-9EAA-D95C845D5E64}"/>
+    <hyperlink ref="F17" r:id="rId10" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{4224CAE8-D477-4CC7-BBE2-9EC01B45D9FA}"/>
+    <hyperlink ref="F18" r:id="rId11" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{1641E57A-493F-4C05-834C-BDA7EFE326BC}"/>
+    <hyperlink ref="F19" r:id="rId12" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{E3AC5E34-DCAB-4B2D-91B7-DB7578DA7DA7}"/>
+    <hyperlink ref="F20" r:id="rId13" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{450A100B-9C54-462D-A844-DDBA03CEF330}"/>
+    <hyperlink ref="F21" r:id="rId14" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{0889437B-D418-49FA-A794-93D1B2A8DA5E}"/>
+    <hyperlink ref="F22" r:id="rId15" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{BEED0499-EB3F-4BC0-9EDD-B86CB5E04A15}"/>
+    <hyperlink ref="F23" r:id="rId16" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{D6FAD608-8B7D-40E7-8782-630B06F5438D}"/>
+    <hyperlink ref="F24" r:id="rId17" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A8B04DA8-15DA-424E-A339-EBF3D5430B4F}"/>
+    <hyperlink ref="F25" r:id="rId18" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{4055ADBA-18D1-49A8-AF10-C2B900AF0C71}"/>
+    <hyperlink ref="F26" r:id="rId19" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{DD5F08E8-4172-45BF-99C6-6877BD8883EF}"/>
+    <hyperlink ref="F27" r:id="rId20" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A6ED9626-4857-447E-8005-4923CC397323}"/>
+    <hyperlink ref="F28" r:id="rId21" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{060B7E8F-B19A-41D8-9F65-568E32450C69}"/>
+    <hyperlink ref="F29" r:id="rId22" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{AA2E7730-A407-494B-B217-60F04820FCD4}"/>
+    <hyperlink ref="F30" r:id="rId23" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{74162190-91F8-476D-8EED-5D782DF17E48}"/>
+    <hyperlink ref="F31" r:id="rId24" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{7498F791-7384-42D1-9284-7F13767D742A}"/>
+    <hyperlink ref="F32:F33" r:id="rId25" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{050B8A83-DABB-488A-A85F-114F7A41BF73}"/>
+    <hyperlink ref="F34:F58" r:id="rId26" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{94B9B623-DFA0-4247-B85F-18BC495D0A60}"/>
+    <hyperlink ref="F39" r:id="rId27" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{BA549CD2-BF8E-4F33-BAA0-710A9A6DB67D}"/>
+    <hyperlink ref="F51" r:id="rId28" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{A15E1050-2C34-46FF-9F75-47F3E14BE3D5}"/>
+    <hyperlink ref="F54" r:id="rId29" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{516C8DDD-DD0B-4386-9826-11FC217EBBD0}"/>
+    <hyperlink ref="F55" r:id="rId30" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{78B541DE-49EF-4FCE-8337-1A697E954BB1}"/>
+    <hyperlink ref="F56" r:id="rId31" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{EEDB3697-71C1-43EC-91D5-4BBDAD2C1152}"/>
+    <hyperlink ref="F57" r:id="rId32" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{8564B7C9-3C2D-425E-9C41-C12DEFF1388B}"/>
     <hyperlink ref="F14" r:id="rId33" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{9F0F1621-D6C1-457F-83C4-4E56356D2DC4}"/>
+    <hyperlink ref="F15" r:id="rId34" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Design/Diagrams/DDD/ClassDiagram%20LearningHub.vpd%20v1.2.pdf_x000a_" xr:uid="{F949F62D-59DD-4DA6-8FA0-61A913D0AB09}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" r:id="rId34"/>
+  <pageSetup orientation="landscape" r:id="rId35"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;"Arial,Bold"&amp;8UP Template Version&amp;"Arial,Regular": 11/30/06&amp;R&amp;8Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId35"/>
+  <legacyDrawing r:id="rId36"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update according to design document
</commit_message>
<xml_diff>
--- a/RTM/Traceability_Matrix learning hub ver 2.xlsx
+++ b/RTM/Traceability_Matrix learning hub ver 2.xlsx
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="294">
   <si>
     <t>For detail regarding the practice of Requirements Management, please refer to the Requirements Management Practices Guide</t>
   </si>
@@ -2085,7 +2085,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2255,53 +2255,8 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2364,9 +2319,6 @@
     <xf numFmtId="49" fontId="8" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2399,6 +2351,51 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="48" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2751,10 +2748,10 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="60"/>
+      <c r="B4" s="94"/>
     </row>
     <row r="5" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="46" t="s">
@@ -2856,8 +2853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D35" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2865,10 +2862,10 @@
     <col min="1" max="1" width="9.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="29.5703125" style="4" customWidth="1"/>
     <col min="3" max="3" width="35.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="55" style="5" customWidth="1"/>
+    <col min="4" max="4" width="55.7109375" style="5" customWidth="1"/>
     <col min="5" max="5" width="29.140625" style="5" customWidth="1"/>
     <col min="6" max="6" width="47.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="47.28515625" style="87" customWidth="1"/>
+    <col min="7" max="7" width="47.28515625" style="72" customWidth="1"/>
     <col min="8" max="8" width="51" style="5" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" style="5" customWidth="1"/>
     <col min="10" max="10" width="17.28515625" style="5" customWidth="1"/>
@@ -2886,7 +2883,7 @@
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
-      <c r="G1" s="83"/>
+      <c r="G1" s="68"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
       <c r="J1" s="10"/>
@@ -2901,16 +2898,16 @@
         <v>21</v>
       </c>
       <c r="B2" s="11"/>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="72"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="97"/>
       <c r="K2" s="28"/>
       <c r="L2" s="28"/>
       <c r="M2" s="29"/>
@@ -2920,16 +2917,16 @@
         <v>23</v>
       </c>
       <c r="B3" s="12"/>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="72"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="97"/>
       <c r="K3" s="28"/>
       <c r="L3" s="28"/>
       <c r="M3" s="29"/>
@@ -2939,16 +2936,16 @@
         <v>25</v>
       </c>
       <c r="B4" s="14"/>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="69"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="101"/>
       <c r="K4" s="28"/>
       <c r="L4" s="28"/>
       <c r="M4" s="30"/>
@@ -2972,10 +2969,10 @@
       <c r="F5" s="57" t="s">
         <v>247</v>
       </c>
-      <c r="G5" s="75" t="s">
+      <c r="G5" s="60" t="s">
         <v>250</v>
       </c>
-      <c r="H5" s="73" t="s">
+      <c r="H5" s="59" t="s">
         <v>219</v>
       </c>
       <c r="I5" s="52" t="s">
@@ -3007,16 +3004,16 @@
       <c r="D6" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="E6" s="77" t="s">
+      <c r="E6" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F6" s="77" t="s">
+      <c r="F6" s="62" t="s">
         <v>248</v>
       </c>
-      <c r="G6" s="84" t="s">
+      <c r="G6" s="69" t="s">
         <v>251</v>
       </c>
-      <c r="H6" s="80" t="s">
+      <c r="H6" s="65" t="s">
         <v>236</v>
       </c>
       <c r="I6" s="18"/>
@@ -3038,16 +3035,16 @@
       <c r="D7" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="E7" s="77" t="s">
+      <c r="E7" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F7" s="76" t="s">
+      <c r="F7" s="61" t="s">
         <v>248</v>
       </c>
-      <c r="G7" s="84" t="s">
+      <c r="G7" s="69" t="s">
         <v>251</v>
       </c>
-      <c r="H7" s="80" t="s">
+      <c r="H7" s="65" t="s">
         <v>236</v>
       </c>
       <c r="I7" s="20"/>
@@ -3069,16 +3066,16 @@
       <c r="D8" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="E8" s="77" t="s">
+      <c r="E8" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F8" s="76" t="s">
+      <c r="F8" s="61" t="s">
         <v>248</v>
       </c>
-      <c r="G8" s="84" t="s">
+      <c r="G8" s="69" t="s">
         <v>251</v>
       </c>
-      <c r="H8" s="80" t="s">
+      <c r="H8" s="65" t="s">
         <v>236</v>
       </c>
       <c r="I8" s="20"/>
@@ -3100,14 +3097,14 @@
       <c r="D9" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="E9" s="77" t="s">
+      <c r="E9" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F9" s="76" t="s">
+      <c r="F9" s="61" t="s">
         <v>248</v>
       </c>
       <c r="G9" s="20"/>
-      <c r="H9" s="80" t="s">
+      <c r="H9" s="65" t="s">
         <v>236</v>
       </c>
       <c r="I9" s="20"/>
@@ -3129,16 +3126,16 @@
       <c r="D10" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="E10" s="77" t="s">
+      <c r="E10" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F10" s="76" t="s">
+      <c r="F10" s="61" t="s">
         <v>248</v>
       </c>
-      <c r="G10" s="84" t="s">
+      <c r="G10" s="69" t="s">
         <v>252</v>
       </c>
-      <c r="H10" s="80" t="s">
+      <c r="H10" s="65" t="s">
         <v>236</v>
       </c>
       <c r="I10" s="20"/>
@@ -3160,16 +3157,16 @@
       <c r="D11" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="E11" s="77" t="s">
+      <c r="E11" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F11" s="76" t="s">
+      <c r="F11" s="61" t="s">
         <v>248</v>
       </c>
-      <c r="G11" s="84" t="s">
+      <c r="G11" s="69" t="s">
         <v>252</v>
       </c>
-      <c r="H11" s="80" t="s">
+      <c r="H11" s="65" t="s">
         <v>236</v>
       </c>
       <c r="I11" s="20"/>
@@ -3191,16 +3188,16 @@
       <c r="D12" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="E12" s="77" t="s">
+      <c r="E12" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F12" s="76" t="s">
+      <c r="F12" s="61" t="s">
         <v>248</v>
       </c>
-      <c r="G12" s="84" t="s">
+      <c r="G12" s="69" t="s">
         <v>252</v>
       </c>
-      <c r="H12" s="80" t="s">
+      <c r="H12" s="65" t="s">
         <v>236</v>
       </c>
       <c r="I12" s="20"/>
@@ -3222,16 +3219,16 @@
       <c r="D13" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="E13" s="77" t="s">
+      <c r="E13" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F13" s="76" t="s">
+      <c r="F13" s="61" t="s">
         <v>248</v>
       </c>
-      <c r="G13" s="84" t="s">
+      <c r="G13" s="69" t="s">
         <v>254</v>
       </c>
-      <c r="H13" s="80" t="s">
+      <c r="H13" s="65" t="s">
         <v>236</v>
       </c>
       <c r="I13" s="20"/>
@@ -3253,14 +3250,14 @@
       <c r="D14" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="E14" s="77" t="s">
+      <c r="E14" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F14" s="76" t="s">
+      <c r="F14" s="61" t="s">
         <v>248</v>
       </c>
       <c r="G14" s="20"/>
-      <c r="H14" s="80" t="s">
+      <c r="H14" s="65" t="s">
         <v>236</v>
       </c>
       <c r="I14" s="20"/>
@@ -3279,17 +3276,17 @@
       <c r="C15" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="90" t="s">
+      <c r="D15" s="75" t="s">
         <v>256</v>
       </c>
-      <c r="E15" s="77" t="s">
+      <c r="E15" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F15" s="88" t="s">
+      <c r="F15" s="73" t="s">
         <v>255</v>
       </c>
-      <c r="G15" s="91"/>
-      <c r="H15" s="81" t="s">
+      <c r="G15" s="76"/>
+      <c r="H15" s="66" t="s">
         <v>237</v>
       </c>
       <c r="I15" s="20"/>
@@ -3308,17 +3305,17 @@
       <c r="C16" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="90" t="s">
+      <c r="D16" s="75" t="s">
         <v>256</v>
       </c>
-      <c r="E16" s="77" t="s">
+      <c r="E16" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F16" s="88" t="s">
+      <c r="F16" s="73" t="s">
         <v>255</v>
       </c>
       <c r="G16" s="56"/>
-      <c r="H16" s="81" t="s">
+      <c r="H16" s="66" t="s">
         <v>237</v>
       </c>
       <c r="I16" s="20"/>
@@ -3337,17 +3334,17 @@
       <c r="C17" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="90" t="s">
+      <c r="D17" s="75" t="s">
         <v>256</v>
       </c>
-      <c r="E17" s="77" t="s">
+      <c r="E17" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F17" s="88" t="s">
+      <c r="F17" s="73" t="s">
         <v>255</v>
       </c>
       <c r="G17" s="56"/>
-      <c r="H17" s="81" t="s">
+      <c r="H17" s="66" t="s">
         <v>237</v>
       </c>
       <c r="I17" s="20"/>
@@ -3367,12 +3364,12 @@
         <v>63</v>
       </c>
       <c r="D18" s="20"/>
-      <c r="E18" s="77" t="s">
+      <c r="E18" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F18" s="78"/>
+      <c r="F18" s="63"/>
       <c r="G18" s="56"/>
-      <c r="H18" s="81" t="s">
+      <c r="H18" s="66" t="s">
         <v>238</v>
       </c>
       <c r="I18" s="20"/>
@@ -3392,12 +3389,12 @@
         <v>212</v>
       </c>
       <c r="D19" s="20"/>
-      <c r="E19" s="77" t="s">
+      <c r="E19" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F19" s="78"/>
+      <c r="F19" s="63"/>
       <c r="G19" s="56"/>
-      <c r="H19" s="81" t="s">
+      <c r="H19" s="66" t="s">
         <v>238</v>
       </c>
       <c r="I19" s="20"/>
@@ -3417,12 +3414,12 @@
         <v>66</v>
       </c>
       <c r="D20" s="20"/>
-      <c r="E20" s="77" t="s">
+      <c r="E20" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F20" s="78"/>
+      <c r="F20" s="63"/>
       <c r="G20" s="56"/>
-      <c r="H20" s="81" t="s">
+      <c r="H20" s="66" t="s">
         <v>238</v>
       </c>
       <c r="I20" s="20"/>
@@ -3442,12 +3439,12 @@
         <v>221</v>
       </c>
       <c r="D21" s="20"/>
-      <c r="E21" s="77" t="s">
+      <c r="E21" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F21" s="78"/>
+      <c r="F21" s="63"/>
       <c r="G21" s="56"/>
-      <c r="H21" s="81" t="s">
+      <c r="H21" s="66" t="s">
         <v>238</v>
       </c>
       <c r="I21" s="20"/>
@@ -3466,19 +3463,19 @@
       <c r="C22" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="90" t="s">
+      <c r="D22" s="75" t="s">
         <v>257</v>
       </c>
-      <c r="E22" s="77" t="s">
+      <c r="E22" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F22" s="88" t="s">
+      <c r="F22" s="73" t="s">
         <v>258</v>
       </c>
-      <c r="G22" s="88" t="s">
+      <c r="G22" s="73" t="s">
         <v>259</v>
       </c>
-      <c r="H22" s="81" t="s">
+      <c r="H22" s="66" t="s">
         <v>239</v>
       </c>
       <c r="I22" s="20"/>
@@ -3497,19 +3494,19 @@
       <c r="C23" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="D23" s="90" t="s">
+      <c r="D23" s="75" t="s">
         <v>257</v>
       </c>
-      <c r="E23" s="77" t="s">
+      <c r="E23" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F23" s="88" t="s">
+      <c r="F23" s="73" t="s">
         <v>258</v>
       </c>
-      <c r="G23" s="88" t="s">
+      <c r="G23" s="73" t="s">
         <v>259</v>
       </c>
-      <c r="H23" s="81" t="s">
+      <c r="H23" s="66" t="s">
         <v>239</v>
       </c>
       <c r="I23" s="20"/>
@@ -3528,17 +3525,19 @@
       <c r="C24" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="90" t="s">
+      <c r="D24" s="75" t="s">
         <v>269</v>
       </c>
-      <c r="E24" s="77" t="s">
+      <c r="E24" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F24" s="88" t="s">
+      <c r="F24" s="73" t="s">
         <v>258</v>
       </c>
-      <c r="G24" s="56"/>
-      <c r="H24" s="81" t="s">
+      <c r="G24" s="73" t="s">
+        <v>259</v>
+      </c>
+      <c r="H24" s="66" t="s">
         <v>239</v>
       </c>
       <c r="I24" s="20"/>
@@ -3557,17 +3556,19 @@
       <c r="C25" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="D25" s="90" t="s">
+      <c r="D25" s="75" t="s">
         <v>269</v>
       </c>
-      <c r="E25" s="77" t="s">
+      <c r="E25" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F25" s="88" t="s">
+      <c r="F25" s="73" t="s">
         <v>258</v>
       </c>
-      <c r="G25" s="56"/>
-      <c r="H25" s="81" t="s">
+      <c r="G25" s="73" t="s">
+        <v>259</v>
+      </c>
+      <c r="H25" s="66" t="s">
         <v>239</v>
       </c>
       <c r="I25" s="20"/>
@@ -3586,17 +3587,19 @@
       <c r="C26" s="23" t="s">
         <v>223</v>
       </c>
-      <c r="D26" s="90" t="s">
+      <c r="D26" s="75" t="s">
         <v>269</v>
       </c>
-      <c r="E26" s="77" t="s">
+      <c r="E26" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F26" s="88" t="s">
+      <c r="F26" s="73" t="s">
         <v>258</v>
       </c>
-      <c r="G26" s="56"/>
-      <c r="H26" s="81" t="s">
+      <c r="G26" s="73" t="s">
+        <v>259</v>
+      </c>
+      <c r="H26" s="66" t="s">
         <v>239</v>
       </c>
       <c r="I26" s="20"/>
@@ -3615,17 +3618,19 @@
       <c r="C27" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="90" t="s">
+      <c r="D27" s="75" t="s">
         <v>269</v>
       </c>
-      <c r="E27" s="77" t="s">
+      <c r="E27" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F27" s="88" t="s">
+      <c r="F27" s="73" t="s">
         <v>258</v>
       </c>
-      <c r="G27" s="56"/>
-      <c r="H27" s="81" t="s">
+      <c r="G27" s="73" t="s">
+        <v>259</v>
+      </c>
+      <c r="H27" s="66" t="s">
         <v>239</v>
       </c>
       <c r="I27" s="20"/>
@@ -3644,17 +3649,19 @@
       <c r="C28" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="D28" s="90" t="s">
+      <c r="D28" s="75" t="s">
         <v>269</v>
       </c>
-      <c r="E28" s="77" t="s">
+      <c r="E28" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F28" s="88" t="s">
+      <c r="F28" s="73" t="s">
         <v>258</v>
       </c>
-      <c r="G28" s="56"/>
-      <c r="H28" s="81" t="s">
+      <c r="G28" s="73" t="s">
+        <v>259</v>
+      </c>
+      <c r="H28" s="66" t="s">
         <v>239</v>
       </c>
       <c r="I28" s="20"/>
@@ -3673,17 +3680,19 @@
       <c r="C29" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="D29" s="90" t="s">
+      <c r="D29" s="75" t="s">
         <v>269</v>
       </c>
-      <c r="E29" s="77" t="s">
+      <c r="E29" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F29" s="88" t="s">
+      <c r="F29" s="73" t="s">
         <v>258</v>
       </c>
-      <c r="G29" s="56"/>
-      <c r="H29" s="81" t="s">
+      <c r="G29" s="73" t="s">
+        <v>259</v>
+      </c>
+      <c r="H29" s="66" t="s">
         <v>239</v>
       </c>
       <c r="I29" s="20"/>
@@ -3692,94 +3701,108 @@
       <c r="L29" s="38"/>
       <c r="M29" s="39"/>
     </row>
-    <row r="30" spans="1:13" s="102" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="93" t="s">
+    <row r="30" spans="1:13" s="86" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A30" s="78" t="s">
         <v>82</v>
       </c>
-      <c r="B30" s="94" t="s">
+      <c r="B30" s="79" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="95" t="s">
+      <c r="C30" s="80" t="s">
         <v>73</v>
       </c>
-      <c r="D30" s="89"/>
-      <c r="E30" s="88" t="s">
+      <c r="D30" s="74"/>
+      <c r="E30" s="73" t="s">
         <v>253</v>
       </c>
-      <c r="F30" s="88" t="s">
+      <c r="F30" s="73" t="s">
         <v>258</v>
       </c>
-      <c r="G30" s="96"/>
-      <c r="H30" s="97" t="s">
+      <c r="G30" s="73" t="s">
+        <v>259</v>
+      </c>
+      <c r="H30" s="81" t="s">
         <v>239</v>
       </c>
-      <c r="I30" s="89"/>
-      <c r="J30" s="98"/>
-      <c r="K30" s="99"/>
-      <c r="L30" s="100"/>
-      <c r="M30" s="101"/>
-    </row>
-    <row r="31" spans="1:13" s="102" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="93" t="s">
+      <c r="I30" s="74"/>
+      <c r="J30" s="82"/>
+      <c r="K30" s="83"/>
+      <c r="L30" s="84"/>
+      <c r="M30" s="85"/>
+    </row>
+    <row r="31" spans="1:13" s="86" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A31" s="78" t="s">
         <v>84</v>
       </c>
-      <c r="B31" s="94" t="s">
+      <c r="B31" s="79" t="s">
         <v>260</v>
       </c>
-      <c r="C31" s="103" t="s">
+      <c r="C31" s="87" t="s">
         <v>262</v>
       </c>
-      <c r="D31" s="89"/>
-      <c r="E31" s="88"/>
-      <c r="F31" s="88"/>
-      <c r="G31" s="96"/>
-      <c r="H31" s="97"/>
-      <c r="I31" s="104"/>
-      <c r="J31" s="105"/>
-      <c r="K31" s="106"/>
-      <c r="L31" s="107"/>
-      <c r="M31" s="108"/>
-    </row>
-    <row r="32" spans="1:13" s="102" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A32" s="93" t="s">
+      <c r="D31" s="74"/>
+      <c r="E31" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="F31" s="73" t="s">
+        <v>258</v>
+      </c>
+      <c r="G31" s="73" t="s">
+        <v>259</v>
+      </c>
+      <c r="H31" s="81"/>
+      <c r="I31" s="88"/>
+      <c r="J31" s="89"/>
+      <c r="K31" s="90"/>
+      <c r="L31" s="91"/>
+      <c r="M31" s="92"/>
+    </row>
+    <row r="32" spans="1:13" s="86" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A32" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="B32" s="94" t="s">
+      <c r="B32" s="79" t="s">
         <v>261</v>
       </c>
-      <c r="C32" s="103" t="s">
+      <c r="C32" s="87" t="s">
         <v>262</v>
       </c>
-      <c r="D32" s="89"/>
-      <c r="E32" s="88"/>
-      <c r="F32" s="88"/>
-      <c r="G32" s="96"/>
-      <c r="H32" s="97"/>
-      <c r="I32" s="104"/>
-      <c r="J32" s="105"/>
-      <c r="K32" s="106"/>
-      <c r="L32" s="107"/>
-      <c r="M32" s="108"/>
-    </row>
-    <row r="33" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="74"/>
+      <c r="E32" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="F32" s="73" t="s">
+        <v>258</v>
+      </c>
+      <c r="G32" s="73" t="s">
+        <v>259</v>
+      </c>
+      <c r="H32" s="81"/>
+      <c r="I32" s="88"/>
+      <c r="J32" s="89"/>
+      <c r="K32" s="90"/>
+      <c r="L32" s="91"/>
+      <c r="M32" s="92"/>
+    </row>
+    <row r="33" spans="1:13" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B33" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="92" t="s">
+      <c r="C33" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="D33" s="90" t="s">
+      <c r="D33" s="75" t="s">
         <v>268</v>
       </c>
-      <c r="E33" s="77" t="s">
+      <c r="E33" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F33" s="78"/>
+      <c r="F33" s="63"/>
       <c r="G33" s="56"/>
-      <c r="H33" s="81" t="s">
+      <c r="H33" s="66" t="s">
         <v>239</v>
       </c>
       <c r="I33" s="25"/>
@@ -3788,25 +3811,25 @@
       <c r="L33" s="41"/>
       <c r="M33" s="42"/>
     </row>
-    <row r="34" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
         <v>275</v>
       </c>
       <c r="B34" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="C34" s="92" t="s">
+      <c r="C34" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="D34" s="90" t="s">
+      <c r="D34" s="75" t="s">
         <v>268</v>
       </c>
-      <c r="E34" s="77" t="s">
+      <c r="E34" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F34" s="78"/>
+      <c r="F34" s="63"/>
       <c r="G34" s="56"/>
-      <c r="H34" s="81" t="s">
+      <c r="H34" s="66" t="s">
         <v>239</v>
       </c>
       <c r="I34" s="25"/>
@@ -3815,25 +3838,25 @@
       <c r="L34" s="41"/>
       <c r="M34" s="42"/>
     </row>
-    <row r="35" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
         <v>276</v>
       </c>
       <c r="B35" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="92" t="s">
+      <c r="C35" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="D35" s="90" t="s">
+      <c r="D35" s="75" t="s">
         <v>268</v>
       </c>
-      <c r="E35" s="77" t="s">
+      <c r="E35" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F35" s="78"/>
+      <c r="F35" s="63"/>
       <c r="G35" s="56"/>
-      <c r="H35" s="81" t="s">
+      <c r="H35" s="66" t="s">
         <v>239</v>
       </c>
       <c r="I35" s="25"/>
@@ -3842,25 +3865,25 @@
       <c r="L35" s="41"/>
       <c r="M35" s="42"/>
     </row>
-    <row r="36" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
         <v>277</v>
       </c>
       <c r="B36" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="C36" s="92" t="s">
+      <c r="C36" s="77" t="s">
         <v>91</v>
       </c>
-      <c r="D36" s="90" t="s">
+      <c r="D36" s="75" t="s">
         <v>268</v>
       </c>
-      <c r="E36" s="77" t="s">
+      <c r="E36" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F36" s="78"/>
+      <c r="F36" s="63"/>
       <c r="G36" s="56"/>
-      <c r="H36" s="81" t="s">
+      <c r="H36" s="66" t="s">
         <v>239</v>
       </c>
       <c r="I36" s="25"/>
@@ -3869,25 +3892,25 @@
       <c r="L36" s="41"/>
       <c r="M36" s="42"/>
     </row>
-    <row r="37" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
         <v>278</v>
       </c>
       <c r="B37" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="C37" s="92" t="s">
+      <c r="C37" s="77" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="90" t="s">
+      <c r="D37" s="75" t="s">
         <v>268</v>
       </c>
-      <c r="E37" s="77" t="s">
+      <c r="E37" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F37" s="78"/>
+      <c r="F37" s="63"/>
       <c r="G37" s="56"/>
-      <c r="H37" s="81" t="s">
+      <c r="H37" s="66" t="s">
         <v>239</v>
       </c>
       <c r="I37" s="25"/>
@@ -3896,25 +3919,25 @@
       <c r="L37" s="41"/>
       <c r="M37" s="42"/>
     </row>
-    <row r="38" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
         <v>279</v>
       </c>
       <c r="B38" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="92" t="s">
+      <c r="C38" s="77" t="s">
         <v>91</v>
       </c>
-      <c r="D38" s="90" t="s">
+      <c r="D38" s="75" t="s">
         <v>268</v>
       </c>
-      <c r="E38" s="77" t="s">
+      <c r="E38" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F38" s="78"/>
+      <c r="F38" s="63"/>
       <c r="G38" s="56"/>
-      <c r="H38" s="81" t="s">
+      <c r="H38" s="66" t="s">
         <v>239</v>
       </c>
       <c r="I38" s="25"/>
@@ -3923,25 +3946,25 @@
       <c r="L38" s="41"/>
       <c r="M38" s="42"/>
     </row>
-    <row r="39" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
         <v>280</v>
       </c>
       <c r="B39" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="C39" s="92" t="s">
+      <c r="C39" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="90" t="s">
+      <c r="D39" s="75" t="s">
         <v>268</v>
       </c>
-      <c r="E39" s="77" t="s">
+      <c r="E39" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F39" s="78"/>
+      <c r="F39" s="63"/>
       <c r="G39" s="56"/>
-      <c r="H39" s="81" t="s">
+      <c r="H39" s="66" t="s">
         <v>239</v>
       </c>
       <c r="I39" s="25"/>
@@ -3950,25 +3973,25 @@
       <c r="L39" s="41"/>
       <c r="M39" s="42"/>
     </row>
-    <row r="40" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
         <v>281</v>
       </c>
       <c r="B40" s="55" t="s">
         <v>225</v>
       </c>
-      <c r="C40" s="92" t="s">
+      <c r="C40" s="77" t="s">
         <v>226</v>
       </c>
-      <c r="D40" s="90" t="s">
+      <c r="D40" s="75" t="s">
         <v>268</v>
       </c>
-      <c r="E40" s="77" t="s">
+      <c r="E40" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F40" s="78"/>
+      <c r="F40" s="63"/>
       <c r="G40" s="56"/>
-      <c r="H40" s="81" t="s">
+      <c r="H40" s="66" t="s">
         <v>239</v>
       </c>
       <c r="I40" s="25"/>
@@ -3977,7 +4000,7 @@
       <c r="L40" s="41"/>
       <c r="M40" s="42"/>
     </row>
-    <row r="41" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
         <v>282</v>
       </c>
@@ -3987,15 +4010,15 @@
       <c r="C41" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="D41" s="90" t="s">
+      <c r="D41" s="75" t="s">
         <v>263</v>
       </c>
-      <c r="E41" s="77" t="s">
+      <c r="E41" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F41" s="78"/>
+      <c r="F41" s="73"/>
       <c r="G41" s="56"/>
-      <c r="H41" s="81" t="s">
+      <c r="H41" s="66" t="s">
         <v>240</v>
       </c>
       <c r="I41" s="25"/>
@@ -4004,7 +4027,7 @@
       <c r="L41" s="41"/>
       <c r="M41" s="42"/>
     </row>
-    <row r="42" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
         <v>283</v>
       </c>
@@ -4014,15 +4037,15 @@
       <c r="C42" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="D42" s="90" t="s">
+      <c r="D42" s="75" t="s">
         <v>263</v>
       </c>
-      <c r="E42" s="77" t="s">
+      <c r="E42" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F42" s="78"/>
+      <c r="F42" s="73"/>
       <c r="G42" s="56"/>
-      <c r="H42" s="81" t="s">
+      <c r="H42" s="66" t="s">
         <v>240</v>
       </c>
       <c r="I42" s="25"/>
@@ -4031,7 +4054,7 @@
       <c r="L42" s="41"/>
       <c r="M42" s="42"/>
     </row>
-    <row r="43" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
         <v>284</v>
       </c>
@@ -4041,15 +4064,15 @@
       <c r="C43" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D43" s="90" t="s">
+      <c r="D43" s="75" t="s">
         <v>270</v>
       </c>
-      <c r="E43" s="77" t="s">
+      <c r="E43" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F43" s="78"/>
+      <c r="F43" s="63"/>
       <c r="G43" s="56"/>
-      <c r="H43" s="81" t="s">
+      <c r="H43" s="66" t="s">
         <v>241</v>
       </c>
       <c r="I43" s="25"/>
@@ -4068,15 +4091,15 @@
       <c r="C44" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D44" s="90" t="s">
+      <c r="D44" s="75" t="s">
         <v>270</v>
       </c>
-      <c r="E44" s="77" t="s">
+      <c r="E44" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F44" s="78"/>
+      <c r="F44" s="63"/>
       <c r="G44" s="56"/>
-      <c r="H44" s="81" t="s">
+      <c r="H44" s="66" t="s">
         <v>241</v>
       </c>
       <c r="I44" s="25"/>
@@ -4095,15 +4118,15 @@
       <c r="C45" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D45" s="90" t="s">
+      <c r="D45" s="75" t="s">
         <v>270</v>
       </c>
-      <c r="E45" s="77" t="s">
+      <c r="E45" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F45" s="78"/>
+      <c r="F45" s="63"/>
       <c r="G45" s="56"/>
-      <c r="H45" s="81" t="s">
+      <c r="H45" s="66" t="s">
         <v>241</v>
       </c>
       <c r="I45" s="25"/>
@@ -4122,15 +4145,15 @@
       <c r="C46" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="90" t="s">
+      <c r="D46" s="75" t="s">
         <v>270</v>
       </c>
-      <c r="E46" s="77" t="s">
+      <c r="E46" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F46" s="78"/>
+      <c r="F46" s="63"/>
       <c r="G46" s="56"/>
-      <c r="H46" s="81" t="s">
+      <c r="H46" s="66" t="s">
         <v>241</v>
       </c>
       <c r="I46" s="25"/>
@@ -4149,15 +4172,15 @@
       <c r="C47" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D47" s="90" t="s">
+      <c r="D47" s="75" t="s">
         <v>270</v>
       </c>
-      <c r="E47" s="77" t="s">
+      <c r="E47" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F47" s="78"/>
+      <c r="F47" s="63"/>
       <c r="G47" s="56"/>
-      <c r="H47" s="81" t="s">
+      <c r="H47" s="66" t="s">
         <v>241</v>
       </c>
       <c r="I47" s="25"/>
@@ -4176,15 +4199,15 @@
       <c r="C48" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D48" s="90" t="s">
+      <c r="D48" s="75" t="s">
         <v>270</v>
       </c>
-      <c r="E48" s="77" t="s">
+      <c r="E48" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F48" s="78"/>
+      <c r="F48" s="63"/>
       <c r="G48" s="56"/>
-      <c r="H48" s="81" t="s">
+      <c r="H48" s="66" t="s">
         <v>241</v>
       </c>
       <c r="I48" s="25"/>
@@ -4203,15 +4226,15 @@
       <c r="C49" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D49" s="90" t="s">
+      <c r="D49" s="75" t="s">
         <v>270</v>
       </c>
-      <c r="E49" s="77" t="s">
+      <c r="E49" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F49" s="78"/>
+      <c r="F49" s="63"/>
       <c r="G49" s="56"/>
-      <c r="H49" s="81" t="s">
+      <c r="H49" s="66" t="s">
         <v>241</v>
       </c>
       <c r="I49" s="25"/>
@@ -4230,15 +4253,15 @@
       <c r="C50" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D50" s="90" t="s">
+      <c r="D50" s="75" t="s">
         <v>270</v>
       </c>
-      <c r="E50" s="77" t="s">
+      <c r="E50" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F50" s="78"/>
+      <c r="F50" s="63"/>
       <c r="G50" s="56"/>
-      <c r="H50" s="81" t="s">
+      <c r="H50" s="66" t="s">
         <v>241</v>
       </c>
       <c r="I50" s="25"/>
@@ -4257,15 +4280,15 @@
       <c r="C51" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="D51" s="90" t="s">
+      <c r="D51" s="75" t="s">
         <v>270</v>
       </c>
-      <c r="E51" s="77" t="s">
+      <c r="E51" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F51" s="78"/>
+      <c r="F51" s="63"/>
       <c r="G51" s="56"/>
-      <c r="H51" s="81" t="s">
+      <c r="H51" s="66" t="s">
         <v>241</v>
       </c>
       <c r="I51" s="25"/>
@@ -4284,15 +4307,15 @@
       <c r="C52" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="D52" s="90" t="s">
+      <c r="D52" s="75" t="s">
         <v>270</v>
       </c>
-      <c r="E52" s="77" t="s">
+      <c r="E52" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F52" s="78"/>
+      <c r="F52" s="63"/>
       <c r="G52" s="56"/>
-      <c r="H52" s="81" t="s">
+      <c r="H52" s="66" t="s">
         <v>241</v>
       </c>
       <c r="I52" s="25"/>
@@ -4311,15 +4334,15 @@
       <c r="C53" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="D53" s="90" t="s">
+      <c r="D53" s="75" t="s">
         <v>271</v>
       </c>
-      <c r="E53" s="77" t="s">
+      <c r="E53" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F53" s="78"/>
+      <c r="F53" s="63"/>
       <c r="G53" s="56"/>
-      <c r="H53" s="81" t="s">
+      <c r="H53" s="66" t="s">
         <v>242</v>
       </c>
       <c r="I53" s="25"/>
@@ -4338,15 +4361,15 @@
       <c r="C54" s="23" t="s">
         <v>229</v>
       </c>
-      <c r="D54" s="90" t="s">
+      <c r="D54" s="75" t="s">
         <v>271</v>
       </c>
-      <c r="E54" s="77" t="s">
+      <c r="E54" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F54" s="78"/>
+      <c r="F54" s="63"/>
       <c r="G54" s="56"/>
-      <c r="H54" s="81" t="s">
+      <c r="H54" s="66" t="s">
         <v>242</v>
       </c>
       <c r="I54" s="25"/>
@@ -4365,19 +4388,19 @@
       <c r="C55" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="D55" s="90" t="s">
+      <c r="D55" s="75" t="s">
         <v>264</v>
       </c>
-      <c r="E55" s="77" t="s">
+      <c r="E55" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F55" s="88" t="s">
+      <c r="F55" s="73" t="s">
         <v>265</v>
       </c>
-      <c r="G55" s="90" t="s">
+      <c r="G55" s="75" t="s">
         <v>267</v>
       </c>
-      <c r="H55" s="81" t="s">
+      <c r="H55" s="66" t="s">
         <v>243</v>
       </c>
       <c r="I55" s="25"/>
@@ -4396,19 +4419,19 @@
       <c r="C56" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="D56" s="90" t="s">
+      <c r="D56" s="75" t="s">
         <v>264</v>
       </c>
-      <c r="E56" s="77" t="s">
+      <c r="E56" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F56" s="88" t="s">
+      <c r="F56" s="73" t="s">
         <v>265</v>
       </c>
-      <c r="G56" s="90" t="s">
+      <c r="G56" s="75" t="s">
         <v>267</v>
       </c>
-      <c r="H56" s="81" t="s">
+      <c r="H56" s="66" t="s">
         <v>243</v>
       </c>
       <c r="I56" s="25"/>
@@ -4427,19 +4450,19 @@
       <c r="C57" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="D57" s="90" t="s">
+      <c r="D57" s="75" t="s">
         <v>264</v>
       </c>
-      <c r="E57" s="77" t="s">
+      <c r="E57" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F57" s="88" t="s">
+      <c r="F57" s="73" t="s">
         <v>265</v>
       </c>
-      <c r="G57" s="90" t="s">
+      <c r="G57" s="75" t="s">
         <v>267</v>
       </c>
-      <c r="H57" s="81" t="s">
+      <c r="H57" s="66" t="s">
         <v>243</v>
       </c>
       <c r="I57" s="25"/>
@@ -4458,19 +4481,19 @@
       <c r="C58" s="23" t="s">
         <v>235</v>
       </c>
-      <c r="D58" s="90" t="s">
+      <c r="D58" s="75" t="s">
         <v>266</v>
       </c>
-      <c r="E58" s="77" t="s">
+      <c r="E58" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F58" s="88" t="s">
+      <c r="F58" s="73" t="s">
         <v>265</v>
       </c>
-      <c r="G58" s="90" t="s">
+      <c r="G58" s="75" t="s">
         <v>267</v>
       </c>
-      <c r="H58" s="81" t="s">
+      <c r="H58" s="66" t="s">
         <v>243</v>
       </c>
       <c r="I58" s="25"/>
@@ -4490,12 +4513,12 @@
         <v>218</v>
       </c>
       <c r="D59" s="20"/>
-      <c r="E59" s="77" t="s">
+      <c r="E59" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="F59" s="78"/>
+      <c r="F59" s="63"/>
       <c r="G59" s="56"/>
-      <c r="H59" s="81" t="s">
+      <c r="H59" s="66" t="s">
         <v>238</v>
       </c>
       <c r="I59" s="25"/>
@@ -4506,12 +4529,12 @@
     </row>
     <row r="60" spans="1:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="24"/>
-      <c r="B60" s="63"/>
-      <c r="C60" s="64"/>
-      <c r="D60" s="64"/>
-      <c r="E60" s="64"/>
-      <c r="F60" s="65"/>
-      <c r="G60" s="85"/>
+      <c r="B60" s="102"/>
+      <c r="C60" s="103"/>
+      <c r="D60" s="103"/>
+      <c r="E60" s="103"/>
+      <c r="F60" s="104"/>
+      <c r="G60" s="70"/>
       <c r="H60" s="58"/>
       <c r="I60" s="25"/>
       <c r="J60" s="26"/>
@@ -4521,12 +4544,12 @@
     </row>
     <row r="61" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="24"/>
-      <c r="B61" s="61"/>
-      <c r="C61" s="66"/>
-      <c r="D61" s="66"/>
-      <c r="E61" s="66"/>
-      <c r="F61" s="62"/>
-      <c r="G61" s="85"/>
+      <c r="B61" s="105"/>
+      <c r="C61" s="106"/>
+      <c r="D61" s="106"/>
+      <c r="E61" s="106"/>
+      <c r="F61" s="107"/>
+      <c r="G61" s="70"/>
       <c r="H61" s="58"/>
       <c r="I61" s="25"/>
       <c r="J61" s="26"/>
@@ -4536,12 +4559,12 @@
     </row>
     <row r="62" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="24"/>
-      <c r="B62" s="61"/>
-      <c r="C62" s="66"/>
-      <c r="D62" s="66"/>
-      <c r="E62" s="66"/>
-      <c r="F62" s="62"/>
-      <c r="G62" s="85"/>
+      <c r="B62" s="105"/>
+      <c r="C62" s="106"/>
+      <c r="D62" s="106"/>
+      <c r="E62" s="106"/>
+      <c r="F62" s="107"/>
+      <c r="G62" s="70"/>
       <c r="H62" s="58"/>
       <c r="I62" s="25"/>
       <c r="J62" s="26"/>
@@ -4551,12 +4574,12 @@
     </row>
     <row r="63" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="24"/>
-      <c r="B63" s="61"/>
-      <c r="C63" s="66"/>
-      <c r="D63" s="66"/>
-      <c r="E63" s="66"/>
-      <c r="F63" s="62"/>
-      <c r="G63" s="85"/>
+      <c r="B63" s="105"/>
+      <c r="C63" s="106"/>
+      <c r="D63" s="106"/>
+      <c r="E63" s="106"/>
+      <c r="F63" s="107"/>
+      <c r="G63" s="70"/>
       <c r="H63" s="58"/>
       <c r="I63" s="25"/>
       <c r="J63" s="26"/>
@@ -4566,12 +4589,12 @@
     </row>
     <row r="64" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="24"/>
-      <c r="B64" s="61"/>
-      <c r="C64" s="66"/>
-      <c r="D64" s="66"/>
-      <c r="E64" s="66"/>
-      <c r="F64" s="62"/>
-      <c r="G64" s="85"/>
+      <c r="B64" s="105"/>
+      <c r="C64" s="106"/>
+      <c r="D64" s="106"/>
+      <c r="E64" s="106"/>
+      <c r="F64" s="107"/>
+      <c r="G64" s="70"/>
       <c r="H64" s="58"/>
       <c r="I64" s="25"/>
       <c r="J64" s="26"/>
@@ -4581,12 +4604,12 @@
     </row>
     <row r="65" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="24"/>
-      <c r="B65" s="61"/>
-      <c r="C65" s="66"/>
-      <c r="D65" s="66"/>
-      <c r="E65" s="66"/>
-      <c r="F65" s="62"/>
-      <c r="G65" s="85"/>
+      <c r="B65" s="105"/>
+      <c r="C65" s="106"/>
+      <c r="D65" s="106"/>
+      <c r="E65" s="106"/>
+      <c r="F65" s="107"/>
+      <c r="G65" s="70"/>
       <c r="H65" s="58"/>
       <c r="I65" s="25"/>
       <c r="J65" s="26"/>
@@ -4596,12 +4619,12 @@
     </row>
     <row r="66" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="24"/>
-      <c r="B66" s="61"/>
-      <c r="C66" s="66"/>
-      <c r="D66" s="66"/>
-      <c r="E66" s="66"/>
-      <c r="F66" s="62"/>
-      <c r="G66" s="85"/>
+      <c r="B66" s="105"/>
+      <c r="C66" s="106"/>
+      <c r="D66" s="106"/>
+      <c r="E66" s="106"/>
+      <c r="F66" s="107"/>
+      <c r="G66" s="70"/>
       <c r="H66" s="58"/>
       <c r="I66" s="25"/>
       <c r="J66" s="26"/>
@@ -4613,12 +4636,12 @@
       <c r="A67" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="B67" s="61"/>
-      <c r="C67" s="66"/>
-      <c r="D67" s="66"/>
-      <c r="E67" s="66"/>
-      <c r="F67" s="62"/>
-      <c r="G67" s="85"/>
+      <c r="B67" s="105"/>
+      <c r="C67" s="106"/>
+      <c r="D67" s="106"/>
+      <c r="E67" s="106"/>
+      <c r="F67" s="107"/>
+      <c r="G67" s="70"/>
       <c r="H67" s="58"/>
       <c r="I67" s="25"/>
       <c r="J67" s="26"/>
@@ -4634,9 +4657,9 @@
       <c r="C68" s="25"/>
       <c r="D68" s="25"/>
       <c r="E68" s="25"/>
-      <c r="F68" s="79"/>
-      <c r="G68" s="86"/>
-      <c r="H68" s="82"/>
+      <c r="F68" s="64"/>
+      <c r="G68" s="71"/>
+      <c r="H68" s="67"/>
       <c r="I68" s="25"/>
       <c r="J68" s="26"/>
       <c r="K68" s="40"/>
@@ -4651,9 +4674,9 @@
       <c r="C69" s="25"/>
       <c r="D69" s="25"/>
       <c r="E69" s="25"/>
-      <c r="F69" s="79"/>
-      <c r="G69" s="86"/>
-      <c r="H69" s="82"/>
+      <c r="F69" s="64"/>
+      <c r="G69" s="71"/>
+      <c r="H69" s="67"/>
       <c r="I69" s="25"/>
       <c r="J69" s="26"/>
       <c r="K69" s="40"/>
@@ -4668,9 +4691,9 @@
       <c r="C70" s="25"/>
       <c r="D70" s="25"/>
       <c r="E70" s="25"/>
-      <c r="F70" s="79"/>
-      <c r="G70" s="86"/>
-      <c r="H70" s="82"/>
+      <c r="F70" s="64"/>
+      <c r="G70" s="71"/>
+      <c r="H70" s="67"/>
       <c r="I70" s="25"/>
       <c r="J70" s="26"/>
       <c r="K70" s="40"/>
@@ -4685,9 +4708,9 @@
       <c r="C71" s="25"/>
       <c r="D71" s="25"/>
       <c r="E71" s="25"/>
-      <c r="F71" s="79"/>
-      <c r="G71" s="86"/>
-      <c r="H71" s="82"/>
+      <c r="F71" s="64"/>
+      <c r="G71" s="71"/>
+      <c r="H71" s="67"/>
       <c r="I71" s="25"/>
       <c r="J71" s="26"/>
       <c r="K71" s="40"/>
@@ -4702,9 +4725,9 @@
       <c r="C72" s="25"/>
       <c r="D72" s="25"/>
       <c r="E72" s="25"/>
-      <c r="F72" s="79"/>
-      <c r="G72" s="86"/>
-      <c r="H72" s="82"/>
+      <c r="F72" s="64"/>
+      <c r="G72" s="71"/>
+      <c r="H72" s="67"/>
       <c r="I72" s="25"/>
       <c r="J72" s="26"/>
       <c r="K72" s="40"/>
@@ -4719,9 +4742,9 @@
       <c r="C73" s="25"/>
       <c r="D73" s="25"/>
       <c r="E73" s="25"/>
-      <c r="F73" s="79"/>
-      <c r="G73" s="86"/>
-      <c r="H73" s="82"/>
+      <c r="F73" s="64"/>
+      <c r="G73" s="71"/>
+      <c r="H73" s="67"/>
       <c r="I73" s="25"/>
       <c r="J73" s="26"/>
       <c r="K73" s="40"/>
@@ -4736,9 +4759,9 @@
       <c r="C74" s="25"/>
       <c r="D74" s="25"/>
       <c r="E74" s="25"/>
-      <c r="F74" s="79"/>
-      <c r="G74" s="86"/>
-      <c r="H74" s="82"/>
+      <c r="F74" s="64"/>
+      <c r="G74" s="71"/>
+      <c r="H74" s="67"/>
       <c r="I74" s="25"/>
       <c r="J74" s="26"/>
       <c r="K74" s="40"/>
@@ -4753,9 +4776,9 @@
       <c r="C75" s="25"/>
       <c r="D75" s="25"/>
       <c r="E75" s="25"/>
-      <c r="F75" s="79"/>
-      <c r="G75" s="86"/>
-      <c r="H75" s="82"/>
+      <c r="F75" s="64"/>
+      <c r="G75" s="71"/>
+      <c r="H75" s="67"/>
       <c r="I75" s="25"/>
       <c r="J75" s="26"/>
       <c r="K75" s="40"/>
@@ -4770,9 +4793,9 @@
       <c r="C76" s="25"/>
       <c r="D76" s="25"/>
       <c r="E76" s="25"/>
-      <c r="F76" s="79"/>
-      <c r="G76" s="86"/>
-      <c r="H76" s="82"/>
+      <c r="F76" s="64"/>
+      <c r="G76" s="71"/>
+      <c r="H76" s="67"/>
       <c r="I76" s="25"/>
       <c r="J76" s="26"/>
       <c r="K76" s="40"/>
@@ -4787,9 +4810,9 @@
       <c r="C77" s="25"/>
       <c r="D77" s="25"/>
       <c r="E77" s="25"/>
-      <c r="F77" s="79"/>
-      <c r="G77" s="86"/>
-      <c r="H77" s="82"/>
+      <c r="F77" s="64"/>
+      <c r="G77" s="71"/>
+      <c r="H77" s="67"/>
       <c r="I77" s="25"/>
       <c r="J77" s="26"/>
       <c r="K77" s="40"/>
@@ -4804,9 +4827,9 @@
       <c r="C78" s="25"/>
       <c r="D78" s="25"/>
       <c r="E78" s="25"/>
-      <c r="F78" s="79"/>
-      <c r="G78" s="86"/>
-      <c r="H78" s="82"/>
+      <c r="F78" s="64"/>
+      <c r="G78" s="71"/>
+      <c r="H78" s="67"/>
       <c r="I78" s="25"/>
       <c r="J78" s="26"/>
       <c r="K78" s="40"/>
@@ -4821,9 +4844,9 @@
       <c r="C79" s="25"/>
       <c r="D79" s="25"/>
       <c r="E79" s="25"/>
-      <c r="F79" s="79"/>
-      <c r="G79" s="86"/>
-      <c r="H79" s="82"/>
+      <c r="F79" s="64"/>
+      <c r="G79" s="71"/>
+      <c r="H79" s="67"/>
       <c r="I79" s="25"/>
       <c r="J79" s="26"/>
       <c r="K79" s="40"/>
@@ -4838,9 +4861,9 @@
       <c r="C80" s="25"/>
       <c r="D80" s="25"/>
       <c r="E80" s="25"/>
-      <c r="F80" s="79"/>
-      <c r="G80" s="86"/>
-      <c r="H80" s="82"/>
+      <c r="F80" s="64"/>
+      <c r="G80" s="71"/>
+      <c r="H80" s="67"/>
       <c r="I80" s="25"/>
       <c r="J80" s="26"/>
       <c r="K80" s="40"/>
@@ -4855,9 +4878,9 @@
       <c r="C81" s="25"/>
       <c r="D81" s="25"/>
       <c r="E81" s="25"/>
-      <c r="F81" s="79"/>
-      <c r="G81" s="86"/>
-      <c r="H81" s="82"/>
+      <c r="F81" s="64"/>
+      <c r="G81" s="71"/>
+      <c r="H81" s="67"/>
       <c r="I81" s="25"/>
       <c r="J81" s="26"/>
       <c r="K81" s="40"/>
@@ -4872,9 +4895,9 @@
       <c r="C82" s="25"/>
       <c r="D82" s="25"/>
       <c r="E82" s="25"/>
-      <c r="F82" s="79"/>
-      <c r="G82" s="86"/>
-      <c r="H82" s="82"/>
+      <c r="F82" s="64"/>
+      <c r="G82" s="71"/>
+      <c r="H82" s="67"/>
       <c r="I82" s="25"/>
       <c r="J82" s="26"/>
       <c r="K82" s="40"/>
@@ -4889,9 +4912,9 @@
       <c r="C83" s="25"/>
       <c r="D83" s="25"/>
       <c r="E83" s="25"/>
-      <c r="F83" s="79"/>
-      <c r="G83" s="86"/>
-      <c r="H83" s="82"/>
+      <c r="F83" s="64"/>
+      <c r="G83" s="71"/>
+      <c r="H83" s="67"/>
       <c r="I83" s="25"/>
       <c r="J83" s="26"/>
       <c r="K83" s="40"/>
@@ -4906,9 +4929,9 @@
       <c r="C84" s="25"/>
       <c r="D84" s="25"/>
       <c r="E84" s="25"/>
-      <c r="F84" s="79"/>
-      <c r="G84" s="86"/>
-      <c r="H84" s="82"/>
+      <c r="F84" s="64"/>
+      <c r="G84" s="71"/>
+      <c r="H84" s="67"/>
       <c r="I84" s="25"/>
       <c r="J84" s="26"/>
       <c r="K84" s="40"/>
@@ -4923,9 +4946,9 @@
       <c r="C85" s="25"/>
       <c r="D85" s="25"/>
       <c r="E85" s="25"/>
-      <c r="F85" s="79"/>
-      <c r="G85" s="86"/>
-      <c r="H85" s="82"/>
+      <c r="F85" s="64"/>
+      <c r="G85" s="71"/>
+      <c r="H85" s="67"/>
       <c r="I85" s="25"/>
       <c r="J85" s="26"/>
       <c r="K85" s="40"/>
@@ -4940,9 +4963,9 @@
       <c r="C86" s="25"/>
       <c r="D86" s="25"/>
       <c r="E86" s="25"/>
-      <c r="F86" s="79"/>
-      <c r="G86" s="86"/>
-      <c r="H86" s="82"/>
+      <c r="F86" s="64"/>
+      <c r="G86" s="71"/>
+      <c r="H86" s="67"/>
       <c r="I86" s="25"/>
       <c r="J86" s="26"/>
       <c r="K86" s="40"/>
@@ -4957,9 +4980,9 @@
       <c r="C87" s="25"/>
       <c r="D87" s="25"/>
       <c r="E87" s="25"/>
-      <c r="F87" s="79"/>
-      <c r="G87" s="86"/>
-      <c r="H87" s="82"/>
+      <c r="F87" s="64"/>
+      <c r="G87" s="71"/>
+      <c r="H87" s="67"/>
       <c r="I87" s="25"/>
       <c r="J87" s="26"/>
       <c r="K87" s="40"/>
@@ -4974,9 +4997,9 @@
       <c r="C88" s="25"/>
       <c r="D88" s="25"/>
       <c r="E88" s="25"/>
-      <c r="F88" s="79"/>
-      <c r="G88" s="86"/>
-      <c r="H88" s="82"/>
+      <c r="F88" s="64"/>
+      <c r="G88" s="71"/>
+      <c r="H88" s="67"/>
       <c r="I88" s="25"/>
       <c r="J88" s="26"/>
       <c r="K88" s="40"/>
@@ -4991,9 +5014,9 @@
       <c r="C89" s="25"/>
       <c r="D89" s="25"/>
       <c r="E89" s="25"/>
-      <c r="F89" s="79"/>
-      <c r="G89" s="86"/>
-      <c r="H89" s="82"/>
+      <c r="F89" s="64"/>
+      <c r="G89" s="71"/>
+      <c r="H89" s="67"/>
       <c r="I89" s="25"/>
       <c r="J89" s="26"/>
       <c r="K89" s="40"/>
@@ -5008,9 +5031,9 @@
       <c r="C90" s="25"/>
       <c r="D90" s="25"/>
       <c r="E90" s="25"/>
-      <c r="F90" s="79"/>
-      <c r="G90" s="86"/>
-      <c r="H90" s="82"/>
+      <c r="F90" s="64"/>
+      <c r="G90" s="71"/>
+      <c r="H90" s="67"/>
       <c r="I90" s="25"/>
       <c r="J90" s="26"/>
       <c r="K90" s="40"/>
@@ -5025,9 +5048,9 @@
       <c r="C91" s="25"/>
       <c r="D91" s="25"/>
       <c r="E91" s="25"/>
-      <c r="F91" s="79"/>
-      <c r="G91" s="86"/>
-      <c r="H91" s="82"/>
+      <c r="F91" s="64"/>
+      <c r="G91" s="71"/>
+      <c r="H91" s="67"/>
       <c r="I91" s="25"/>
       <c r="J91" s="26"/>
       <c r="K91" s="40"/>
@@ -5042,9 +5065,9 @@
       <c r="C92" s="25"/>
       <c r="D92" s="25"/>
       <c r="E92" s="25"/>
-      <c r="F92" s="79"/>
-      <c r="G92" s="86"/>
-      <c r="H92" s="82"/>
+      <c r="F92" s="64"/>
+      <c r="G92" s="71"/>
+      <c r="H92" s="67"/>
       <c r="I92" s="25"/>
       <c r="J92" s="26"/>
       <c r="K92" s="40"/>
@@ -5059,9 +5082,9 @@
       <c r="C93" s="25"/>
       <c r="D93" s="25"/>
       <c r="E93" s="25"/>
-      <c r="F93" s="79"/>
-      <c r="G93" s="86"/>
-      <c r="H93" s="82"/>
+      <c r="F93" s="64"/>
+      <c r="G93" s="71"/>
+      <c r="H93" s="67"/>
       <c r="I93" s="25"/>
       <c r="J93" s="26"/>
       <c r="K93" s="40"/>
@@ -5076,9 +5099,9 @@
       <c r="C94" s="25"/>
       <c r="D94" s="25"/>
       <c r="E94" s="25"/>
-      <c r="F94" s="79"/>
-      <c r="G94" s="86"/>
-      <c r="H94" s="82"/>
+      <c r="F94" s="64"/>
+      <c r="G94" s="71"/>
+      <c r="H94" s="67"/>
       <c r="I94" s="25"/>
       <c r="J94" s="26"/>
       <c r="K94" s="40"/>
@@ -5093,9 +5116,9 @@
       <c r="C95" s="25"/>
       <c r="D95" s="25"/>
       <c r="E95" s="25"/>
-      <c r="F95" s="79"/>
-      <c r="G95" s="86"/>
-      <c r="H95" s="82"/>
+      <c r="F95" s="64"/>
+      <c r="G95" s="71"/>
+      <c r="H95" s="67"/>
       <c r="I95" s="25"/>
       <c r="J95" s="26"/>
       <c r="K95" s="40"/>
@@ -5110,9 +5133,9 @@
       <c r="C96" s="25"/>
       <c r="D96" s="25"/>
       <c r="E96" s="25"/>
-      <c r="F96" s="79"/>
-      <c r="G96" s="86"/>
-      <c r="H96" s="82"/>
+      <c r="F96" s="64"/>
+      <c r="G96" s="71"/>
+      <c r="H96" s="67"/>
       <c r="I96" s="25"/>
       <c r="J96" s="26"/>
       <c r="K96" s="40"/>
@@ -5127,9 +5150,9 @@
       <c r="C97" s="25"/>
       <c r="D97" s="25"/>
       <c r="E97" s="25"/>
-      <c r="F97" s="79"/>
-      <c r="G97" s="86"/>
-      <c r="H97" s="82"/>
+      <c r="F97" s="64"/>
+      <c r="G97" s="71"/>
+      <c r="H97" s="67"/>
       <c r="I97" s="25"/>
       <c r="J97" s="26"/>
       <c r="K97" s="40"/>
@@ -5144,9 +5167,9 @@
       <c r="C98" s="25"/>
       <c r="D98" s="25"/>
       <c r="E98" s="25"/>
-      <c r="F98" s="79"/>
-      <c r="G98" s="86"/>
-      <c r="H98" s="82"/>
+      <c r="F98" s="64"/>
+      <c r="G98" s="71"/>
+      <c r="H98" s="67"/>
       <c r="I98" s="25"/>
       <c r="J98" s="26"/>
       <c r="K98" s="40"/>
@@ -5161,9 +5184,9 @@
       <c r="C99" s="25"/>
       <c r="D99" s="25"/>
       <c r="E99" s="25"/>
-      <c r="F99" s="79"/>
-      <c r="G99" s="86"/>
-      <c r="H99" s="82"/>
+      <c r="F99" s="64"/>
+      <c r="G99" s="71"/>
+      <c r="H99" s="67"/>
       <c r="I99" s="25"/>
       <c r="J99" s="26"/>
       <c r="K99" s="40"/>
@@ -5178,9 +5201,9 @@
       <c r="C100" s="25"/>
       <c r="D100" s="25"/>
       <c r="E100" s="25"/>
-      <c r="F100" s="79"/>
-      <c r="G100" s="86"/>
-      <c r="H100" s="82"/>
+      <c r="F100" s="64"/>
+      <c r="G100" s="71"/>
+      <c r="H100" s="67"/>
       <c r="I100" s="25"/>
       <c r="J100" s="26"/>
       <c r="K100" s="40"/>
@@ -5195,9 +5218,9 @@
       <c r="C101" s="25"/>
       <c r="D101" s="25"/>
       <c r="E101" s="25"/>
-      <c r="F101" s="79"/>
-      <c r="G101" s="86"/>
-      <c r="H101" s="82"/>
+      <c r="F101" s="64"/>
+      <c r="G101" s="71"/>
+      <c r="H101" s="67"/>
       <c r="I101" s="25"/>
       <c r="J101" s="26"/>
       <c r="K101" s="40"/>
@@ -5212,9 +5235,9 @@
       <c r="C102" s="25"/>
       <c r="D102" s="25"/>
       <c r="E102" s="25"/>
-      <c r="F102" s="79"/>
-      <c r="G102" s="86"/>
-      <c r="H102" s="82"/>
+      <c r="F102" s="64"/>
+      <c r="G102" s="71"/>
+      <c r="H102" s="67"/>
       <c r="I102" s="25"/>
       <c r="J102" s="26"/>
       <c r="K102" s="40"/>
@@ -5229,9 +5252,9 @@
       <c r="C103" s="25"/>
       <c r="D103" s="25"/>
       <c r="E103" s="25"/>
-      <c r="F103" s="79"/>
-      <c r="G103" s="86"/>
-      <c r="H103" s="82"/>
+      <c r="F103" s="64"/>
+      <c r="G103" s="71"/>
+      <c r="H103" s="67"/>
       <c r="I103" s="25"/>
       <c r="J103" s="26"/>
       <c r="K103" s="40"/>
@@ -5246,9 +5269,9 @@
       <c r="C104" s="25"/>
       <c r="D104" s="25"/>
       <c r="E104" s="25"/>
-      <c r="F104" s="79"/>
-      <c r="G104" s="86"/>
-      <c r="H104" s="82"/>
+      <c r="F104" s="64"/>
+      <c r="G104" s="71"/>
+      <c r="H104" s="67"/>
       <c r="I104" s="25"/>
       <c r="J104" s="26"/>
       <c r="K104" s="40"/>
@@ -5263,9 +5286,9 @@
       <c r="C105" s="25"/>
       <c r="D105" s="25"/>
       <c r="E105" s="25"/>
-      <c r="F105" s="79"/>
-      <c r="G105" s="86"/>
-      <c r="H105" s="82"/>
+      <c r="F105" s="64"/>
+      <c r="G105" s="71"/>
+      <c r="H105" s="67"/>
       <c r="I105" s="25"/>
       <c r="J105" s="26"/>
       <c r="K105" s="40"/>
@@ -5280,9 +5303,9 @@
       <c r="C106" s="25"/>
       <c r="D106" s="25"/>
       <c r="E106" s="25"/>
-      <c r="F106" s="79"/>
-      <c r="G106" s="86"/>
-      <c r="H106" s="82"/>
+      <c r="F106" s="64"/>
+      <c r="G106" s="71"/>
+      <c r="H106" s="67"/>
       <c r="I106" s="25"/>
       <c r="J106" s="26"/>
       <c r="K106" s="40"/>
@@ -5297,9 +5320,9 @@
       <c r="C107" s="25"/>
       <c r="D107" s="25"/>
       <c r="E107" s="25"/>
-      <c r="F107" s="79"/>
-      <c r="G107" s="86"/>
-      <c r="H107" s="82"/>
+      <c r="F107" s="64"/>
+      <c r="G107" s="71"/>
+      <c r="H107" s="67"/>
       <c r="I107" s="25"/>
       <c r="J107" s="26"/>
       <c r="K107" s="40"/>
@@ -5314,9 +5337,9 @@
       <c r="C108" s="25"/>
       <c r="D108" s="25"/>
       <c r="E108" s="25"/>
-      <c r="F108" s="79"/>
-      <c r="G108" s="86"/>
-      <c r="H108" s="82"/>
+      <c r="F108" s="64"/>
+      <c r="G108" s="71"/>
+      <c r="H108" s="67"/>
       <c r="I108" s="25"/>
       <c r="J108" s="26"/>
       <c r="K108" s="40"/>
@@ -5331,9 +5354,9 @@
       <c r="C109" s="25"/>
       <c r="D109" s="25"/>
       <c r="E109" s="25"/>
-      <c r="F109" s="79"/>
-      <c r="G109" s="86"/>
-      <c r="H109" s="82"/>
+      <c r="F109" s="64"/>
+      <c r="G109" s="71"/>
+      <c r="H109" s="67"/>
       <c r="I109" s="25"/>
       <c r="J109" s="26"/>
       <c r="K109" s="40"/>
@@ -5348,9 +5371,9 @@
       <c r="C110" s="25"/>
       <c r="D110" s="25"/>
       <c r="E110" s="25"/>
-      <c r="F110" s="79"/>
-      <c r="G110" s="86"/>
-      <c r="H110" s="82"/>
+      <c r="F110" s="64"/>
+      <c r="G110" s="71"/>
+      <c r="H110" s="67"/>
       <c r="I110" s="25"/>
       <c r="J110" s="26"/>
       <c r="K110" s="40"/>
@@ -5365,9 +5388,9 @@
       <c r="C111" s="25"/>
       <c r="D111" s="25"/>
       <c r="E111" s="25"/>
-      <c r="F111" s="79"/>
-      <c r="G111" s="86"/>
-      <c r="H111" s="82"/>
+      <c r="F111" s="64"/>
+      <c r="G111" s="71"/>
+      <c r="H111" s="67"/>
       <c r="I111" s="25"/>
       <c r="J111" s="26"/>
       <c r="K111" s="40"/>
@@ -5382,9 +5405,9 @@
       <c r="C112" s="25"/>
       <c r="D112" s="25"/>
       <c r="E112" s="25"/>
-      <c r="F112" s="79"/>
-      <c r="G112" s="86"/>
-      <c r="H112" s="82"/>
+      <c r="F112" s="64"/>
+      <c r="G112" s="71"/>
+      <c r="H112" s="67"/>
       <c r="I112" s="25"/>
       <c r="J112" s="26"/>
       <c r="K112" s="40"/>
@@ -5399,9 +5422,9 @@
       <c r="C113" s="25"/>
       <c r="D113" s="25"/>
       <c r="E113" s="25"/>
-      <c r="F113" s="79"/>
-      <c r="G113" s="86"/>
-      <c r="H113" s="82"/>
+      <c r="F113" s="64"/>
+      <c r="G113" s="71"/>
+      <c r="H113" s="67"/>
       <c r="I113" s="25"/>
       <c r="J113" s="26"/>
       <c r="K113" s="40"/>
@@ -5416,9 +5439,9 @@
       <c r="C114" s="25"/>
       <c r="D114" s="25"/>
       <c r="E114" s="25"/>
-      <c r="F114" s="79"/>
-      <c r="G114" s="86"/>
-      <c r="H114" s="82"/>
+      <c r="F114" s="64"/>
+      <c r="G114" s="71"/>
+      <c r="H114" s="67"/>
       <c r="I114" s="25"/>
       <c r="J114" s="26"/>
       <c r="K114" s="40"/>
@@ -5433,9 +5456,9 @@
       <c r="C115" s="25"/>
       <c r="D115" s="25"/>
       <c r="E115" s="25"/>
-      <c r="F115" s="79"/>
-      <c r="G115" s="86"/>
-      <c r="H115" s="82"/>
+      <c r="F115" s="64"/>
+      <c r="G115" s="71"/>
+      <c r="H115" s="67"/>
       <c r="I115" s="25"/>
       <c r="J115" s="26"/>
       <c r="K115" s="40"/>
@@ -5450,9 +5473,9 @@
       <c r="C116" s="25"/>
       <c r="D116" s="25"/>
       <c r="E116" s="25"/>
-      <c r="F116" s="79"/>
-      <c r="G116" s="86"/>
-      <c r="H116" s="82"/>
+      <c r="F116" s="64"/>
+      <c r="G116" s="71"/>
+      <c r="H116" s="67"/>
       <c r="I116" s="25"/>
       <c r="J116" s="26"/>
       <c r="K116" s="40"/>
@@ -5467,9 +5490,9 @@
       <c r="C117" s="25"/>
       <c r="D117" s="25"/>
       <c r="E117" s="25"/>
-      <c r="F117" s="79"/>
-      <c r="G117" s="86"/>
-      <c r="H117" s="82"/>
+      <c r="F117" s="64"/>
+      <c r="G117" s="71"/>
+      <c r="H117" s="67"/>
       <c r="I117" s="25"/>
       <c r="J117" s="26"/>
       <c r="K117" s="40"/>
@@ -5484,9 +5507,9 @@
       <c r="C118" s="25"/>
       <c r="D118" s="25"/>
       <c r="E118" s="25"/>
-      <c r="F118" s="79"/>
-      <c r="G118" s="86"/>
-      <c r="H118" s="82"/>
+      <c r="F118" s="64"/>
+      <c r="G118" s="71"/>
+      <c r="H118" s="67"/>
       <c r="I118" s="25"/>
       <c r="J118" s="26"/>
       <c r="K118" s="40"/>
@@ -5501,9 +5524,9 @@
       <c r="C119" s="25"/>
       <c r="D119" s="25"/>
       <c r="E119" s="25"/>
-      <c r="F119" s="79"/>
-      <c r="G119" s="86"/>
-      <c r="H119" s="82"/>
+      <c r="F119" s="64"/>
+      <c r="G119" s="71"/>
+      <c r="H119" s="67"/>
       <c r="I119" s="25"/>
       <c r="J119" s="26"/>
       <c r="K119" s="40"/>
@@ -5518,9 +5541,9 @@
       <c r="C120" s="25"/>
       <c r="D120" s="25"/>
       <c r="E120" s="25"/>
-      <c r="F120" s="79"/>
-      <c r="G120" s="86"/>
-      <c r="H120" s="82"/>
+      <c r="F120" s="64"/>
+      <c r="G120" s="71"/>
+      <c r="H120" s="67"/>
       <c r="I120" s="25"/>
       <c r="J120" s="26"/>
       <c r="K120" s="40"/>
@@ -5535,9 +5558,9 @@
       <c r="C121" s="25"/>
       <c r="D121" s="25"/>
       <c r="E121" s="25"/>
-      <c r="F121" s="79"/>
-      <c r="G121" s="86"/>
-      <c r="H121" s="82"/>
+      <c r="F121" s="64"/>
+      <c r="G121" s="71"/>
+      <c r="H121" s="67"/>
       <c r="I121" s="25"/>
       <c r="J121" s="26"/>
       <c r="K121" s="40"/>
@@ -5552,9 +5575,9 @@
       <c r="C122" s="25"/>
       <c r="D122" s="25"/>
       <c r="E122" s="25"/>
-      <c r="F122" s="79"/>
-      <c r="G122" s="86"/>
-      <c r="H122" s="82"/>
+      <c r="F122" s="64"/>
+      <c r="G122" s="71"/>
+      <c r="H122" s="67"/>
       <c r="I122" s="25"/>
       <c r="J122" s="26"/>
       <c r="K122" s="40"/>
@@ -5569,9 +5592,9 @@
       <c r="C123" s="25"/>
       <c r="D123" s="25"/>
       <c r="E123" s="25"/>
-      <c r="F123" s="79"/>
-      <c r="G123" s="86"/>
-      <c r="H123" s="82"/>
+      <c r="F123" s="64"/>
+      <c r="G123" s="71"/>
+      <c r="H123" s="67"/>
       <c r="I123" s="25"/>
       <c r="J123" s="26"/>
       <c r="K123" s="40"/>
@@ -5586,9 +5609,9 @@
       <c r="C124" s="25"/>
       <c r="D124" s="25"/>
       <c r="E124" s="25"/>
-      <c r="F124" s="79"/>
-      <c r="G124" s="86"/>
-      <c r="H124" s="82"/>
+      <c r="F124" s="64"/>
+      <c r="G124" s="71"/>
+      <c r="H124" s="67"/>
       <c r="I124" s="25"/>
       <c r="J124" s="26"/>
       <c r="K124" s="40"/>
@@ -5603,9 +5626,9 @@
       <c r="C125" s="25"/>
       <c r="D125" s="25"/>
       <c r="E125" s="25"/>
-      <c r="F125" s="79"/>
-      <c r="G125" s="86"/>
-      <c r="H125" s="82"/>
+      <c r="F125" s="64"/>
+      <c r="G125" s="71"/>
+      <c r="H125" s="67"/>
       <c r="I125" s="25"/>
       <c r="J125" s="26"/>
       <c r="K125" s="40"/>
@@ -5620,9 +5643,9 @@
       <c r="C126" s="25"/>
       <c r="D126" s="25"/>
       <c r="E126" s="25"/>
-      <c r="F126" s="79"/>
-      <c r="G126" s="86"/>
-      <c r="H126" s="82"/>
+      <c r="F126" s="64"/>
+      <c r="G126" s="71"/>
+      <c r="H126" s="67"/>
       <c r="I126" s="25"/>
       <c r="J126" s="26"/>
       <c r="K126" s="40"/>
@@ -5637,9 +5660,9 @@
       <c r="C127" s="25"/>
       <c r="D127" s="25"/>
       <c r="E127" s="25"/>
-      <c r="F127" s="79"/>
-      <c r="G127" s="86"/>
-      <c r="H127" s="82"/>
+      <c r="F127" s="64"/>
+      <c r="G127" s="71"/>
+      <c r="H127" s="67"/>
       <c r="I127" s="25"/>
       <c r="J127" s="26"/>
       <c r="K127" s="40"/>
@@ -5654,9 +5677,9 @@
       <c r="C128" s="25"/>
       <c r="D128" s="25"/>
       <c r="E128" s="25"/>
-      <c r="F128" s="79"/>
-      <c r="G128" s="86"/>
-      <c r="H128" s="82"/>
+      <c r="F128" s="64"/>
+      <c r="G128" s="71"/>
+      <c r="H128" s="67"/>
       <c r="I128" s="25"/>
       <c r="J128" s="26"/>
       <c r="K128" s="40"/>
@@ -5671,9 +5694,9 @@
       <c r="C129" s="25"/>
       <c r="D129" s="25"/>
       <c r="E129" s="25"/>
-      <c r="F129" s="79"/>
-      <c r="G129" s="86"/>
-      <c r="H129" s="82"/>
+      <c r="F129" s="64"/>
+      <c r="G129" s="71"/>
+      <c r="H129" s="67"/>
       <c r="I129" s="25"/>
       <c r="J129" s="26"/>
       <c r="K129" s="40"/>
@@ -5688,9 +5711,9 @@
       <c r="C130" s="25"/>
       <c r="D130" s="25"/>
       <c r="E130" s="25"/>
-      <c r="F130" s="79"/>
-      <c r="G130" s="86"/>
-      <c r="H130" s="82"/>
+      <c r="F130" s="64"/>
+      <c r="G130" s="71"/>
+      <c r="H130" s="67"/>
       <c r="I130" s="25"/>
       <c r="J130" s="26"/>
       <c r="K130" s="40"/>
@@ -5705,9 +5728,9 @@
       <c r="C131" s="25"/>
       <c r="D131" s="25"/>
       <c r="E131" s="25"/>
-      <c r="F131" s="79"/>
-      <c r="G131" s="86"/>
-      <c r="H131" s="82"/>
+      <c r="F131" s="64"/>
+      <c r="G131" s="71"/>
+      <c r="H131" s="67"/>
       <c r="I131" s="25"/>
       <c r="J131" s="26"/>
       <c r="K131" s="40"/>
@@ -5722,9 +5745,9 @@
       <c r="C132" s="25"/>
       <c r="D132" s="25"/>
       <c r="E132" s="25"/>
-      <c r="F132" s="79"/>
-      <c r="G132" s="86"/>
-      <c r="H132" s="82"/>
+      <c r="F132" s="64"/>
+      <c r="G132" s="71"/>
+      <c r="H132" s="67"/>
       <c r="I132" s="25"/>
       <c r="J132" s="26"/>
       <c r="K132" s="40"/>
@@ -5739,9 +5762,9 @@
       <c r="C133" s="25"/>
       <c r="D133" s="25"/>
       <c r="E133" s="25"/>
-      <c r="F133" s="79"/>
-      <c r="G133" s="86"/>
-      <c r="H133" s="82"/>
+      <c r="F133" s="64"/>
+      <c r="G133" s="71"/>
+      <c r="H133" s="67"/>
       <c r="I133" s="25"/>
       <c r="J133" s="26"/>
       <c r="K133" s="40"/>
@@ -5756,9 +5779,9 @@
       <c r="C134" s="25"/>
       <c r="D134" s="25"/>
       <c r="E134" s="25"/>
-      <c r="F134" s="79"/>
-      <c r="G134" s="86"/>
-      <c r="H134" s="82"/>
+      <c r="F134" s="64"/>
+      <c r="G134" s="71"/>
+      <c r="H134" s="67"/>
       <c r="I134" s="25"/>
       <c r="J134" s="26"/>
       <c r="K134" s="40"/>
@@ -5773,9 +5796,9 @@
       <c r="C135" s="25"/>
       <c r="D135" s="25"/>
       <c r="E135" s="25"/>
-      <c r="F135" s="79"/>
-      <c r="G135" s="86"/>
-      <c r="H135" s="82"/>
+      <c r="F135" s="64"/>
+      <c r="G135" s="71"/>
+      <c r="H135" s="67"/>
       <c r="I135" s="25"/>
       <c r="J135" s="26"/>
       <c r="K135" s="40"/>
@@ -5790,9 +5813,9 @@
       <c r="C136" s="25"/>
       <c r="D136" s="25"/>
       <c r="E136" s="25"/>
-      <c r="F136" s="79"/>
-      <c r="G136" s="86"/>
-      <c r="H136" s="82"/>
+      <c r="F136" s="64"/>
+      <c r="G136" s="71"/>
+      <c r="H136" s="67"/>
       <c r="I136" s="25"/>
       <c r="J136" s="26"/>
       <c r="K136" s="40"/>
@@ -5807,9 +5830,9 @@
       <c r="C137" s="25"/>
       <c r="D137" s="25"/>
       <c r="E137" s="25"/>
-      <c r="F137" s="79"/>
-      <c r="G137" s="86"/>
-      <c r="H137" s="82"/>
+      <c r="F137" s="64"/>
+      <c r="G137" s="71"/>
+      <c r="H137" s="67"/>
       <c r="I137" s="25"/>
       <c r="J137" s="26"/>
       <c r="K137" s="40"/>
@@ -5824,9 +5847,9 @@
       <c r="C138" s="25"/>
       <c r="D138" s="25"/>
       <c r="E138" s="25"/>
-      <c r="F138" s="79"/>
-      <c r="G138" s="86"/>
-      <c r="H138" s="82"/>
+      <c r="F138" s="64"/>
+      <c r="G138" s="71"/>
+      <c r="H138" s="67"/>
       <c r="I138" s="25"/>
       <c r="J138" s="26"/>
       <c r="K138" s="40"/>
@@ -5841,9 +5864,9 @@
       <c r="C139" s="25"/>
       <c r="D139" s="25"/>
       <c r="E139" s="25"/>
-      <c r="F139" s="79"/>
-      <c r="G139" s="86"/>
-      <c r="H139" s="82"/>
+      <c r="F139" s="64"/>
+      <c r="G139" s="71"/>
+      <c r="H139" s="67"/>
       <c r="I139" s="25"/>
       <c r="J139" s="26"/>
       <c r="K139" s="40"/>
@@ -5858,9 +5881,9 @@
       <c r="C140" s="25"/>
       <c r="D140" s="25"/>
       <c r="E140" s="25"/>
-      <c r="F140" s="79"/>
-      <c r="G140" s="86"/>
-      <c r="H140" s="82"/>
+      <c r="F140" s="64"/>
+      <c r="G140" s="71"/>
+      <c r="H140" s="67"/>
       <c r="I140" s="25"/>
       <c r="J140" s="26"/>
       <c r="K140" s="40"/>
@@ -5875,9 +5898,9 @@
       <c r="C141" s="25"/>
       <c r="D141" s="25"/>
       <c r="E141" s="25"/>
-      <c r="F141" s="79"/>
-      <c r="G141" s="86"/>
-      <c r="H141" s="82"/>
+      <c r="F141" s="64"/>
+      <c r="G141" s="71"/>
+      <c r="H141" s="67"/>
       <c r="I141" s="25"/>
       <c r="J141" s="26"/>
       <c r="K141" s="40"/>
@@ -5892,9 +5915,9 @@
       <c r="C142" s="25"/>
       <c r="D142" s="25"/>
       <c r="E142" s="25"/>
-      <c r="F142" s="79"/>
-      <c r="G142" s="86"/>
-      <c r="H142" s="82"/>
+      <c r="F142" s="64"/>
+      <c r="G142" s="71"/>
+      <c r="H142" s="67"/>
       <c r="I142" s="25"/>
       <c r="J142" s="26"/>
       <c r="K142" s="40"/>
@@ -5909,9 +5932,9 @@
       <c r="C143" s="25"/>
       <c r="D143" s="25"/>
       <c r="E143" s="25"/>
-      <c r="F143" s="79"/>
-      <c r="G143" s="86"/>
-      <c r="H143" s="82"/>
+      <c r="F143" s="64"/>
+      <c r="G143" s="71"/>
+      <c r="H143" s="67"/>
       <c r="I143" s="25"/>
       <c r="J143" s="26"/>
       <c r="K143" s="40"/>
@@ -5926,9 +5949,9 @@
       <c r="C144" s="25"/>
       <c r="D144" s="25"/>
       <c r="E144" s="25"/>
-      <c r="F144" s="79"/>
-      <c r="G144" s="86"/>
-      <c r="H144" s="82"/>
+      <c r="F144" s="64"/>
+      <c r="G144" s="71"/>
+      <c r="H144" s="67"/>
       <c r="I144" s="25"/>
       <c r="J144" s="26"/>
       <c r="K144" s="40"/>
@@ -5943,9 +5966,9 @@
       <c r="C145" s="25"/>
       <c r="D145" s="25"/>
       <c r="E145" s="25"/>
-      <c r="F145" s="79"/>
-      <c r="G145" s="86"/>
-      <c r="H145" s="82"/>
+      <c r="F145" s="64"/>
+      <c r="G145" s="71"/>
+      <c r="H145" s="67"/>
       <c r="I145" s="25"/>
       <c r="J145" s="26"/>
       <c r="K145" s="40"/>
@@ -5960,9 +5983,9 @@
       <c r="C146" s="25"/>
       <c r="D146" s="25"/>
       <c r="E146" s="25"/>
-      <c r="F146" s="79"/>
-      <c r="G146" s="86"/>
-      <c r="H146" s="82"/>
+      <c r="F146" s="64"/>
+      <c r="G146" s="71"/>
+      <c r="H146" s="67"/>
       <c r="I146" s="25"/>
       <c r="J146" s="26"/>
       <c r="K146" s="40"/>
@@ -5977,9 +6000,9 @@
       <c r="C147" s="25"/>
       <c r="D147" s="25"/>
       <c r="E147" s="25"/>
-      <c r="F147" s="79"/>
-      <c r="G147" s="86"/>
-      <c r="H147" s="82"/>
+      <c r="F147" s="64"/>
+      <c r="G147" s="71"/>
+      <c r="H147" s="67"/>
       <c r="I147" s="25"/>
       <c r="J147" s="26"/>
       <c r="K147" s="40"/>
@@ -5994,9 +6017,9 @@
       <c r="C148" s="25"/>
       <c r="D148" s="25"/>
       <c r="E148" s="25"/>
-      <c r="F148" s="79"/>
-      <c r="G148" s="86"/>
-      <c r="H148" s="82"/>
+      <c r="F148" s="64"/>
+      <c r="G148" s="71"/>
+      <c r="H148" s="67"/>
       <c r="I148" s="25"/>
       <c r="J148" s="26"/>
       <c r="K148" s="40"/>
@@ -6011,9 +6034,9 @@
       <c r="C149" s="25"/>
       <c r="D149" s="25"/>
       <c r="E149" s="25"/>
-      <c r="F149" s="79"/>
-      <c r="G149" s="86"/>
-      <c r="H149" s="82"/>
+      <c r="F149" s="64"/>
+      <c r="G149" s="71"/>
+      <c r="H149" s="67"/>
       <c r="I149" s="25"/>
       <c r="J149" s="26"/>
       <c r="K149" s="40"/>
@@ -6028,9 +6051,9 @@
       <c r="C150" s="25"/>
       <c r="D150" s="25"/>
       <c r="E150" s="25"/>
-      <c r="F150" s="79"/>
-      <c r="G150" s="86"/>
-      <c r="H150" s="82"/>
+      <c r="F150" s="64"/>
+      <c r="G150" s="71"/>
+      <c r="H150" s="67"/>
       <c r="I150" s="25"/>
       <c r="J150" s="26"/>
       <c r="K150" s="40"/>
@@ -6045,9 +6068,9 @@
       <c r="C151" s="25"/>
       <c r="D151" s="25"/>
       <c r="E151" s="25"/>
-      <c r="F151" s="79"/>
-      <c r="G151" s="86"/>
-      <c r="H151" s="82"/>
+      <c r="F151" s="64"/>
+      <c r="G151" s="71"/>
+      <c r="H151" s="67"/>
       <c r="I151" s="25"/>
       <c r="J151" s="26"/>
       <c r="K151" s="40"/>
@@ -6062,9 +6085,9 @@
       <c r="C152" s="25"/>
       <c r="D152" s="25"/>
       <c r="E152" s="25"/>
-      <c r="F152" s="79"/>
-      <c r="G152" s="86"/>
-      <c r="H152" s="82"/>
+      <c r="F152" s="64"/>
+      <c r="G152" s="71"/>
+      <c r="H152" s="67"/>
       <c r="I152" s="25"/>
       <c r="J152" s="26"/>
       <c r="K152" s="40"/>
@@ -6079,9 +6102,9 @@
       <c r="C153" s="25"/>
       <c r="D153" s="25"/>
       <c r="E153" s="25"/>
-      <c r="F153" s="79"/>
-      <c r="G153" s="86"/>
-      <c r="H153" s="82"/>
+      <c r="F153" s="64"/>
+      <c r="G153" s="71"/>
+      <c r="H153" s="67"/>
       <c r="I153" s="25"/>
       <c r="J153" s="26"/>
       <c r="K153" s="40"/>
@@ -6096,9 +6119,9 @@
       <c r="C154" s="25"/>
       <c r="D154" s="25"/>
       <c r="E154" s="25"/>
-      <c r="F154" s="79"/>
-      <c r="G154" s="86"/>
-      <c r="H154" s="82"/>
+      <c r="F154" s="64"/>
+      <c r="G154" s="71"/>
+      <c r="H154" s="67"/>
       <c r="I154" s="25"/>
       <c r="J154" s="26"/>
       <c r="K154" s="40"/>
@@ -6113,9 +6136,9 @@
       <c r="C155" s="25"/>
       <c r="D155" s="25"/>
       <c r="E155" s="25"/>
-      <c r="F155" s="79"/>
-      <c r="G155" s="86"/>
-      <c r="H155" s="82"/>
+      <c r="F155" s="64"/>
+      <c r="G155" s="71"/>
+      <c r="H155" s="67"/>
       <c r="I155" s="25"/>
       <c r="J155" s="26"/>
       <c r="K155" s="40"/>
@@ -6130,9 +6153,9 @@
       <c r="C156" s="25"/>
       <c r="D156" s="25"/>
       <c r="E156" s="25"/>
-      <c r="F156" s="79"/>
-      <c r="G156" s="86"/>
-      <c r="H156" s="82"/>
+      <c r="F156" s="64"/>
+      <c r="G156" s="71"/>
+      <c r="H156" s="67"/>
       <c r="I156" s="25"/>
       <c r="J156" s="26"/>
       <c r="K156" s="40"/>
@@ -6147,9 +6170,9 @@
       <c r="C157" s="25"/>
       <c r="D157" s="25"/>
       <c r="E157" s="25"/>
-      <c r="F157" s="79"/>
-      <c r="G157" s="86"/>
-      <c r="H157" s="82"/>
+      <c r="F157" s="64"/>
+      <c r="G157" s="71"/>
+      <c r="H157" s="67"/>
       <c r="I157" s="25"/>
       <c r="J157" s="26"/>
       <c r="K157" s="40"/>
@@ -6164,9 +6187,9 @@
       <c r="C158" s="25"/>
       <c r="D158" s="25"/>
       <c r="E158" s="25"/>
-      <c r="F158" s="79"/>
-      <c r="G158" s="86"/>
-      <c r="H158" s="82"/>
+      <c r="F158" s="64"/>
+      <c r="G158" s="71"/>
+      <c r="H158" s="67"/>
       <c r="I158" s="25"/>
       <c r="J158" s="26"/>
       <c r="K158" s="40"/>

</xml_diff>

<commit_message>
update srs and rtm for adding requirment in del user
</commit_message>
<xml_diff>
--- a/RTM/Traceability_Matrix learning hub ver 2.xlsx
+++ b/RTM/Traceability_Matrix learning hub ver 2.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed Mazrouaa\Documents\GitHub\learning-hub\RTM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95F1CC9-15DA-40C8-87C1-2E9AE3409296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" state="hidden" r:id="rId1"/>
@@ -20,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>eze3</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -44,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -63,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -82,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0">
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -101,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0">
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -120,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0">
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -139,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0">
+    <comment ref="K5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -158,7 +164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L5" authorId="0">
+    <comment ref="L5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -182,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="304">
   <si>
     <t>For detail regarding the practice of Requirements Management, please refer to the Requirements Management Practices Guide</t>
   </si>
@@ -766,54 +772,6 @@
     <t>SRS-LOGOUT-001</t>
   </si>
   <si>
-    <t>084</t>
-  </si>
-  <si>
-    <t>085</t>
-  </si>
-  <si>
-    <t>086</t>
-  </si>
-  <si>
-    <t>087</t>
-  </si>
-  <si>
-    <t>088</t>
-  </si>
-  <si>
-    <t>089</t>
-  </si>
-  <si>
-    <t>090</t>
-  </si>
-  <si>
-    <t>091</t>
-  </si>
-  <si>
-    <t>092</t>
-  </si>
-  <si>
-    <t>093</t>
-  </si>
-  <si>
-    <t>094</t>
-  </si>
-  <si>
-    <t>095</t>
-  </si>
-  <si>
-    <t>096</t>
-  </si>
-  <si>
-    <t>097</t>
-  </si>
-  <si>
-    <t>098</t>
-  </si>
-  <si>
-    <t>099</t>
-  </si>
-  <si>
     <t>100</t>
   </si>
   <si>
@@ -1300,11 +1258,89 @@
   <si>
     <t>054</t>
   </si>
+  <si>
+    <t>SRS-DELUSR-003</t>
+  </si>
+  <si>
+    <t>055</t>
+  </si>
+  <si>
+    <t>056</t>
+  </si>
+  <si>
+    <t>057</t>
+  </si>
+  <si>
+    <t>058</t>
+  </si>
+  <si>
+    <t>059</t>
+  </si>
+  <si>
+    <t>060</t>
+  </si>
+  <si>
+    <t>061</t>
+  </si>
+  <si>
+    <t>062</t>
+  </si>
+  <si>
+    <t>063</t>
+  </si>
+  <si>
+    <t>064</t>
+  </si>
+  <si>
+    <t>065</t>
+  </si>
+  <si>
+    <t>066</t>
+  </si>
+  <si>
+    <t>067</t>
+  </si>
+  <si>
+    <t>068</t>
+  </si>
+  <si>
+    <t>069</t>
+  </si>
+  <si>
+    <t>070</t>
+  </si>
+  <si>
+    <t>071</t>
+  </si>
+  <si>
+    <t>072</t>
+  </si>
+  <si>
+    <t>073</t>
+  </si>
+  <si>
+    <t>074</t>
+  </si>
+  <si>
+    <t>075</t>
+  </si>
+  <si>
+    <t>076</t>
+  </si>
+  <si>
+    <t>077</t>
+  </si>
+  <si>
+    <t>078</t>
+  </si>
+  <si>
+    <t>CRS-8.3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -2392,7 +2428,7 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2728,32 +2764,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B20"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="43" customWidth="1"/>
-    <col min="2" max="2" width="58.85546875" style="44" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="44"/>
+    <col min="1" max="1" width="5.33203125" style="43" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" style="44" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="44"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B2" s="45" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A4" s="93" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="94"/>
     </row>
-    <row r="5" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
         <v>2</v>
       </c>
@@ -2761,7 +2797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
         <v>4</v>
       </c>
@@ -2769,72 +2805,72 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B7" s="50" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B8" s="50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B9" s="50" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B10" s="50" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B11" s="50" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B12" s="50" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B13" s="50" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B14" s="50" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B15" s="50" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B16" s="50" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B17" s="50" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B18" s="50" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B19" s="50" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B20" s="51" t="s">
         <v>19</v>
       </c>
@@ -2850,31 +2886,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M158"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54:H55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="55.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="47.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="47.28515625" style="72" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="35.88671875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="55.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="47.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="47.33203125" style="72" customWidth="1"/>
     <col min="8" max="8" width="51" style="5" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" style="6" customWidth="1"/>
     <col min="13" max="13" width="86" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>20</v>
       </c>
@@ -2893,7 +2929,7 @@
       <c r="L1" s="9"/>
       <c r="M1" s="10"/>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
@@ -2912,7 +2948,7 @@
       <c r="L2" s="28"/>
       <c r="M2" s="29"/>
     </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>23</v>
       </c>
@@ -2931,7 +2967,7 @@
       <c r="L3" s="28"/>
       <c r="M3" s="29"/>
     </row>
-    <row r="4" spans="1:13" s="2" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="2" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>25</v>
       </c>
@@ -2950,7 +2986,7 @@
       <c r="L4" s="28"/>
       <c r="M4" s="30"/>
     </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="3" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
@@ -2961,19 +2997,19 @@
         <v>29</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="F5" s="57" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="G5" s="60" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="H5" s="59" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="I5" s="52" t="s">
         <v>30</v>
@@ -2991,7 +3027,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>35</v>
       </c>
@@ -3002,19 +3038,19 @@
         <v>37</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="E6" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F6" s="62" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="G6" s="69" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="H6" s="65" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="I6" s="18"/>
       <c r="J6" s="19"/>
@@ -3022,7 +3058,7 @@
       <c r="L6" s="35"/>
       <c r="M6" s="36"/>
     </row>
-    <row r="7" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>38</v>
       </c>
@@ -3033,19 +3069,19 @@
         <v>37</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="E7" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F7" s="61" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="G7" s="69" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="H7" s="65" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="I7" s="20"/>
       <c r="J7" s="21"/>
@@ -3053,7 +3089,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="39"/>
     </row>
-    <row r="8" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>40</v>
       </c>
@@ -3064,19 +3100,19 @@
         <v>37</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="E8" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F8" s="61" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="G8" s="69" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="H8" s="65" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="I8" s="20"/>
       <c r="J8" s="21"/>
@@ -3084,7 +3120,7 @@
       <c r="L8" s="38"/>
       <c r="M8" s="39"/>
     </row>
-    <row r="9" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>42</v>
       </c>
@@ -3095,17 +3131,17 @@
         <v>44</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="E9" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F9" s="61" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="65" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="I9" s="20"/>
       <c r="J9" s="21"/>
@@ -3113,7 +3149,7 @@
       <c r="L9" s="38"/>
       <c r="M9" s="39"/>
     </row>
-    <row r="10" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>45</v>
       </c>
@@ -3124,19 +3160,19 @@
         <v>47</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="E10" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F10" s="61" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="G10" s="69" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="H10" s="65" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="I10" s="20"/>
       <c r="J10" s="21"/>
@@ -3144,7 +3180,7 @@
       <c r="L10" s="38"/>
       <c r="M10" s="39"/>
     </row>
-    <row r="11" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>48</v>
       </c>
@@ -3155,19 +3191,19 @@
         <v>47</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="E11" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F11" s="61" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="G11" s="69" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="H11" s="65" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="I11" s="20"/>
       <c r="J11" s="21"/>
@@ -3175,7 +3211,7 @@
       <c r="L11" s="38"/>
       <c r="M11" s="39"/>
     </row>
-    <row r="12" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>50</v>
       </c>
@@ -3186,19 +3222,19 @@
         <v>47</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="E12" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F12" s="61" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="G12" s="69" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="H12" s="65" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="I12" s="20"/>
       <c r="J12" s="21"/>
@@ -3206,7 +3242,7 @@
       <c r="L12" s="38"/>
       <c r="M12" s="39"/>
     </row>
-    <row r="13" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>52</v>
       </c>
@@ -3217,19 +3253,19 @@
         <v>47</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="E13" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F13" s="61" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="G13" s="69" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="H13" s="65" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="I13" s="20"/>
       <c r="J13" s="21"/>
@@ -3237,28 +3273,28 @@
       <c r="L13" s="38"/>
       <c r="M13" s="39"/>
     </row>
-    <row r="14" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="B14" s="54" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="C14" s="23" t="s">
         <v>47</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="E14" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F14" s="61" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="65" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="I14" s="20"/>
       <c r="J14" s="21"/>
@@ -3266,7 +3302,7 @@
       <c r="L14" s="38"/>
       <c r="M14" s="39"/>
     </row>
-    <row r="15" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>54</v>
       </c>
@@ -3277,17 +3313,17 @@
         <v>56</v>
       </c>
       <c r="D15" s="75" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="E15" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F15" s="73" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="G15" s="76"/>
       <c r="H15" s="66" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="I15" s="20"/>
       <c r="J15" s="21"/>
@@ -3295,9 +3331,9 @@
       <c r="L15" s="38"/>
       <c r="M15" s="39"/>
     </row>
-    <row r="16" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="B16" s="55" t="s">
         <v>57</v>
@@ -3306,17 +3342,17 @@
         <v>56</v>
       </c>
       <c r="D16" s="75" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="E16" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F16" s="73" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="G16" s="56"/>
       <c r="H16" s="66" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="I16" s="20"/>
       <c r="J16" s="21"/>
@@ -3324,7 +3360,7 @@
       <c r="L16" s="38"/>
       <c r="M16" s="39"/>
     </row>
-    <row r="17" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>58</v>
       </c>
@@ -3335,17 +3371,17 @@
         <v>56</v>
       </c>
       <c r="D17" s="75" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="E17" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F17" s="73" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="G17" s="56"/>
       <c r="H17" s="66" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="I17" s="20"/>
       <c r="J17" s="21"/>
@@ -3353,7 +3389,7 @@
       <c r="L17" s="38"/>
       <c r="M17" s="39"/>
     </row>
-    <row r="18" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>60</v>
       </c>
@@ -3365,12 +3401,12 @@
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F18" s="63"/>
       <c r="G18" s="56"/>
       <c r="H18" s="66" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="I18" s="20"/>
       <c r="J18" s="21"/>
@@ -3378,24 +3414,24 @@
       <c r="L18" s="38"/>
       <c r="M18" s="39"/>
     </row>
-    <row r="19" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
       <c r="B19" s="55" t="s">
         <v>65</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F19" s="63"/>
       <c r="G19" s="56"/>
       <c r="H19" s="66" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="I19" s="20"/>
       <c r="J19" s="21"/>
@@ -3403,7 +3439,7 @@
       <c r="L19" s="38"/>
       <c r="M19" s="39"/>
     </row>
-    <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>61</v>
       </c>
@@ -3415,12 +3451,12 @@
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F20" s="63"/>
       <c r="G20" s="56"/>
       <c r="H20" s="66" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="I20" s="20"/>
       <c r="J20" s="21"/>
@@ -3428,7 +3464,7 @@
       <c r="L20" s="38"/>
       <c r="M20" s="39"/>
     </row>
-    <row r="21" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>64</v>
       </c>
@@ -3436,16 +3472,16 @@
         <v>70</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F21" s="63"/>
       <c r="G21" s="56"/>
       <c r="H21" s="66" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="I21" s="20"/>
       <c r="J21" s="21"/>
@@ -3453,7 +3489,7 @@
       <c r="L21" s="38"/>
       <c r="M21" s="39"/>
     </row>
-    <row r="22" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>67</v>
       </c>
@@ -3464,19 +3500,19 @@
         <v>73</v>
       </c>
       <c r="D22" s="75" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="E22" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F22" s="73" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="G22" s="73" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="H22" s="66" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="I22" s="20"/>
       <c r="J22" s="21"/>
@@ -3484,7 +3520,7 @@
       <c r="L22" s="38"/>
       <c r="M22" s="39"/>
     </row>
-    <row r="23" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>69</v>
       </c>
@@ -3492,22 +3528,22 @@
         <v>75</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="D23" s="75" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="E23" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F23" s="73" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="G23" s="73" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="H23" s="66" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="I23" s="20"/>
       <c r="J23" s="21"/>
@@ -3515,9 +3551,9 @@
       <c r="L23" s="38"/>
       <c r="M23" s="39"/>
     </row>
-    <row r="24" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="B24" s="55" t="s">
         <v>77</v>
@@ -3526,19 +3562,19 @@
         <v>73</v>
       </c>
       <c r="D24" s="75" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="E24" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F24" s="73" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="G24" s="73" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="H24" s="66" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="I24" s="20"/>
       <c r="J24" s="21"/>
@@ -3546,7 +3582,7 @@
       <c r="L24" s="38"/>
       <c r="M24" s="39"/>
     </row>
-    <row r="25" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
         <v>71</v>
       </c>
@@ -3554,22 +3590,22 @@
         <v>79</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="D25" s="75" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="E25" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F25" s="73" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="G25" s="73" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="H25" s="66" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="I25" s="20"/>
       <c r="J25" s="21"/>
@@ -3577,7 +3613,7 @@
       <c r="L25" s="38"/>
       <c r="M25" s="39"/>
     </row>
-    <row r="26" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
         <v>74</v>
       </c>
@@ -3585,22 +3621,22 @@
         <v>81</v>
       </c>
       <c r="C26" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="D26" s="75" t="s">
+        <v>253</v>
+      </c>
+      <c r="E26" s="62" t="s">
+        <v>237</v>
+      </c>
+      <c r="F26" s="73" t="s">
+        <v>242</v>
+      </c>
+      <c r="G26" s="73" t="s">
+        <v>243</v>
+      </c>
+      <c r="H26" s="66" t="s">
         <v>223</v>
-      </c>
-      <c r="D26" s="75" t="s">
-        <v>269</v>
-      </c>
-      <c r="E26" s="62" t="s">
-        <v>253</v>
-      </c>
-      <c r="F26" s="73" t="s">
-        <v>258</v>
-      </c>
-      <c r="G26" s="73" t="s">
-        <v>259</v>
-      </c>
-      <c r="H26" s="66" t="s">
-        <v>239</v>
       </c>
       <c r="I26" s="20"/>
       <c r="J26" s="21"/>
@@ -3608,7 +3644,7 @@
       <c r="L26" s="38"/>
       <c r="M26" s="39"/>
     </row>
-    <row r="27" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
         <v>76</v>
       </c>
@@ -3619,19 +3655,19 @@
         <v>73</v>
       </c>
       <c r="D27" s="75" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="E27" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F27" s="73" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="G27" s="73" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="H27" s="66" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="I27" s="20"/>
       <c r="J27" s="21"/>
@@ -3639,7 +3675,7 @@
       <c r="L27" s="38"/>
       <c r="M27" s="39"/>
     </row>
-    <row r="28" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
         <v>78</v>
       </c>
@@ -3647,22 +3683,22 @@
         <v>85</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="D28" s="75" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="E28" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F28" s="73" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="G28" s="73" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="H28" s="66" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="I28" s="20"/>
       <c r="J28" s="21"/>
@@ -3670,7 +3706,7 @@
       <c r="L28" s="38"/>
       <c r="M28" s="39"/>
     </row>
-    <row r="29" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
         <v>80</v>
       </c>
@@ -3678,22 +3714,22 @@
         <v>87</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="D29" s="75" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="E29" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F29" s="73" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="G29" s="73" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="H29" s="66" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="I29" s="20"/>
       <c r="J29" s="21"/>
@@ -3701,7 +3737,7 @@
       <c r="L29" s="38"/>
       <c r="M29" s="39"/>
     </row>
-    <row r="30" spans="1:13" s="86" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="86" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A30" s="78" t="s">
         <v>82</v>
       </c>
@@ -3713,16 +3749,16 @@
       </c>
       <c r="D30" s="74"/>
       <c r="E30" s="73" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F30" s="73" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="G30" s="73" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="H30" s="81" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="I30" s="74"/>
       <c r="J30" s="82"/>
@@ -3730,25 +3766,25 @@
       <c r="L30" s="84"/>
       <c r="M30" s="85"/>
     </row>
-    <row r="31" spans="1:13" s="86" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="86" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="78" t="s">
         <v>84</v>
       </c>
       <c r="B31" s="79" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="C31" s="87" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="D31" s="74"/>
       <c r="E31" s="73" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F31" s="73" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="G31" s="73" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="H31" s="81"/>
       <c r="I31" s="88"/>
@@ -3757,25 +3793,25 @@
       <c r="L31" s="91"/>
       <c r="M31" s="92"/>
     </row>
-    <row r="32" spans="1:13" s="86" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" s="86" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="78" t="s">
         <v>86</v>
       </c>
       <c r="B32" s="79" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="C32" s="87" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="D32" s="74"/>
       <c r="E32" s="73" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F32" s="73" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="G32" s="73" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="H32" s="81"/>
       <c r="I32" s="88"/>
@@ -3784,7 +3820,7 @@
       <c r="L32" s="91"/>
       <c r="M32" s="92"/>
     </row>
-    <row r="33" spans="1:13" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="17" t="s">
         <v>88</v>
       </c>
@@ -3795,15 +3831,15 @@
         <v>90</v>
       </c>
       <c r="D33" s="75" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="E33" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F33" s="63"/>
       <c r="G33" s="56"/>
       <c r="H33" s="66" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="I33" s="25"/>
       <c r="J33" s="26"/>
@@ -3811,9 +3847,9 @@
       <c r="L33" s="41"/>
       <c r="M33" s="42"/>
     </row>
-    <row r="34" spans="1:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="B34" s="55" t="s">
         <v>95</v>
@@ -3822,15 +3858,15 @@
         <v>90</v>
       </c>
       <c r="D34" s="75" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="E34" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F34" s="63"/>
       <c r="G34" s="56"/>
       <c r="H34" s="66" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="I34" s="25"/>
       <c r="J34" s="26"/>
@@ -3838,9 +3874,9 @@
       <c r="L34" s="41"/>
       <c r="M34" s="42"/>
     </row>
-    <row r="35" spans="1:13" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="17" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="B35" s="55" t="s">
         <v>97</v>
@@ -3849,15 +3885,15 @@
         <v>90</v>
       </c>
       <c r="D35" s="75" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="E35" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F35" s="63"/>
       <c r="G35" s="56"/>
       <c r="H35" s="66" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="I35" s="25"/>
       <c r="J35" s="26"/>
@@ -3865,9 +3901,9 @@
       <c r="L35" s="41"/>
       <c r="M35" s="42"/>
     </row>
-    <row r="36" spans="1:13" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="17" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="B36" s="55" t="s">
         <v>99</v>
@@ -3876,15 +3912,15 @@
         <v>91</v>
       </c>
       <c r="D36" s="75" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="E36" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F36" s="63"/>
       <c r="G36" s="56"/>
       <c r="H36" s="66" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="I36" s="25"/>
       <c r="J36" s="26"/>
@@ -3892,9 +3928,9 @@
       <c r="L36" s="41"/>
       <c r="M36" s="42"/>
     </row>
-    <row r="37" spans="1:13" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="17" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="B37" s="55" t="s">
         <v>101</v>
@@ -3903,15 +3939,15 @@
         <v>91</v>
       </c>
       <c r="D37" s="75" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="E37" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F37" s="63"/>
       <c r="G37" s="56"/>
       <c r="H37" s="66" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="I37" s="25"/>
       <c r="J37" s="26"/>
@@ -3919,9 +3955,9 @@
       <c r="L37" s="41"/>
       <c r="M37" s="42"/>
     </row>
-    <row r="38" spans="1:13" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="17" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="B38" s="55" t="s">
         <v>103</v>
@@ -3930,15 +3966,15 @@
         <v>91</v>
       </c>
       <c r="D38" s="75" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="E38" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F38" s="63"/>
       <c r="G38" s="56"/>
       <c r="H38" s="66" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="I38" s="25"/>
       <c r="J38" s="26"/>
@@ -3946,9 +3982,9 @@
       <c r="L38" s="41"/>
       <c r="M38" s="42"/>
     </row>
-    <row r="39" spans="1:13" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="17" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="B39" s="55" t="s">
         <v>105</v>
@@ -3957,15 +3993,15 @@
         <v>90</v>
       </c>
       <c r="D39" s="75" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="E39" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F39" s="63"/>
       <c r="G39" s="56"/>
       <c r="H39" s="66" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="I39" s="25"/>
       <c r="J39" s="26"/>
@@ -3973,26 +4009,26 @@
       <c r="L39" s="41"/>
       <c r="M39" s="42"/>
     </row>
-    <row r="40" spans="1:13" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="17" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="B40" s="55" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="C40" s="77" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="D40" s="75" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="E40" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F40" s="63"/>
       <c r="G40" s="56"/>
       <c r="H40" s="66" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="I40" s="25"/>
       <c r="J40" s="26"/>
@@ -4000,26 +4036,26 @@
       <c r="L40" s="41"/>
       <c r="M40" s="42"/>
     </row>
-    <row r="41" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="17" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="B41" s="55" t="s">
         <v>106</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="D41" s="75" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="E41" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F41" s="73"/>
       <c r="G41" s="56"/>
       <c r="H41" s="66" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="I41" s="25"/>
       <c r="J41" s="26"/>
@@ -4027,26 +4063,26 @@
       <c r="L41" s="41"/>
       <c r="M41" s="42"/>
     </row>
-    <row r="42" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="17" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="B42" s="55" t="s">
         <v>107</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="D42" s="75" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="E42" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F42" s="73"/>
       <c r="G42" s="56"/>
       <c r="H42" s="66" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="I42" s="25"/>
       <c r="J42" s="26"/>
@@ -4054,9 +4090,9 @@
       <c r="L42" s="41"/>
       <c r="M42" s="42"/>
     </row>
-    <row r="43" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="17" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="B43" s="55" t="s">
         <v>108</v>
@@ -4065,15 +4101,15 @@
         <v>37</v>
       </c>
       <c r="D43" s="75" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="E43" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F43" s="63"/>
       <c r="G43" s="56"/>
       <c r="H43" s="66" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="I43" s="25"/>
       <c r="J43" s="26"/>
@@ -4081,9 +4117,9 @@
       <c r="L43" s="41"/>
       <c r="M43" s="42"/>
     </row>
-    <row r="44" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="17" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
       <c r="B44" s="55" t="s">
         <v>109</v>
@@ -4092,15 +4128,15 @@
         <v>37</v>
       </c>
       <c r="D44" s="75" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="E44" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F44" s="63"/>
       <c r="G44" s="56"/>
       <c r="H44" s="66" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="I44" s="25"/>
       <c r="J44" s="26"/>
@@ -4108,9 +4144,9 @@
       <c r="L44" s="41"/>
       <c r="M44" s="42"/>
     </row>
-    <row r="45" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="17" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="B45" s="55" t="s">
         <v>110</v>
@@ -4119,15 +4155,15 @@
         <v>37</v>
       </c>
       <c r="D45" s="75" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="E45" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F45" s="63"/>
       <c r="G45" s="56"/>
       <c r="H45" s="66" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="I45" s="25"/>
       <c r="J45" s="26"/>
@@ -4135,9 +4171,9 @@
       <c r="L45" s="41"/>
       <c r="M45" s="42"/>
     </row>
-    <row r="46" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="17" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="B46" s="55" t="s">
         <v>111</v>
@@ -4146,15 +4182,15 @@
         <v>44</v>
       </c>
       <c r="D46" s="75" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="E46" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F46" s="63"/>
       <c r="G46" s="56"/>
       <c r="H46" s="66" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="I46" s="25"/>
       <c r="J46" s="26"/>
@@ -4162,9 +4198,9 @@
       <c r="L46" s="41"/>
       <c r="M46" s="42"/>
     </row>
-    <row r="47" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="17" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="B47" s="55" t="s">
         <v>112</v>
@@ -4173,15 +4209,15 @@
         <v>47</v>
       </c>
       <c r="D47" s="75" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="E47" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F47" s="63"/>
       <c r="G47" s="56"/>
       <c r="H47" s="66" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="I47" s="25"/>
       <c r="J47" s="26"/>
@@ -4189,7 +4225,7 @@
       <c r="L47" s="41"/>
       <c r="M47" s="42"/>
     </row>
-    <row r="48" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="17" t="s">
         <v>92</v>
       </c>
@@ -4200,15 +4236,15 @@
         <v>47</v>
       </c>
       <c r="D48" s="75" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="E48" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F48" s="63"/>
       <c r="G48" s="56"/>
       <c r="H48" s="66" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="I48" s="25"/>
       <c r="J48" s="26"/>
@@ -4216,7 +4252,7 @@
       <c r="L48" s="41"/>
       <c r="M48" s="42"/>
     </row>
-    <row r="49" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="17" t="s">
         <v>94</v>
       </c>
@@ -4227,15 +4263,15 @@
         <v>47</v>
       </c>
       <c r="D49" s="75" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="E49" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F49" s="63"/>
       <c r="G49" s="56"/>
       <c r="H49" s="66" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="I49" s="25"/>
       <c r="J49" s="26"/>
@@ -4243,7 +4279,7 @@
       <c r="L49" s="41"/>
       <c r="M49" s="42"/>
     </row>
-    <row r="50" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="17" t="s">
         <v>96</v>
       </c>
@@ -4254,15 +4290,15 @@
         <v>47</v>
       </c>
       <c r="D50" s="75" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="E50" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F50" s="63"/>
       <c r="G50" s="56"/>
       <c r="H50" s="66" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="I50" s="25"/>
       <c r="J50" s="26"/>
@@ -4270,7 +4306,7 @@
       <c r="L50" s="41"/>
       <c r="M50" s="42"/>
     </row>
-    <row r="51" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="17" t="s">
         <v>98</v>
       </c>
@@ -4278,18 +4314,18 @@
         <v>116</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="D51" s="75" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="E51" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F51" s="63"/>
       <c r="G51" s="56"/>
       <c r="H51" s="66" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="I51" s="25"/>
       <c r="J51" s="26"/>
@@ -4297,26 +4333,26 @@
       <c r="L51" s="41"/>
       <c r="M51" s="42"/>
     </row>
-    <row r="52" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="17" t="s">
         <v>100</v>
       </c>
       <c r="B52" s="55" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="D52" s="75" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="E52" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F52" s="63"/>
       <c r="G52" s="56"/>
       <c r="H52" s="66" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="I52" s="25"/>
       <c r="J52" s="26"/>
@@ -4324,7 +4360,7 @@
       <c r="L52" s="41"/>
       <c r="M52" s="42"/>
     </row>
-    <row r="53" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="17" t="s">
         <v>102</v>
       </c>
@@ -4332,18 +4368,18 @@
         <v>117</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="D53" s="75" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="E53" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F53" s="63"/>
       <c r="G53" s="56"/>
       <c r="H53" s="66" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="I53" s="25"/>
       <c r="J53" s="26"/>
@@ -4351,7 +4387,7 @@
       <c r="L53" s="41"/>
       <c r="M53" s="42"/>
     </row>
-    <row r="54" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="17" t="s">
         <v>104</v>
       </c>
@@ -4359,18 +4395,18 @@
         <v>118</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="D54" s="75" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="E54" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F54" s="63"/>
       <c r="G54" s="56"/>
       <c r="H54" s="66" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="I54" s="25"/>
       <c r="J54" s="26"/>
@@ -4378,30 +4414,26 @@
       <c r="L54" s="41"/>
       <c r="M54" s="42"/>
     </row>
-    <row r="55" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="B55" s="55" t="s">
-        <v>230</v>
+        <v>273</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>278</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>217</v>
+        <v>303</v>
       </c>
       <c r="D55" s="75" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="E55" s="62" t="s">
-        <v>253</v>
-      </c>
-      <c r="F55" s="73" t="s">
-        <v>265</v>
-      </c>
-      <c r="G55" s="75" t="s">
-        <v>267</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="F55" s="63"/>
+      <c r="G55" s="56"/>
       <c r="H55" s="66" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="I55" s="25"/>
       <c r="J55" s="26"/>
@@ -4409,30 +4441,30 @@
       <c r="L55" s="41"/>
       <c r="M55" s="42"/>
     </row>
-    <row r="56" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="17" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="B56" s="55" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>234</v>
+        <v>201</v>
       </c>
       <c r="D56" s="75" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="E56" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F56" s="73" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="G56" s="75" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="H56" s="66" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="I56" s="25"/>
       <c r="J56" s="26"/>
@@ -4440,30 +4472,30 @@
       <c r="L56" s="41"/>
       <c r="M56" s="42"/>
     </row>
-    <row r="57" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
       <c r="B57" s="55" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D57" s="75" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="E57" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F57" s="73" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="G57" s="75" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="H57" s="66" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="I57" s="25"/>
       <c r="J57" s="26"/>
@@ -4471,30 +4503,30 @@
       <c r="L57" s="41"/>
       <c r="M57" s="42"/>
     </row>
-    <row r="58" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="17" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="B58" s="55" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>235</v>
+        <v>201</v>
       </c>
       <c r="D58" s="75" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="E58" s="62" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F58" s="73" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="G58" s="75" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="H58" s="66" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="I58" s="25"/>
       <c r="J58" s="26"/>
@@ -4502,24 +4534,30 @@
       <c r="L58" s="41"/>
       <c r="M58" s="42"/>
     </row>
-    <row r="59" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="B59" s="55" t="s">
-        <v>119</v>
+        <v>217</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="D59" s="20"/>
+        <v>219</v>
+      </c>
+      <c r="D59" s="75" t="s">
+        <v>250</v>
+      </c>
       <c r="E59" s="62" t="s">
-        <v>253</v>
-      </c>
-      <c r="F59" s="63"/>
-      <c r="G59" s="56"/>
+        <v>237</v>
+      </c>
+      <c r="F59" s="73" t="s">
+        <v>249</v>
+      </c>
+      <c r="G59" s="75" t="s">
+        <v>251</v>
+      </c>
       <c r="H59" s="66" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="I59" s="25"/>
       <c r="J59" s="26"/>
@@ -4527,28 +4565,40 @@
       <c r="L59" s="41"/>
       <c r="M59" s="42"/>
     </row>
-    <row r="60" spans="1:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="24"/>
-      <c r="B60" s="102"/>
-      <c r="C60" s="103"/>
-      <c r="D60" s="103"/>
-      <c r="E60" s="103"/>
-      <c r="F60" s="104"/>
-      <c r="G60" s="70"/>
-      <c r="H60" s="58"/>
+    <row r="60" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="B60" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="C60" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="D60" s="20"/>
+      <c r="E60" s="62" t="s">
+        <v>237</v>
+      </c>
+      <c r="F60" s="63"/>
+      <c r="G60" s="56"/>
+      <c r="H60" s="66" t="s">
+        <v>222</v>
+      </c>
       <c r="I60" s="25"/>
       <c r="J60" s="26"/>
       <c r="K60" s="40"/>
       <c r="L60" s="41"/>
       <c r="M60" s="42"/>
     </row>
-    <row r="61" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="24"/>
-      <c r="B61" s="105"/>
-      <c r="C61" s="106"/>
-      <c r="D61" s="106"/>
-      <c r="E61" s="106"/>
-      <c r="F61" s="107"/>
+    <row r="61" spans="1:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="B61" s="102"/>
+      <c r="C61" s="103"/>
+      <c r="D61" s="103"/>
+      <c r="E61" s="103"/>
+      <c r="F61" s="104"/>
       <c r="G61" s="70"/>
       <c r="H61" s="58"/>
       <c r="I61" s="25"/>
@@ -4557,8 +4607,10 @@
       <c r="L61" s="41"/>
       <c r="M61" s="42"/>
     </row>
-    <row r="62" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="24"/>
+    <row r="62" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="17" t="s">
+        <v>281</v>
+      </c>
       <c r="B62" s="105"/>
       <c r="C62" s="106"/>
       <c r="D62" s="106"/>
@@ -4572,8 +4624,10 @@
       <c r="L62" s="41"/>
       <c r="M62" s="42"/>
     </row>
-    <row r="63" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="24"/>
+    <row r="63" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="17" t="s">
+        <v>282</v>
+      </c>
       <c r="B63" s="105"/>
       <c r="C63" s="106"/>
       <c r="D63" s="106"/>
@@ -4587,8 +4641,10 @@
       <c r="L63" s="41"/>
       <c r="M63" s="42"/>
     </row>
-    <row r="64" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="24"/>
+    <row r="64" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="17" t="s">
+        <v>283</v>
+      </c>
       <c r="B64" s="105"/>
       <c r="C64" s="106"/>
       <c r="D64" s="106"/>
@@ -4602,8 +4658,10 @@
       <c r="L64" s="41"/>
       <c r="M64" s="42"/>
     </row>
-    <row r="65" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="24"/>
+    <row r="65" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="17" t="s">
+        <v>284</v>
+      </c>
       <c r="B65" s="105"/>
       <c r="C65" s="106"/>
       <c r="D65" s="106"/>
@@ -4617,8 +4675,10 @@
       <c r="L65" s="41"/>
       <c r="M65" s="42"/>
     </row>
-    <row r="66" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="24"/>
+    <row r="66" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="17" t="s">
+        <v>285</v>
+      </c>
       <c r="B66" s="105"/>
       <c r="C66" s="106"/>
       <c r="D66" s="106"/>
@@ -4632,9 +4692,9 @@
       <c r="L66" s="41"/>
       <c r="M66" s="42"/>
     </row>
-    <row r="67" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="24" t="s">
-        <v>120</v>
+    <row r="67" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="17" t="s">
+        <v>286</v>
       </c>
       <c r="B67" s="105"/>
       <c r="C67" s="106"/>
@@ -4649,26 +4709,26 @@
       <c r="L67" s="41"/>
       <c r="M67" s="42"/>
     </row>
-    <row r="68" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="B68" s="22"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="64"/>
-      <c r="G68" s="71"/>
-      <c r="H68" s="67"/>
+    <row r="68" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="B68" s="105"/>
+      <c r="C68" s="106"/>
+      <c r="D68" s="106"/>
+      <c r="E68" s="106"/>
+      <c r="F68" s="107"/>
+      <c r="G68" s="70"/>
+      <c r="H68" s="58"/>
       <c r="I68" s="25"/>
       <c r="J68" s="26"/>
       <c r="K68" s="40"/>
       <c r="L68" s="41"/>
       <c r="M68" s="42"/>
     </row>
-    <row r="69" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="24" t="s">
-        <v>122</v>
+    <row r="69" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="17" t="s">
+        <v>288</v>
       </c>
       <c r="B69" s="22"/>
       <c r="C69" s="25"/>
@@ -4683,9 +4743,9 @@
       <c r="L69" s="41"/>
       <c r="M69" s="42"/>
     </row>
-    <row r="70" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="24" t="s">
-        <v>123</v>
+    <row r="70" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="17" t="s">
+        <v>289</v>
       </c>
       <c r="B70" s="22"/>
       <c r="C70" s="25"/>
@@ -4700,9 +4760,9 @@
       <c r="L70" s="41"/>
       <c r="M70" s="42"/>
     </row>
-    <row r="71" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="24" t="s">
-        <v>124</v>
+    <row r="71" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="17" t="s">
+        <v>290</v>
       </c>
       <c r="B71" s="22"/>
       <c r="C71" s="25"/>
@@ -4717,9 +4777,9 @@
       <c r="L71" s="41"/>
       <c r="M71" s="42"/>
     </row>
-    <row r="72" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="24" t="s">
-        <v>125</v>
+    <row r="72" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="17" t="s">
+        <v>291</v>
       </c>
       <c r="B72" s="22"/>
       <c r="C72" s="25"/>
@@ -4734,9 +4794,9 @@
       <c r="L72" s="41"/>
       <c r="M72" s="42"/>
     </row>
-    <row r="73" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="24" t="s">
-        <v>126</v>
+    <row r="73" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="17" t="s">
+        <v>292</v>
       </c>
       <c r="B73" s="22"/>
       <c r="C73" s="25"/>
@@ -4751,9 +4811,9 @@
       <c r="L73" s="41"/>
       <c r="M73" s="42"/>
     </row>
-    <row r="74" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="24" t="s">
-        <v>127</v>
+    <row r="74" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="17" t="s">
+        <v>293</v>
       </c>
       <c r="B74" s="22"/>
       <c r="C74" s="25"/>
@@ -4768,9 +4828,9 @@
       <c r="L74" s="41"/>
       <c r="M74" s="42"/>
     </row>
-    <row r="75" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="24" t="s">
-        <v>128</v>
+    <row r="75" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="17" t="s">
+        <v>294</v>
       </c>
       <c r="B75" s="22"/>
       <c r="C75" s="25"/>
@@ -4785,9 +4845,9 @@
       <c r="L75" s="41"/>
       <c r="M75" s="42"/>
     </row>
-    <row r="76" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="24" t="s">
-        <v>129</v>
+    <row r="76" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="17" t="s">
+        <v>295</v>
       </c>
       <c r="B76" s="22"/>
       <c r="C76" s="25"/>
@@ -4802,9 +4862,9 @@
       <c r="L76" s="41"/>
       <c r="M76" s="42"/>
     </row>
-    <row r="77" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="24" t="s">
-        <v>130</v>
+    <row r="77" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="17" t="s">
+        <v>296</v>
       </c>
       <c r="B77" s="22"/>
       <c r="C77" s="25"/>
@@ -4819,9 +4879,9 @@
       <c r="L77" s="41"/>
       <c r="M77" s="42"/>
     </row>
-    <row r="78" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="24" t="s">
-        <v>131</v>
+    <row r="78" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="17" t="s">
+        <v>297</v>
       </c>
       <c r="B78" s="22"/>
       <c r="C78" s="25"/>
@@ -4836,9 +4896,9 @@
       <c r="L78" s="41"/>
       <c r="M78" s="42"/>
     </row>
-    <row r="79" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="24" t="s">
-        <v>132</v>
+    <row r="79" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="17" t="s">
+        <v>298</v>
       </c>
       <c r="B79" s="22"/>
       <c r="C79" s="25"/>
@@ -4853,9 +4913,9 @@
       <c r="L79" s="41"/>
       <c r="M79" s="42"/>
     </row>
-    <row r="80" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="24" t="s">
-        <v>133</v>
+    <row r="80" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="17" t="s">
+        <v>299</v>
       </c>
       <c r="B80" s="22"/>
       <c r="C80" s="25"/>
@@ -4870,9 +4930,9 @@
       <c r="L80" s="41"/>
       <c r="M80" s="42"/>
     </row>
-    <row r="81" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="24" t="s">
-        <v>134</v>
+    <row r="81" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="17" t="s">
+        <v>300</v>
       </c>
       <c r="B81" s="22"/>
       <c r="C81" s="25"/>
@@ -4887,9 +4947,9 @@
       <c r="L81" s="41"/>
       <c r="M81" s="42"/>
     </row>
-    <row r="82" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="24" t="s">
-        <v>135</v>
+    <row r="82" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="17" t="s">
+        <v>301</v>
       </c>
       <c r="B82" s="22"/>
       <c r="C82" s="25"/>
@@ -4904,9 +4964,9 @@
       <c r="L82" s="41"/>
       <c r="M82" s="42"/>
     </row>
-    <row r="83" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="24" t="s">
-        <v>136</v>
+    <row r="83" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="17" t="s">
+        <v>302</v>
       </c>
       <c r="B83" s="22"/>
       <c r="C83" s="25"/>
@@ -4921,9 +4981,9 @@
       <c r="L83" s="41"/>
       <c r="M83" s="42"/>
     </row>
-    <row r="84" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="24" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B84" s="22"/>
       <c r="C84" s="25"/>
@@ -4938,9 +4998,9 @@
       <c r="L84" s="41"/>
       <c r="M84" s="42"/>
     </row>
-    <row r="85" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="24" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B85" s="22"/>
       <c r="C85" s="25"/>
@@ -4955,9 +5015,9 @@
       <c r="L85" s="41"/>
       <c r="M85" s="42"/>
     </row>
-    <row r="86" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="24" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="B86" s="22"/>
       <c r="C86" s="25"/>
@@ -4972,9 +5032,9 @@
       <c r="L86" s="41"/>
       <c r="M86" s="42"/>
     </row>
-    <row r="87" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="24" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="B87" s="22"/>
       <c r="C87" s="25"/>
@@ -4989,9 +5049,9 @@
       <c r="L87" s="41"/>
       <c r="M87" s="42"/>
     </row>
-    <row r="88" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="24" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B88" s="22"/>
       <c r="C88" s="25"/>
@@ -5006,9 +5066,9 @@
       <c r="L88" s="41"/>
       <c r="M88" s="42"/>
     </row>
-    <row r="89" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="24" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="B89" s="22"/>
       <c r="C89" s="25"/>
@@ -5023,9 +5083,9 @@
       <c r="L89" s="41"/>
       <c r="M89" s="42"/>
     </row>
-    <row r="90" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="24" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="B90" s="22"/>
       <c r="C90" s="25"/>
@@ -5040,9 +5100,9 @@
       <c r="L90" s="41"/>
       <c r="M90" s="42"/>
     </row>
-    <row r="91" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="24" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="B91" s="22"/>
       <c r="C91" s="25"/>
@@ -5057,9 +5117,9 @@
       <c r="L91" s="41"/>
       <c r="M91" s="42"/>
     </row>
-    <row r="92" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="24" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="B92" s="22"/>
       <c r="C92" s="25"/>
@@ -5074,9 +5134,9 @@
       <c r="L92" s="41"/>
       <c r="M92" s="42"/>
     </row>
-    <row r="93" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="24" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="B93" s="22"/>
       <c r="C93" s="25"/>
@@ -5091,9 +5151,9 @@
       <c r="L93" s="41"/>
       <c r="M93" s="42"/>
     </row>
-    <row r="94" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="24" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="B94" s="22"/>
       <c r="C94" s="25"/>
@@ -5108,9 +5168,9 @@
       <c r="L94" s="41"/>
       <c r="M94" s="42"/>
     </row>
-    <row r="95" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="24" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="B95" s="22"/>
       <c r="C95" s="25"/>
@@ -5125,9 +5185,9 @@
       <c r="L95" s="41"/>
       <c r="M95" s="42"/>
     </row>
-    <row r="96" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="24" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="B96" s="22"/>
       <c r="C96" s="25"/>
@@ -5142,9 +5202,9 @@
       <c r="L96" s="41"/>
       <c r="M96" s="42"/>
     </row>
-    <row r="97" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="24" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B97" s="22"/>
       <c r="C97" s="25"/>
@@ -5159,9 +5219,9 @@
       <c r="L97" s="41"/>
       <c r="M97" s="42"/>
     </row>
-    <row r="98" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="24" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="B98" s="22"/>
       <c r="C98" s="25"/>
@@ -5176,9 +5236,9 @@
       <c r="L98" s="41"/>
       <c r="M98" s="42"/>
     </row>
-    <row r="99" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="24" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="B99" s="22"/>
       <c r="C99" s="25"/>
@@ -5193,9 +5253,9 @@
       <c r="L99" s="41"/>
       <c r="M99" s="42"/>
     </row>
-    <row r="100" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="24" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="B100" s="22"/>
       <c r="C100" s="25"/>
@@ -5210,9 +5270,9 @@
       <c r="L100" s="41"/>
       <c r="M100" s="42"/>
     </row>
-    <row r="101" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="24" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B101" s="22"/>
       <c r="C101" s="25"/>
@@ -5227,9 +5287,9 @@
       <c r="L101" s="41"/>
       <c r="M101" s="42"/>
     </row>
-    <row r="102" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="24" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="B102" s="22"/>
       <c r="C102" s="25"/>
@@ -5244,9 +5304,9 @@
       <c r="L102" s="41"/>
       <c r="M102" s="42"/>
     </row>
-    <row r="103" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="24" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="B103" s="22"/>
       <c r="C103" s="25"/>
@@ -5261,9 +5321,9 @@
       <c r="L103" s="41"/>
       <c r="M103" s="42"/>
     </row>
-    <row r="104" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="24" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="B104" s="22"/>
       <c r="C104" s="25"/>
@@ -5278,9 +5338,9 @@
       <c r="L104" s="41"/>
       <c r="M104" s="42"/>
     </row>
-    <row r="105" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="24" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B105" s="22"/>
       <c r="C105" s="25"/>
@@ -5295,9 +5355,9 @@
       <c r="L105" s="41"/>
       <c r="M105" s="42"/>
     </row>
-    <row r="106" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="24" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="B106" s="22"/>
       <c r="C106" s="25"/>
@@ -5312,9 +5372,9 @@
       <c r="L106" s="41"/>
       <c r="M106" s="42"/>
     </row>
-    <row r="107" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="24" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="B107" s="22"/>
       <c r="C107" s="25"/>
@@ -5329,9 +5389,9 @@
       <c r="L107" s="41"/>
       <c r="M107" s="42"/>
     </row>
-    <row r="108" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="24" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="B108" s="22"/>
       <c r="C108" s="25"/>
@@ -5346,9 +5406,9 @@
       <c r="L108" s="41"/>
       <c r="M108" s="42"/>
     </row>
-    <row r="109" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="24" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="B109" s="22"/>
       <c r="C109" s="25"/>
@@ -5363,9 +5423,9 @@
       <c r="L109" s="41"/>
       <c r="M109" s="42"/>
     </row>
-    <row r="110" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="24" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="B110" s="22"/>
       <c r="C110" s="25"/>
@@ -5380,9 +5440,9 @@
       <c r="L110" s="41"/>
       <c r="M110" s="42"/>
     </row>
-    <row r="111" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="24" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="B111" s="22"/>
       <c r="C111" s="25"/>
@@ -5397,9 +5457,9 @@
       <c r="L111" s="41"/>
       <c r="M111" s="42"/>
     </row>
-    <row r="112" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="24" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="B112" s="22"/>
       <c r="C112" s="25"/>
@@ -5414,9 +5474,9 @@
       <c r="L112" s="41"/>
       <c r="M112" s="42"/>
     </row>
-    <row r="113" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="24" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="B113" s="22"/>
       <c r="C113" s="25"/>
@@ -5431,9 +5491,9 @@
       <c r="L113" s="41"/>
       <c r="M113" s="42"/>
     </row>
-    <row r="114" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="24" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="B114" s="22"/>
       <c r="C114" s="25"/>
@@ -5448,9 +5508,9 @@
       <c r="L114" s="41"/>
       <c r="M114" s="42"/>
     </row>
-    <row r="115" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="24" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="B115" s="22"/>
       <c r="C115" s="25"/>
@@ -5465,9 +5525,9 @@
       <c r="L115" s="41"/>
       <c r="M115" s="42"/>
     </row>
-    <row r="116" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="24" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="B116" s="22"/>
       <c r="C116" s="25"/>
@@ -5482,9 +5542,9 @@
       <c r="L116" s="41"/>
       <c r="M116" s="42"/>
     </row>
-    <row r="117" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="24" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="B117" s="22"/>
       <c r="C117" s="25"/>
@@ -5499,9 +5559,9 @@
       <c r="L117" s="41"/>
       <c r="M117" s="42"/>
     </row>
-    <row r="118" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="24" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="B118" s="22"/>
       <c r="C118" s="25"/>
@@ -5516,9 +5576,9 @@
       <c r="L118" s="41"/>
       <c r="M118" s="42"/>
     </row>
-    <row r="119" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="24" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="B119" s="22"/>
       <c r="C119" s="25"/>
@@ -5533,9 +5593,9 @@
       <c r="L119" s="41"/>
       <c r="M119" s="42"/>
     </row>
-    <row r="120" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="24" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="B120" s="22"/>
       <c r="C120" s="25"/>
@@ -5550,9 +5610,9 @@
       <c r="L120" s="41"/>
       <c r="M120" s="42"/>
     </row>
-    <row r="121" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="24" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="B121" s="22"/>
       <c r="C121" s="25"/>
@@ -5567,9 +5627,9 @@
       <c r="L121" s="41"/>
       <c r="M121" s="42"/>
     </row>
-    <row r="122" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="24" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="B122" s="22"/>
       <c r="C122" s="25"/>
@@ -5584,9 +5644,9 @@
       <c r="L122" s="41"/>
       <c r="M122" s="42"/>
     </row>
-    <row r="123" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="24" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="B123" s="22"/>
       <c r="C123" s="25"/>
@@ -5601,9 +5661,9 @@
       <c r="L123" s="41"/>
       <c r="M123" s="42"/>
     </row>
-    <row r="124" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="24" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="B124" s="22"/>
       <c r="C124" s="25"/>
@@ -5618,9 +5678,9 @@
       <c r="L124" s="41"/>
       <c r="M124" s="42"/>
     </row>
-    <row r="125" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="24" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="B125" s="22"/>
       <c r="C125" s="25"/>
@@ -5635,9 +5695,9 @@
       <c r="L125" s="41"/>
       <c r="M125" s="42"/>
     </row>
-    <row r="126" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="24" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="B126" s="22"/>
       <c r="C126" s="25"/>
@@ -5652,9 +5712,9 @@
       <c r="L126" s="41"/>
       <c r="M126" s="42"/>
     </row>
-    <row r="127" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="24" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="B127" s="22"/>
       <c r="C127" s="25"/>
@@ -5669,9 +5729,9 @@
       <c r="L127" s="41"/>
       <c r="M127" s="42"/>
     </row>
-    <row r="128" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="24" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="B128" s="22"/>
       <c r="C128" s="25"/>
@@ -5686,9 +5746,9 @@
       <c r="L128" s="41"/>
       <c r="M128" s="42"/>
     </row>
-    <row r="129" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="24" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="B129" s="22"/>
       <c r="C129" s="25"/>
@@ -5703,9 +5763,9 @@
       <c r="L129" s="41"/>
       <c r="M129" s="42"/>
     </row>
-    <row r="130" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="24" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="B130" s="22"/>
       <c r="C130" s="25"/>
@@ -5720,9 +5780,9 @@
       <c r="L130" s="41"/>
       <c r="M130" s="42"/>
     </row>
-    <row r="131" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="24" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="B131" s="22"/>
       <c r="C131" s="25"/>
@@ -5737,9 +5797,9 @@
       <c r="L131" s="41"/>
       <c r="M131" s="42"/>
     </row>
-    <row r="132" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A132" s="24" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="B132" s="22"/>
       <c r="C132" s="25"/>
@@ -5754,9 +5814,9 @@
       <c r="L132" s="41"/>
       <c r="M132" s="42"/>
     </row>
-    <row r="133" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A133" s="24" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="B133" s="22"/>
       <c r="C133" s="25"/>
@@ -5771,9 +5831,9 @@
       <c r="L133" s="41"/>
       <c r="M133" s="42"/>
     </row>
-    <row r="134" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A134" s="24" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="B134" s="22"/>
       <c r="C134" s="25"/>
@@ -5788,9 +5848,9 @@
       <c r="L134" s="41"/>
       <c r="M134" s="42"/>
     </row>
-    <row r="135" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A135" s="24" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="B135" s="22"/>
       <c r="C135" s="25"/>
@@ -5805,9 +5865,9 @@
       <c r="L135" s="41"/>
       <c r="M135" s="42"/>
     </row>
-    <row r="136" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A136" s="24" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="B136" s="22"/>
       <c r="C136" s="25"/>
@@ -5822,9 +5882,9 @@
       <c r="L136" s="41"/>
       <c r="M136" s="42"/>
     </row>
-    <row r="137" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A137" s="24" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="B137" s="22"/>
       <c r="C137" s="25"/>
@@ -5839,9 +5899,9 @@
       <c r="L137" s="41"/>
       <c r="M137" s="42"/>
     </row>
-    <row r="138" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="24" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="B138" s="22"/>
       <c r="C138" s="25"/>
@@ -5856,9 +5916,9 @@
       <c r="L138" s="41"/>
       <c r="M138" s="42"/>
     </row>
-    <row r="139" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="24" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="B139" s="22"/>
       <c r="C139" s="25"/>
@@ -5873,9 +5933,9 @@
       <c r="L139" s="41"/>
       <c r="M139" s="42"/>
     </row>
-    <row r="140" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="24" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="B140" s="22"/>
       <c r="C140" s="25"/>
@@ -5890,9 +5950,9 @@
       <c r="L140" s="41"/>
       <c r="M140" s="42"/>
     </row>
-    <row r="141" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="24" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="B141" s="22"/>
       <c r="C141" s="25"/>
@@ -5907,9 +5967,9 @@
       <c r="L141" s="41"/>
       <c r="M141" s="42"/>
     </row>
-    <row r="142" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="24" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="B142" s="22"/>
       <c r="C142" s="25"/>
@@ -5924,9 +5984,9 @@
       <c r="L142" s="41"/>
       <c r="M142" s="42"/>
     </row>
-    <row r="143" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="24" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="B143" s="22"/>
       <c r="C143" s="25"/>
@@ -5941,9 +6001,9 @@
       <c r="L143" s="41"/>
       <c r="M143" s="42"/>
     </row>
-    <row r="144" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="24" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="B144" s="22"/>
       <c r="C144" s="25"/>
@@ -5958,9 +6018,9 @@
       <c r="L144" s="41"/>
       <c r="M144" s="42"/>
     </row>
-    <row r="145" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="24" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B145" s="22"/>
       <c r="C145" s="25"/>
@@ -5975,9 +6035,9 @@
       <c r="L145" s="41"/>
       <c r="M145" s="42"/>
     </row>
-    <row r="146" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="24" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="B146" s="22"/>
       <c r="C146" s="25"/>
@@ -5992,9 +6052,9 @@
       <c r="L146" s="41"/>
       <c r="M146" s="42"/>
     </row>
-    <row r="147" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A147" s="24" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="B147" s="22"/>
       <c r="C147" s="25"/>
@@ -6009,9 +6069,9 @@
       <c r="L147" s="41"/>
       <c r="M147" s="42"/>
     </row>
-    <row r="148" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A148" s="24" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="B148" s="22"/>
       <c r="C148" s="25"/>
@@ -6026,9 +6086,9 @@
       <c r="L148" s="41"/>
       <c r="M148" s="42"/>
     </row>
-    <row r="149" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A149" s="24" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="B149" s="22"/>
       <c r="C149" s="25"/>
@@ -6043,9 +6103,9 @@
       <c r="L149" s="41"/>
       <c r="M149" s="42"/>
     </row>
-    <row r="150" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A150" s="24" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="B150" s="22"/>
       <c r="C150" s="25"/>
@@ -6060,9 +6120,9 @@
       <c r="L150" s="41"/>
       <c r="M150" s="42"/>
     </row>
-    <row r="151" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A151" s="24" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="B151" s="22"/>
       <c r="C151" s="25"/>
@@ -6077,9 +6137,9 @@
       <c r="L151" s="41"/>
       <c r="M151" s="42"/>
     </row>
-    <row r="152" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A152" s="24" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="B152" s="22"/>
       <c r="C152" s="25"/>
@@ -6094,9 +6154,9 @@
       <c r="L152" s="41"/>
       <c r="M152" s="42"/>
     </row>
-    <row r="153" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A153" s="24" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="B153" s="22"/>
       <c r="C153" s="25"/>
@@ -6111,9 +6171,9 @@
       <c r="L153" s="41"/>
       <c r="M153" s="42"/>
     </row>
-    <row r="154" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A154" s="24" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="B154" s="22"/>
       <c r="C154" s="25"/>
@@ -6128,9 +6188,9 @@
       <c r="L154" s="41"/>
       <c r="M154" s="42"/>
     </row>
-    <row r="155" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="24" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="B155" s="22"/>
       <c r="C155" s="25"/>
@@ -6145,9 +6205,9 @@
       <c r="L155" s="41"/>
       <c r="M155" s="42"/>
     </row>
-    <row r="156" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A156" s="24" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="B156" s="22"/>
       <c r="C156" s="25"/>
@@ -6162,9 +6222,9 @@
       <c r="L156" s="41"/>
       <c r="M156" s="42"/>
     </row>
-    <row r="157" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A157" s="24" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="B157" s="22"/>
       <c r="C157" s="25"/>
@@ -6179,9 +6239,9 @@
       <c r="L157" s="41"/>
       <c r="M157" s="42"/>
     </row>
-    <row r="158" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A158" s="24" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="B158" s="22"/>
       <c r="C158" s="25"/>
@@ -6196,15 +6256,32 @@
       <c r="L158" s="41"/>
       <c r="M158" s="42"/>
     </row>
+    <row r="159" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A159" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="B159" s="22"/>
+      <c r="C159" s="25"/>
+      <c r="D159" s="25"/>
+      <c r="E159" s="25"/>
+      <c r="F159" s="64"/>
+      <c r="G159" s="71"/>
+      <c r="H159" s="67"/>
+      <c r="I159" s="25"/>
+      <c r="J159" s="26"/>
+      <c r="K159" s="40"/>
+      <c r="L159" s="41"/>
+      <c r="M159" s="42"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="C3:J3"/>
     <mergeCell ref="C4:J4"/>
-    <mergeCell ref="B60:F67"/>
+    <mergeCell ref="B61:F68"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
-  <conditionalFormatting sqref="C1:J1 M1 L5:M5 C159:J65514">
+  <conditionalFormatting sqref="C1:J1 M1 L5:M5 C160:J65515">
     <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
@@ -6215,7 +6292,7 @@
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F68:H158">
+  <conditionalFormatting sqref="F69:H159">
     <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
@@ -6227,7 +6304,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F68:H158">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F69:H159" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"In Progress, Testing, Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
srs add user message requirment added
</commit_message>
<xml_diff>
--- a/RTM/Traceability_Matrix learning hub ver 2.xlsx
+++ b/RTM/Traceability_Matrix learning hub ver 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed Mazrouaa\Documents\GitHub\learning-hub\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95F1CC9-15DA-40C8-87C1-2E9AE3409296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74716B5E-3B28-4FB7-84F0-38E8E86C01E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="306">
   <si>
     <t>For detail regarding the practice of Requirements Management, please refer to the Requirements Management Practices Guide</t>
   </si>
@@ -1335,6 +1335,12 @@
   </si>
   <si>
     <t>CRS-8.3</t>
+  </si>
+  <si>
+    <t>SRS-ADDUSR-011</t>
+  </si>
+  <si>
+    <t>SRS-DELUSR-004</t>
   </si>
 </sst>
 </file>
@@ -2887,10 +2893,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M159"/>
+  <dimension ref="A1:M161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54:H55"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4365,13 +4371,13 @@
         <v>102</v>
       </c>
       <c r="B53" s="55" t="s">
-        <v>117</v>
+        <v>304</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="D53" s="75" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E53" s="62" t="s">
         <v>237</v>
@@ -4379,7 +4385,7 @@
       <c r="F53" s="63"/>
       <c r="G53" s="56"/>
       <c r="H53" s="66" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I53" s="25"/>
       <c r="J53" s="26"/>
@@ -4392,10 +4398,10 @@
         <v>104</v>
       </c>
       <c r="B54" s="55" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="D54" s="75" t="s">
         <v>255</v>
@@ -4418,11 +4424,11 @@
       <c r="A55" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="B55" s="22" t="s">
-        <v>278</v>
+      <c r="B55" s="55" t="s">
+        <v>118</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>303</v>
+        <v>213</v>
       </c>
       <c r="D55" s="75" t="s">
         <v>255</v>
@@ -4441,30 +4447,26 @@
       <c r="L55" s="41"/>
       <c r="M55" s="42"/>
     </row>
-    <row r="56" spans="1:13" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="B56" s="55" t="s">
-        <v>214</v>
+      <c r="B56" s="22" t="s">
+        <v>278</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>201</v>
+        <v>303</v>
       </c>
       <c r="D56" s="75" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="E56" s="62" t="s">
         <v>237</v>
       </c>
-      <c r="F56" s="73" t="s">
-        <v>249</v>
-      </c>
-      <c r="G56" s="75" t="s">
-        <v>251</v>
-      </c>
+      <c r="F56" s="63"/>
+      <c r="G56" s="56"/>
       <c r="H56" s="66" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I56" s="25"/>
       <c r="J56" s="26"/>
@@ -4472,30 +4474,26 @@
       <c r="L56" s="41"/>
       <c r="M56" s="42"/>
     </row>
-    <row r="57" spans="1:13" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="B57" s="55" t="s">
-        <v>215</v>
+      <c r="B57" s="22" t="s">
+        <v>305</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>218</v>
+        <v>303</v>
       </c>
       <c r="D57" s="75" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="E57" s="62" t="s">
         <v>237</v>
       </c>
-      <c r="F57" s="73" t="s">
-        <v>249</v>
-      </c>
-      <c r="G57" s="75" t="s">
-        <v>251</v>
-      </c>
+      <c r="F57" s="63"/>
+      <c r="G57" s="56"/>
       <c r="H57" s="66" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I57" s="25"/>
       <c r="J57" s="26"/>
@@ -4508,7 +4506,7 @@
         <v>276</v>
       </c>
       <c r="B58" s="55" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C58" s="23" t="s">
         <v>201</v>
@@ -4539,13 +4537,13 @@
         <v>277</v>
       </c>
       <c r="B59" s="55" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D59" s="75" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E59" s="62" t="s">
         <v>237</v>
@@ -4565,24 +4563,30 @@
       <c r="L59" s="41"/>
       <c r="M59" s="42"/>
     </row>
-    <row r="60" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="17" t="s">
         <v>279</v>
       </c>
       <c r="B60" s="55" t="s">
-        <v>119</v>
+        <v>216</v>
       </c>
       <c r="C60" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="D60" s="20"/>
+        <v>201</v>
+      </c>
+      <c r="D60" s="75" t="s">
+        <v>248</v>
+      </c>
       <c r="E60" s="62" t="s">
         <v>237</v>
       </c>
-      <c r="F60" s="63"/>
-      <c r="G60" s="56"/>
+      <c r="F60" s="73" t="s">
+        <v>249</v>
+      </c>
+      <c r="G60" s="75" t="s">
+        <v>251</v>
+      </c>
       <c r="H60" s="66" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="I60" s="25"/>
       <c r="J60" s="26"/>
@@ -4590,17 +4594,31 @@
       <c r="L60" s="41"/>
       <c r="M60" s="42"/>
     </row>
-    <row r="61" spans="1:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="B61" s="102"/>
-      <c r="C61" s="103"/>
-      <c r="D61" s="103"/>
-      <c r="E61" s="103"/>
-      <c r="F61" s="104"/>
-      <c r="G61" s="70"/>
-      <c r="H61" s="58"/>
+      <c r="B61" s="55" t="s">
+        <v>217</v>
+      </c>
+      <c r="C61" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="D61" s="75" t="s">
+        <v>250</v>
+      </c>
+      <c r="E61" s="62" t="s">
+        <v>237</v>
+      </c>
+      <c r="F61" s="73" t="s">
+        <v>249</v>
+      </c>
+      <c r="G61" s="75" t="s">
+        <v>251</v>
+      </c>
+      <c r="H61" s="66" t="s">
+        <v>227</v>
+      </c>
       <c r="I61" s="25"/>
       <c r="J61" s="26"/>
       <c r="K61" s="40"/>
@@ -4611,28 +4629,36 @@
       <c r="A62" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="B62" s="105"/>
-      <c r="C62" s="106"/>
-      <c r="D62" s="106"/>
-      <c r="E62" s="106"/>
-      <c r="F62" s="107"/>
-      <c r="G62" s="70"/>
-      <c r="H62" s="58"/>
+      <c r="B62" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="D62" s="20"/>
+      <c r="E62" s="62" t="s">
+        <v>237</v>
+      </c>
+      <c r="F62" s="63"/>
+      <c r="G62" s="56"/>
+      <c r="H62" s="66" t="s">
+        <v>222</v>
+      </c>
       <c r="I62" s="25"/>
       <c r="J62" s="26"/>
       <c r="K62" s="40"/>
       <c r="L62" s="41"/>
       <c r="M62" s="42"/>
     </row>
-    <row r="63" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="B63" s="105"/>
-      <c r="C63" s="106"/>
-      <c r="D63" s="106"/>
-      <c r="E63" s="106"/>
-      <c r="F63" s="107"/>
+      <c r="B63" s="102"/>
+      <c r="C63" s="103"/>
+      <c r="D63" s="103"/>
+      <c r="E63" s="103"/>
+      <c r="F63" s="104"/>
       <c r="G63" s="70"/>
       <c r="H63" s="58"/>
       <c r="I63" s="25"/>
@@ -4660,7 +4686,7 @@
     </row>
     <row r="65" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B65" s="105"/>
       <c r="C65" s="106"/>
@@ -4677,7 +4703,7 @@
     </row>
     <row r="66" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B66" s="105"/>
       <c r="C66" s="106"/>
@@ -4694,7 +4720,7 @@
     </row>
     <row r="67" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B67" s="105"/>
       <c r="C67" s="106"/>
@@ -4711,7 +4737,7 @@
     </row>
     <row r="68" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B68" s="105"/>
       <c r="C68" s="106"/>
@@ -4728,15 +4754,15 @@
     </row>
     <row r="69" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="17" t="s">
-        <v>288</v>
-      </c>
-      <c r="B69" s="22"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="64"/>
-      <c r="G69" s="71"/>
-      <c r="H69" s="67"/>
+        <v>286</v>
+      </c>
+      <c r="B69" s="105"/>
+      <c r="C69" s="106"/>
+      <c r="D69" s="106"/>
+      <c r="E69" s="106"/>
+      <c r="F69" s="107"/>
+      <c r="G69" s="70"/>
+      <c r="H69" s="58"/>
       <c r="I69" s="25"/>
       <c r="J69" s="26"/>
       <c r="K69" s="40"/>
@@ -4745,15 +4771,15 @@
     </row>
     <row r="70" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="B70" s="22"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="64"/>
-      <c r="G70" s="71"/>
-      <c r="H70" s="67"/>
+        <v>287</v>
+      </c>
+      <c r="B70" s="105"/>
+      <c r="C70" s="106"/>
+      <c r="D70" s="106"/>
+      <c r="E70" s="106"/>
+      <c r="F70" s="107"/>
+      <c r="G70" s="70"/>
+      <c r="H70" s="58"/>
       <c r="I70" s="25"/>
       <c r="J70" s="26"/>
       <c r="K70" s="40"/>
@@ -4762,7 +4788,7 @@
     </row>
     <row r="71" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B71" s="22"/>
       <c r="C71" s="25"/>
@@ -4779,7 +4805,7 @@
     </row>
     <row r="72" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="17" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B72" s="22"/>
       <c r="C72" s="25"/>
@@ -4796,7 +4822,7 @@
     </row>
     <row r="73" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="17" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B73" s="22"/>
       <c r="C73" s="25"/>
@@ -4813,7 +4839,7 @@
     </row>
     <row r="74" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="17" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B74" s="22"/>
       <c r="C74" s="25"/>
@@ -4830,7 +4856,7 @@
     </row>
     <row r="75" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="17" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B75" s="22"/>
       <c r="C75" s="25"/>
@@ -4847,7 +4873,7 @@
     </row>
     <row r="76" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="17" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B76" s="22"/>
       <c r="C76" s="25"/>
@@ -4864,7 +4890,7 @@
     </row>
     <row r="77" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="17" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B77" s="22"/>
       <c r="C77" s="25"/>
@@ -4881,7 +4907,7 @@
     </row>
     <row r="78" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="17" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B78" s="22"/>
       <c r="C78" s="25"/>
@@ -4898,7 +4924,7 @@
     </row>
     <row r="79" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="17" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B79" s="22"/>
       <c r="C79" s="25"/>
@@ -4915,7 +4941,7 @@
     </row>
     <row r="80" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="17" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B80" s="22"/>
       <c r="C80" s="25"/>
@@ -4932,7 +4958,7 @@
     </row>
     <row r="81" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="17" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B81" s="22"/>
       <c r="C81" s="25"/>
@@ -4949,7 +4975,7 @@
     </row>
     <row r="82" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="17" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B82" s="22"/>
       <c r="C82" s="25"/>
@@ -4966,7 +4992,7 @@
     </row>
     <row r="83" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="17" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B83" s="22"/>
       <c r="C83" s="25"/>
@@ -4982,8 +5008,8 @@
       <c r="M83" s="42"/>
     </row>
     <row r="84" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="24" t="s">
-        <v>120</v>
+      <c r="A84" s="17" t="s">
+        <v>301</v>
       </c>
       <c r="B84" s="22"/>
       <c r="C84" s="25"/>
@@ -4999,8 +5025,8 @@
       <c r="M84" s="42"/>
     </row>
     <row r="85" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="24" t="s">
-        <v>121</v>
+      <c r="A85" s="17" t="s">
+        <v>302</v>
       </c>
       <c r="B85" s="22"/>
       <c r="C85" s="25"/>
@@ -5017,7 +5043,7 @@
     </row>
     <row r="86" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B86" s="22"/>
       <c r="C86" s="25"/>
@@ -5034,7 +5060,7 @@
     </row>
     <row r="87" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B87" s="22"/>
       <c r="C87" s="25"/>
@@ -5051,7 +5077,7 @@
     </row>
     <row r="88" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B88" s="22"/>
       <c r="C88" s="25"/>
@@ -5068,7 +5094,7 @@
     </row>
     <row r="89" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="24" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B89" s="22"/>
       <c r="C89" s="25"/>
@@ -5085,7 +5111,7 @@
     </row>
     <row r="90" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B90" s="22"/>
       <c r="C90" s="25"/>
@@ -5102,7 +5128,7 @@
     </row>
     <row r="91" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B91" s="22"/>
       <c r="C91" s="25"/>
@@ -5119,7 +5145,7 @@
     </row>
     <row r="92" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B92" s="22"/>
       <c r="C92" s="25"/>
@@ -5136,7 +5162,7 @@
     </row>
     <row r="93" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B93" s="22"/>
       <c r="C93" s="25"/>
@@ -5153,7 +5179,7 @@
     </row>
     <row r="94" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="24" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B94" s="22"/>
       <c r="C94" s="25"/>
@@ -5170,7 +5196,7 @@
     </row>
     <row r="95" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B95" s="22"/>
       <c r="C95" s="25"/>
@@ -5187,7 +5213,7 @@
     </row>
     <row r="96" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B96" s="22"/>
       <c r="C96" s="25"/>
@@ -5204,7 +5230,7 @@
     </row>
     <row r="97" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B97" s="22"/>
       <c r="C97" s="25"/>
@@ -5221,7 +5247,7 @@
     </row>
     <row r="98" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B98" s="22"/>
       <c r="C98" s="25"/>
@@ -5238,7 +5264,7 @@
     </row>
     <row r="99" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B99" s="22"/>
       <c r="C99" s="25"/>
@@ -5255,7 +5281,7 @@
     </row>
     <row r="100" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B100" s="22"/>
       <c r="C100" s="25"/>
@@ -5272,7 +5298,7 @@
     </row>
     <row r="101" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B101" s="22"/>
       <c r="C101" s="25"/>
@@ -5289,7 +5315,7 @@
     </row>
     <row r="102" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="24" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B102" s="22"/>
       <c r="C102" s="25"/>
@@ -5306,7 +5332,7 @@
     </row>
     <row r="103" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B103" s="22"/>
       <c r="C103" s="25"/>
@@ -5323,7 +5349,7 @@
     </row>
     <row r="104" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="24" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B104" s="22"/>
       <c r="C104" s="25"/>
@@ -5340,7 +5366,7 @@
     </row>
     <row r="105" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B105" s="22"/>
       <c r="C105" s="25"/>
@@ -5357,7 +5383,7 @@
     </row>
     <row r="106" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B106" s="22"/>
       <c r="C106" s="25"/>
@@ -5374,7 +5400,7 @@
     </row>
     <row r="107" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="24" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B107" s="22"/>
       <c r="C107" s="25"/>
@@ -5391,7 +5417,7 @@
     </row>
     <row r="108" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B108" s="22"/>
       <c r="C108" s="25"/>
@@ -5408,7 +5434,7 @@
     </row>
     <row r="109" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B109" s="22"/>
       <c r="C109" s="25"/>
@@ -5425,7 +5451,7 @@
     </row>
     <row r="110" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B110" s="22"/>
       <c r="C110" s="25"/>
@@ -5442,7 +5468,7 @@
     </row>
     <row r="111" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B111" s="22"/>
       <c r="C111" s="25"/>
@@ -5459,7 +5485,7 @@
     </row>
     <row r="112" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B112" s="22"/>
       <c r="C112" s="25"/>
@@ -5476,7 +5502,7 @@
     </row>
     <row r="113" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B113" s="22"/>
       <c r="C113" s="25"/>
@@ -5493,7 +5519,7 @@
     </row>
     <row r="114" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B114" s="22"/>
       <c r="C114" s="25"/>
@@ -5510,7 +5536,7 @@
     </row>
     <row r="115" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B115" s="22"/>
       <c r="C115" s="25"/>
@@ -5527,7 +5553,7 @@
     </row>
     <row r="116" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="24" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B116" s="22"/>
       <c r="C116" s="25"/>
@@ -5544,7 +5570,7 @@
     </row>
     <row r="117" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B117" s="22"/>
       <c r="C117" s="25"/>
@@ -5561,7 +5587,7 @@
     </row>
     <row r="118" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B118" s="22"/>
       <c r="C118" s="25"/>
@@ -5578,7 +5604,7 @@
     </row>
     <row r="119" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B119" s="22"/>
       <c r="C119" s="25"/>
@@ -5595,7 +5621,7 @@
     </row>
     <row r="120" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B120" s="22"/>
       <c r="C120" s="25"/>
@@ -5612,7 +5638,7 @@
     </row>
     <row r="121" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="24" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B121" s="22"/>
       <c r="C121" s="25"/>
@@ -5629,7 +5655,7 @@
     </row>
     <row r="122" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B122" s="22"/>
       <c r="C122" s="25"/>
@@ -5646,7 +5672,7 @@
     </row>
     <row r="123" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="24" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B123" s="22"/>
       <c r="C123" s="25"/>
@@ -5663,7 +5689,7 @@
     </row>
     <row r="124" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B124" s="22"/>
       <c r="C124" s="25"/>
@@ -5680,7 +5706,7 @@
     </row>
     <row r="125" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B125" s="22"/>
       <c r="C125" s="25"/>
@@ -5697,7 +5723,7 @@
     </row>
     <row r="126" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B126" s="22"/>
       <c r="C126" s="25"/>
@@ -5714,7 +5740,7 @@
     </row>
     <row r="127" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="24" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B127" s="22"/>
       <c r="C127" s="25"/>
@@ -5731,7 +5757,7 @@
     </row>
     <row r="128" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B128" s="22"/>
       <c r="C128" s="25"/>
@@ -5748,7 +5774,7 @@
     </row>
     <row r="129" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B129" s="22"/>
       <c r="C129" s="25"/>
@@ -5765,7 +5791,7 @@
     </row>
     <row r="130" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="24" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B130" s="22"/>
       <c r="C130" s="25"/>
@@ -5782,7 +5808,7 @@
     </row>
     <row r="131" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B131" s="22"/>
       <c r="C131" s="25"/>
@@ -5799,7 +5825,7 @@
     </row>
     <row r="132" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A132" s="24" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B132" s="22"/>
       <c r="C132" s="25"/>
@@ -5816,7 +5842,7 @@
     </row>
     <row r="133" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A133" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B133" s="22"/>
       <c r="C133" s="25"/>
@@ -5833,7 +5859,7 @@
     </row>
     <row r="134" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A134" s="24" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B134" s="22"/>
       <c r="C134" s="25"/>
@@ -5850,7 +5876,7 @@
     </row>
     <row r="135" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A135" s="24" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B135" s="22"/>
       <c r="C135" s="25"/>
@@ -5867,7 +5893,7 @@
     </row>
     <row r="136" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A136" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B136" s="22"/>
       <c r="C136" s="25"/>
@@ -5884,7 +5910,7 @@
     </row>
     <row r="137" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A137" s="24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B137" s="22"/>
       <c r="C137" s="25"/>
@@ -5901,7 +5927,7 @@
     </row>
     <row r="138" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="24" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B138" s="22"/>
       <c r="C138" s="25"/>
@@ -5918,7 +5944,7 @@
     </row>
     <row r="139" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B139" s="22"/>
       <c r="C139" s="25"/>
@@ -5935,7 +5961,7 @@
     </row>
     <row r="140" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B140" s="22"/>
       <c r="C140" s="25"/>
@@ -5952,7 +5978,7 @@
     </row>
     <row r="141" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B141" s="22"/>
       <c r="C141" s="25"/>
@@ -5969,7 +5995,7 @@
     </row>
     <row r="142" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B142" s="22"/>
       <c r="C142" s="25"/>
@@ -5986,7 +6012,7 @@
     </row>
     <row r="143" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B143" s="22"/>
       <c r="C143" s="25"/>
@@ -6003,7 +6029,7 @@
     </row>
     <row r="144" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B144" s="22"/>
       <c r="C144" s="25"/>
@@ -6020,7 +6046,7 @@
     </row>
     <row r="145" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="24" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B145" s="22"/>
       <c r="C145" s="25"/>
@@ -6037,7 +6063,7 @@
     </row>
     <row r="146" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B146" s="22"/>
       <c r="C146" s="25"/>
@@ -6054,7 +6080,7 @@
     </row>
     <row r="147" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A147" s="24" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B147" s="22"/>
       <c r="C147" s="25"/>
@@ -6071,7 +6097,7 @@
     </row>
     <row r="148" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A148" s="24" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B148" s="22"/>
       <c r="C148" s="25"/>
@@ -6088,7 +6114,7 @@
     </row>
     <row r="149" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A149" s="24" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B149" s="22"/>
       <c r="C149" s="25"/>
@@ -6105,7 +6131,7 @@
     </row>
     <row r="150" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A150" s="24" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B150" s="22"/>
       <c r="C150" s="25"/>
@@ -6122,7 +6148,7 @@
     </row>
     <row r="151" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A151" s="24" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B151" s="22"/>
       <c r="C151" s="25"/>
@@ -6139,7 +6165,7 @@
     </row>
     <row r="152" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A152" s="24" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B152" s="22"/>
       <c r="C152" s="25"/>
@@ -6156,7 +6182,7 @@
     </row>
     <row r="153" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A153" s="24" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B153" s="22"/>
       <c r="C153" s="25"/>
@@ -6173,7 +6199,7 @@
     </row>
     <row r="154" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A154" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B154" s="22"/>
       <c r="C154" s="25"/>
@@ -6190,7 +6216,7 @@
     </row>
     <row r="155" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="24" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B155" s="22"/>
       <c r="C155" s="25"/>
@@ -6207,7 +6233,7 @@
     </row>
     <row r="156" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A156" s="24" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B156" s="22"/>
       <c r="C156" s="25"/>
@@ -6224,7 +6250,7 @@
     </row>
     <row r="157" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A157" s="24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B157" s="22"/>
       <c r="C157" s="25"/>
@@ -6241,7 +6267,7 @@
     </row>
     <row r="158" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A158" s="24" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B158" s="22"/>
       <c r="C158" s="25"/>
@@ -6258,7 +6284,7 @@
     </row>
     <row r="159" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A159" s="24" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B159" s="22"/>
       <c r="C159" s="25"/>
@@ -6273,15 +6299,49 @@
       <c r="L159" s="41"/>
       <c r="M159" s="42"/>
     </row>
+    <row r="160" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A160" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="B160" s="22"/>
+      <c r="C160" s="25"/>
+      <c r="D160" s="25"/>
+      <c r="E160" s="25"/>
+      <c r="F160" s="64"/>
+      <c r="G160" s="71"/>
+      <c r="H160" s="67"/>
+      <c r="I160" s="25"/>
+      <c r="J160" s="26"/>
+      <c r="K160" s="40"/>
+      <c r="L160" s="41"/>
+      <c r="M160" s="42"/>
+    </row>
+    <row r="161" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A161" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="B161" s="22"/>
+      <c r="C161" s="25"/>
+      <c r="D161" s="25"/>
+      <c r="E161" s="25"/>
+      <c r="F161" s="64"/>
+      <c r="G161" s="71"/>
+      <c r="H161" s="67"/>
+      <c r="I161" s="25"/>
+      <c r="J161" s="26"/>
+      <c r="K161" s="40"/>
+      <c r="L161" s="41"/>
+      <c r="M161" s="42"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="C3:J3"/>
     <mergeCell ref="C4:J4"/>
-    <mergeCell ref="B61:F68"/>
+    <mergeCell ref="B63:F70"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
-  <conditionalFormatting sqref="C1:J1 M1 L5:M5 C160:J65515">
+  <conditionalFormatting sqref="C1:J1 M1 L5:M5 C162:J65517">
     <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
@@ -6292,7 +6352,7 @@
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F69:H159">
+  <conditionalFormatting sqref="F71:H161">
     <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
@@ -6304,7 +6364,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F69:H159" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F71:H161" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"In Progress, Testing, Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
testcases of register and add user is added, RTM is updated, Reviews is updated
</commit_message>
<xml_diff>
--- a/RTM/Traceability_Matrix learning hub ver 2.xlsx
+++ b/RTM/Traceability_Matrix learning hub ver 2.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad\Documents\GitHub\learning-hub\RTM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91035FC9-8CF5-472C-9236-2401478109CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" state="hidden" r:id="rId1"/>
@@ -20,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>eze3</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -44,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -63,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -82,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0">
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -101,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0">
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -120,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0">
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -139,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0">
+    <comment ref="K5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -158,13 +164,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="L5" authorId="0">
+    <comment ref="L5" authorId="0" shapeId="0" xr:uid="{7D60CAF8-4D99-4CE1-80A1-1548DC799F01}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="8"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">• Test Case Number: </t>
         </r>
@@ -172,6 +179,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> This column should be populated with the test case number linked to the functional requirement.</t>
         </r>
@@ -182,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="326">
   <si>
     <t>For detail regarding the practice of Requirements Management, please refer to the Requirements Management Practices Guide</t>
   </si>
@@ -413,10 +421,6 @@
   <si>
     <t>Software
 Module(s)</t>
-  </si>
-  <si>
-    <t>Test Case
-Number</t>
   </si>
   <si>
     <t>Additional
@@ -1342,15 +1346,73 @@
   <si>
     <t>Design Document (3.8.2 classDiagram_Delete User)</t>
   </si>
+  <si>
+    <t>Test Case
+ID</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_Register_002</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_Register_004</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_Register_005</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_Register_006</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_Register_007</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_Register_008</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_Register_009</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_Register_001</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_002</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_003</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_004</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_005</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_006</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_007</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_008</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_009</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_001</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_010</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1467,6 +1529,17 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1648,7 +1721,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1753,12 +1826,6 @@
     <xf numFmtId="49" fontId="10" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1768,14 +1835,8 @@
     <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1801,15 +1862,57 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2134,32 +2237,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B20"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="58.85546875" style="12" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="5.33203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" style="12" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="12"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="39"/>
-    </row>
-    <row r="5" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B4" s="51"/>
+    </row>
+    <row r="5" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
@@ -2167,7 +2270,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
@@ -2175,72 +2278,72 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B20" s="19" t="s">
         <v>19</v>
       </c>
@@ -2256,32 +2359,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F42" sqref="F33:F42"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="55.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="47.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="47.28515625" style="28" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="35.88671875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="55.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="47.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="47.33203125" style="28" customWidth="1"/>
     <col min="8" max="8" width="51" style="5" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="28.109375" style="57" customWidth="1"/>
     <col min="13" max="13" width="86" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="24"/>
@@ -2293,71 +2396,71 @@
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
-      <c r="K1" s="41" t="s">
+      <c r="K1" s="39" t="s">
         <v>20</v>
       </c>
       <c r="L1" s="24"/>
       <c r="M1" s="24"/>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="43" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
-      <c r="M2" s="44"/>
-    </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
+      <c r="M2" s="41"/>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="43" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
-      <c r="M3" s="44"/>
-    </row>
-    <row r="4" spans="1:13" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
+      <c r="M3" s="41"/>
+    </row>
+    <row r="4" spans="1:13" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="45" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
-      <c r="M4" s="46"/>
-    </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="M4" s="42"/>
+    </row>
+    <row r="5" spans="1:13" s="3" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="23" t="s">
@@ -2367,19 +2470,19 @@
         <v>29</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E5" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="F5" s="23" t="s">
-        <v>231</v>
-      </c>
       <c r="G5" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I5" s="23" t="s">
         <v>30</v>
@@ -2390,1663 +2493,1703 @@
       <c r="K5" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="48" t="s">
+      <c r="L5" s="44" t="s">
+        <v>307</v>
+      </c>
+      <c r="M5" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="48" t="s">
+    </row>
+    <row r="6" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="45" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="B6" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="C6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>37</v>
-      </c>
       <c r="D6" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E6" s="50" t="s">
-        <v>237</v>
-      </c>
-      <c r="F6" s="50" t="s">
         <v>232</v>
       </c>
+      <c r="E6" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F6" s="46" t="s">
+        <v>231</v>
+      </c>
       <c r="G6" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="H6" s="51" t="s">
-        <v>220</v>
+        <v>234</v>
+      </c>
+      <c r="H6" s="47" t="s">
+        <v>219</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
-      <c r="L6" s="10"/>
+      <c r="L6" s="55" t="s">
+        <v>308</v>
+      </c>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="49" t="s">
+    <row r="7" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A7" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>39</v>
-      </c>
       <c r="C7" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E7" s="50" t="s">
-        <v>237</v>
+        <v>232</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="H7" s="51" t="s">
-        <v>220</v>
+        <v>234</v>
+      </c>
+      <c r="H7" s="47" t="s">
+        <v>219</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
-      <c r="L7" s="10"/>
+      <c r="L7" s="55" t="s">
+        <v>308</v>
+      </c>
       <c r="M7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+    <row r="8" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A8" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>41</v>
-      </c>
       <c r="C8" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E8" s="50" t="s">
-        <v>237</v>
+        <v>232</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="H8" s="51" t="s">
-        <v>220</v>
+        <v>234</v>
+      </c>
+      <c r="H8" s="47" t="s">
+        <v>219</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="10"/>
+      <c r="L8" s="55" t="s">
+        <v>309</v>
+      </c>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
+    <row r="9" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A9" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="C9" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="D9" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E9" s="50" t="s">
-        <v>237</v>
+        <v>232</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="51" t="s">
-        <v>220</v>
+      <c r="H9" s="47" t="s">
+        <v>219</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
-      <c r="L9" s="10"/>
+      <c r="L9" s="55" t="s">
+        <v>310</v>
+      </c>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
+    <row r="10" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A10" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="C10" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="D10" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E10" s="50" t="s">
-        <v>237</v>
+        <v>232</v>
+      </c>
+      <c r="E10" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>236</v>
-      </c>
-      <c r="H10" s="51" t="s">
-        <v>220</v>
+        <v>235</v>
+      </c>
+      <c r="H10" s="47" t="s">
+        <v>219</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
-      <c r="L10" s="10"/>
+      <c r="L10" s="55" t="s">
+        <v>311</v>
+      </c>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+    <row r="11" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A11" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>49</v>
-      </c>
       <c r="C11" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E11" s="50" t="s">
-        <v>237</v>
+        <v>232</v>
+      </c>
+      <c r="E11" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>236</v>
-      </c>
-      <c r="H11" s="51" t="s">
-        <v>220</v>
+        <v>235</v>
+      </c>
+      <c r="H11" s="47" t="s">
+        <v>219</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
-      <c r="L11" s="10"/>
+      <c r="L11" s="55" t="s">
+        <v>312</v>
+      </c>
       <c r="M11" s="10"/>
     </row>
-    <row r="12" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
+    <row r="12" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A12" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>51</v>
-      </c>
       <c r="C12" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E12" s="50" t="s">
-        <v>237</v>
+        <v>232</v>
+      </c>
+      <c r="E12" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>236</v>
-      </c>
-      <c r="H12" s="51" t="s">
-        <v>220</v>
+        <v>235</v>
+      </c>
+      <c r="H12" s="47" t="s">
+        <v>219</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
-      <c r="L12" s="10"/>
+      <c r="L12" s="55" t="s">
+        <v>313</v>
+      </c>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="49" t="s">
+    <row r="13" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A13" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="20" t="s">
-        <v>53</v>
-      </c>
       <c r="C13" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E13" s="50" t="s">
+        <v>232</v>
+      </c>
+      <c r="E13" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="G13" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="G13" s="25" t="s">
-        <v>238</v>
-      </c>
-      <c r="H13" s="51" t="s">
-        <v>220</v>
+      <c r="H13" s="47" t="s">
+        <v>219</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
-      <c r="L13" s="10"/>
+      <c r="L13" s="55" t="s">
+        <v>314</v>
+      </c>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="49" t="s">
-        <v>229</v>
+    <row r="14" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="45" t="s">
+        <v>228</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E14" s="50" t="s">
-        <v>237</v>
+        <v>232</v>
+      </c>
+      <c r="E14" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="51" t="s">
-        <v>220</v>
+      <c r="H14" s="47" t="s">
+        <v>219</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="10"/>
+      <c r="L14" s="55" t="s">
+        <v>315</v>
+      </c>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="s">
+    <row r="15" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="C15" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="D15" s="30" t="s">
-        <v>240</v>
-      </c>
-      <c r="E15" s="50" t="s">
-        <v>237</v>
+        <v>239</v>
+      </c>
+      <c r="E15" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G15" s="31"/>
-      <c r="H15" s="51" t="s">
-        <v>221</v>
+      <c r="H15" s="47" t="s">
+        <v>220</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
-      <c r="L15" s="10"/>
+      <c r="L15" s="55"/>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="s">
-        <v>256</v>
+    <row r="16" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="45" t="s">
+        <v>255</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>240</v>
-      </c>
-      <c r="E16" s="50" t="s">
-        <v>237</v>
+        <v>239</v>
+      </c>
+      <c r="E16" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G16" s="22"/>
-      <c r="H16" s="51" t="s">
-        <v>221</v>
+      <c r="H16" s="47" t="s">
+        <v>220</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
-      <c r="L16" s="10"/>
+      <c r="L16" s="55"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="49" t="s">
+    <row r="17" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="21" t="s">
-        <v>59</v>
-      </c>
       <c r="C17" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>240</v>
-      </c>
-      <c r="E17" s="50" t="s">
-        <v>237</v>
+        <v>239</v>
+      </c>
+      <c r="E17" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F17" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G17" s="22"/>
-      <c r="H17" s="51" t="s">
-        <v>221</v>
+      <c r="H17" s="47" t="s">
+        <v>220</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
-      <c r="L17" s="10"/>
+      <c r="L17" s="55"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="s">
-        <v>60</v>
+    <row r="18" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A18" s="45" t="s">
+        <v>59</v>
       </c>
       <c r="B18" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="50" t="s">
-        <v>237</v>
+      <c r="E18" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="51" t="s">
-        <v>222</v>
+      <c r="H18" s="47" t="s">
+        <v>221</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
-      <c r="L18" s="10"/>
+      <c r="L18" s="55"/>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="49" t="s">
-        <v>257</v>
+    <row r="19" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A19" s="45" t="s">
+        <v>256</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D19" s="7"/>
-      <c r="E19" s="50" t="s">
-        <v>237</v>
+      <c r="E19" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
-      <c r="H19" s="51" t="s">
-        <v>222</v>
+      <c r="H19" s="47" t="s">
+        <v>221</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
-      <c r="L19" s="10"/>
+      <c r="L19" s="55"/>
       <c r="M19" s="10"/>
     </row>
-    <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="49" t="s">
-        <v>61</v>
+    <row r="20" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A20" s="45" t="s">
+        <v>60</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20" s="7"/>
-      <c r="E20" s="50" t="s">
-        <v>237</v>
+      <c r="E20" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
-      <c r="H20" s="51" t="s">
-        <v>222</v>
+      <c r="H20" s="47" t="s">
+        <v>221</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
-      <c r="L20" s="10"/>
+      <c r="L20" s="55"/>
       <c r="M20" s="10"/>
     </row>
-    <row r="21" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="s">
-        <v>64</v>
+    <row r="21" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A21" s="45" t="s">
+        <v>63</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D21" s="7"/>
-      <c r="E21" s="50" t="s">
-        <v>237</v>
+      <c r="E21" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="51" t="s">
-        <v>222</v>
+      <c r="H21" s="47" t="s">
+        <v>221</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
-      <c r="L21" s="10"/>
+      <c r="L21" s="55"/>
       <c r="M21" s="10"/>
     </row>
-    <row r="22" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="49" t="s">
-        <v>67</v>
+    <row r="22" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="45" t="s">
+        <v>66</v>
       </c>
       <c r="B22" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>73</v>
-      </c>
       <c r="D22" s="30" t="s">
+        <v>240</v>
+      </c>
+      <c r="E22" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F22" s="30" t="s">
         <v>241</v>
       </c>
-      <c r="E22" s="50" t="s">
-        <v>237</v>
-      </c>
-      <c r="F22" s="30" t="s">
+      <c r="G22" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G22" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H22" s="51" t="s">
-        <v>223</v>
+      <c r="H22" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
-      <c r="L22" s="10"/>
+      <c r="L22" s="55"/>
       <c r="M22" s="10"/>
     </row>
-    <row r="23" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="49" t="s">
-        <v>69</v>
+    <row r="23" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="45" t="s">
+        <v>68</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D23" s="30" t="s">
+        <v>240</v>
+      </c>
+      <c r="E23" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F23" s="30" t="s">
         <v>241</v>
       </c>
-      <c r="E23" s="50" t="s">
-        <v>237</v>
-      </c>
-      <c r="F23" s="30" t="s">
+      <c r="G23" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G23" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H23" s="51" t="s">
-        <v>223</v>
+      <c r="H23" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
-      <c r="L23" s="10"/>
+      <c r="L23" s="55"/>
       <c r="M23" s="10"/>
     </row>
-    <row r="24" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="49" t="s">
-        <v>258</v>
+    <row r="24" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A24" s="45" t="s">
+        <v>257</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="E24" s="50" t="s">
-        <v>237</v>
+        <v>252</v>
+      </c>
+      <c r="E24" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F24" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G24" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G24" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H24" s="51" t="s">
-        <v>223</v>
+      <c r="H24" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
-      <c r="L24" s="10"/>
+      <c r="L24" s="55"/>
       <c r="M24" s="10"/>
     </row>
-    <row r="25" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="49" t="s">
-        <v>71</v>
+    <row r="25" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A25" s="45" t="s">
+        <v>70</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="E25" s="50" t="s">
-        <v>237</v>
+        <v>252</v>
+      </c>
+      <c r="E25" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F25" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G25" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G25" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H25" s="51" t="s">
-        <v>223</v>
+      <c r="H25" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
-      <c r="L25" s="10"/>
+      <c r="L25" s="55"/>
       <c r="M25" s="10"/>
     </row>
-    <row r="26" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" s="49" t="s">
-        <v>74</v>
+    <row r="26" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A26" s="45" t="s">
+        <v>73</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="E26" s="50" t="s">
-        <v>237</v>
+        <v>252</v>
+      </c>
+      <c r="E26" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F26" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G26" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G26" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H26" s="51" t="s">
-        <v>223</v>
+      <c r="H26" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
-      <c r="L26" s="10"/>
+      <c r="L26" s="55"/>
       <c r="M26" s="10"/>
     </row>
-    <row r="27" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="49" t="s">
-        <v>76</v>
+    <row r="27" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A27" s="45" t="s">
+        <v>75</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="E27" s="50" t="s">
-        <v>237</v>
+        <v>252</v>
+      </c>
+      <c r="E27" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F27" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G27" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G27" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H27" s="51" t="s">
-        <v>223</v>
+      <c r="H27" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
-      <c r="L27" s="10"/>
+      <c r="L27" s="55"/>
       <c r="M27" s="10"/>
     </row>
-    <row r="28" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="49" t="s">
-        <v>78</v>
+    <row r="28" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A28" s="45" t="s">
+        <v>77</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="E28" s="50" t="s">
-        <v>237</v>
+        <v>252</v>
+      </c>
+      <c r="E28" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F28" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G28" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G28" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H28" s="51" t="s">
-        <v>223</v>
+      <c r="H28" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
-      <c r="L28" s="10"/>
+      <c r="L28" s="55"/>
       <c r="M28" s="10"/>
     </row>
-    <row r="29" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A29" s="49" t="s">
-        <v>80</v>
+    <row r="29" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A29" s="45" t="s">
+        <v>79</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="E29" s="50" t="s">
-        <v>237</v>
+        <v>252</v>
+      </c>
+      <c r="E29" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F29" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G29" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G29" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H29" s="51" t="s">
-        <v>223</v>
+      <c r="H29" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
-      <c r="L29" s="10"/>
+      <c r="L29" s="55"/>
       <c r="M29" s="10"/>
     </row>
-    <row r="30" spans="1:13" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="52" t="s">
-        <v>82</v>
+    <row r="30" spans="1:13" s="36" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A30" s="48" t="s">
+        <v>81</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D30" s="29"/>
       <c r="E30" s="30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F30" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G30" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G30" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H30" s="53" t="s">
-        <v>223</v>
+      <c r="H30" s="49" t="s">
+        <v>222</v>
       </c>
       <c r="I30" s="29"/>
       <c r="J30" s="29"/>
       <c r="K30" s="29"/>
-      <c r="L30" s="35"/>
+      <c r="L30" s="56"/>
       <c r="M30" s="35"/>
     </row>
-    <row r="31" spans="1:13" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="52" t="s">
-        <v>84</v>
+    <row r="31" spans="1:13" s="36" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A31" s="48" t="s">
+        <v>83</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D31" s="29"/>
       <c r="E31" s="30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F31" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G31" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G31" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H31" s="53"/>
+      <c r="H31" s="49"/>
       <c r="I31" s="29"/>
       <c r="J31" s="29"/>
       <c r="K31" s="29"/>
-      <c r="L31" s="35"/>
+      <c r="L31" s="56"/>
       <c r="M31" s="35"/>
     </row>
-    <row r="32" spans="1:13" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A32" s="52" t="s">
-        <v>86</v>
+    <row r="32" spans="1:13" s="36" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A32" s="48" t="s">
+        <v>85</v>
       </c>
       <c r="B32" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="C32" s="37" t="s">
         <v>245</v>
-      </c>
-      <c r="C32" s="37" t="s">
-        <v>246</v>
       </c>
       <c r="D32" s="29"/>
       <c r="E32" s="30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F32" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G32" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G32" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H32" s="53"/>
+      <c r="H32" s="49"/>
       <c r="I32" s="29"/>
       <c r="J32" s="29"/>
       <c r="K32" s="29"/>
-      <c r="L32" s="35"/>
+      <c r="L32" s="56"/>
       <c r="M32" s="35"/>
     </row>
-    <row r="33" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="49" t="s">
-        <v>88</v>
+    <row r="33" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="45" t="s">
+        <v>87</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="E33" s="50" t="s">
-        <v>237</v>
+        <v>251</v>
+      </c>
+      <c r="E33" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F33" s="22"/>
       <c r="G33" s="30"/>
-      <c r="H33" s="51" t="s">
-        <v>223</v>
+      <c r="H33" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
-      <c r="L33" s="10"/>
+      <c r="L33" s="55"/>
       <c r="M33" s="10"/>
     </row>
-    <row r="34" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="49" t="s">
-        <v>259</v>
+    <row r="34" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="45" t="s">
+        <v>258</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="E34" s="50" t="s">
-        <v>237</v>
+        <v>251</v>
+      </c>
+      <c r="E34" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="30"/>
-      <c r="H34" s="51" t="s">
-        <v>223</v>
+      <c r="H34" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
-      <c r="L34" s="10"/>
+      <c r="L34" s="55"/>
       <c r="M34" s="10"/>
     </row>
-    <row r="35" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="49" t="s">
-        <v>260</v>
+    <row r="35" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="45" t="s">
+        <v>259</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="E35" s="50" t="s">
-        <v>237</v>
+        <v>251</v>
+      </c>
+      <c r="E35" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="30"/>
-      <c r="H35" s="51" t="s">
-        <v>223</v>
+      <c r="H35" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
-      <c r="L35" s="10"/>
+      <c r="L35" s="55"/>
       <c r="M35" s="10"/>
     </row>
-    <row r="36" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="49" t="s">
-        <v>261</v>
+    <row r="36" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="45" t="s">
+        <v>260</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="E36" s="50" t="s">
-        <v>237</v>
+        <v>251</v>
+      </c>
+      <c r="E36" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F36" s="22"/>
       <c r="G36" s="30"/>
-      <c r="H36" s="51" t="s">
-        <v>223</v>
+      <c r="H36" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
-      <c r="L36" s="10"/>
+      <c r="L36" s="55"/>
       <c r="M36" s="10"/>
     </row>
-    <row r="37" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="49" t="s">
-        <v>262</v>
+    <row r="37" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="45" t="s">
+        <v>261</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="E37" s="50" t="s">
-        <v>237</v>
+        <v>251</v>
+      </c>
+      <c r="E37" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F37" s="22"/>
       <c r="G37" s="30"/>
-      <c r="H37" s="51" t="s">
-        <v>223</v>
+      <c r="H37" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="10"/>
+      <c r="L37" s="55"/>
       <c r="M37" s="10"/>
     </row>
-    <row r="38" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="49" t="s">
-        <v>263</v>
+    <row r="38" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="45" t="s">
+        <v>262</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="E38" s="50" t="s">
-        <v>237</v>
+        <v>251</v>
+      </c>
+      <c r="E38" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F38" s="22"/>
       <c r="G38" s="30"/>
-      <c r="H38" s="51" t="s">
-        <v>223</v>
+      <c r="H38" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
-      <c r="L38" s="10"/>
+      <c r="L38" s="55"/>
       <c r="M38" s="10"/>
     </row>
-    <row r="39" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="49" t="s">
-        <v>264</v>
+    <row r="39" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="45" t="s">
+        <v>263</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="E39" s="50" t="s">
-        <v>237</v>
+        <v>251</v>
+      </c>
+      <c r="E39" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F39" s="22"/>
       <c r="G39" s="30"/>
-      <c r="H39" s="51" t="s">
-        <v>223</v>
+      <c r="H39" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
-      <c r="L39" s="10"/>
+      <c r="L39" s="55"/>
       <c r="M39" s="10"/>
     </row>
-    <row r="40" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="49" t="s">
-        <v>265</v>
+    <row r="40" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="45" t="s">
+        <v>264</v>
       </c>
       <c r="B40" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="C40" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="C40" s="32" t="s">
-        <v>210</v>
-      </c>
       <c r="D40" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="E40" s="50" t="s">
-        <v>237</v>
+        <v>251</v>
+      </c>
+      <c r="E40" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F40" s="22"/>
       <c r="G40" s="30"/>
-      <c r="H40" s="51" t="s">
-        <v>223</v>
+      <c r="H40" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
-      <c r="L40" s="10"/>
+      <c r="L40" s="55"/>
       <c r="M40" s="10"/>
     </row>
-    <row r="41" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A41" s="49" t="s">
-        <v>266</v>
+    <row r="41" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A41" s="45" t="s">
+        <v>265</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D41" s="30" t="s">
-        <v>247</v>
-      </c>
-      <c r="E41" s="50" t="s">
-        <v>237</v>
+        <v>246</v>
+      </c>
+      <c r="E41" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F41" s="30"/>
       <c r="G41" s="30"/>
-      <c r="H41" s="51" t="s">
-        <v>224</v>
+      <c r="H41" s="47" t="s">
+        <v>223</v>
       </c>
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
-      <c r="L41" s="10"/>
+      <c r="L41" s="55"/>
       <c r="M41" s="10"/>
     </row>
-    <row r="42" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A42" s="49" t="s">
-        <v>267</v>
+    <row r="42" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A42" s="45" t="s">
+        <v>266</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D42" s="30" t="s">
-        <v>247</v>
-      </c>
-      <c r="E42" s="50" t="s">
-        <v>237</v>
+        <v>246</v>
+      </c>
+      <c r="E42" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F42" s="30"/>
       <c r="G42" s="30"/>
-      <c r="H42" s="51" t="s">
-        <v>224</v>
+      <c r="H42" s="47" t="s">
+        <v>223</v>
       </c>
       <c r="I42" s="7"/>
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
-      <c r="L42" s="10"/>
+      <c r="L42" s="55"/>
       <c r="M42" s="10"/>
     </row>
-    <row r="43" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A43" s="49" t="s">
-        <v>268</v>
+    <row r="43" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A43" s="45" t="s">
+        <v>267</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D43" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E43" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E43" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F43" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G43" s="30"/>
-      <c r="H43" s="51" t="s">
-        <v>225</v>
+      <c r="H43" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
-      <c r="L43" s="10"/>
+      <c r="L43" s="55" t="s">
+        <v>316</v>
+      </c>
       <c r="M43" s="10"/>
     </row>
-    <row r="44" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A44" s="49" t="s">
-        <v>269</v>
+    <row r="44" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A44" s="45" t="s">
+        <v>268</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D44" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E44" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E44" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F44" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G44" s="30"/>
-      <c r="H44" s="51" t="s">
-        <v>225</v>
+      <c r="H44" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I44" s="7"/>
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
-      <c r="L44" s="10"/>
+      <c r="L44" s="55" t="s">
+        <v>317</v>
+      </c>
       <c r="M44" s="10"/>
     </row>
-    <row r="45" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A45" s="49" t="s">
-        <v>270</v>
+    <row r="45" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A45" s="45" t="s">
+        <v>269</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D45" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E45" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E45" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F45" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G45" s="22"/>
-      <c r="H45" s="51" t="s">
-        <v>225</v>
+      <c r="H45" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
-      <c r="L45" s="10"/>
+      <c r="L45" s="55" t="s">
+        <v>318</v>
+      </c>
       <c r="M45" s="10"/>
     </row>
-    <row r="46" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A46" s="49" t="s">
-        <v>271</v>
+    <row r="46" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A46" s="45" t="s">
+        <v>270</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D46" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E46" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E46" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F46" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G46" s="22"/>
-      <c r="H46" s="51" t="s">
-        <v>225</v>
+      <c r="H46" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I46" s="7"/>
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
-      <c r="L46" s="10"/>
+      <c r="L46" s="55" t="s">
+        <v>319</v>
+      </c>
       <c r="M46" s="10"/>
     </row>
-    <row r="47" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A47" s="49" t="s">
-        <v>272</v>
+    <row r="47" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A47" s="45" t="s">
+        <v>271</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D47" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E47" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E47" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F47" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G47" s="22"/>
-      <c r="H47" s="51" t="s">
-        <v>225</v>
+      <c r="H47" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
-      <c r="L47" s="10"/>
+      <c r="L47" s="55" t="s">
+        <v>320</v>
+      </c>
       <c r="M47" s="10"/>
     </row>
-    <row r="48" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A48" s="49" t="s">
-        <v>92</v>
+    <row r="48" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A48" s="45" t="s">
+        <v>91</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D48" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E48" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E48" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F48" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G48" s="22"/>
-      <c r="H48" s="51" t="s">
-        <v>225</v>
+      <c r="H48" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I48" s="7"/>
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
-      <c r="L48" s="10"/>
+      <c r="L48" s="55" t="s">
+        <v>321</v>
+      </c>
       <c r="M48" s="10"/>
     </row>
-    <row r="49" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A49" s="49" t="s">
-        <v>94</v>
+    <row r="49" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A49" s="45" t="s">
+        <v>93</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D49" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E49" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E49" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F49" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G49" s="22"/>
-      <c r="H49" s="51" t="s">
-        <v>225</v>
+      <c r="H49" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
-      <c r="L49" s="10"/>
+      <c r="L49" s="55" t="s">
+        <v>322</v>
+      </c>
       <c r="M49" s="10"/>
     </row>
-    <row r="50" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A50" s="49" t="s">
-        <v>96</v>
+    <row r="50" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A50" s="45" t="s">
+        <v>95</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D50" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E50" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E50" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F50" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G50" s="22"/>
-      <c r="H50" s="51" t="s">
-        <v>225</v>
+      <c r="H50" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
-      <c r="L50" s="10"/>
+      <c r="L50" s="55" t="s">
+        <v>323</v>
+      </c>
       <c r="M50" s="10"/>
     </row>
-    <row r="51" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A51" s="49" t="s">
-        <v>98</v>
+    <row r="51" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A51" s="45" t="s">
+        <v>97</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E51" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E51" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F51" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G51" s="22"/>
-      <c r="H51" s="51" t="s">
-        <v>225</v>
+      <c r="H51" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
       <c r="K51" s="7"/>
-      <c r="L51" s="10"/>
+      <c r="L51" s="55" t="s">
+        <v>324</v>
+      </c>
       <c r="M51" s="10"/>
     </row>
-    <row r="52" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A52" s="49" t="s">
-        <v>100</v>
+    <row r="52" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A52" s="45" t="s">
+        <v>99</v>
       </c>
       <c r="B52" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>212</v>
-      </c>
       <c r="D52" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E52" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E52" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F52" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G52" s="22"/>
-      <c r="H52" s="51" t="s">
-        <v>225</v>
+      <c r="H52" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I52" s="7"/>
       <c r="J52" s="7"/>
       <c r="K52" s="7"/>
-      <c r="L52" s="10"/>
+      <c r="L52" s="55" t="s">
+        <v>325</v>
+      </c>
       <c r="M52" s="10"/>
     </row>
-    <row r="53" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A53" s="49" t="s">
-        <v>102</v>
+    <row r="53" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A53" s="45" t="s">
+        <v>101</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D53" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E53" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E53" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F53" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G53" s="22"/>
-      <c r="H53" s="51" t="s">
-        <v>225</v>
+      <c r="H53" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
       <c r="K53" s="7"/>
-      <c r="L53" s="10"/>
+      <c r="L53" s="55" t="s">
+        <v>324</v>
+      </c>
       <c r="M53" s="10"/>
     </row>
-    <row r="54" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A54" s="49" t="s">
-        <v>104</v>
+    <row r="54" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A54" s="45" t="s">
+        <v>103</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D54" s="30" t="s">
-        <v>255</v>
-      </c>
-      <c r="E54" s="50" t="s">
-        <v>237</v>
+        <v>254</v>
+      </c>
+      <c r="E54" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F54" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G54" s="22"/>
-      <c r="H54" s="51" t="s">
-        <v>226</v>
+      <c r="H54" s="47" t="s">
+        <v>225</v>
       </c>
       <c r="I54" s="7"/>
       <c r="J54" s="7"/>
       <c r="K54" s="7"/>
-      <c r="L54" s="10"/>
+      <c r="L54" s="55"/>
       <c r="M54" s="10"/>
     </row>
-    <row r="55" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A55" s="49" t="s">
-        <v>273</v>
+    <row r="55" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A55" s="45" t="s">
+        <v>272</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D55" s="30" t="s">
-        <v>255</v>
-      </c>
-      <c r="E55" s="50" t="s">
-        <v>237</v>
+        <v>254</v>
+      </c>
+      <c r="E55" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F55" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G55" s="22"/>
-      <c r="H55" s="51" t="s">
-        <v>226</v>
+      <c r="H55" s="47" t="s">
+        <v>225</v>
       </c>
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
       <c r="K55" s="7"/>
-      <c r="L55" s="10"/>
+      <c r="L55" s="55"/>
       <c r="M55" s="10"/>
     </row>
-    <row r="56" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="49" t="s">
-        <v>274</v>
+    <row r="56" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A56" s="45" t="s">
+        <v>273</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D56" s="30" t="s">
-        <v>255</v>
-      </c>
-      <c r="E56" s="50" t="s">
-        <v>237</v>
+        <v>254</v>
+      </c>
+      <c r="E56" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F56" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G56" s="22"/>
-      <c r="H56" s="51" t="s">
-        <v>226</v>
+      <c r="H56" s="47" t="s">
+        <v>225</v>
       </c>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
-      <c r="L56" s="10"/>
+      <c r="L56" s="55"/>
       <c r="M56" s="10"/>
     </row>
-    <row r="57" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A57" s="49" t="s">
-        <v>275</v>
+    <row r="57" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A57" s="45" t="s">
+        <v>274</v>
       </c>
       <c r="B57" s="21" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D57" s="30" t="s">
-        <v>255</v>
-      </c>
-      <c r="E57" s="50" t="s">
-        <v>237</v>
+        <v>254</v>
+      </c>
+      <c r="E57" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F57" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G57" s="22"/>
-      <c r="H57" s="51" t="s">
-        <v>226</v>
+      <c r="H57" s="47" t="s">
+        <v>225</v>
       </c>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
       <c r="K57" s="7"/>
-      <c r="L57" s="10"/>
+      <c r="L57" s="55"/>
       <c r="M57" s="10"/>
     </row>
-    <row r="58" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="49" t="s">
-        <v>276</v>
+    <row r="58" spans="1:13" ht="27" x14ac:dyDescent="0.3">
+      <c r="A58" s="45" t="s">
+        <v>275</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D58" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="E58" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F58" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="E58" s="50" t="s">
-        <v>237</v>
-      </c>
-      <c r="F58" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="G58" s="30" t="s">
-        <v>251</v>
-      </c>
-      <c r="H58" s="51" t="s">
-        <v>227</v>
+        <v>250</v>
+      </c>
+      <c r="H58" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
-      <c r="L58" s="10"/>
+      <c r="L58" s="55"/>
       <c r="M58" s="10"/>
     </row>
-    <row r="59" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="49" t="s">
-        <v>277</v>
+    <row r="59" spans="1:13" ht="27" x14ac:dyDescent="0.3">
+      <c r="A59" s="45" t="s">
+        <v>276</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D59" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="E59" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F59" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="E59" s="50" t="s">
-        <v>237</v>
-      </c>
-      <c r="F59" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="G59" s="30" t="s">
-        <v>251</v>
-      </c>
-      <c r="H59" s="51" t="s">
-        <v>227</v>
+        <v>250</v>
+      </c>
+      <c r="H59" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
-      <c r="L59" s="10"/>
+      <c r="L59" s="55"/>
       <c r="M59" s="10"/>
     </row>
-    <row r="60" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A60" s="49" t="s">
-        <v>279</v>
+    <row r="60" spans="1:13" ht="27" x14ac:dyDescent="0.3">
+      <c r="A60" s="45" t="s">
+        <v>278</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D60" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="E60" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F60" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="E60" s="50" t="s">
-        <v>237</v>
-      </c>
-      <c r="F60" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="G60" s="30" t="s">
-        <v>251</v>
-      </c>
-      <c r="H60" s="51" t="s">
-        <v>227</v>
+        <v>250</v>
+      </c>
+      <c r="H60" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
-      <c r="L60" s="10"/>
+      <c r="L60" s="55"/>
       <c r="M60" s="10"/>
     </row>
-    <row r="61" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A61" s="49" t="s">
-        <v>280</v>
+    <row r="61" spans="1:13" ht="27" x14ac:dyDescent="0.3">
+      <c r="A61" s="45" t="s">
+        <v>279</v>
       </c>
       <c r="B61" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D61" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="E61" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F61" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="G61" s="30" t="s">
         <v>250</v>
       </c>
-      <c r="E61" s="50" t="s">
-        <v>237</v>
-      </c>
-      <c r="F61" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="G61" s="30" t="s">
-        <v>251</v>
-      </c>
-      <c r="H61" s="51" t="s">
-        <v>227</v>
+      <c r="H61" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
-      <c r="L61" s="10"/>
+      <c r="L61" s="55"/>
       <c r="M61" s="10"/>
     </row>
-    <row r="62" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A62" s="49" t="s">
-        <v>281</v>
+    <row r="62" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A62" s="45" t="s">
+        <v>280</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D62" s="7"/>
-      <c r="E62" s="50" t="s">
-        <v>237</v>
+      <c r="E62" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F62" s="22"/>
       <c r="G62" s="22"/>
-      <c r="H62" s="51" t="s">
-        <v>222</v>
+      <c r="H62" s="47" t="s">
+        <v>221</v>
       </c>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
-      <c r="L62" s="10"/>
+      <c r="L62" s="55"/>
       <c r="M62" s="10"/>
     </row>
-    <row r="63" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="49" t="s">
-        <v>282</v>
+    <row r="63" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="45" t="s">
+        <v>281</v>
       </c>
       <c r="B63" s="54"/>
       <c r="C63" s="54"/>
@@ -4058,12 +4201,12 @@
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
-      <c r="L63" s="10"/>
+      <c r="L63" s="55"/>
       <c r="M63" s="10"/>
     </row>
-    <row r="64" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A64" s="49" t="s">
-        <v>283</v>
+    <row r="64" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A64" s="45" t="s">
+        <v>282</v>
       </c>
       <c r="B64" s="54"/>
       <c r="C64" s="54"/>
@@ -4075,12 +4218,12 @@
       <c r="I64" s="7"/>
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
-      <c r="L64" s="10"/>
+      <c r="L64" s="55"/>
       <c r="M64" s="10"/>
     </row>
-    <row r="65" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A65" s="49" t="s">
-        <v>283</v>
+    <row r="65" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A65" s="45" t="s">
+        <v>282</v>
       </c>
       <c r="B65" s="54"/>
       <c r="C65" s="54"/>
@@ -4092,12 +4235,12 @@
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
-      <c r="L65" s="10"/>
+      <c r="L65" s="55"/>
       <c r="M65" s="10"/>
     </row>
-    <row r="66" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A66" s="49" t="s">
-        <v>284</v>
+    <row r="66" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A66" s="45" t="s">
+        <v>283</v>
       </c>
       <c r="B66" s="54"/>
       <c r="C66" s="54"/>
@@ -4109,12 +4252,12 @@
       <c r="I66" s="7"/>
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
-      <c r="L66" s="10"/>
+      <c r="L66" s="55"/>
       <c r="M66" s="10"/>
     </row>
-    <row r="67" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A67" s="49" t="s">
-        <v>285</v>
+    <row r="67" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A67" s="45" t="s">
+        <v>284</v>
       </c>
       <c r="B67" s="54"/>
       <c r="C67" s="54"/>
@@ -4126,12 +4269,12 @@
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
-      <c r="L67" s="10"/>
+      <c r="L67" s="55"/>
       <c r="M67" s="10"/>
     </row>
-    <row r="68" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A68" s="49" t="s">
-        <v>286</v>
+    <row r="68" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A68" s="45" t="s">
+        <v>285</v>
       </c>
       <c r="B68" s="54"/>
       <c r="C68" s="54"/>
@@ -4143,12 +4286,12 @@
       <c r="I68" s="7"/>
       <c r="J68" s="7"/>
       <c r="K68" s="7"/>
-      <c r="L68" s="10"/>
+      <c r="L68" s="55"/>
       <c r="M68" s="10"/>
     </row>
-    <row r="69" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A69" s="49" t="s">
-        <v>286</v>
+    <row r="69" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A69" s="45" t="s">
+        <v>285</v>
       </c>
       <c r="B69" s="54"/>
       <c r="C69" s="54"/>
@@ -4160,12 +4303,12 @@
       <c r="I69" s="7"/>
       <c r="J69" s="7"/>
       <c r="K69" s="7"/>
-      <c r="L69" s="10"/>
+      <c r="L69" s="55"/>
       <c r="M69" s="10"/>
     </row>
-    <row r="70" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A70" s="49" t="s">
-        <v>287</v>
+    <row r="70" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A70" s="45" t="s">
+        <v>286</v>
       </c>
       <c r="B70" s="54"/>
       <c r="C70" s="54"/>
@@ -4177,12 +4320,12 @@
       <c r="I70" s="7"/>
       <c r="J70" s="7"/>
       <c r="K70" s="7"/>
-      <c r="L70" s="10"/>
+      <c r="L70" s="55"/>
       <c r="M70" s="10"/>
     </row>
-    <row r="71" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A71" s="49" t="s">
-        <v>288</v>
+    <row r="71" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A71" s="45" t="s">
+        <v>287</v>
       </c>
       <c r="B71" s="21"/>
       <c r="C71" s="7"/>
@@ -4194,12 +4337,12 @@
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
       <c r="K71" s="7"/>
-      <c r="L71" s="10"/>
+      <c r="L71" s="55"/>
       <c r="M71" s="10"/>
     </row>
-    <row r="72" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A72" s="49" t="s">
-        <v>289</v>
+    <row r="72" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A72" s="45" t="s">
+        <v>288</v>
       </c>
       <c r="B72" s="21"/>
       <c r="C72" s="7"/>
@@ -4211,12 +4354,12 @@
       <c r="I72" s="7"/>
       <c r="J72" s="7"/>
       <c r="K72" s="7"/>
-      <c r="L72" s="10"/>
+      <c r="L72" s="55"/>
       <c r="M72" s="10"/>
     </row>
-    <row r="73" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A73" s="49" t="s">
-        <v>290</v>
+    <row r="73" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A73" s="45" t="s">
+        <v>289</v>
       </c>
       <c r="B73" s="21"/>
       <c r="C73" s="7"/>
@@ -4228,12 +4371,12 @@
       <c r="I73" s="7"/>
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
-      <c r="L73" s="10"/>
+      <c r="L73" s="55"/>
       <c r="M73" s="10"/>
     </row>
-    <row r="74" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A74" s="49" t="s">
-        <v>291</v>
+    <row r="74" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A74" s="45" t="s">
+        <v>290</v>
       </c>
       <c r="B74" s="21"/>
       <c r="C74" s="7"/>
@@ -4245,12 +4388,12 @@
       <c r="I74" s="7"/>
       <c r="J74" s="7"/>
       <c r="K74" s="7"/>
-      <c r="L74" s="10"/>
+      <c r="L74" s="55"/>
       <c r="M74" s="10"/>
     </row>
-    <row r="75" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A75" s="49" t="s">
-        <v>292</v>
+    <row r="75" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A75" s="45" t="s">
+        <v>291</v>
       </c>
       <c r="B75" s="21"/>
       <c r="C75" s="7"/>
@@ -4262,12 +4405,12 @@
       <c r="I75" s="7"/>
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
-      <c r="L75" s="10"/>
+      <c r="L75" s="55"/>
       <c r="M75" s="10"/>
     </row>
-    <row r="76" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A76" s="49" t="s">
-        <v>293</v>
+    <row r="76" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A76" s="45" t="s">
+        <v>292</v>
       </c>
       <c r="B76" s="21"/>
       <c r="C76" s="7"/>
@@ -4279,12 +4422,12 @@
       <c r="I76" s="7"/>
       <c r="J76" s="7"/>
       <c r="K76" s="7"/>
-      <c r="L76" s="10"/>
+      <c r="L76" s="55"/>
       <c r="M76" s="10"/>
     </row>
-    <row r="77" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A77" s="49" t="s">
-        <v>294</v>
+    <row r="77" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A77" s="45" t="s">
+        <v>293</v>
       </c>
       <c r="B77" s="21"/>
       <c r="C77" s="7"/>
@@ -4296,12 +4439,12 @@
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
-      <c r="L77" s="10"/>
+      <c r="L77" s="55"/>
       <c r="M77" s="10"/>
     </row>
-    <row r="78" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A78" s="49" t="s">
-        <v>295</v>
+    <row r="78" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A78" s="45" t="s">
+        <v>294</v>
       </c>
       <c r="B78" s="21"/>
       <c r="C78" s="7"/>
@@ -4313,12 +4456,12 @@
       <c r="I78" s="7"/>
       <c r="J78" s="7"/>
       <c r="K78" s="7"/>
-      <c r="L78" s="10"/>
+      <c r="L78" s="55"/>
       <c r="M78" s="10"/>
     </row>
-    <row r="79" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A79" s="49" t="s">
-        <v>296</v>
+    <row r="79" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A79" s="45" t="s">
+        <v>295</v>
       </c>
       <c r="B79" s="21"/>
       <c r="C79" s="7"/>
@@ -4330,12 +4473,12 @@
       <c r="I79" s="7"/>
       <c r="J79" s="7"/>
       <c r="K79" s="7"/>
-      <c r="L79" s="10"/>
+      <c r="L79" s="55"/>
       <c r="M79" s="10"/>
     </row>
-    <row r="80" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A80" s="49" t="s">
-        <v>297</v>
+    <row r="80" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A80" s="45" t="s">
+        <v>296</v>
       </c>
       <c r="B80" s="21"/>
       <c r="C80" s="7"/>
@@ -4347,12 +4490,12 @@
       <c r="I80" s="7"/>
       <c r="J80" s="7"/>
       <c r="K80" s="7"/>
-      <c r="L80" s="10"/>
+      <c r="L80" s="55"/>
       <c r="M80" s="10"/>
     </row>
-    <row r="81" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A81" s="49" t="s">
-        <v>298</v>
+    <row r="81" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A81" s="45" t="s">
+        <v>297</v>
       </c>
       <c r="B81" s="21"/>
       <c r="C81" s="7"/>
@@ -4364,12 +4507,12 @@
       <c r="I81" s="7"/>
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
-      <c r="L81" s="10"/>
+      <c r="L81" s="55"/>
       <c r="M81" s="10"/>
     </row>
-    <row r="82" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A82" s="49" t="s">
-        <v>299</v>
+    <row r="82" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A82" s="45" t="s">
+        <v>298</v>
       </c>
       <c r="B82" s="21"/>
       <c r="C82" s="7"/>
@@ -4381,12 +4524,12 @@
       <c r="I82" s="7"/>
       <c r="J82" s="7"/>
       <c r="K82" s="7"/>
-      <c r="L82" s="10"/>
+      <c r="L82" s="55"/>
       <c r="M82" s="10"/>
     </row>
-    <row r="83" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A83" s="49" t="s">
-        <v>300</v>
+    <row r="83" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A83" s="45" t="s">
+        <v>299</v>
       </c>
       <c r="B83" s="21"/>
       <c r="C83" s="7"/>
@@ -4398,12 +4541,12 @@
       <c r="I83" s="7"/>
       <c r="J83" s="7"/>
       <c r="K83" s="7"/>
-      <c r="L83" s="10"/>
+      <c r="L83" s="55"/>
       <c r="M83" s="10"/>
     </row>
-    <row r="84" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A84" s="49" t="s">
-        <v>301</v>
+    <row r="84" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A84" s="45" t="s">
+        <v>300</v>
       </c>
       <c r="B84" s="21"/>
       <c r="C84" s="7"/>
@@ -4415,12 +4558,12 @@
       <c r="I84" s="7"/>
       <c r="J84" s="7"/>
       <c r="K84" s="7"/>
-      <c r="L84" s="10"/>
+      <c r="L84" s="55"/>
       <c r="M84" s="10"/>
     </row>
-    <row r="85" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A85" s="49" t="s">
-        <v>302</v>
+    <row r="85" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A85" s="45" t="s">
+        <v>301</v>
       </c>
       <c r="B85" s="21"/>
       <c r="C85" s="7"/>
@@ -4432,12 +4575,12 @@
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
       <c r="K85" s="7"/>
-      <c r="L85" s="10"/>
+      <c r="L85" s="55"/>
       <c r="M85" s="10"/>
     </row>
-    <row r="86" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A86" s="49" t="s">
-        <v>120</v>
+    <row r="86" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A86" s="45" t="s">
+        <v>119</v>
       </c>
       <c r="B86" s="21"/>
       <c r="C86" s="7"/>
@@ -4449,12 +4592,12 @@
       <c r="I86" s="7"/>
       <c r="J86" s="7"/>
       <c r="K86" s="7"/>
-      <c r="L86" s="10"/>
+      <c r="L86" s="55"/>
       <c r="M86" s="10"/>
     </row>
-    <row r="87" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A87" s="49" t="s">
-        <v>121</v>
+    <row r="87" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A87" s="45" t="s">
+        <v>120</v>
       </c>
       <c r="B87" s="21"/>
       <c r="C87" s="7"/>
@@ -4466,12 +4609,12 @@
       <c r="I87" s="7"/>
       <c r="J87" s="7"/>
       <c r="K87" s="7"/>
-      <c r="L87" s="10"/>
+      <c r="L87" s="55"/>
       <c r="M87" s="10"/>
     </row>
-    <row r="88" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A88" s="49" t="s">
-        <v>122</v>
+    <row r="88" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A88" s="45" t="s">
+        <v>121</v>
       </c>
       <c r="B88" s="21"/>
       <c r="C88" s="7"/>
@@ -4483,12 +4626,12 @@
       <c r="I88" s="7"/>
       <c r="J88" s="7"/>
       <c r="K88" s="7"/>
-      <c r="L88" s="10"/>
+      <c r="L88" s="55"/>
       <c r="M88" s="10"/>
     </row>
-    <row r="89" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A89" s="49" t="s">
-        <v>123</v>
+    <row r="89" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A89" s="45" t="s">
+        <v>122</v>
       </c>
       <c r="B89" s="21"/>
       <c r="C89" s="7"/>
@@ -4500,12 +4643,12 @@
       <c r="I89" s="7"/>
       <c r="J89" s="7"/>
       <c r="K89" s="7"/>
-      <c r="L89" s="10"/>
+      <c r="L89" s="55"/>
       <c r="M89" s="10"/>
     </row>
-    <row r="90" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A90" s="49" t="s">
-        <v>124</v>
+    <row r="90" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A90" s="45" t="s">
+        <v>123</v>
       </c>
       <c r="B90" s="21"/>
       <c r="C90" s="7"/>
@@ -4517,12 +4660,12 @@
       <c r="I90" s="7"/>
       <c r="J90" s="7"/>
       <c r="K90" s="7"/>
-      <c r="L90" s="10"/>
+      <c r="L90" s="55"/>
       <c r="M90" s="10"/>
     </row>
-    <row r="91" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A91" s="49" t="s">
-        <v>125</v>
+    <row r="91" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A91" s="45" t="s">
+        <v>124</v>
       </c>
       <c r="B91" s="21"/>
       <c r="C91" s="7"/>
@@ -4534,12 +4677,12 @@
       <c r="I91" s="7"/>
       <c r="J91" s="7"/>
       <c r="K91" s="7"/>
-      <c r="L91" s="10"/>
+      <c r="L91" s="55"/>
       <c r="M91" s="10"/>
     </row>
-    <row r="92" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A92" s="49" t="s">
-        <v>126</v>
+    <row r="92" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A92" s="45" t="s">
+        <v>125</v>
       </c>
       <c r="B92" s="21"/>
       <c r="C92" s="7"/>
@@ -4551,12 +4694,12 @@
       <c r="I92" s="7"/>
       <c r="J92" s="7"/>
       <c r="K92" s="7"/>
-      <c r="L92" s="10"/>
+      <c r="L92" s="55"/>
       <c r="M92" s="10"/>
     </row>
-    <row r="93" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A93" s="49" t="s">
-        <v>127</v>
+    <row r="93" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A93" s="45" t="s">
+        <v>126</v>
       </c>
       <c r="B93" s="21"/>
       <c r="C93" s="7"/>
@@ -4568,12 +4711,12 @@
       <c r="I93" s="7"/>
       <c r="J93" s="7"/>
       <c r="K93" s="7"/>
-      <c r="L93" s="10"/>
+      <c r="L93" s="55"/>
       <c r="M93" s="10"/>
     </row>
-    <row r="94" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A94" s="49" t="s">
-        <v>128</v>
+    <row r="94" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A94" s="45" t="s">
+        <v>127</v>
       </c>
       <c r="B94" s="21"/>
       <c r="C94" s="7"/>
@@ -4585,12 +4728,12 @@
       <c r="I94" s="7"/>
       <c r="J94" s="7"/>
       <c r="K94" s="7"/>
-      <c r="L94" s="10"/>
+      <c r="L94" s="55"/>
       <c r="M94" s="10"/>
     </row>
-    <row r="95" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A95" s="49" t="s">
-        <v>129</v>
+    <row r="95" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A95" s="45" t="s">
+        <v>128</v>
       </c>
       <c r="B95" s="21"/>
       <c r="C95" s="7"/>
@@ -4602,12 +4745,12 @@
       <c r="I95" s="7"/>
       <c r="J95" s="7"/>
       <c r="K95" s="7"/>
-      <c r="L95" s="10"/>
+      <c r="L95" s="55"/>
       <c r="M95" s="10"/>
     </row>
-    <row r="96" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A96" s="49" t="s">
-        <v>130</v>
+    <row r="96" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A96" s="45" t="s">
+        <v>129</v>
       </c>
       <c r="B96" s="21"/>
       <c r="C96" s="7"/>
@@ -4619,12 +4762,12 @@
       <c r="I96" s="7"/>
       <c r="J96" s="7"/>
       <c r="K96" s="7"/>
-      <c r="L96" s="10"/>
+      <c r="L96" s="55"/>
       <c r="M96" s="10"/>
     </row>
-    <row r="97" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A97" s="49" t="s">
-        <v>131</v>
+    <row r="97" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A97" s="45" t="s">
+        <v>130</v>
       </c>
       <c r="B97" s="21"/>
       <c r="C97" s="7"/>
@@ -4636,12 +4779,12 @@
       <c r="I97" s="7"/>
       <c r="J97" s="7"/>
       <c r="K97" s="7"/>
-      <c r="L97" s="10"/>
+      <c r="L97" s="55"/>
       <c r="M97" s="10"/>
     </row>
-    <row r="98" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A98" s="49" t="s">
-        <v>132</v>
+    <row r="98" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A98" s="45" t="s">
+        <v>131</v>
       </c>
       <c r="B98" s="21"/>
       <c r="C98" s="7"/>
@@ -4653,12 +4796,12 @@
       <c r="I98" s="7"/>
       <c r="J98" s="7"/>
       <c r="K98" s="7"/>
-      <c r="L98" s="10"/>
+      <c r="L98" s="55"/>
       <c r="M98" s="10"/>
     </row>
-    <row r="99" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A99" s="49" t="s">
-        <v>133</v>
+    <row r="99" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A99" s="45" t="s">
+        <v>132</v>
       </c>
       <c r="B99" s="21"/>
       <c r="C99" s="7"/>
@@ -4670,12 +4813,12 @@
       <c r="I99" s="7"/>
       <c r="J99" s="7"/>
       <c r="K99" s="7"/>
-      <c r="L99" s="10"/>
+      <c r="L99" s="55"/>
       <c r="M99" s="10"/>
     </row>
-    <row r="100" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A100" s="49" t="s">
-        <v>134</v>
+    <row r="100" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A100" s="45" t="s">
+        <v>133</v>
       </c>
       <c r="B100" s="21"/>
       <c r="C100" s="7"/>
@@ -4687,12 +4830,12 @@
       <c r="I100" s="7"/>
       <c r="J100" s="7"/>
       <c r="K100" s="7"/>
-      <c r="L100" s="10"/>
+      <c r="L100" s="55"/>
       <c r="M100" s="10"/>
     </row>
-    <row r="101" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A101" s="49" t="s">
-        <v>135</v>
+    <row r="101" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A101" s="45" t="s">
+        <v>134</v>
       </c>
       <c r="B101" s="21"/>
       <c r="C101" s="7"/>
@@ -4704,12 +4847,12 @@
       <c r="I101" s="7"/>
       <c r="J101" s="7"/>
       <c r="K101" s="7"/>
-      <c r="L101" s="10"/>
+      <c r="L101" s="55"/>
       <c r="M101" s="10"/>
     </row>
-    <row r="102" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A102" s="49" t="s">
-        <v>136</v>
+    <row r="102" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A102" s="45" t="s">
+        <v>135</v>
       </c>
       <c r="B102" s="21"/>
       <c r="C102" s="7"/>
@@ -4721,12 +4864,12 @@
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
       <c r="K102" s="7"/>
-      <c r="L102" s="10"/>
+      <c r="L102" s="55"/>
       <c r="M102" s="10"/>
     </row>
-    <row r="103" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A103" s="49" t="s">
-        <v>137</v>
+    <row r="103" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A103" s="45" t="s">
+        <v>136</v>
       </c>
       <c r="B103" s="21"/>
       <c r="C103" s="7"/>
@@ -4738,12 +4881,12 @@
       <c r="I103" s="7"/>
       <c r="J103" s="7"/>
       <c r="K103" s="7"/>
-      <c r="L103" s="10"/>
+      <c r="L103" s="55"/>
       <c r="M103" s="10"/>
     </row>
-    <row r="104" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A104" s="49" t="s">
-        <v>138</v>
+    <row r="104" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A104" s="45" t="s">
+        <v>137</v>
       </c>
       <c r="B104" s="21"/>
       <c r="C104" s="7"/>
@@ -4755,12 +4898,12 @@
       <c r="I104" s="7"/>
       <c r="J104" s="7"/>
       <c r="K104" s="7"/>
-      <c r="L104" s="10"/>
+      <c r="L104" s="55"/>
       <c r="M104" s="10"/>
     </row>
-    <row r="105" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A105" s="49" t="s">
-        <v>139</v>
+    <row r="105" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A105" s="45" t="s">
+        <v>138</v>
       </c>
       <c r="B105" s="21"/>
       <c r="C105" s="7"/>
@@ -4772,12 +4915,12 @@
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
       <c r="K105" s="7"/>
-      <c r="L105" s="10"/>
+      <c r="L105" s="55"/>
       <c r="M105" s="10"/>
     </row>
-    <row r="106" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A106" s="49" t="s">
-        <v>140</v>
+    <row r="106" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A106" s="45" t="s">
+        <v>139</v>
       </c>
       <c r="B106" s="21"/>
       <c r="C106" s="7"/>
@@ -4789,12 +4932,12 @@
       <c r="I106" s="7"/>
       <c r="J106" s="7"/>
       <c r="K106" s="7"/>
-      <c r="L106" s="10"/>
+      <c r="L106" s="55"/>
       <c r="M106" s="10"/>
     </row>
-    <row r="107" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A107" s="49" t="s">
-        <v>141</v>
+    <row r="107" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A107" s="45" t="s">
+        <v>140</v>
       </c>
       <c r="B107" s="21"/>
       <c r="C107" s="7"/>
@@ -4806,12 +4949,12 @@
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
       <c r="K107" s="7"/>
-      <c r="L107" s="10"/>
+      <c r="L107" s="55"/>
       <c r="M107" s="10"/>
     </row>
-    <row r="108" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A108" s="49" t="s">
-        <v>142</v>
+    <row r="108" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A108" s="45" t="s">
+        <v>141</v>
       </c>
       <c r="B108" s="21"/>
       <c r="C108" s="7"/>
@@ -4823,12 +4966,12 @@
       <c r="I108" s="7"/>
       <c r="J108" s="7"/>
       <c r="K108" s="7"/>
-      <c r="L108" s="10"/>
+      <c r="L108" s="55"/>
       <c r="M108" s="10"/>
     </row>
-    <row r="109" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A109" s="49" t="s">
-        <v>143</v>
+    <row r="109" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A109" s="45" t="s">
+        <v>142</v>
       </c>
       <c r="B109" s="21"/>
       <c r="C109" s="7"/>
@@ -4840,12 +4983,12 @@
       <c r="I109" s="7"/>
       <c r="J109" s="7"/>
       <c r="K109" s="7"/>
-      <c r="L109" s="10"/>
+      <c r="L109" s="55"/>
       <c r="M109" s="10"/>
     </row>
-    <row r="110" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A110" s="49" t="s">
-        <v>144</v>
+    <row r="110" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A110" s="45" t="s">
+        <v>143</v>
       </c>
       <c r="B110" s="21"/>
       <c r="C110" s="7"/>
@@ -4857,12 +5000,12 @@
       <c r="I110" s="7"/>
       <c r="J110" s="7"/>
       <c r="K110" s="7"/>
-      <c r="L110" s="10"/>
+      <c r="L110" s="55"/>
       <c r="M110" s="10"/>
     </row>
-    <row r="111" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A111" s="49" t="s">
-        <v>145</v>
+    <row r="111" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A111" s="45" t="s">
+        <v>144</v>
       </c>
       <c r="B111" s="21"/>
       <c r="C111" s="7"/>
@@ -4874,12 +5017,12 @@
       <c r="I111" s="7"/>
       <c r="J111" s="7"/>
       <c r="K111" s="7"/>
-      <c r="L111" s="10"/>
+      <c r="L111" s="55"/>
       <c r="M111" s="10"/>
     </row>
-    <row r="112" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A112" s="49" t="s">
-        <v>146</v>
+    <row r="112" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A112" s="45" t="s">
+        <v>145</v>
       </c>
       <c r="B112" s="21"/>
       <c r="C112" s="7"/>
@@ -4891,12 +5034,12 @@
       <c r="I112" s="7"/>
       <c r="J112" s="7"/>
       <c r="K112" s="7"/>
-      <c r="L112" s="10"/>
+      <c r="L112" s="55"/>
       <c r="M112" s="10"/>
     </row>
-    <row r="113" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A113" s="49" t="s">
-        <v>147</v>
+    <row r="113" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A113" s="45" t="s">
+        <v>146</v>
       </c>
       <c r="B113" s="21"/>
       <c r="C113" s="7"/>
@@ -4908,12 +5051,12 @@
       <c r="I113" s="7"/>
       <c r="J113" s="7"/>
       <c r="K113" s="7"/>
-      <c r="L113" s="10"/>
+      <c r="L113" s="55"/>
       <c r="M113" s="10"/>
     </row>
-    <row r="114" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A114" s="49" t="s">
-        <v>148</v>
+    <row r="114" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A114" s="45" t="s">
+        <v>147</v>
       </c>
       <c r="B114" s="21"/>
       <c r="C114" s="7"/>
@@ -4925,12 +5068,12 @@
       <c r="I114" s="7"/>
       <c r="J114" s="7"/>
       <c r="K114" s="7"/>
-      <c r="L114" s="10"/>
+      <c r="L114" s="55"/>
       <c r="M114" s="10"/>
     </row>
-    <row r="115" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A115" s="49" t="s">
-        <v>149</v>
+    <row r="115" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A115" s="45" t="s">
+        <v>148</v>
       </c>
       <c r="B115" s="21"/>
       <c r="C115" s="7"/>
@@ -4942,12 +5085,12 @@
       <c r="I115" s="7"/>
       <c r="J115" s="7"/>
       <c r="K115" s="7"/>
-      <c r="L115" s="10"/>
+      <c r="L115" s="55"/>
       <c r="M115" s="10"/>
     </row>
-    <row r="116" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A116" s="49" t="s">
-        <v>150</v>
+    <row r="116" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A116" s="45" t="s">
+        <v>149</v>
       </c>
       <c r="B116" s="21"/>
       <c r="C116" s="7"/>
@@ -4959,12 +5102,12 @@
       <c r="I116" s="7"/>
       <c r="J116" s="7"/>
       <c r="K116" s="7"/>
-      <c r="L116" s="10"/>
+      <c r="L116" s="55"/>
       <c r="M116" s="10"/>
     </row>
-    <row r="117" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A117" s="49" t="s">
-        <v>151</v>
+    <row r="117" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A117" s="45" t="s">
+        <v>150</v>
       </c>
       <c r="B117" s="21"/>
       <c r="C117" s="7"/>
@@ -4976,12 +5119,12 @@
       <c r="I117" s="7"/>
       <c r="J117" s="7"/>
       <c r="K117" s="7"/>
-      <c r="L117" s="10"/>
+      <c r="L117" s="55"/>
       <c r="M117" s="10"/>
     </row>
-    <row r="118" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A118" s="49" t="s">
-        <v>152</v>
+    <row r="118" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A118" s="45" t="s">
+        <v>151</v>
       </c>
       <c r="B118" s="21"/>
       <c r="C118" s="7"/>
@@ -4993,12 +5136,12 @@
       <c r="I118" s="7"/>
       <c r="J118" s="7"/>
       <c r="K118" s="7"/>
-      <c r="L118" s="10"/>
+      <c r="L118" s="55"/>
       <c r="M118" s="10"/>
     </row>
-    <row r="119" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A119" s="49" t="s">
-        <v>153</v>
+    <row r="119" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A119" s="45" t="s">
+        <v>152</v>
       </c>
       <c r="B119" s="21"/>
       <c r="C119" s="7"/>
@@ -5010,12 +5153,12 @@
       <c r="I119" s="7"/>
       <c r="J119" s="7"/>
       <c r="K119" s="7"/>
-      <c r="L119" s="10"/>
+      <c r="L119" s="55"/>
       <c r="M119" s="10"/>
     </row>
-    <row r="120" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A120" s="49" t="s">
-        <v>154</v>
+    <row r="120" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A120" s="45" t="s">
+        <v>153</v>
       </c>
       <c r="B120" s="21"/>
       <c r="C120" s="7"/>
@@ -5027,12 +5170,12 @@
       <c r="I120" s="7"/>
       <c r="J120" s="7"/>
       <c r="K120" s="7"/>
-      <c r="L120" s="10"/>
+      <c r="L120" s="55"/>
       <c r="M120" s="10"/>
     </row>
-    <row r="121" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A121" s="49" t="s">
-        <v>155</v>
+    <row r="121" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A121" s="45" t="s">
+        <v>154</v>
       </c>
       <c r="B121" s="21"/>
       <c r="C121" s="7"/>
@@ -5044,12 +5187,12 @@
       <c r="I121" s="7"/>
       <c r="J121" s="7"/>
       <c r="K121" s="7"/>
-      <c r="L121" s="10"/>
+      <c r="L121" s="55"/>
       <c r="M121" s="10"/>
     </row>
-    <row r="122" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A122" s="49" t="s">
-        <v>156</v>
+    <row r="122" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A122" s="45" t="s">
+        <v>155</v>
       </c>
       <c r="B122" s="21"/>
       <c r="C122" s="7"/>
@@ -5061,12 +5204,12 @@
       <c r="I122" s="7"/>
       <c r="J122" s="7"/>
       <c r="K122" s="7"/>
-      <c r="L122" s="10"/>
+      <c r="L122" s="55"/>
       <c r="M122" s="10"/>
     </row>
-    <row r="123" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A123" s="49" t="s">
-        <v>157</v>
+    <row r="123" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A123" s="45" t="s">
+        <v>156</v>
       </c>
       <c r="B123" s="21"/>
       <c r="C123" s="7"/>
@@ -5078,12 +5221,12 @@
       <c r="I123" s="7"/>
       <c r="J123" s="7"/>
       <c r="K123" s="7"/>
-      <c r="L123" s="10"/>
+      <c r="L123" s="55"/>
       <c r="M123" s="10"/>
     </row>
-    <row r="124" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A124" s="49" t="s">
-        <v>158</v>
+    <row r="124" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A124" s="45" t="s">
+        <v>157</v>
       </c>
       <c r="B124" s="21"/>
       <c r="C124" s="7"/>
@@ -5095,12 +5238,12 @@
       <c r="I124" s="7"/>
       <c r="J124" s="7"/>
       <c r="K124" s="7"/>
-      <c r="L124" s="10"/>
+      <c r="L124" s="55"/>
       <c r="M124" s="10"/>
     </row>
-    <row r="125" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A125" s="49" t="s">
-        <v>159</v>
+    <row r="125" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A125" s="45" t="s">
+        <v>158</v>
       </c>
       <c r="B125" s="21"/>
       <c r="C125" s="7"/>
@@ -5112,12 +5255,12 @@
       <c r="I125" s="7"/>
       <c r="J125" s="7"/>
       <c r="K125" s="7"/>
-      <c r="L125" s="10"/>
+      <c r="L125" s="55"/>
       <c r="M125" s="10"/>
     </row>
-    <row r="126" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A126" s="49" t="s">
-        <v>160</v>
+    <row r="126" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A126" s="45" t="s">
+        <v>159</v>
       </c>
       <c r="B126" s="21"/>
       <c r="C126" s="7"/>
@@ -5129,12 +5272,12 @@
       <c r="I126" s="7"/>
       <c r="J126" s="7"/>
       <c r="K126" s="7"/>
-      <c r="L126" s="10"/>
+      <c r="L126" s="55"/>
       <c r="M126" s="10"/>
     </row>
-    <row r="127" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A127" s="49" t="s">
-        <v>161</v>
+    <row r="127" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A127" s="45" t="s">
+        <v>160</v>
       </c>
       <c r="B127" s="21"/>
       <c r="C127" s="7"/>
@@ -5146,12 +5289,12 @@
       <c r="I127" s="7"/>
       <c r="J127" s="7"/>
       <c r="K127" s="7"/>
-      <c r="L127" s="10"/>
+      <c r="L127" s="55"/>
       <c r="M127" s="10"/>
     </row>
-    <row r="128" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A128" s="49" t="s">
-        <v>162</v>
+    <row r="128" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A128" s="45" t="s">
+        <v>161</v>
       </c>
       <c r="B128" s="21"/>
       <c r="C128" s="7"/>
@@ -5163,12 +5306,12 @@
       <c r="I128" s="7"/>
       <c r="J128" s="7"/>
       <c r="K128" s="7"/>
-      <c r="L128" s="10"/>
+      <c r="L128" s="55"/>
       <c r="M128" s="10"/>
     </row>
-    <row r="129" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A129" s="49" t="s">
-        <v>163</v>
+    <row r="129" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A129" s="45" t="s">
+        <v>162</v>
       </c>
       <c r="B129" s="21"/>
       <c r="C129" s="7"/>
@@ -5180,12 +5323,12 @@
       <c r="I129" s="7"/>
       <c r="J129" s="7"/>
       <c r="K129" s="7"/>
-      <c r="L129" s="10"/>
+      <c r="L129" s="55"/>
       <c r="M129" s="10"/>
     </row>
-    <row r="130" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A130" s="49" t="s">
-        <v>164</v>
+    <row r="130" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A130" s="45" t="s">
+        <v>163</v>
       </c>
       <c r="B130" s="21"/>
       <c r="C130" s="7"/>
@@ -5197,12 +5340,12 @@
       <c r="I130" s="7"/>
       <c r="J130" s="7"/>
       <c r="K130" s="7"/>
-      <c r="L130" s="10"/>
+      <c r="L130" s="55"/>
       <c r="M130" s="10"/>
     </row>
-    <row r="131" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A131" s="49" t="s">
-        <v>165</v>
+    <row r="131" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A131" s="45" t="s">
+        <v>164</v>
       </c>
       <c r="B131" s="21"/>
       <c r="C131" s="7"/>
@@ -5214,12 +5357,12 @@
       <c r="I131" s="7"/>
       <c r="J131" s="7"/>
       <c r="K131" s="7"/>
-      <c r="L131" s="10"/>
+      <c r="L131" s="55"/>
       <c r="M131" s="10"/>
     </row>
-    <row r="132" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A132" s="49" t="s">
-        <v>166</v>
+    <row r="132" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A132" s="45" t="s">
+        <v>165</v>
       </c>
       <c r="B132" s="21"/>
       <c r="C132" s="7"/>
@@ -5231,12 +5374,12 @@
       <c r="I132" s="7"/>
       <c r="J132" s="7"/>
       <c r="K132" s="7"/>
-      <c r="L132" s="10"/>
+      <c r="L132" s="55"/>
       <c r="M132" s="10"/>
     </row>
-    <row r="133" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A133" s="49" t="s">
-        <v>167</v>
+    <row r="133" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A133" s="45" t="s">
+        <v>166</v>
       </c>
       <c r="B133" s="21"/>
       <c r="C133" s="7"/>
@@ -5248,12 +5391,12 @@
       <c r="I133" s="7"/>
       <c r="J133" s="7"/>
       <c r="K133" s="7"/>
-      <c r="L133" s="10"/>
+      <c r="L133" s="55"/>
       <c r="M133" s="10"/>
     </row>
-    <row r="134" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A134" s="49" t="s">
-        <v>168</v>
+    <row r="134" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A134" s="45" t="s">
+        <v>167</v>
       </c>
       <c r="B134" s="21"/>
       <c r="C134" s="7"/>
@@ -5265,12 +5408,12 @@
       <c r="I134" s="7"/>
       <c r="J134" s="7"/>
       <c r="K134" s="7"/>
-      <c r="L134" s="10"/>
+      <c r="L134" s="55"/>
       <c r="M134" s="10"/>
     </row>
-    <row r="135" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A135" s="49" t="s">
-        <v>169</v>
+    <row r="135" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A135" s="45" t="s">
+        <v>168</v>
       </c>
       <c r="B135" s="21"/>
       <c r="C135" s="7"/>
@@ -5282,12 +5425,12 @@
       <c r="I135" s="7"/>
       <c r="J135" s="7"/>
       <c r="K135" s="7"/>
-      <c r="L135" s="10"/>
+      <c r="L135" s="55"/>
       <c r="M135" s="10"/>
     </row>
-    <row r="136" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A136" s="49" t="s">
-        <v>170</v>
+    <row r="136" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A136" s="45" t="s">
+        <v>169</v>
       </c>
       <c r="B136" s="21"/>
       <c r="C136" s="7"/>
@@ -5299,12 +5442,12 @@
       <c r="I136" s="7"/>
       <c r="J136" s="7"/>
       <c r="K136" s="7"/>
-      <c r="L136" s="10"/>
+      <c r="L136" s="55"/>
       <c r="M136" s="10"/>
     </row>
-    <row r="137" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A137" s="49" t="s">
-        <v>171</v>
+    <row r="137" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A137" s="45" t="s">
+        <v>170</v>
       </c>
       <c r="B137" s="21"/>
       <c r="C137" s="7"/>
@@ -5316,12 +5459,12 @@
       <c r="I137" s="7"/>
       <c r="J137" s="7"/>
       <c r="K137" s="7"/>
-      <c r="L137" s="10"/>
+      <c r="L137" s="55"/>
       <c r="M137" s="10"/>
     </row>
-    <row r="138" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A138" s="49" t="s">
-        <v>172</v>
+    <row r="138" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A138" s="45" t="s">
+        <v>171</v>
       </c>
       <c r="B138" s="21"/>
       <c r="C138" s="7"/>
@@ -5333,12 +5476,12 @@
       <c r="I138" s="7"/>
       <c r="J138" s="7"/>
       <c r="K138" s="7"/>
-      <c r="L138" s="10"/>
+      <c r="L138" s="55"/>
       <c r="M138" s="10"/>
     </row>
-    <row r="139" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A139" s="49" t="s">
-        <v>173</v>
+    <row r="139" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A139" s="45" t="s">
+        <v>172</v>
       </c>
       <c r="B139" s="21"/>
       <c r="C139" s="7"/>
@@ -5350,12 +5493,12 @@
       <c r="I139" s="7"/>
       <c r="J139" s="7"/>
       <c r="K139" s="7"/>
-      <c r="L139" s="10"/>
+      <c r="L139" s="55"/>
       <c r="M139" s="10"/>
     </row>
-    <row r="140" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A140" s="49" t="s">
-        <v>174</v>
+    <row r="140" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A140" s="45" t="s">
+        <v>173</v>
       </c>
       <c r="B140" s="21"/>
       <c r="C140" s="7"/>
@@ -5367,12 +5510,12 @@
       <c r="I140" s="7"/>
       <c r="J140" s="7"/>
       <c r="K140" s="7"/>
-      <c r="L140" s="10"/>
+      <c r="L140" s="55"/>
       <c r="M140" s="10"/>
     </row>
-    <row r="141" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A141" s="49" t="s">
-        <v>175</v>
+    <row r="141" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A141" s="45" t="s">
+        <v>174</v>
       </c>
       <c r="B141" s="21"/>
       <c r="C141" s="7"/>
@@ -5384,12 +5527,12 @@
       <c r="I141" s="7"/>
       <c r="J141" s="7"/>
       <c r="K141" s="7"/>
-      <c r="L141" s="10"/>
+      <c r="L141" s="55"/>
       <c r="M141" s="10"/>
     </row>
-    <row r="142" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A142" s="49" t="s">
-        <v>176</v>
+    <row r="142" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A142" s="45" t="s">
+        <v>175</v>
       </c>
       <c r="B142" s="21"/>
       <c r="C142" s="7"/>
@@ -5401,12 +5544,12 @@
       <c r="I142" s="7"/>
       <c r="J142" s="7"/>
       <c r="K142" s="7"/>
-      <c r="L142" s="10"/>
+      <c r="L142" s="55"/>
       <c r="M142" s="10"/>
     </row>
-    <row r="143" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A143" s="49" t="s">
-        <v>177</v>
+    <row r="143" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A143" s="45" t="s">
+        <v>176</v>
       </c>
       <c r="B143" s="21"/>
       <c r="C143" s="7"/>
@@ -5418,12 +5561,12 @@
       <c r="I143" s="7"/>
       <c r="J143" s="7"/>
       <c r="K143" s="7"/>
-      <c r="L143" s="10"/>
+      <c r="L143" s="55"/>
       <c r="M143" s="10"/>
     </row>
-    <row r="144" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A144" s="49" t="s">
-        <v>178</v>
+    <row r="144" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A144" s="45" t="s">
+        <v>177</v>
       </c>
       <c r="B144" s="21"/>
       <c r="C144" s="7"/>
@@ -5435,12 +5578,12 @@
       <c r="I144" s="7"/>
       <c r="J144" s="7"/>
       <c r="K144" s="7"/>
-      <c r="L144" s="10"/>
+      <c r="L144" s="55"/>
       <c r="M144" s="10"/>
     </row>
-    <row r="145" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A145" s="49" t="s">
-        <v>179</v>
+    <row r="145" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A145" s="45" t="s">
+        <v>178</v>
       </c>
       <c r="B145" s="21"/>
       <c r="C145" s="7"/>
@@ -5452,12 +5595,12 @@
       <c r="I145" s="7"/>
       <c r="J145" s="7"/>
       <c r="K145" s="7"/>
-      <c r="L145" s="10"/>
+      <c r="L145" s="55"/>
       <c r="M145" s="10"/>
     </row>
-    <row r="146" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A146" s="49" t="s">
-        <v>180</v>
+    <row r="146" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A146" s="45" t="s">
+        <v>179</v>
       </c>
       <c r="B146" s="21"/>
       <c r="C146" s="7"/>
@@ -5469,12 +5612,12 @@
       <c r="I146" s="7"/>
       <c r="J146" s="7"/>
       <c r="K146" s="7"/>
-      <c r="L146" s="10"/>
+      <c r="L146" s="55"/>
       <c r="M146" s="10"/>
     </row>
-    <row r="147" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A147" s="49" t="s">
-        <v>181</v>
+    <row r="147" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A147" s="45" t="s">
+        <v>180</v>
       </c>
       <c r="B147" s="21"/>
       <c r="C147" s="7"/>
@@ -5486,12 +5629,12 @@
       <c r="I147" s="7"/>
       <c r="J147" s="7"/>
       <c r="K147" s="7"/>
-      <c r="L147" s="10"/>
+      <c r="L147" s="55"/>
       <c r="M147" s="10"/>
     </row>
-    <row r="148" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A148" s="49" t="s">
-        <v>182</v>
+    <row r="148" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A148" s="45" t="s">
+        <v>181</v>
       </c>
       <c r="B148" s="21"/>
       <c r="C148" s="7"/>
@@ -5503,12 +5646,12 @@
       <c r="I148" s="7"/>
       <c r="J148" s="7"/>
       <c r="K148" s="7"/>
-      <c r="L148" s="10"/>
+      <c r="L148" s="55"/>
       <c r="M148" s="10"/>
     </row>
-    <row r="149" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A149" s="49" t="s">
-        <v>183</v>
+    <row r="149" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A149" s="45" t="s">
+        <v>182</v>
       </c>
       <c r="B149" s="21"/>
       <c r="C149" s="7"/>
@@ -5520,12 +5663,12 @@
       <c r="I149" s="7"/>
       <c r="J149" s="7"/>
       <c r="K149" s="7"/>
-      <c r="L149" s="10"/>
+      <c r="L149" s="55"/>
       <c r="M149" s="10"/>
     </row>
-    <row r="150" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A150" s="49" t="s">
-        <v>184</v>
+    <row r="150" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A150" s="45" t="s">
+        <v>183</v>
       </c>
       <c r="B150" s="21"/>
       <c r="C150" s="7"/>
@@ -5537,12 +5680,12 @@
       <c r="I150" s="7"/>
       <c r="J150" s="7"/>
       <c r="K150" s="7"/>
-      <c r="L150" s="10"/>
+      <c r="L150" s="55"/>
       <c r="M150" s="10"/>
     </row>
-    <row r="151" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A151" s="49" t="s">
-        <v>185</v>
+    <row r="151" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A151" s="45" t="s">
+        <v>184</v>
       </c>
       <c r="B151" s="21"/>
       <c r="C151" s="7"/>
@@ -5554,12 +5697,12 @@
       <c r="I151" s="7"/>
       <c r="J151" s="7"/>
       <c r="K151" s="7"/>
-      <c r="L151" s="10"/>
+      <c r="L151" s="55"/>
       <c r="M151" s="10"/>
     </row>
-    <row r="152" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A152" s="49" t="s">
-        <v>186</v>
+    <row r="152" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A152" s="45" t="s">
+        <v>185</v>
       </c>
       <c r="B152" s="21"/>
       <c r="C152" s="7"/>
@@ -5571,12 +5714,12 @@
       <c r="I152" s="7"/>
       <c r="J152" s="7"/>
       <c r="K152" s="7"/>
-      <c r="L152" s="10"/>
+      <c r="L152" s="55"/>
       <c r="M152" s="10"/>
     </row>
-    <row r="153" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A153" s="49" t="s">
-        <v>187</v>
+    <row r="153" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A153" s="45" t="s">
+        <v>186</v>
       </c>
       <c r="B153" s="21"/>
       <c r="C153" s="7"/>
@@ -5588,12 +5731,12 @@
       <c r="I153" s="7"/>
       <c r="J153" s="7"/>
       <c r="K153" s="7"/>
-      <c r="L153" s="10"/>
+      <c r="L153" s="55"/>
       <c r="M153" s="10"/>
     </row>
-    <row r="154" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A154" s="49" t="s">
-        <v>188</v>
+    <row r="154" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A154" s="45" t="s">
+        <v>187</v>
       </c>
       <c r="B154" s="21"/>
       <c r="C154" s="7"/>
@@ -5605,12 +5748,12 @@
       <c r="I154" s="7"/>
       <c r="J154" s="7"/>
       <c r="K154" s="7"/>
-      <c r="L154" s="10"/>
+      <c r="L154" s="55"/>
       <c r="M154" s="10"/>
     </row>
-    <row r="155" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A155" s="49" t="s">
-        <v>189</v>
+    <row r="155" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A155" s="45" t="s">
+        <v>188</v>
       </c>
       <c r="B155" s="21"/>
       <c r="C155" s="7"/>
@@ -5622,12 +5765,12 @@
       <c r="I155" s="7"/>
       <c r="J155" s="7"/>
       <c r="K155" s="7"/>
-      <c r="L155" s="10"/>
+      <c r="L155" s="55"/>
       <c r="M155" s="10"/>
     </row>
-    <row r="156" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A156" s="49" t="s">
-        <v>190</v>
+    <row r="156" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A156" s="45" t="s">
+        <v>189</v>
       </c>
       <c r="B156" s="21"/>
       <c r="C156" s="7"/>
@@ -5639,12 +5782,12 @@
       <c r="I156" s="7"/>
       <c r="J156" s="7"/>
       <c r="K156" s="7"/>
-      <c r="L156" s="10"/>
+      <c r="L156" s="55"/>
       <c r="M156" s="10"/>
     </row>
-    <row r="157" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A157" s="49" t="s">
-        <v>191</v>
+    <row r="157" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A157" s="45" t="s">
+        <v>190</v>
       </c>
       <c r="B157" s="21"/>
       <c r="C157" s="7"/>
@@ -5656,12 +5799,12 @@
       <c r="I157" s="7"/>
       <c r="J157" s="7"/>
       <c r="K157" s="7"/>
-      <c r="L157" s="10"/>
+      <c r="L157" s="55"/>
       <c r="M157" s="10"/>
     </row>
-    <row r="158" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A158" s="49" t="s">
-        <v>192</v>
+    <row r="158" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A158" s="45" t="s">
+        <v>191</v>
       </c>
       <c r="B158" s="21"/>
       <c r="C158" s="7"/>
@@ -5673,12 +5816,12 @@
       <c r="I158" s="7"/>
       <c r="J158" s="7"/>
       <c r="K158" s="7"/>
-      <c r="L158" s="10"/>
+      <c r="L158" s="55"/>
       <c r="M158" s="10"/>
     </row>
-    <row r="159" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A159" s="49" t="s">
-        <v>193</v>
+    <row r="159" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A159" s="45" t="s">
+        <v>192</v>
       </c>
       <c r="B159" s="21"/>
       <c r="C159" s="7"/>
@@ -5690,12 +5833,12 @@
       <c r="I159" s="7"/>
       <c r="J159" s="7"/>
       <c r="K159" s="7"/>
-      <c r="L159" s="10"/>
+      <c r="L159" s="55"/>
       <c r="M159" s="10"/>
     </row>
-    <row r="160" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A160" s="49" t="s">
-        <v>194</v>
+    <row r="160" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A160" s="45" t="s">
+        <v>193</v>
       </c>
       <c r="B160" s="21"/>
       <c r="C160" s="7"/>
@@ -5707,12 +5850,12 @@
       <c r="I160" s="7"/>
       <c r="J160" s="7"/>
       <c r="K160" s="7"/>
-      <c r="L160" s="10"/>
+      <c r="L160" s="55"/>
       <c r="M160" s="10"/>
     </row>
-    <row r="161" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A161" s="49" t="s">
-        <v>195</v>
+    <row r="161" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A161" s="45" t="s">
+        <v>194</v>
       </c>
       <c r="B161" s="21"/>
       <c r="C161" s="7"/>
@@ -5724,11 +5867,11 @@
       <c r="I161" s="7"/>
       <c r="J161" s="7"/>
       <c r="K161" s="7"/>
-      <c r="L161" s="10"/>
+      <c r="L161" s="55"/>
       <c r="M161" s="10"/>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G162" s="40"/>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G162" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5738,30 +5881,41 @@
     <mergeCell ref="B63:F70"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
-  <conditionalFormatting sqref="C1:J1 M1 L5:M5 C162:J65517">
-    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="C1:J1 M1 M5 C162:J65517">
+    <cfRule type="cellIs" dxfId="8" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F71:H161">
-    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" stopIfTrue="1" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Testing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="L5">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Critical"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F71:H161">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F71:H161" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"In Progress, Testing, Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
register and add user testcases are updated, RTM is updated, Review history is updated
</commit_message>
<xml_diff>
--- a/RTM/Traceability_Matrix learning hub ver 2.xlsx
+++ b/RTM/Traceability_Matrix learning hub ver 2.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad\Documents\GitHub\learning-hub\RTM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91035FC9-8CF5-472C-9236-2401478109CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" state="hidden" r:id="rId1"/>
@@ -20,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>eze3</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -44,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -63,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -82,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0">
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -101,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0">
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -120,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0">
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -139,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0">
+    <comment ref="K5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -158,13 +164,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="L5" authorId="0">
+    <comment ref="L5" authorId="0" shapeId="0" xr:uid="{7D60CAF8-4D99-4CE1-80A1-1548DC799F01}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="8"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">• Test Case Number: </t>
         </r>
@@ -172,6 +179,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> This column should be populated with the test case number linked to the functional requirement.</t>
         </r>
@@ -182,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="326">
   <si>
     <t>For detail regarding the practice of Requirements Management, please refer to the Requirements Management Practices Guide</t>
   </si>
@@ -413,10 +421,6 @@
   <si>
     <t>Software
 Module(s)</t>
-  </si>
-  <si>
-    <t>Test Case
-Number</t>
   </si>
   <si>
     <t>Additional
@@ -1342,15 +1346,73 @@
   <si>
     <t>Design Document (3.8.2 classDiagram_Delete User)</t>
   </si>
+  <si>
+    <t>Test Case
+ID</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_Register_002</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_Register_004</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_Register_005</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_Register_006</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_Register_007</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_Register_008</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_Register_009</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_Register_001</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_002</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_003</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_004</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_005</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_006</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_007</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_008</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_009</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_001</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_010</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1467,6 +1529,17 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1648,7 +1721,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1753,12 +1826,6 @@
     <xf numFmtId="49" fontId="10" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1768,14 +1835,8 @@
     <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1801,15 +1862,57 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2134,32 +2237,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B20"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="58.85546875" style="12" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="5.33203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" style="12" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="12"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="39"/>
-    </row>
-    <row r="5" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B4" s="51"/>
+    </row>
+    <row r="5" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
@@ -2167,7 +2270,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
@@ -2175,72 +2278,72 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B20" s="19" t="s">
         <v>19</v>
       </c>
@@ -2256,32 +2359,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F42" sqref="F33:F42"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="55.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="47.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="47.28515625" style="28" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="35.88671875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="55.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="47.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="47.33203125" style="28" customWidth="1"/>
     <col min="8" max="8" width="51" style="5" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="28.109375" style="57" customWidth="1"/>
     <col min="13" max="13" width="86" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="24"/>
@@ -2293,71 +2396,71 @@
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
-      <c r="K1" s="41" t="s">
+      <c r="K1" s="39" t="s">
         <v>20</v>
       </c>
       <c r="L1" s="24"/>
       <c r="M1" s="24"/>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="43" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
-      <c r="M2" s="44"/>
-    </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
+      <c r="M2" s="41"/>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="43" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
-      <c r="M3" s="44"/>
-    </row>
-    <row r="4" spans="1:13" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
+      <c r="M3" s="41"/>
+    </row>
+    <row r="4" spans="1:13" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="45" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
-      <c r="M4" s="46"/>
-    </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="M4" s="42"/>
+    </row>
+    <row r="5" spans="1:13" s="3" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="23" t="s">
@@ -2367,19 +2470,19 @@
         <v>29</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E5" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="F5" s="23" t="s">
-        <v>231</v>
-      </c>
       <c r="G5" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I5" s="23" t="s">
         <v>30</v>
@@ -2390,1663 +2493,1703 @@
       <c r="K5" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="48" t="s">
+      <c r="L5" s="44" t="s">
+        <v>307</v>
+      </c>
+      <c r="M5" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="48" t="s">
+    </row>
+    <row r="6" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="45" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="B6" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="C6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>37</v>
-      </c>
       <c r="D6" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E6" s="50" t="s">
-        <v>237</v>
-      </c>
-      <c r="F6" s="50" t="s">
         <v>232</v>
       </c>
+      <c r="E6" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F6" s="46" t="s">
+        <v>231</v>
+      </c>
       <c r="G6" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="H6" s="51" t="s">
-        <v>220</v>
+        <v>234</v>
+      </c>
+      <c r="H6" s="47" t="s">
+        <v>219</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
-      <c r="L6" s="10"/>
+      <c r="L6" s="55" t="s">
+        <v>308</v>
+      </c>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="49" t="s">
+    <row r="7" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A7" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>39</v>
-      </c>
       <c r="C7" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E7" s="50" t="s">
-        <v>237</v>
+        <v>232</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="H7" s="51" t="s">
-        <v>220</v>
+        <v>234</v>
+      </c>
+      <c r="H7" s="47" t="s">
+        <v>219</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
-      <c r="L7" s="10"/>
+      <c r="L7" s="55" t="s">
+        <v>308</v>
+      </c>
       <c r="M7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+    <row r="8" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A8" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>41</v>
-      </c>
       <c r="C8" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E8" s="50" t="s">
-        <v>237</v>
+        <v>232</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="H8" s="51" t="s">
-        <v>220</v>
+        <v>234</v>
+      </c>
+      <c r="H8" s="47" t="s">
+        <v>219</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="10"/>
+      <c r="L8" s="55" t="s">
+        <v>309</v>
+      </c>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
+    <row r="9" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A9" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="C9" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="D9" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E9" s="50" t="s">
-        <v>237</v>
+        <v>232</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="51" t="s">
-        <v>220</v>
+      <c r="H9" s="47" t="s">
+        <v>219</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
-      <c r="L9" s="10"/>
+      <c r="L9" s="55" t="s">
+        <v>310</v>
+      </c>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
+    <row r="10" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A10" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="C10" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="D10" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E10" s="50" t="s">
-        <v>237</v>
+        <v>232</v>
+      </c>
+      <c r="E10" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>236</v>
-      </c>
-      <c r="H10" s="51" t="s">
-        <v>220</v>
+        <v>235</v>
+      </c>
+      <c r="H10" s="47" t="s">
+        <v>219</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
-      <c r="L10" s="10"/>
+      <c r="L10" s="55" t="s">
+        <v>311</v>
+      </c>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+    <row r="11" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A11" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>49</v>
-      </c>
       <c r="C11" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E11" s="50" t="s">
-        <v>237</v>
+        <v>232</v>
+      </c>
+      <c r="E11" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>236</v>
-      </c>
-      <c r="H11" s="51" t="s">
-        <v>220</v>
+        <v>235</v>
+      </c>
+      <c r="H11" s="47" t="s">
+        <v>219</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
-      <c r="L11" s="10"/>
+      <c r="L11" s="55" t="s">
+        <v>312</v>
+      </c>
       <c r="M11" s="10"/>
     </row>
-    <row r="12" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
+    <row r="12" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A12" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>51</v>
-      </c>
       <c r="C12" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E12" s="50" t="s">
-        <v>237</v>
+        <v>232</v>
+      </c>
+      <c r="E12" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>236</v>
-      </c>
-      <c r="H12" s="51" t="s">
-        <v>220</v>
+        <v>235</v>
+      </c>
+      <c r="H12" s="47" t="s">
+        <v>219</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
-      <c r="L12" s="10"/>
+      <c r="L12" s="55" t="s">
+        <v>313</v>
+      </c>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="49" t="s">
+    <row r="13" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A13" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="20" t="s">
-        <v>53</v>
-      </c>
       <c r="C13" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E13" s="50" t="s">
+        <v>232</v>
+      </c>
+      <c r="E13" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="G13" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="G13" s="25" t="s">
-        <v>238</v>
-      </c>
-      <c r="H13" s="51" t="s">
-        <v>220</v>
+      <c r="H13" s="47" t="s">
+        <v>219</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
-      <c r="L13" s="10"/>
+      <c r="L13" s="55" t="s">
+        <v>314</v>
+      </c>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="49" t="s">
-        <v>229</v>
+    <row r="14" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="45" t="s">
+        <v>228</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E14" s="50" t="s">
-        <v>237</v>
+        <v>232</v>
+      </c>
+      <c r="E14" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="51" t="s">
-        <v>220</v>
+      <c r="H14" s="47" t="s">
+        <v>219</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="10"/>
+      <c r="L14" s="55" t="s">
+        <v>315</v>
+      </c>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="s">
+    <row r="15" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="C15" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="D15" s="30" t="s">
-        <v>240</v>
-      </c>
-      <c r="E15" s="50" t="s">
-        <v>237</v>
+        <v>239</v>
+      </c>
+      <c r="E15" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G15" s="31"/>
-      <c r="H15" s="51" t="s">
-        <v>221</v>
+      <c r="H15" s="47" t="s">
+        <v>220</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
-      <c r="L15" s="10"/>
+      <c r="L15" s="55"/>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="s">
-        <v>256</v>
+    <row r="16" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="45" t="s">
+        <v>255</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>240</v>
-      </c>
-      <c r="E16" s="50" t="s">
-        <v>237</v>
+        <v>239</v>
+      </c>
+      <c r="E16" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G16" s="22"/>
-      <c r="H16" s="51" t="s">
-        <v>221</v>
+      <c r="H16" s="47" t="s">
+        <v>220</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
-      <c r="L16" s="10"/>
+      <c r="L16" s="55"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="49" t="s">
+    <row r="17" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="21" t="s">
-        <v>59</v>
-      </c>
       <c r="C17" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>240</v>
-      </c>
-      <c r="E17" s="50" t="s">
-        <v>237</v>
+        <v>239</v>
+      </c>
+      <c r="E17" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F17" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G17" s="22"/>
-      <c r="H17" s="51" t="s">
-        <v>221</v>
+      <c r="H17" s="47" t="s">
+        <v>220</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
-      <c r="L17" s="10"/>
+      <c r="L17" s="55"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="s">
-        <v>60</v>
+    <row r="18" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A18" s="45" t="s">
+        <v>59</v>
       </c>
       <c r="B18" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="50" t="s">
-        <v>237</v>
+      <c r="E18" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="51" t="s">
-        <v>222</v>
+      <c r="H18" s="47" t="s">
+        <v>221</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
-      <c r="L18" s="10"/>
+      <c r="L18" s="55"/>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="49" t="s">
-        <v>257</v>
+    <row r="19" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A19" s="45" t="s">
+        <v>256</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D19" s="7"/>
-      <c r="E19" s="50" t="s">
-        <v>237</v>
+      <c r="E19" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
-      <c r="H19" s="51" t="s">
-        <v>222</v>
+      <c r="H19" s="47" t="s">
+        <v>221</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
-      <c r="L19" s="10"/>
+      <c r="L19" s="55"/>
       <c r="M19" s="10"/>
     </row>
-    <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="49" t="s">
-        <v>61</v>
+    <row r="20" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A20" s="45" t="s">
+        <v>60</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20" s="7"/>
-      <c r="E20" s="50" t="s">
-        <v>237</v>
+      <c r="E20" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
-      <c r="H20" s="51" t="s">
-        <v>222</v>
+      <c r="H20" s="47" t="s">
+        <v>221</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
-      <c r="L20" s="10"/>
+      <c r="L20" s="55"/>
       <c r="M20" s="10"/>
     </row>
-    <row r="21" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="s">
-        <v>64</v>
+    <row r="21" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A21" s="45" t="s">
+        <v>63</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D21" s="7"/>
-      <c r="E21" s="50" t="s">
-        <v>237</v>
+      <c r="E21" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="51" t="s">
-        <v>222</v>
+      <c r="H21" s="47" t="s">
+        <v>221</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
-      <c r="L21" s="10"/>
+      <c r="L21" s="55"/>
       <c r="M21" s="10"/>
     </row>
-    <row r="22" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="49" t="s">
-        <v>67</v>
+    <row r="22" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="45" t="s">
+        <v>66</v>
       </c>
       <c r="B22" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>73</v>
-      </c>
       <c r="D22" s="30" t="s">
+        <v>240</v>
+      </c>
+      <c r="E22" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F22" s="30" t="s">
         <v>241</v>
       </c>
-      <c r="E22" s="50" t="s">
-        <v>237</v>
-      </c>
-      <c r="F22" s="30" t="s">
+      <c r="G22" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G22" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H22" s="51" t="s">
-        <v>223</v>
+      <c r="H22" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
-      <c r="L22" s="10"/>
+      <c r="L22" s="55"/>
       <c r="M22" s="10"/>
     </row>
-    <row r="23" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="49" t="s">
-        <v>69</v>
+    <row r="23" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="45" t="s">
+        <v>68</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D23" s="30" t="s">
+        <v>240</v>
+      </c>
+      <c r="E23" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F23" s="30" t="s">
         <v>241</v>
       </c>
-      <c r="E23" s="50" t="s">
-        <v>237</v>
-      </c>
-      <c r="F23" s="30" t="s">
+      <c r="G23" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G23" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H23" s="51" t="s">
-        <v>223</v>
+      <c r="H23" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
-      <c r="L23" s="10"/>
+      <c r="L23" s="55"/>
       <c r="M23" s="10"/>
     </row>
-    <row r="24" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="49" t="s">
-        <v>258</v>
+    <row r="24" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A24" s="45" t="s">
+        <v>257</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="E24" s="50" t="s">
-        <v>237</v>
+        <v>252</v>
+      </c>
+      <c r="E24" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F24" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G24" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G24" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H24" s="51" t="s">
-        <v>223</v>
+      <c r="H24" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
-      <c r="L24" s="10"/>
+      <c r="L24" s="55"/>
       <c r="M24" s="10"/>
     </row>
-    <row r="25" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="49" t="s">
-        <v>71</v>
+    <row r="25" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A25" s="45" t="s">
+        <v>70</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="E25" s="50" t="s">
-        <v>237</v>
+        <v>252</v>
+      </c>
+      <c r="E25" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F25" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G25" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G25" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H25" s="51" t="s">
-        <v>223</v>
+      <c r="H25" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
-      <c r="L25" s="10"/>
+      <c r="L25" s="55"/>
       <c r="M25" s="10"/>
     </row>
-    <row r="26" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" s="49" t="s">
-        <v>74</v>
+    <row r="26" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A26" s="45" t="s">
+        <v>73</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="E26" s="50" t="s">
-        <v>237</v>
+        <v>252</v>
+      </c>
+      <c r="E26" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F26" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G26" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G26" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H26" s="51" t="s">
-        <v>223</v>
+      <c r="H26" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
-      <c r="L26" s="10"/>
+      <c r="L26" s="55"/>
       <c r="M26" s="10"/>
     </row>
-    <row r="27" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="49" t="s">
-        <v>76</v>
+    <row r="27" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A27" s="45" t="s">
+        <v>75</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="E27" s="50" t="s">
-        <v>237</v>
+        <v>252</v>
+      </c>
+      <c r="E27" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F27" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G27" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G27" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H27" s="51" t="s">
-        <v>223</v>
+      <c r="H27" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
-      <c r="L27" s="10"/>
+      <c r="L27" s="55"/>
       <c r="M27" s="10"/>
     </row>
-    <row r="28" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="49" t="s">
-        <v>78</v>
+    <row r="28" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A28" s="45" t="s">
+        <v>77</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="E28" s="50" t="s">
-        <v>237</v>
+        <v>252</v>
+      </c>
+      <c r="E28" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F28" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G28" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G28" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H28" s="51" t="s">
-        <v>223</v>
+      <c r="H28" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
-      <c r="L28" s="10"/>
+      <c r="L28" s="55"/>
       <c r="M28" s="10"/>
     </row>
-    <row r="29" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A29" s="49" t="s">
-        <v>80</v>
+    <row r="29" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A29" s="45" t="s">
+        <v>79</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="E29" s="50" t="s">
-        <v>237</v>
+        <v>252</v>
+      </c>
+      <c r="E29" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F29" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G29" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G29" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H29" s="51" t="s">
-        <v>223</v>
+      <c r="H29" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
-      <c r="L29" s="10"/>
+      <c r="L29" s="55"/>
       <c r="M29" s="10"/>
     </row>
-    <row r="30" spans="1:13" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="52" t="s">
-        <v>82</v>
+    <row r="30" spans="1:13" s="36" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A30" s="48" t="s">
+        <v>81</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D30" s="29"/>
       <c r="E30" s="30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F30" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G30" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G30" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H30" s="53" t="s">
-        <v>223</v>
+      <c r="H30" s="49" t="s">
+        <v>222</v>
       </c>
       <c r="I30" s="29"/>
       <c r="J30" s="29"/>
       <c r="K30" s="29"/>
-      <c r="L30" s="35"/>
+      <c r="L30" s="56"/>
       <c r="M30" s="35"/>
     </row>
-    <row r="31" spans="1:13" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="52" t="s">
-        <v>84</v>
+    <row r="31" spans="1:13" s="36" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A31" s="48" t="s">
+        <v>83</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D31" s="29"/>
       <c r="E31" s="30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F31" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G31" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G31" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H31" s="53"/>
+      <c r="H31" s="49"/>
       <c r="I31" s="29"/>
       <c r="J31" s="29"/>
       <c r="K31" s="29"/>
-      <c r="L31" s="35"/>
+      <c r="L31" s="56"/>
       <c r="M31" s="35"/>
     </row>
-    <row r="32" spans="1:13" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A32" s="52" t="s">
-        <v>86</v>
+    <row r="32" spans="1:13" s="36" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A32" s="48" t="s">
+        <v>85</v>
       </c>
       <c r="B32" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="C32" s="37" t="s">
         <v>245</v>
-      </c>
-      <c r="C32" s="37" t="s">
-        <v>246</v>
       </c>
       <c r="D32" s="29"/>
       <c r="E32" s="30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F32" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G32" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="G32" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="H32" s="53"/>
+      <c r="H32" s="49"/>
       <c r="I32" s="29"/>
       <c r="J32" s="29"/>
       <c r="K32" s="29"/>
-      <c r="L32" s="35"/>
+      <c r="L32" s="56"/>
       <c r="M32" s="35"/>
     </row>
-    <row r="33" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="49" t="s">
-        <v>88</v>
+    <row r="33" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="45" t="s">
+        <v>87</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="E33" s="50" t="s">
-        <v>237</v>
+        <v>251</v>
+      </c>
+      <c r="E33" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F33" s="22"/>
       <c r="G33" s="30"/>
-      <c r="H33" s="51" t="s">
-        <v>223</v>
+      <c r="H33" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
-      <c r="L33" s="10"/>
+      <c r="L33" s="55"/>
       <c r="M33" s="10"/>
     </row>
-    <row r="34" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="49" t="s">
-        <v>259</v>
+    <row r="34" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="45" t="s">
+        <v>258</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="E34" s="50" t="s">
-        <v>237</v>
+        <v>251</v>
+      </c>
+      <c r="E34" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="30"/>
-      <c r="H34" s="51" t="s">
-        <v>223</v>
+      <c r="H34" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
-      <c r="L34" s="10"/>
+      <c r="L34" s="55"/>
       <c r="M34" s="10"/>
     </row>
-    <row r="35" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="49" t="s">
-        <v>260</v>
+    <row r="35" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="45" t="s">
+        <v>259</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="E35" s="50" t="s">
-        <v>237</v>
+        <v>251</v>
+      </c>
+      <c r="E35" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="30"/>
-      <c r="H35" s="51" t="s">
-        <v>223</v>
+      <c r="H35" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
-      <c r="L35" s="10"/>
+      <c r="L35" s="55"/>
       <c r="M35" s="10"/>
     </row>
-    <row r="36" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="49" t="s">
-        <v>261</v>
+    <row r="36" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="45" t="s">
+        <v>260</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="E36" s="50" t="s">
-        <v>237</v>
+        <v>251</v>
+      </c>
+      <c r="E36" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F36" s="22"/>
       <c r="G36" s="30"/>
-      <c r="H36" s="51" t="s">
-        <v>223</v>
+      <c r="H36" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
-      <c r="L36" s="10"/>
+      <c r="L36" s="55"/>
       <c r="M36" s="10"/>
     </row>
-    <row r="37" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="49" t="s">
-        <v>262</v>
+    <row r="37" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="45" t="s">
+        <v>261</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="E37" s="50" t="s">
-        <v>237</v>
+        <v>251</v>
+      </c>
+      <c r="E37" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F37" s="22"/>
       <c r="G37" s="30"/>
-      <c r="H37" s="51" t="s">
-        <v>223</v>
+      <c r="H37" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="10"/>
+      <c r="L37" s="55"/>
       <c r="M37" s="10"/>
     </row>
-    <row r="38" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="49" t="s">
-        <v>263</v>
+    <row r="38" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="45" t="s">
+        <v>262</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="E38" s="50" t="s">
-        <v>237</v>
+        <v>251</v>
+      </c>
+      <c r="E38" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F38" s="22"/>
       <c r="G38" s="30"/>
-      <c r="H38" s="51" t="s">
-        <v>223</v>
+      <c r="H38" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
-      <c r="L38" s="10"/>
+      <c r="L38" s="55"/>
       <c r="M38" s="10"/>
     </row>
-    <row r="39" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="49" t="s">
-        <v>264</v>
+    <row r="39" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="45" t="s">
+        <v>263</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="E39" s="50" t="s">
-        <v>237</v>
+        <v>251</v>
+      </c>
+      <c r="E39" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F39" s="22"/>
       <c r="G39" s="30"/>
-      <c r="H39" s="51" t="s">
-        <v>223</v>
+      <c r="H39" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
-      <c r="L39" s="10"/>
+      <c r="L39" s="55"/>
       <c r="M39" s="10"/>
     </row>
-    <row r="40" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="49" t="s">
-        <v>265</v>
+    <row r="40" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="45" t="s">
+        <v>264</v>
       </c>
       <c r="B40" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="C40" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="C40" s="32" t="s">
-        <v>210</v>
-      </c>
       <c r="D40" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="E40" s="50" t="s">
-        <v>237</v>
+        <v>251</v>
+      </c>
+      <c r="E40" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F40" s="22"/>
       <c r="G40" s="30"/>
-      <c r="H40" s="51" t="s">
-        <v>223</v>
+      <c r="H40" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
-      <c r="L40" s="10"/>
+      <c r="L40" s="55"/>
       <c r="M40" s="10"/>
     </row>
-    <row r="41" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A41" s="49" t="s">
-        <v>266</v>
+    <row r="41" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A41" s="45" t="s">
+        <v>265</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D41" s="30" t="s">
-        <v>247</v>
-      </c>
-      <c r="E41" s="50" t="s">
-        <v>237</v>
+        <v>246</v>
+      </c>
+      <c r="E41" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F41" s="30"/>
       <c r="G41" s="30"/>
-      <c r="H41" s="51" t="s">
-        <v>224</v>
+      <c r="H41" s="47" t="s">
+        <v>223</v>
       </c>
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
-      <c r="L41" s="10"/>
+      <c r="L41" s="55"/>
       <c r="M41" s="10"/>
     </row>
-    <row r="42" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A42" s="49" t="s">
-        <v>267</v>
+    <row r="42" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A42" s="45" t="s">
+        <v>266</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D42" s="30" t="s">
-        <v>247</v>
-      </c>
-      <c r="E42" s="50" t="s">
-        <v>237</v>
+        <v>246</v>
+      </c>
+      <c r="E42" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F42" s="30"/>
       <c r="G42" s="30"/>
-      <c r="H42" s="51" t="s">
-        <v>224</v>
+      <c r="H42" s="47" t="s">
+        <v>223</v>
       </c>
       <c r="I42" s="7"/>
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
-      <c r="L42" s="10"/>
+      <c r="L42" s="55"/>
       <c r="M42" s="10"/>
     </row>
-    <row r="43" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A43" s="49" t="s">
-        <v>268</v>
+    <row r="43" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A43" s="45" t="s">
+        <v>267</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D43" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E43" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E43" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F43" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G43" s="30"/>
-      <c r="H43" s="51" t="s">
-        <v>225</v>
+      <c r="H43" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
-      <c r="L43" s="10"/>
+      <c r="L43" s="55" t="s">
+        <v>316</v>
+      </c>
       <c r="M43" s="10"/>
     </row>
-    <row r="44" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A44" s="49" t="s">
-        <v>269</v>
+    <row r="44" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A44" s="45" t="s">
+        <v>268</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D44" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E44" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E44" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F44" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G44" s="30"/>
-      <c r="H44" s="51" t="s">
-        <v>225</v>
+      <c r="H44" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I44" s="7"/>
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
-      <c r="L44" s="10"/>
+      <c r="L44" s="55" t="s">
+        <v>317</v>
+      </c>
       <c r="M44" s="10"/>
     </row>
-    <row r="45" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A45" s="49" t="s">
-        <v>270</v>
+    <row r="45" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A45" s="45" t="s">
+        <v>269</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D45" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E45" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E45" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F45" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G45" s="22"/>
-      <c r="H45" s="51" t="s">
-        <v>225</v>
+      <c r="H45" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
-      <c r="L45" s="10"/>
+      <c r="L45" s="55" t="s">
+        <v>318</v>
+      </c>
       <c r="M45" s="10"/>
     </row>
-    <row r="46" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A46" s="49" t="s">
-        <v>271</v>
+    <row r="46" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A46" s="45" t="s">
+        <v>270</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D46" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E46" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E46" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F46" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G46" s="22"/>
-      <c r="H46" s="51" t="s">
-        <v>225</v>
+      <c r="H46" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I46" s="7"/>
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
-      <c r="L46" s="10"/>
+      <c r="L46" s="55" t="s">
+        <v>319</v>
+      </c>
       <c r="M46" s="10"/>
     </row>
-    <row r="47" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A47" s="49" t="s">
-        <v>272</v>
+    <row r="47" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A47" s="45" t="s">
+        <v>271</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D47" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E47" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E47" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F47" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G47" s="22"/>
-      <c r="H47" s="51" t="s">
-        <v>225</v>
+      <c r="H47" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
-      <c r="L47" s="10"/>
+      <c r="L47" s="55" t="s">
+        <v>320</v>
+      </c>
       <c r="M47" s="10"/>
     </row>
-    <row r="48" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A48" s="49" t="s">
-        <v>92</v>
+    <row r="48" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A48" s="45" t="s">
+        <v>91</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D48" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E48" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E48" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F48" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G48" s="22"/>
-      <c r="H48" s="51" t="s">
-        <v>225</v>
+      <c r="H48" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I48" s="7"/>
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
-      <c r="L48" s="10"/>
+      <c r="L48" s="55" t="s">
+        <v>321</v>
+      </c>
       <c r="M48" s="10"/>
     </row>
-    <row r="49" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A49" s="49" t="s">
-        <v>94</v>
+    <row r="49" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A49" s="45" t="s">
+        <v>93</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D49" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E49" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E49" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F49" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G49" s="22"/>
-      <c r="H49" s="51" t="s">
-        <v>225</v>
+      <c r="H49" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
-      <c r="L49" s="10"/>
+      <c r="L49" s="55" t="s">
+        <v>322</v>
+      </c>
       <c r="M49" s="10"/>
     </row>
-    <row r="50" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A50" s="49" t="s">
-        <v>96</v>
+    <row r="50" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A50" s="45" t="s">
+        <v>95</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D50" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E50" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E50" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F50" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G50" s="22"/>
-      <c r="H50" s="51" t="s">
-        <v>225</v>
+      <c r="H50" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
-      <c r="L50" s="10"/>
+      <c r="L50" s="55" t="s">
+        <v>323</v>
+      </c>
       <c r="M50" s="10"/>
     </row>
-    <row r="51" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A51" s="49" t="s">
-        <v>98</v>
+    <row r="51" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A51" s="45" t="s">
+        <v>97</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E51" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E51" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F51" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G51" s="22"/>
-      <c r="H51" s="51" t="s">
-        <v>225</v>
+      <c r="H51" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
       <c r="K51" s="7"/>
-      <c r="L51" s="10"/>
+      <c r="L51" s="55" t="s">
+        <v>324</v>
+      </c>
       <c r="M51" s="10"/>
     </row>
-    <row r="52" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A52" s="49" t="s">
-        <v>100</v>
+    <row r="52" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A52" s="45" t="s">
+        <v>99</v>
       </c>
       <c r="B52" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>212</v>
-      </c>
       <c r="D52" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E52" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E52" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F52" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G52" s="22"/>
-      <c r="H52" s="51" t="s">
-        <v>225</v>
+      <c r="H52" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I52" s="7"/>
       <c r="J52" s="7"/>
       <c r="K52" s="7"/>
-      <c r="L52" s="10"/>
+      <c r="L52" s="55" t="s">
+        <v>325</v>
+      </c>
       <c r="M52" s="10"/>
     </row>
-    <row r="53" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A53" s="49" t="s">
-        <v>102</v>
+    <row r="53" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A53" s="45" t="s">
+        <v>101</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D53" s="30" t="s">
-        <v>254</v>
-      </c>
-      <c r="E53" s="50" t="s">
-        <v>237</v>
+        <v>253</v>
+      </c>
+      <c r="E53" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F53" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G53" s="22"/>
-      <c r="H53" s="51" t="s">
-        <v>225</v>
+      <c r="H53" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
       <c r="K53" s="7"/>
-      <c r="L53" s="10"/>
+      <c r="L53" s="55" t="s">
+        <v>324</v>
+      </c>
       <c r="M53" s="10"/>
     </row>
-    <row r="54" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A54" s="49" t="s">
-        <v>104</v>
+    <row r="54" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A54" s="45" t="s">
+        <v>103</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D54" s="30" t="s">
-        <v>255</v>
-      </c>
-      <c r="E54" s="50" t="s">
-        <v>237</v>
+        <v>254</v>
+      </c>
+      <c r="E54" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F54" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G54" s="22"/>
-      <c r="H54" s="51" t="s">
-        <v>226</v>
+      <c r="H54" s="47" t="s">
+        <v>225</v>
       </c>
       <c r="I54" s="7"/>
       <c r="J54" s="7"/>
       <c r="K54" s="7"/>
-      <c r="L54" s="10"/>
+      <c r="L54" s="55"/>
       <c r="M54" s="10"/>
     </row>
-    <row r="55" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A55" s="49" t="s">
-        <v>273</v>
+    <row r="55" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A55" s="45" t="s">
+        <v>272</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D55" s="30" t="s">
-        <v>255</v>
-      </c>
-      <c r="E55" s="50" t="s">
-        <v>237</v>
+        <v>254</v>
+      </c>
+      <c r="E55" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F55" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G55" s="22"/>
-      <c r="H55" s="51" t="s">
-        <v>226</v>
+      <c r="H55" s="47" t="s">
+        <v>225</v>
       </c>
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
       <c r="K55" s="7"/>
-      <c r="L55" s="10"/>
+      <c r="L55" s="55"/>
       <c r="M55" s="10"/>
     </row>
-    <row r="56" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="49" t="s">
-        <v>274</v>
+    <row r="56" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A56" s="45" t="s">
+        <v>273</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D56" s="30" t="s">
-        <v>255</v>
-      </c>
-      <c r="E56" s="50" t="s">
-        <v>237</v>
+        <v>254</v>
+      </c>
+      <c r="E56" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F56" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G56" s="22"/>
-      <c r="H56" s="51" t="s">
-        <v>226</v>
+      <c r="H56" s="47" t="s">
+        <v>225</v>
       </c>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
-      <c r="L56" s="10"/>
+      <c r="L56" s="55"/>
       <c r="M56" s="10"/>
     </row>
-    <row r="57" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A57" s="49" t="s">
-        <v>275</v>
+    <row r="57" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A57" s="45" t="s">
+        <v>274</v>
       </c>
       <c r="B57" s="21" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D57" s="30" t="s">
-        <v>255</v>
-      </c>
-      <c r="E57" s="50" t="s">
-        <v>237</v>
+        <v>254</v>
+      </c>
+      <c r="E57" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F57" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G57" s="22"/>
-      <c r="H57" s="51" t="s">
-        <v>226</v>
+      <c r="H57" s="47" t="s">
+        <v>225</v>
       </c>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
       <c r="K57" s="7"/>
-      <c r="L57" s="10"/>
+      <c r="L57" s="55"/>
       <c r="M57" s="10"/>
     </row>
-    <row r="58" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="49" t="s">
-        <v>276</v>
+    <row r="58" spans="1:13" ht="27" x14ac:dyDescent="0.3">
+      <c r="A58" s="45" t="s">
+        <v>275</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D58" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="E58" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F58" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="E58" s="50" t="s">
-        <v>237</v>
-      </c>
-      <c r="F58" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="G58" s="30" t="s">
-        <v>251</v>
-      </c>
-      <c r="H58" s="51" t="s">
-        <v>227</v>
+        <v>250</v>
+      </c>
+      <c r="H58" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
-      <c r="L58" s="10"/>
+      <c r="L58" s="55"/>
       <c r="M58" s="10"/>
     </row>
-    <row r="59" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="49" t="s">
-        <v>277</v>
+    <row r="59" spans="1:13" ht="27" x14ac:dyDescent="0.3">
+      <c r="A59" s="45" t="s">
+        <v>276</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D59" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="E59" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F59" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="E59" s="50" t="s">
-        <v>237</v>
-      </c>
-      <c r="F59" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="G59" s="30" t="s">
-        <v>251</v>
-      </c>
-      <c r="H59" s="51" t="s">
-        <v>227</v>
+        <v>250</v>
+      </c>
+      <c r="H59" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
-      <c r="L59" s="10"/>
+      <c r="L59" s="55"/>
       <c r="M59" s="10"/>
     </row>
-    <row r="60" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A60" s="49" t="s">
-        <v>279</v>
+    <row r="60" spans="1:13" ht="27" x14ac:dyDescent="0.3">
+      <c r="A60" s="45" t="s">
+        <v>278</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D60" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="E60" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F60" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="E60" s="50" t="s">
-        <v>237</v>
-      </c>
-      <c r="F60" s="30" t="s">
-        <v>249</v>
-      </c>
       <c r="G60" s="30" t="s">
-        <v>251</v>
-      </c>
-      <c r="H60" s="51" t="s">
-        <v>227</v>
+        <v>250</v>
+      </c>
+      <c r="H60" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
-      <c r="L60" s="10"/>
+      <c r="L60" s="55"/>
       <c r="M60" s="10"/>
     </row>
-    <row r="61" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A61" s="49" t="s">
-        <v>280</v>
+    <row r="61" spans="1:13" ht="27" x14ac:dyDescent="0.3">
+      <c r="A61" s="45" t="s">
+        <v>279</v>
       </c>
       <c r="B61" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D61" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="E61" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F61" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="G61" s="30" t="s">
         <v>250</v>
       </c>
-      <c r="E61" s="50" t="s">
-        <v>237</v>
-      </c>
-      <c r="F61" s="30" t="s">
-        <v>249</v>
-      </c>
-      <c r="G61" s="30" t="s">
-        <v>251</v>
-      </c>
-      <c r="H61" s="51" t="s">
-        <v>227</v>
+      <c r="H61" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
-      <c r="L61" s="10"/>
+      <c r="L61" s="55"/>
       <c r="M61" s="10"/>
     </row>
-    <row r="62" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A62" s="49" t="s">
-        <v>281</v>
+    <row r="62" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A62" s="45" t="s">
+        <v>280</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D62" s="7"/>
-      <c r="E62" s="50" t="s">
-        <v>237</v>
+      <c r="E62" s="46" t="s">
+        <v>236</v>
       </c>
       <c r="F62" s="22"/>
       <c r="G62" s="22"/>
-      <c r="H62" s="51" t="s">
-        <v>222</v>
+      <c r="H62" s="47" t="s">
+        <v>221</v>
       </c>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
-      <c r="L62" s="10"/>
+      <c r="L62" s="55"/>
       <c r="M62" s="10"/>
     </row>
-    <row r="63" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="49" t="s">
-        <v>282</v>
+    <row r="63" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="45" t="s">
+        <v>281</v>
       </c>
       <c r="B63" s="54"/>
       <c r="C63" s="54"/>
@@ -4058,12 +4201,12 @@
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
-      <c r="L63" s="10"/>
+      <c r="L63" s="55"/>
       <c r="M63" s="10"/>
     </row>
-    <row r="64" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A64" s="49" t="s">
-        <v>283</v>
+    <row r="64" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A64" s="45" t="s">
+        <v>282</v>
       </c>
       <c r="B64" s="54"/>
       <c r="C64" s="54"/>
@@ -4075,12 +4218,12 @@
       <c r="I64" s="7"/>
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
-      <c r="L64" s="10"/>
+      <c r="L64" s="55"/>
       <c r="M64" s="10"/>
     </row>
-    <row r="65" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A65" s="49" t="s">
-        <v>283</v>
+    <row r="65" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A65" s="45" t="s">
+        <v>282</v>
       </c>
       <c r="B65" s="54"/>
       <c r="C65" s="54"/>
@@ -4092,12 +4235,12 @@
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
-      <c r="L65" s="10"/>
+      <c r="L65" s="55"/>
       <c r="M65" s="10"/>
     </row>
-    <row r="66" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A66" s="49" t="s">
-        <v>284</v>
+    <row r="66" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A66" s="45" t="s">
+        <v>283</v>
       </c>
       <c r="B66" s="54"/>
       <c r="C66" s="54"/>
@@ -4109,12 +4252,12 @@
       <c r="I66" s="7"/>
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
-      <c r="L66" s="10"/>
+      <c r="L66" s="55"/>
       <c r="M66" s="10"/>
     </row>
-    <row r="67" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A67" s="49" t="s">
-        <v>285</v>
+    <row r="67" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A67" s="45" t="s">
+        <v>284</v>
       </c>
       <c r="B67" s="54"/>
       <c r="C67" s="54"/>
@@ -4126,12 +4269,12 @@
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
-      <c r="L67" s="10"/>
+      <c r="L67" s="55"/>
       <c r="M67" s="10"/>
     </row>
-    <row r="68" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A68" s="49" t="s">
-        <v>286</v>
+    <row r="68" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A68" s="45" t="s">
+        <v>285</v>
       </c>
       <c r="B68" s="54"/>
       <c r="C68" s="54"/>
@@ -4143,12 +4286,12 @@
       <c r="I68" s="7"/>
       <c r="J68" s="7"/>
       <c r="K68" s="7"/>
-      <c r="L68" s="10"/>
+      <c r="L68" s="55"/>
       <c r="M68" s="10"/>
     </row>
-    <row r="69" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A69" s="49" t="s">
-        <v>286</v>
+    <row r="69" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A69" s="45" t="s">
+        <v>285</v>
       </c>
       <c r="B69" s="54"/>
       <c r="C69" s="54"/>
@@ -4160,12 +4303,12 @@
       <c r="I69" s="7"/>
       <c r="J69" s="7"/>
       <c r="K69" s="7"/>
-      <c r="L69" s="10"/>
+      <c r="L69" s="55"/>
       <c r="M69" s="10"/>
     </row>
-    <row r="70" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A70" s="49" t="s">
-        <v>287</v>
+    <row r="70" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A70" s="45" t="s">
+        <v>286</v>
       </c>
       <c r="B70" s="54"/>
       <c r="C70" s="54"/>
@@ -4177,12 +4320,12 @@
       <c r="I70" s="7"/>
       <c r="J70" s="7"/>
       <c r="K70" s="7"/>
-      <c r="L70" s="10"/>
+      <c r="L70" s="55"/>
       <c r="M70" s="10"/>
     </row>
-    <row r="71" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A71" s="49" t="s">
-        <v>288</v>
+    <row r="71" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A71" s="45" t="s">
+        <v>287</v>
       </c>
       <c r="B71" s="21"/>
       <c r="C71" s="7"/>
@@ -4194,12 +4337,12 @@
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
       <c r="K71" s="7"/>
-      <c r="L71" s="10"/>
+      <c r="L71" s="55"/>
       <c r="M71" s="10"/>
     </row>
-    <row r="72" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A72" s="49" t="s">
-        <v>289</v>
+    <row r="72" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A72" s="45" t="s">
+        <v>288</v>
       </c>
       <c r="B72" s="21"/>
       <c r="C72" s="7"/>
@@ -4211,12 +4354,12 @@
       <c r="I72" s="7"/>
       <c r="J72" s="7"/>
       <c r="K72" s="7"/>
-      <c r="L72" s="10"/>
+      <c r="L72" s="55"/>
       <c r="M72" s="10"/>
     </row>
-    <row r="73" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A73" s="49" t="s">
-        <v>290</v>
+    <row r="73" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A73" s="45" t="s">
+        <v>289</v>
       </c>
       <c r="B73" s="21"/>
       <c r="C73" s="7"/>
@@ -4228,12 +4371,12 @@
       <c r="I73" s="7"/>
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
-      <c r="L73" s="10"/>
+      <c r="L73" s="55"/>
       <c r="M73" s="10"/>
     </row>
-    <row r="74" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A74" s="49" t="s">
-        <v>291</v>
+    <row r="74" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A74" s="45" t="s">
+        <v>290</v>
       </c>
       <c r="B74" s="21"/>
       <c r="C74" s="7"/>
@@ -4245,12 +4388,12 @@
       <c r="I74" s="7"/>
       <c r="J74" s="7"/>
       <c r="K74" s="7"/>
-      <c r="L74" s="10"/>
+      <c r="L74" s="55"/>
       <c r="M74" s="10"/>
     </row>
-    <row r="75" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A75" s="49" t="s">
-        <v>292</v>
+    <row r="75" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A75" s="45" t="s">
+        <v>291</v>
       </c>
       <c r="B75" s="21"/>
       <c r="C75" s="7"/>
@@ -4262,12 +4405,12 @@
       <c r="I75" s="7"/>
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
-      <c r="L75" s="10"/>
+      <c r="L75" s="55"/>
       <c r="M75" s="10"/>
     </row>
-    <row r="76" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A76" s="49" t="s">
-        <v>293</v>
+    <row r="76" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A76" s="45" t="s">
+        <v>292</v>
       </c>
       <c r="B76" s="21"/>
       <c r="C76" s="7"/>
@@ -4279,12 +4422,12 @@
       <c r="I76" s="7"/>
       <c r="J76" s="7"/>
       <c r="K76" s="7"/>
-      <c r="L76" s="10"/>
+      <c r="L76" s="55"/>
       <c r="M76" s="10"/>
     </row>
-    <row r="77" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A77" s="49" t="s">
-        <v>294</v>
+    <row r="77" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A77" s="45" t="s">
+        <v>293</v>
       </c>
       <c r="B77" s="21"/>
       <c r="C77" s="7"/>
@@ -4296,12 +4439,12 @@
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
-      <c r="L77" s="10"/>
+      <c r="L77" s="55"/>
       <c r="M77" s="10"/>
     </row>
-    <row r="78" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A78" s="49" t="s">
-        <v>295</v>
+    <row r="78" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A78" s="45" t="s">
+        <v>294</v>
       </c>
       <c r="B78" s="21"/>
       <c r="C78" s="7"/>
@@ -4313,12 +4456,12 @@
       <c r="I78" s="7"/>
       <c r="J78" s="7"/>
       <c r="K78" s="7"/>
-      <c r="L78" s="10"/>
+      <c r="L78" s="55"/>
       <c r="M78" s="10"/>
     </row>
-    <row r="79" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A79" s="49" t="s">
-        <v>296</v>
+    <row r="79" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A79" s="45" t="s">
+        <v>295</v>
       </c>
       <c r="B79" s="21"/>
       <c r="C79" s="7"/>
@@ -4330,12 +4473,12 @@
       <c r="I79" s="7"/>
       <c r="J79" s="7"/>
       <c r="K79" s="7"/>
-      <c r="L79" s="10"/>
+      <c r="L79" s="55"/>
       <c r="M79" s="10"/>
     </row>
-    <row r="80" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A80" s="49" t="s">
-        <v>297</v>
+    <row r="80" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A80" s="45" t="s">
+        <v>296</v>
       </c>
       <c r="B80" s="21"/>
       <c r="C80" s="7"/>
@@ -4347,12 +4490,12 @@
       <c r="I80" s="7"/>
       <c r="J80" s="7"/>
       <c r="K80" s="7"/>
-      <c r="L80" s="10"/>
+      <c r="L80" s="55"/>
       <c r="M80" s="10"/>
     </row>
-    <row r="81" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A81" s="49" t="s">
-        <v>298</v>
+    <row r="81" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A81" s="45" t="s">
+        <v>297</v>
       </c>
       <c r="B81" s="21"/>
       <c r="C81" s="7"/>
@@ -4364,12 +4507,12 @@
       <c r="I81" s="7"/>
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
-      <c r="L81" s="10"/>
+      <c r="L81" s="55"/>
       <c r="M81" s="10"/>
     </row>
-    <row r="82" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A82" s="49" t="s">
-        <v>299</v>
+    <row r="82" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A82" s="45" t="s">
+        <v>298</v>
       </c>
       <c r="B82" s="21"/>
       <c r="C82" s="7"/>
@@ -4381,12 +4524,12 @@
       <c r="I82" s="7"/>
       <c r="J82" s="7"/>
       <c r="K82" s="7"/>
-      <c r="L82" s="10"/>
+      <c r="L82" s="55"/>
       <c r="M82" s="10"/>
     </row>
-    <row r="83" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A83" s="49" t="s">
-        <v>300</v>
+    <row r="83" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A83" s="45" t="s">
+        <v>299</v>
       </c>
       <c r="B83" s="21"/>
       <c r="C83" s="7"/>
@@ -4398,12 +4541,12 @@
       <c r="I83" s="7"/>
       <c r="J83" s="7"/>
       <c r="K83" s="7"/>
-      <c r="L83" s="10"/>
+      <c r="L83" s="55"/>
       <c r="M83" s="10"/>
     </row>
-    <row r="84" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A84" s="49" t="s">
-        <v>301</v>
+    <row r="84" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A84" s="45" t="s">
+        <v>300</v>
       </c>
       <c r="B84" s="21"/>
       <c r="C84" s="7"/>
@@ -4415,12 +4558,12 @@
       <c r="I84" s="7"/>
       <c r="J84" s="7"/>
       <c r="K84" s="7"/>
-      <c r="L84" s="10"/>
+      <c r="L84" s="55"/>
       <c r="M84" s="10"/>
     </row>
-    <row r="85" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A85" s="49" t="s">
-        <v>302</v>
+    <row r="85" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A85" s="45" t="s">
+        <v>301</v>
       </c>
       <c r="B85" s="21"/>
       <c r="C85" s="7"/>
@@ -4432,12 +4575,12 @@
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
       <c r="K85" s="7"/>
-      <c r="L85" s="10"/>
+      <c r="L85" s="55"/>
       <c r="M85" s="10"/>
     </row>
-    <row r="86" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A86" s="49" t="s">
-        <v>120</v>
+    <row r="86" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A86" s="45" t="s">
+        <v>119</v>
       </c>
       <c r="B86" s="21"/>
       <c r="C86" s="7"/>
@@ -4449,12 +4592,12 @@
       <c r="I86" s="7"/>
       <c r="J86" s="7"/>
       <c r="K86" s="7"/>
-      <c r="L86" s="10"/>
+      <c r="L86" s="55"/>
       <c r="M86" s="10"/>
     </row>
-    <row r="87" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A87" s="49" t="s">
-        <v>121</v>
+    <row r="87" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A87" s="45" t="s">
+        <v>120</v>
       </c>
       <c r="B87" s="21"/>
       <c r="C87" s="7"/>
@@ -4466,12 +4609,12 @@
       <c r="I87" s="7"/>
       <c r="J87" s="7"/>
       <c r="K87" s="7"/>
-      <c r="L87" s="10"/>
+      <c r="L87" s="55"/>
       <c r="M87" s="10"/>
     </row>
-    <row r="88" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A88" s="49" t="s">
-        <v>122</v>
+    <row r="88" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A88" s="45" t="s">
+        <v>121</v>
       </c>
       <c r="B88" s="21"/>
       <c r="C88" s="7"/>
@@ -4483,12 +4626,12 @@
       <c r="I88" s="7"/>
       <c r="J88" s="7"/>
       <c r="K88" s="7"/>
-      <c r="L88" s="10"/>
+      <c r="L88" s="55"/>
       <c r="M88" s="10"/>
     </row>
-    <row r="89" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A89" s="49" t="s">
-        <v>123</v>
+    <row r="89" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A89" s="45" t="s">
+        <v>122</v>
       </c>
       <c r="B89" s="21"/>
       <c r="C89" s="7"/>
@@ -4500,12 +4643,12 @@
       <c r="I89" s="7"/>
       <c r="J89" s="7"/>
       <c r="K89" s="7"/>
-      <c r="L89" s="10"/>
+      <c r="L89" s="55"/>
       <c r="M89" s="10"/>
     </row>
-    <row r="90" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A90" s="49" t="s">
-        <v>124</v>
+    <row r="90" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A90" s="45" t="s">
+        <v>123</v>
       </c>
       <c r="B90" s="21"/>
       <c r="C90" s="7"/>
@@ -4517,12 +4660,12 @@
       <c r="I90" s="7"/>
       <c r="J90" s="7"/>
       <c r="K90" s="7"/>
-      <c r="L90" s="10"/>
+      <c r="L90" s="55"/>
       <c r="M90" s="10"/>
     </row>
-    <row r="91" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A91" s="49" t="s">
-        <v>125</v>
+    <row r="91" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A91" s="45" t="s">
+        <v>124</v>
       </c>
       <c r="B91" s="21"/>
       <c r="C91" s="7"/>
@@ -4534,12 +4677,12 @@
       <c r="I91" s="7"/>
       <c r="J91" s="7"/>
       <c r="K91" s="7"/>
-      <c r="L91" s="10"/>
+      <c r="L91" s="55"/>
       <c r="M91" s="10"/>
     </row>
-    <row r="92" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A92" s="49" t="s">
-        <v>126</v>
+    <row r="92" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A92" s="45" t="s">
+        <v>125</v>
       </c>
       <c r="B92" s="21"/>
       <c r="C92" s="7"/>
@@ -4551,12 +4694,12 @@
       <c r="I92" s="7"/>
       <c r="J92" s="7"/>
       <c r="K92" s="7"/>
-      <c r="L92" s="10"/>
+      <c r="L92" s="55"/>
       <c r="M92" s="10"/>
     </row>
-    <row r="93" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A93" s="49" t="s">
-        <v>127</v>
+    <row r="93" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A93" s="45" t="s">
+        <v>126</v>
       </c>
       <c r="B93" s="21"/>
       <c r="C93" s="7"/>
@@ -4568,12 +4711,12 @@
       <c r="I93" s="7"/>
       <c r="J93" s="7"/>
       <c r="K93" s="7"/>
-      <c r="L93" s="10"/>
+      <c r="L93" s="55"/>
       <c r="M93" s="10"/>
     </row>
-    <row r="94" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A94" s="49" t="s">
-        <v>128</v>
+    <row r="94" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A94" s="45" t="s">
+        <v>127</v>
       </c>
       <c r="B94" s="21"/>
       <c r="C94" s="7"/>
@@ -4585,12 +4728,12 @@
       <c r="I94" s="7"/>
       <c r="J94" s="7"/>
       <c r="K94" s="7"/>
-      <c r="L94" s="10"/>
+      <c r="L94" s="55"/>
       <c r="M94" s="10"/>
     </row>
-    <row r="95" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A95" s="49" t="s">
-        <v>129</v>
+    <row r="95" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A95" s="45" t="s">
+        <v>128</v>
       </c>
       <c r="B95" s="21"/>
       <c r="C95" s="7"/>
@@ -4602,12 +4745,12 @@
       <c r="I95" s="7"/>
       <c r="J95" s="7"/>
       <c r="K95" s="7"/>
-      <c r="L95" s="10"/>
+      <c r="L95" s="55"/>
       <c r="M95" s="10"/>
     </row>
-    <row r="96" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A96" s="49" t="s">
-        <v>130</v>
+    <row r="96" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A96" s="45" t="s">
+        <v>129</v>
       </c>
       <c r="B96" s="21"/>
       <c r="C96" s="7"/>
@@ -4619,12 +4762,12 @@
       <c r="I96" s="7"/>
       <c r="J96" s="7"/>
       <c r="K96" s="7"/>
-      <c r="L96" s="10"/>
+      <c r="L96" s="55"/>
       <c r="M96" s="10"/>
     </row>
-    <row r="97" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A97" s="49" t="s">
-        <v>131</v>
+    <row r="97" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A97" s="45" t="s">
+        <v>130</v>
       </c>
       <c r="B97" s="21"/>
       <c r="C97" s="7"/>
@@ -4636,12 +4779,12 @@
       <c r="I97" s="7"/>
       <c r="J97" s="7"/>
       <c r="K97" s="7"/>
-      <c r="L97" s="10"/>
+      <c r="L97" s="55"/>
       <c r="M97" s="10"/>
     </row>
-    <row r="98" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A98" s="49" t="s">
-        <v>132</v>
+    <row r="98" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A98" s="45" t="s">
+        <v>131</v>
       </c>
       <c r="B98" s="21"/>
       <c r="C98" s="7"/>
@@ -4653,12 +4796,12 @@
       <c r="I98" s="7"/>
       <c r="J98" s="7"/>
       <c r="K98" s="7"/>
-      <c r="L98" s="10"/>
+      <c r="L98" s="55"/>
       <c r="M98" s="10"/>
     </row>
-    <row r="99" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A99" s="49" t="s">
-        <v>133</v>
+    <row r="99" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A99" s="45" t="s">
+        <v>132</v>
       </c>
       <c r="B99" s="21"/>
       <c r="C99" s="7"/>
@@ -4670,12 +4813,12 @@
       <c r="I99" s="7"/>
       <c r="J99" s="7"/>
       <c r="K99" s="7"/>
-      <c r="L99" s="10"/>
+      <c r="L99" s="55"/>
       <c r="M99" s="10"/>
     </row>
-    <row r="100" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A100" s="49" t="s">
-        <v>134</v>
+    <row r="100" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A100" s="45" t="s">
+        <v>133</v>
       </c>
       <c r="B100" s="21"/>
       <c r="C100" s="7"/>
@@ -4687,12 +4830,12 @@
       <c r="I100" s="7"/>
       <c r="J100" s="7"/>
       <c r="K100" s="7"/>
-      <c r="L100" s="10"/>
+      <c r="L100" s="55"/>
       <c r="M100" s="10"/>
     </row>
-    <row r="101" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A101" s="49" t="s">
-        <v>135</v>
+    <row r="101" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A101" s="45" t="s">
+        <v>134</v>
       </c>
       <c r="B101" s="21"/>
       <c r="C101" s="7"/>
@@ -4704,12 +4847,12 @@
       <c r="I101" s="7"/>
       <c r="J101" s="7"/>
       <c r="K101" s="7"/>
-      <c r="L101" s="10"/>
+      <c r="L101" s="55"/>
       <c r="M101" s="10"/>
     </row>
-    <row r="102" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A102" s="49" t="s">
-        <v>136</v>
+    <row r="102" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A102" s="45" t="s">
+        <v>135</v>
       </c>
       <c r="B102" s="21"/>
       <c r="C102" s="7"/>
@@ -4721,12 +4864,12 @@
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
       <c r="K102" s="7"/>
-      <c r="L102" s="10"/>
+      <c r="L102" s="55"/>
       <c r="M102" s="10"/>
     </row>
-    <row r="103" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A103" s="49" t="s">
-        <v>137</v>
+    <row r="103" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A103" s="45" t="s">
+        <v>136</v>
       </c>
       <c r="B103" s="21"/>
       <c r="C103" s="7"/>
@@ -4738,12 +4881,12 @@
       <c r="I103" s="7"/>
       <c r="J103" s="7"/>
       <c r="K103" s="7"/>
-      <c r="L103" s="10"/>
+      <c r="L103" s="55"/>
       <c r="M103" s="10"/>
     </row>
-    <row r="104" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A104" s="49" t="s">
-        <v>138</v>
+    <row r="104" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A104" s="45" t="s">
+        <v>137</v>
       </c>
       <c r="B104" s="21"/>
       <c r="C104" s="7"/>
@@ -4755,12 +4898,12 @@
       <c r="I104" s="7"/>
       <c r="J104" s="7"/>
       <c r="K104" s="7"/>
-      <c r="L104" s="10"/>
+      <c r="L104" s="55"/>
       <c r="M104" s="10"/>
     </row>
-    <row r="105" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A105" s="49" t="s">
-        <v>139</v>
+    <row r="105" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A105" s="45" t="s">
+        <v>138</v>
       </c>
       <c r="B105" s="21"/>
       <c r="C105" s="7"/>
@@ -4772,12 +4915,12 @@
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
       <c r="K105" s="7"/>
-      <c r="L105" s="10"/>
+      <c r="L105" s="55"/>
       <c r="M105" s="10"/>
     </row>
-    <row r="106" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A106" s="49" t="s">
-        <v>140</v>
+    <row r="106" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A106" s="45" t="s">
+        <v>139</v>
       </c>
       <c r="B106" s="21"/>
       <c r="C106" s="7"/>
@@ -4789,12 +4932,12 @@
       <c r="I106" s="7"/>
       <c r="J106" s="7"/>
       <c r="K106" s="7"/>
-      <c r="L106" s="10"/>
+      <c r="L106" s="55"/>
       <c r="M106" s="10"/>
     </row>
-    <row r="107" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A107" s="49" t="s">
-        <v>141</v>
+    <row r="107" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A107" s="45" t="s">
+        <v>140</v>
       </c>
       <c r="B107" s="21"/>
       <c r="C107" s="7"/>
@@ -4806,12 +4949,12 @@
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
       <c r="K107" s="7"/>
-      <c r="L107" s="10"/>
+      <c r="L107" s="55"/>
       <c r="M107" s="10"/>
     </row>
-    <row r="108" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A108" s="49" t="s">
-        <v>142</v>
+    <row r="108" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A108" s="45" t="s">
+        <v>141</v>
       </c>
       <c r="B108" s="21"/>
       <c r="C108" s="7"/>
@@ -4823,12 +4966,12 @@
       <c r="I108" s="7"/>
       <c r="J108" s="7"/>
       <c r="K108" s="7"/>
-      <c r="L108" s="10"/>
+      <c r="L108" s="55"/>
       <c r="M108" s="10"/>
     </row>
-    <row r="109" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A109" s="49" t="s">
-        <v>143</v>
+    <row r="109" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A109" s="45" t="s">
+        <v>142</v>
       </c>
       <c r="B109" s="21"/>
       <c r="C109" s="7"/>
@@ -4840,12 +4983,12 @@
       <c r="I109" s="7"/>
       <c r="J109" s="7"/>
       <c r="K109" s="7"/>
-      <c r="L109" s="10"/>
+      <c r="L109" s="55"/>
       <c r="M109" s="10"/>
     </row>
-    <row r="110" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A110" s="49" t="s">
-        <v>144</v>
+    <row r="110" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A110" s="45" t="s">
+        <v>143</v>
       </c>
       <c r="B110" s="21"/>
       <c r="C110" s="7"/>
@@ -4857,12 +5000,12 @@
       <c r="I110" s="7"/>
       <c r="J110" s="7"/>
       <c r="K110" s="7"/>
-      <c r="L110" s="10"/>
+      <c r="L110" s="55"/>
       <c r="M110" s="10"/>
     </row>
-    <row r="111" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A111" s="49" t="s">
-        <v>145</v>
+    <row r="111" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A111" s="45" t="s">
+        <v>144</v>
       </c>
       <c r="B111" s="21"/>
       <c r="C111" s="7"/>
@@ -4874,12 +5017,12 @@
       <c r="I111" s="7"/>
       <c r="J111" s="7"/>
       <c r="K111" s="7"/>
-      <c r="L111" s="10"/>
+      <c r="L111" s="55"/>
       <c r="M111" s="10"/>
     </row>
-    <row r="112" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A112" s="49" t="s">
-        <v>146</v>
+    <row r="112" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A112" s="45" t="s">
+        <v>145</v>
       </c>
       <c r="B112" s="21"/>
       <c r="C112" s="7"/>
@@ -4891,12 +5034,12 @@
       <c r="I112" s="7"/>
       <c r="J112" s="7"/>
       <c r="K112" s="7"/>
-      <c r="L112" s="10"/>
+      <c r="L112" s="55"/>
       <c r="M112" s="10"/>
     </row>
-    <row r="113" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A113" s="49" t="s">
-        <v>147</v>
+    <row r="113" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A113" s="45" t="s">
+        <v>146</v>
       </c>
       <c r="B113" s="21"/>
       <c r="C113" s="7"/>
@@ -4908,12 +5051,12 @@
       <c r="I113" s="7"/>
       <c r="J113" s="7"/>
       <c r="K113" s="7"/>
-      <c r="L113" s="10"/>
+      <c r="L113" s="55"/>
       <c r="M113" s="10"/>
     </row>
-    <row r="114" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A114" s="49" t="s">
-        <v>148</v>
+    <row r="114" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A114" s="45" t="s">
+        <v>147</v>
       </c>
       <c r="B114" s="21"/>
       <c r="C114" s="7"/>
@@ -4925,12 +5068,12 @@
       <c r="I114" s="7"/>
       <c r="J114" s="7"/>
       <c r="K114" s="7"/>
-      <c r="L114" s="10"/>
+      <c r="L114" s="55"/>
       <c r="M114" s="10"/>
     </row>
-    <row r="115" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A115" s="49" t="s">
-        <v>149</v>
+    <row r="115" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A115" s="45" t="s">
+        <v>148</v>
       </c>
       <c r="B115" s="21"/>
       <c r="C115" s="7"/>
@@ -4942,12 +5085,12 @@
       <c r="I115" s="7"/>
       <c r="J115" s="7"/>
       <c r="K115" s="7"/>
-      <c r="L115" s="10"/>
+      <c r="L115" s="55"/>
       <c r="M115" s="10"/>
     </row>
-    <row r="116" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A116" s="49" t="s">
-        <v>150</v>
+    <row r="116" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A116" s="45" t="s">
+        <v>149</v>
       </c>
       <c r="B116" s="21"/>
       <c r="C116" s="7"/>
@@ -4959,12 +5102,12 @@
       <c r="I116" s="7"/>
       <c r="J116" s="7"/>
       <c r="K116" s="7"/>
-      <c r="L116" s="10"/>
+      <c r="L116" s="55"/>
       <c r="M116" s="10"/>
     </row>
-    <row r="117" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A117" s="49" t="s">
-        <v>151</v>
+    <row r="117" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A117" s="45" t="s">
+        <v>150</v>
       </c>
       <c r="B117" s="21"/>
       <c r="C117" s="7"/>
@@ -4976,12 +5119,12 @@
       <c r="I117" s="7"/>
       <c r="J117" s="7"/>
       <c r="K117" s="7"/>
-      <c r="L117" s="10"/>
+      <c r="L117" s="55"/>
       <c r="M117" s="10"/>
     </row>
-    <row r="118" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A118" s="49" t="s">
-        <v>152</v>
+    <row r="118" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A118" s="45" t="s">
+        <v>151</v>
       </c>
       <c r="B118" s="21"/>
       <c r="C118" s="7"/>
@@ -4993,12 +5136,12 @@
       <c r="I118" s="7"/>
       <c r="J118" s="7"/>
       <c r="K118" s="7"/>
-      <c r="L118" s="10"/>
+      <c r="L118" s="55"/>
       <c r="M118" s="10"/>
     </row>
-    <row r="119" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A119" s="49" t="s">
-        <v>153</v>
+    <row r="119" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A119" s="45" t="s">
+        <v>152</v>
       </c>
       <c r="B119" s="21"/>
       <c r="C119" s="7"/>
@@ -5010,12 +5153,12 @@
       <c r="I119" s="7"/>
       <c r="J119" s="7"/>
       <c r="K119" s="7"/>
-      <c r="L119" s="10"/>
+      <c r="L119" s="55"/>
       <c r="M119" s="10"/>
     </row>
-    <row r="120" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A120" s="49" t="s">
-        <v>154</v>
+    <row r="120" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A120" s="45" t="s">
+        <v>153</v>
       </c>
       <c r="B120" s="21"/>
       <c r="C120" s="7"/>
@@ -5027,12 +5170,12 @@
       <c r="I120" s="7"/>
       <c r="J120" s="7"/>
       <c r="K120" s="7"/>
-      <c r="L120" s="10"/>
+      <c r="L120" s="55"/>
       <c r="M120" s="10"/>
     </row>
-    <row r="121" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A121" s="49" t="s">
-        <v>155</v>
+    <row r="121" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A121" s="45" t="s">
+        <v>154</v>
       </c>
       <c r="B121" s="21"/>
       <c r="C121" s="7"/>
@@ -5044,12 +5187,12 @@
       <c r="I121" s="7"/>
       <c r="J121" s="7"/>
       <c r="K121" s="7"/>
-      <c r="L121" s="10"/>
+      <c r="L121" s="55"/>
       <c r="M121" s="10"/>
     </row>
-    <row r="122" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A122" s="49" t="s">
-        <v>156</v>
+    <row r="122" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A122" s="45" t="s">
+        <v>155</v>
       </c>
       <c r="B122" s="21"/>
       <c r="C122" s="7"/>
@@ -5061,12 +5204,12 @@
       <c r="I122" s="7"/>
       <c r="J122" s="7"/>
       <c r="K122" s="7"/>
-      <c r="L122" s="10"/>
+      <c r="L122" s="55"/>
       <c r="M122" s="10"/>
     </row>
-    <row r="123" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A123" s="49" t="s">
-        <v>157</v>
+    <row r="123" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A123" s="45" t="s">
+        <v>156</v>
       </c>
       <c r="B123" s="21"/>
       <c r="C123" s="7"/>
@@ -5078,12 +5221,12 @@
       <c r="I123" s="7"/>
       <c r="J123" s="7"/>
       <c r="K123" s="7"/>
-      <c r="L123" s="10"/>
+      <c r="L123" s="55"/>
       <c r="M123" s="10"/>
     </row>
-    <row r="124" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A124" s="49" t="s">
-        <v>158</v>
+    <row r="124" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A124" s="45" t="s">
+        <v>157</v>
       </c>
       <c r="B124" s="21"/>
       <c r="C124" s="7"/>
@@ -5095,12 +5238,12 @@
       <c r="I124" s="7"/>
       <c r="J124" s="7"/>
       <c r="K124" s="7"/>
-      <c r="L124" s="10"/>
+      <c r="L124" s="55"/>
       <c r="M124" s="10"/>
     </row>
-    <row r="125" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A125" s="49" t="s">
-        <v>159</v>
+    <row r="125" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A125" s="45" t="s">
+        <v>158</v>
       </c>
       <c r="B125" s="21"/>
       <c r="C125" s="7"/>
@@ -5112,12 +5255,12 @@
       <c r="I125" s="7"/>
       <c r="J125" s="7"/>
       <c r="K125" s="7"/>
-      <c r="L125" s="10"/>
+      <c r="L125" s="55"/>
       <c r="M125" s="10"/>
     </row>
-    <row r="126" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A126" s="49" t="s">
-        <v>160</v>
+    <row r="126" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A126" s="45" t="s">
+        <v>159</v>
       </c>
       <c r="B126" s="21"/>
       <c r="C126" s="7"/>
@@ -5129,12 +5272,12 @@
       <c r="I126" s="7"/>
       <c r="J126" s="7"/>
       <c r="K126" s="7"/>
-      <c r="L126" s="10"/>
+      <c r="L126" s="55"/>
       <c r="M126" s="10"/>
     </row>
-    <row r="127" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A127" s="49" t="s">
-        <v>161</v>
+    <row r="127" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A127" s="45" t="s">
+        <v>160</v>
       </c>
       <c r="B127" s="21"/>
       <c r="C127" s="7"/>
@@ -5146,12 +5289,12 @@
       <c r="I127" s="7"/>
       <c r="J127" s="7"/>
       <c r="K127" s="7"/>
-      <c r="L127" s="10"/>
+      <c r="L127" s="55"/>
       <c r="M127" s="10"/>
     </row>
-    <row r="128" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A128" s="49" t="s">
-        <v>162</v>
+    <row r="128" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A128" s="45" t="s">
+        <v>161</v>
       </c>
       <c r="B128" s="21"/>
       <c r="C128" s="7"/>
@@ -5163,12 +5306,12 @@
       <c r="I128" s="7"/>
       <c r="J128" s="7"/>
       <c r="K128" s="7"/>
-      <c r="L128" s="10"/>
+      <c r="L128" s="55"/>
       <c r="M128" s="10"/>
     </row>
-    <row r="129" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A129" s="49" t="s">
-        <v>163</v>
+    <row r="129" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A129" s="45" t="s">
+        <v>162</v>
       </c>
       <c r="B129" s="21"/>
       <c r="C129" s="7"/>
@@ -5180,12 +5323,12 @@
       <c r="I129" s="7"/>
       <c r="J129" s="7"/>
       <c r="K129" s="7"/>
-      <c r="L129" s="10"/>
+      <c r="L129" s="55"/>
       <c r="M129" s="10"/>
     </row>
-    <row r="130" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A130" s="49" t="s">
-        <v>164</v>
+    <row r="130" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A130" s="45" t="s">
+        <v>163</v>
       </c>
       <c r="B130" s="21"/>
       <c r="C130" s="7"/>
@@ -5197,12 +5340,12 @@
       <c r="I130" s="7"/>
       <c r="J130" s="7"/>
       <c r="K130" s="7"/>
-      <c r="L130" s="10"/>
+      <c r="L130" s="55"/>
       <c r="M130" s="10"/>
     </row>
-    <row r="131" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A131" s="49" t="s">
-        <v>165</v>
+    <row r="131" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A131" s="45" t="s">
+        <v>164</v>
       </c>
       <c r="B131" s="21"/>
       <c r="C131" s="7"/>
@@ -5214,12 +5357,12 @@
       <c r="I131" s="7"/>
       <c r="J131" s="7"/>
       <c r="K131" s="7"/>
-      <c r="L131" s="10"/>
+      <c r="L131" s="55"/>
       <c r="M131" s="10"/>
     </row>
-    <row r="132" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A132" s="49" t="s">
-        <v>166</v>
+    <row r="132" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A132" s="45" t="s">
+        <v>165</v>
       </c>
       <c r="B132" s="21"/>
       <c r="C132" s="7"/>
@@ -5231,12 +5374,12 @@
       <c r="I132" s="7"/>
       <c r="J132" s="7"/>
       <c r="K132" s="7"/>
-      <c r="L132" s="10"/>
+      <c r="L132" s="55"/>
       <c r="M132" s="10"/>
     </row>
-    <row r="133" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A133" s="49" t="s">
-        <v>167</v>
+    <row r="133" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A133" s="45" t="s">
+        <v>166</v>
       </c>
       <c r="B133" s="21"/>
       <c r="C133" s="7"/>
@@ -5248,12 +5391,12 @@
       <c r="I133" s="7"/>
       <c r="J133" s="7"/>
       <c r="K133" s="7"/>
-      <c r="L133" s="10"/>
+      <c r="L133" s="55"/>
       <c r="M133" s="10"/>
     </row>
-    <row r="134" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A134" s="49" t="s">
-        <v>168</v>
+    <row r="134" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A134" s="45" t="s">
+        <v>167</v>
       </c>
       <c r="B134" s="21"/>
       <c r="C134" s="7"/>
@@ -5265,12 +5408,12 @@
       <c r="I134" s="7"/>
       <c r="J134" s="7"/>
       <c r="K134" s="7"/>
-      <c r="L134" s="10"/>
+      <c r="L134" s="55"/>
       <c r="M134" s="10"/>
     </row>
-    <row r="135" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A135" s="49" t="s">
-        <v>169</v>
+    <row r="135" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A135" s="45" t="s">
+        <v>168</v>
       </c>
       <c r="B135" s="21"/>
       <c r="C135" s="7"/>
@@ -5282,12 +5425,12 @@
       <c r="I135" s="7"/>
       <c r="J135" s="7"/>
       <c r="K135" s="7"/>
-      <c r="L135" s="10"/>
+      <c r="L135" s="55"/>
       <c r="M135" s="10"/>
     </row>
-    <row r="136" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A136" s="49" t="s">
-        <v>170</v>
+    <row r="136" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A136" s="45" t="s">
+        <v>169</v>
       </c>
       <c r="B136" s="21"/>
       <c r="C136" s="7"/>
@@ -5299,12 +5442,12 @@
       <c r="I136" s="7"/>
       <c r="J136" s="7"/>
       <c r="K136" s="7"/>
-      <c r="L136" s="10"/>
+      <c r="L136" s="55"/>
       <c r="M136" s="10"/>
     </row>
-    <row r="137" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A137" s="49" t="s">
-        <v>171</v>
+    <row r="137" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A137" s="45" t="s">
+        <v>170</v>
       </c>
       <c r="B137" s="21"/>
       <c r="C137" s="7"/>
@@ -5316,12 +5459,12 @@
       <c r="I137" s="7"/>
       <c r="J137" s="7"/>
       <c r="K137" s="7"/>
-      <c r="L137" s="10"/>
+      <c r="L137" s="55"/>
       <c r="M137" s="10"/>
     </row>
-    <row r="138" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A138" s="49" t="s">
-        <v>172</v>
+    <row r="138" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A138" s="45" t="s">
+        <v>171</v>
       </c>
       <c r="B138" s="21"/>
       <c r="C138" s="7"/>
@@ -5333,12 +5476,12 @@
       <c r="I138" s="7"/>
       <c r="J138" s="7"/>
       <c r="K138" s="7"/>
-      <c r="L138" s="10"/>
+      <c r="L138" s="55"/>
       <c r="M138" s="10"/>
     </row>
-    <row r="139" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A139" s="49" t="s">
-        <v>173</v>
+    <row r="139" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A139" s="45" t="s">
+        <v>172</v>
       </c>
       <c r="B139" s="21"/>
       <c r="C139" s="7"/>
@@ -5350,12 +5493,12 @@
       <c r="I139" s="7"/>
       <c r="J139" s="7"/>
       <c r="K139" s="7"/>
-      <c r="L139" s="10"/>
+      <c r="L139" s="55"/>
       <c r="M139" s="10"/>
     </row>
-    <row r="140" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A140" s="49" t="s">
-        <v>174</v>
+    <row r="140" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A140" s="45" t="s">
+        <v>173</v>
       </c>
       <c r="B140" s="21"/>
       <c r="C140" s="7"/>
@@ -5367,12 +5510,12 @@
       <c r="I140" s="7"/>
       <c r="J140" s="7"/>
       <c r="K140" s="7"/>
-      <c r="L140" s="10"/>
+      <c r="L140" s="55"/>
       <c r="M140" s="10"/>
     </row>
-    <row r="141" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A141" s="49" t="s">
-        <v>175</v>
+    <row r="141" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A141" s="45" t="s">
+        <v>174</v>
       </c>
       <c r="B141" s="21"/>
       <c r="C141" s="7"/>
@@ -5384,12 +5527,12 @@
       <c r="I141" s="7"/>
       <c r="J141" s="7"/>
       <c r="K141" s="7"/>
-      <c r="L141" s="10"/>
+      <c r="L141" s="55"/>
       <c r="M141" s="10"/>
     </row>
-    <row r="142" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A142" s="49" t="s">
-        <v>176</v>
+    <row r="142" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A142" s="45" t="s">
+        <v>175</v>
       </c>
       <c r="B142" s="21"/>
       <c r="C142" s="7"/>
@@ -5401,12 +5544,12 @@
       <c r="I142" s="7"/>
       <c r="J142" s="7"/>
       <c r="K142" s="7"/>
-      <c r="L142" s="10"/>
+      <c r="L142" s="55"/>
       <c r="M142" s="10"/>
     </row>
-    <row r="143" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A143" s="49" t="s">
-        <v>177</v>
+    <row r="143" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A143" s="45" t="s">
+        <v>176</v>
       </c>
       <c r="B143" s="21"/>
       <c r="C143" s="7"/>
@@ -5418,12 +5561,12 @@
       <c r="I143" s="7"/>
       <c r="J143" s="7"/>
       <c r="K143" s="7"/>
-      <c r="L143" s="10"/>
+      <c r="L143" s="55"/>
       <c r="M143" s="10"/>
     </row>
-    <row r="144" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A144" s="49" t="s">
-        <v>178</v>
+    <row r="144" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A144" s="45" t="s">
+        <v>177</v>
       </c>
       <c r="B144" s="21"/>
       <c r="C144" s="7"/>
@@ -5435,12 +5578,12 @@
       <c r="I144" s="7"/>
       <c r="J144" s="7"/>
       <c r="K144" s="7"/>
-      <c r="L144" s="10"/>
+      <c r="L144" s="55"/>
       <c r="M144" s="10"/>
     </row>
-    <row r="145" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A145" s="49" t="s">
-        <v>179</v>
+    <row r="145" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A145" s="45" t="s">
+        <v>178</v>
       </c>
       <c r="B145" s="21"/>
       <c r="C145" s="7"/>
@@ -5452,12 +5595,12 @@
       <c r="I145" s="7"/>
       <c r="J145" s="7"/>
       <c r="K145" s="7"/>
-      <c r="L145" s="10"/>
+      <c r="L145" s="55"/>
       <c r="M145" s="10"/>
     </row>
-    <row r="146" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A146" s="49" t="s">
-        <v>180</v>
+    <row r="146" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A146" s="45" t="s">
+        <v>179</v>
       </c>
       <c r="B146" s="21"/>
       <c r="C146" s="7"/>
@@ -5469,12 +5612,12 @@
       <c r="I146" s="7"/>
       <c r="J146" s="7"/>
       <c r="K146" s="7"/>
-      <c r="L146" s="10"/>
+      <c r="L146" s="55"/>
       <c r="M146" s="10"/>
     </row>
-    <row r="147" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A147" s="49" t="s">
-        <v>181</v>
+    <row r="147" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A147" s="45" t="s">
+        <v>180</v>
       </c>
       <c r="B147" s="21"/>
       <c r="C147" s="7"/>
@@ -5486,12 +5629,12 @@
       <c r="I147" s="7"/>
       <c r="J147" s="7"/>
       <c r="K147" s="7"/>
-      <c r="L147" s="10"/>
+      <c r="L147" s="55"/>
       <c r="M147" s="10"/>
     </row>
-    <row r="148" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A148" s="49" t="s">
-        <v>182</v>
+    <row r="148" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A148" s="45" t="s">
+        <v>181</v>
       </c>
       <c r="B148" s="21"/>
       <c r="C148" s="7"/>
@@ -5503,12 +5646,12 @@
       <c r="I148" s="7"/>
       <c r="J148" s="7"/>
       <c r="K148" s="7"/>
-      <c r="L148" s="10"/>
+      <c r="L148" s="55"/>
       <c r="M148" s="10"/>
     </row>
-    <row r="149" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A149" s="49" t="s">
-        <v>183</v>
+    <row r="149" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A149" s="45" t="s">
+        <v>182</v>
       </c>
       <c r="B149" s="21"/>
       <c r="C149" s="7"/>
@@ -5520,12 +5663,12 @@
       <c r="I149" s="7"/>
       <c r="J149" s="7"/>
       <c r="K149" s="7"/>
-      <c r="L149" s="10"/>
+      <c r="L149" s="55"/>
       <c r="M149" s="10"/>
     </row>
-    <row r="150" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A150" s="49" t="s">
-        <v>184</v>
+    <row r="150" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A150" s="45" t="s">
+        <v>183</v>
       </c>
       <c r="B150" s="21"/>
       <c r="C150" s="7"/>
@@ -5537,12 +5680,12 @@
       <c r="I150" s="7"/>
       <c r="J150" s="7"/>
       <c r="K150" s="7"/>
-      <c r="L150" s="10"/>
+      <c r="L150" s="55"/>
       <c r="M150" s="10"/>
     </row>
-    <row r="151" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A151" s="49" t="s">
-        <v>185</v>
+    <row r="151" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A151" s="45" t="s">
+        <v>184</v>
       </c>
       <c r="B151" s="21"/>
       <c r="C151" s="7"/>
@@ -5554,12 +5697,12 @@
       <c r="I151" s="7"/>
       <c r="J151" s="7"/>
       <c r="K151" s="7"/>
-      <c r="L151" s="10"/>
+      <c r="L151" s="55"/>
       <c r="M151" s="10"/>
     </row>
-    <row r="152" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A152" s="49" t="s">
-        <v>186</v>
+    <row r="152" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A152" s="45" t="s">
+        <v>185</v>
       </c>
       <c r="B152" s="21"/>
       <c r="C152" s="7"/>
@@ -5571,12 +5714,12 @@
       <c r="I152" s="7"/>
       <c r="J152" s="7"/>
       <c r="K152" s="7"/>
-      <c r="L152" s="10"/>
+      <c r="L152" s="55"/>
       <c r="M152" s="10"/>
     </row>
-    <row r="153" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A153" s="49" t="s">
-        <v>187</v>
+    <row r="153" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A153" s="45" t="s">
+        <v>186</v>
       </c>
       <c r="B153" s="21"/>
       <c r="C153" s="7"/>
@@ -5588,12 +5731,12 @@
       <c r="I153" s="7"/>
       <c r="J153" s="7"/>
       <c r="K153" s="7"/>
-      <c r="L153" s="10"/>
+      <c r="L153" s="55"/>
       <c r="M153" s="10"/>
     </row>
-    <row r="154" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A154" s="49" t="s">
-        <v>188</v>
+    <row r="154" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A154" s="45" t="s">
+        <v>187</v>
       </c>
       <c r="B154" s="21"/>
       <c r="C154" s="7"/>
@@ -5605,12 +5748,12 @@
       <c r="I154" s="7"/>
       <c r="J154" s="7"/>
       <c r="K154" s="7"/>
-      <c r="L154" s="10"/>
+      <c r="L154" s="55"/>
       <c r="M154" s="10"/>
     </row>
-    <row r="155" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A155" s="49" t="s">
-        <v>189</v>
+    <row r="155" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A155" s="45" t="s">
+        <v>188</v>
       </c>
       <c r="B155" s="21"/>
       <c r="C155" s="7"/>
@@ -5622,12 +5765,12 @@
       <c r="I155" s="7"/>
       <c r="J155" s="7"/>
       <c r="K155" s="7"/>
-      <c r="L155" s="10"/>
+      <c r="L155" s="55"/>
       <c r="M155" s="10"/>
     </row>
-    <row r="156" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A156" s="49" t="s">
-        <v>190</v>
+    <row r="156" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A156" s="45" t="s">
+        <v>189</v>
       </c>
       <c r="B156" s="21"/>
       <c r="C156" s="7"/>
@@ -5639,12 +5782,12 @@
       <c r="I156" s="7"/>
       <c r="J156" s="7"/>
       <c r="K156" s="7"/>
-      <c r="L156" s="10"/>
+      <c r="L156" s="55"/>
       <c r="M156" s="10"/>
     </row>
-    <row r="157" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A157" s="49" t="s">
-        <v>191</v>
+    <row r="157" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A157" s="45" t="s">
+        <v>190</v>
       </c>
       <c r="B157" s="21"/>
       <c r="C157" s="7"/>
@@ -5656,12 +5799,12 @@
       <c r="I157" s="7"/>
       <c r="J157" s="7"/>
       <c r="K157" s="7"/>
-      <c r="L157" s="10"/>
+      <c r="L157" s="55"/>
       <c r="M157" s="10"/>
     </row>
-    <row r="158" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A158" s="49" t="s">
-        <v>192</v>
+    <row r="158" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A158" s="45" t="s">
+        <v>191</v>
       </c>
       <c r="B158" s="21"/>
       <c r="C158" s="7"/>
@@ -5673,12 +5816,12 @@
       <c r="I158" s="7"/>
       <c r="J158" s="7"/>
       <c r="K158" s="7"/>
-      <c r="L158" s="10"/>
+      <c r="L158" s="55"/>
       <c r="M158" s="10"/>
     </row>
-    <row r="159" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A159" s="49" t="s">
-        <v>193</v>
+    <row r="159" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A159" s="45" t="s">
+        <v>192</v>
       </c>
       <c r="B159" s="21"/>
       <c r="C159" s="7"/>
@@ -5690,12 +5833,12 @@
       <c r="I159" s="7"/>
       <c r="J159" s="7"/>
       <c r="K159" s="7"/>
-      <c r="L159" s="10"/>
+      <c r="L159" s="55"/>
       <c r="M159" s="10"/>
     </row>
-    <row r="160" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A160" s="49" t="s">
-        <v>194</v>
+    <row r="160" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A160" s="45" t="s">
+        <v>193</v>
       </c>
       <c r="B160" s="21"/>
       <c r="C160" s="7"/>
@@ -5707,12 +5850,12 @@
       <c r="I160" s="7"/>
       <c r="J160" s="7"/>
       <c r="K160" s="7"/>
-      <c r="L160" s="10"/>
+      <c r="L160" s="55"/>
       <c r="M160" s="10"/>
     </row>
-    <row r="161" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A161" s="49" t="s">
-        <v>195</v>
+    <row r="161" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A161" s="45" t="s">
+        <v>194</v>
       </c>
       <c r="B161" s="21"/>
       <c r="C161" s="7"/>
@@ -5724,11 +5867,11 @@
       <c r="I161" s="7"/>
       <c r="J161" s="7"/>
       <c r="K161" s="7"/>
-      <c r="L161" s="10"/>
+      <c r="L161" s="55"/>
       <c r="M161" s="10"/>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G162" s="40"/>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G162" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5738,30 +5881,41 @@
     <mergeCell ref="B63:F70"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
-  <conditionalFormatting sqref="C1:J1 M1 L5:M5 C162:J65517">
-    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="C1:J1 M1 M5 C162:J65517">
+    <cfRule type="cellIs" dxfId="8" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F71:H161">
-    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" stopIfTrue="1" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Testing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" stopIfTrue="1" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="L5">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Critical"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F71:H161">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F71:H161" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"In Progress, Testing, Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add test cases to RTM
add test cases delete , navigate features  to RTM
 update delete feature regarding review comments
</commit_message>
<xml_diff>
--- a/RTM/Traceability_Matrix learning hub ver 2.xlsx
+++ b/RTM/Traceability_Matrix learning hub ver 2.xlsx
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="320">
   <si>
     <t>For detail regarding the practice of Requirements Management, please refer to the Requirements Management Practices Guide</t>
   </si>
@@ -1342,6 +1342,46 @@
   <si>
     <t>Design Document (3.8.2 classDiagram_Delete User)</t>
   </si>
+  <si>
+    <t>TC_LearningHub_NAV_001 -003 
+TC_LearningHub_NAV_008 -10</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_NAV_004
+TC_LearningHub_NAV_011</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_NAV_005 -006
+TC_LearningHub_NAV_012 - 013</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_NAV_007
+TC_LearningHub_NAV_014</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_DELETE _001 -004</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_DELETE _005 -008</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_DELETE _009 -012</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_DELETE _013 -016</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_DELETE _017 -020</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_DELETE _021 -024</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_DELETE _025 -026</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_DELETE _027</t>
+  </si>
 </sst>
 </file>
 
@@ -1350,7 +1390,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1468,6 +1508,13 @@
       <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1648,7 +1695,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1753,12 +1800,6 @@
     <xf numFmtId="49" fontId="10" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1768,14 +1809,8 @@
     <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1801,8 +1836,23 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2154,10 +2204,10 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="39"/>
+      <c r="B4" s="51"/>
     </row>
     <row r="5" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
@@ -2259,8 +2309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F42" sqref="F33:F42"/>
+    <sheetView tabSelected="1" topLeftCell="H17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2275,13 +2325,13 @@
     <col min="8" max="8" width="51" style="5" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" style="5" customWidth="1"/>
     <col min="10" max="10" width="17.28515625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="6" customWidth="1"/>
-    <col min="13" max="13" width="86" style="6" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="6" customWidth="1"/>
+    <col min="12" max="12" width="34.140625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="30.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="39" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="24"/>
@@ -2293,71 +2343,71 @@
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
-      <c r="K1" s="41" t="s">
+      <c r="K1" s="39" t="s">
         <v>20</v>
       </c>
       <c r="L1" s="24"/>
       <c r="M1" s="24"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="43" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
-      <c r="M2" s="44"/>
+      <c r="M2" s="41"/>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="43" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
-      <c r="M3" s="44"/>
+      <c r="M3" s="41"/>
     </row>
     <row r="4" spans="1:13" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="45" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
-      <c r="M4" s="46"/>
+      <c r="M4" s="42"/>
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="43" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="23" t="s">
@@ -2390,15 +2440,15 @@
       <c r="K5" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="48" t="s">
+      <c r="L5" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="48" t="s">
+      <c r="M5" s="44" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="45" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -2410,16 +2460,16 @@
       <c r="D6" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="E6" s="50" t="s">
+      <c r="E6" s="46" t="s">
         <v>237</v>
       </c>
-      <c r="F6" s="50" t="s">
+      <c r="F6" s="46" t="s">
         <v>232</v>
       </c>
       <c r="G6" s="25" t="s">
         <v>235</v>
       </c>
-      <c r="H6" s="51" t="s">
+      <c r="H6" s="47" t="s">
         <v>220</v>
       </c>
       <c r="I6" s="7"/>
@@ -2429,7 +2479,7 @@
       <c r="M6" s="10"/>
     </row>
     <row r="7" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="45" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="20" t="s">
@@ -2441,7 +2491,7 @@
       <c r="D7" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F7" s="7" t="s">
@@ -2450,7 +2500,7 @@
       <c r="G7" s="25" t="s">
         <v>235</v>
       </c>
-      <c r="H7" s="51" t="s">
+      <c r="H7" s="47" t="s">
         <v>220</v>
       </c>
       <c r="I7" s="7"/>
@@ -2460,7 +2510,7 @@
       <c r="M7" s="10"/>
     </row>
     <row r="8" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="45" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="20" t="s">
@@ -2472,7 +2522,7 @@
       <c r="D8" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="E8" s="50" t="s">
+      <c r="E8" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F8" s="7" t="s">
@@ -2481,7 +2531,7 @@
       <c r="G8" s="25" t="s">
         <v>235</v>
       </c>
-      <c r="H8" s="51" t="s">
+      <c r="H8" s="47" t="s">
         <v>220</v>
       </c>
       <c r="I8" s="7"/>
@@ -2491,7 +2541,7 @@
       <c r="M8" s="10"/>
     </row>
     <row r="9" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="45" t="s">
         <v>42</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -2503,14 +2553,14 @@
       <c r="D9" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="E9" s="50" t="s">
+      <c r="E9" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>232</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="51" t="s">
+      <c r="H9" s="47" t="s">
         <v>220</v>
       </c>
       <c r="I9" s="7"/>
@@ -2520,7 +2570,7 @@
       <c r="M9" s="10"/>
     </row>
     <row r="10" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="45" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="20" t="s">
@@ -2532,7 +2582,7 @@
       <c r="D10" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="E10" s="50" t="s">
+      <c r="E10" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F10" s="7" t="s">
@@ -2541,7 +2591,7 @@
       <c r="G10" s="25" t="s">
         <v>236</v>
       </c>
-      <c r="H10" s="51" t="s">
+      <c r="H10" s="47" t="s">
         <v>220</v>
       </c>
       <c r="I10" s="7"/>
@@ -2551,7 +2601,7 @@
       <c r="M10" s="10"/>
     </row>
     <row r="11" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="45" t="s">
         <v>48</v>
       </c>
       <c r="B11" s="20" t="s">
@@ -2563,7 +2613,7 @@
       <c r="D11" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="E11" s="50" t="s">
+      <c r="E11" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F11" s="7" t="s">
@@ -2572,7 +2622,7 @@
       <c r="G11" s="25" t="s">
         <v>236</v>
       </c>
-      <c r="H11" s="51" t="s">
+      <c r="H11" s="47" t="s">
         <v>220</v>
       </c>
       <c r="I11" s="7"/>
@@ -2582,7 +2632,7 @@
       <c r="M11" s="10"/>
     </row>
     <row r="12" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="45" t="s">
         <v>50</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -2594,7 +2644,7 @@
       <c r="D12" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="E12" s="50" t="s">
+      <c r="E12" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F12" s="7" t="s">
@@ -2603,7 +2653,7 @@
       <c r="G12" s="25" t="s">
         <v>236</v>
       </c>
-      <c r="H12" s="51" t="s">
+      <c r="H12" s="47" t="s">
         <v>220</v>
       </c>
       <c r="I12" s="7"/>
@@ -2613,7 +2663,7 @@
       <c r="M12" s="10"/>
     </row>
     <row r="13" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="45" t="s">
         <v>52</v>
       </c>
       <c r="B13" s="20" t="s">
@@ -2625,7 +2675,7 @@
       <c r="D13" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="E13" s="50" t="s">
+      <c r="E13" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F13" s="7" t="s">
@@ -2634,7 +2684,7 @@
       <c r="G13" s="25" t="s">
         <v>238</v>
       </c>
-      <c r="H13" s="51" t="s">
+      <c r="H13" s="47" t="s">
         <v>220</v>
       </c>
       <c r="I13" s="7"/>
@@ -2644,7 +2694,7 @@
       <c r="M13" s="10"/>
     </row>
     <row r="14" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="49" t="s">
+      <c r="A14" s="45" t="s">
         <v>229</v>
       </c>
       <c r="B14" s="20" t="s">
@@ -2656,14 +2706,14 @@
       <c r="D14" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="E14" s="50" t="s">
+      <c r="E14" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>232</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="51" t="s">
+      <c r="H14" s="47" t="s">
         <v>220</v>
       </c>
       <c r="I14" s="7"/>
@@ -2673,7 +2723,7 @@
       <c r="M14" s="10"/>
     </row>
     <row r="15" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="45" t="s">
         <v>54</v>
       </c>
       <c r="B15" s="21" t="s">
@@ -2685,14 +2735,14 @@
       <c r="D15" s="30" t="s">
         <v>240</v>
       </c>
-      <c r="E15" s="50" t="s">
+      <c r="E15" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F15" s="30" t="s">
         <v>239</v>
       </c>
       <c r="G15" s="31"/>
-      <c r="H15" s="51" t="s">
+      <c r="H15" s="47" t="s">
         <v>221</v>
       </c>
       <c r="I15" s="7"/>
@@ -2702,7 +2752,7 @@
       <c r="M15" s="10"/>
     </row>
     <row r="16" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="45" t="s">
         <v>256</v>
       </c>
       <c r="B16" s="21" t="s">
@@ -2714,14 +2764,14 @@
       <c r="D16" s="30" t="s">
         <v>240</v>
       </c>
-      <c r="E16" s="50" t="s">
+      <c r="E16" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F16" s="30" t="s">
         <v>239</v>
       </c>
       <c r="G16" s="22"/>
-      <c r="H16" s="51" t="s">
+      <c r="H16" s="47" t="s">
         <v>221</v>
       </c>
       <c r="I16" s="7"/>
@@ -2731,7 +2781,7 @@
       <c r="M16" s="10"/>
     </row>
     <row r="17" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="45" t="s">
         <v>58</v>
       </c>
       <c r="B17" s="21" t="s">
@@ -2743,14 +2793,14 @@
       <c r="D17" s="30" t="s">
         <v>240</v>
       </c>
-      <c r="E17" s="50" t="s">
+      <c r="E17" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F17" s="30" t="s">
         <v>239</v>
       </c>
       <c r="G17" s="22"/>
-      <c r="H17" s="51" t="s">
+      <c r="H17" s="47" t="s">
         <v>221</v>
       </c>
       <c r="I17" s="7"/>
@@ -2759,8 +2809,8 @@
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="s">
+    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="45" t="s">
         <v>60</v>
       </c>
       <c r="B18" s="21" t="s">
@@ -2770,22 +2820,24 @@
         <v>63</v>
       </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="50" t="s">
+      <c r="E18" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="51" t="s">
+      <c r="H18" s="47" t="s">
         <v>222</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
-      <c r="L18" s="10"/>
+      <c r="L18" s="55" t="s">
+        <v>308</v>
+      </c>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="49" t="s">
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="45" t="s">
         <v>257</v>
       </c>
       <c r="B19" s="21" t="s">
@@ -2795,22 +2847,24 @@
         <v>196</v>
       </c>
       <c r="D19" s="7"/>
-      <c r="E19" s="50" t="s">
+      <c r="E19" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
-      <c r="H19" s="51" t="s">
+      <c r="H19" s="47" t="s">
         <v>222</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
-      <c r="L19" s="10"/>
+      <c r="L19" s="55" t="s">
+        <v>309</v>
+      </c>
       <c r="M19" s="10"/>
     </row>
-    <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="49" t="s">
+    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="45" t="s">
         <v>61</v>
       </c>
       <c r="B20" s="21" t="s">
@@ -2820,22 +2874,24 @@
         <v>66</v>
       </c>
       <c r="D20" s="7"/>
-      <c r="E20" s="50" t="s">
+      <c r="E20" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
-      <c r="H20" s="51" t="s">
+      <c r="H20" s="47" t="s">
         <v>222</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
-      <c r="L20" s="10"/>
+      <c r="L20" s="55" t="s">
+        <v>310</v>
+      </c>
       <c r="M20" s="10"/>
     </row>
-    <row r="21" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="s">
+    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="45" t="s">
         <v>64</v>
       </c>
       <c r="B21" s="21" t="s">
@@ -2845,22 +2901,24 @@
         <v>205</v>
       </c>
       <c r="D21" s="7"/>
-      <c r="E21" s="50" t="s">
+      <c r="E21" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="51" t="s">
+      <c r="H21" s="47" t="s">
         <v>222</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
-      <c r="L21" s="10"/>
+      <c r="L21" s="55" t="s">
+        <v>311</v>
+      </c>
       <c r="M21" s="10"/>
     </row>
     <row r="22" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="45" t="s">
         <v>67</v>
       </c>
       <c r="B22" s="21" t="s">
@@ -2872,7 +2930,7 @@
       <c r="D22" s="30" t="s">
         <v>241</v>
       </c>
-      <c r="E22" s="50" t="s">
+      <c r="E22" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F22" s="30" t="s">
@@ -2881,7 +2939,7 @@
       <c r="G22" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="H22" s="51" t="s">
+      <c r="H22" s="47" t="s">
         <v>223</v>
       </c>
       <c r="I22" s="7"/>
@@ -2891,7 +2949,7 @@
       <c r="M22" s="10"/>
     </row>
     <row r="23" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="45" t="s">
         <v>69</v>
       </c>
       <c r="B23" s="21" t="s">
@@ -2903,7 +2961,7 @@
       <c r="D23" s="30" t="s">
         <v>241</v>
       </c>
-      <c r="E23" s="50" t="s">
+      <c r="E23" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F23" s="30" t="s">
@@ -2912,7 +2970,7 @@
       <c r="G23" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="H23" s="51" t="s">
+      <c r="H23" s="47" t="s">
         <v>223</v>
       </c>
       <c r="I23" s="7"/>
@@ -2922,7 +2980,7 @@
       <c r="M23" s="10"/>
     </row>
     <row r="24" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="45" t="s">
         <v>258</v>
       </c>
       <c r="B24" s="21" t="s">
@@ -2934,7 +2992,7 @@
       <c r="D24" s="30" t="s">
         <v>253</v>
       </c>
-      <c r="E24" s="50" t="s">
+      <c r="E24" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F24" s="30" t="s">
@@ -2943,7 +3001,7 @@
       <c r="G24" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="H24" s="51" t="s">
+      <c r="H24" s="47" t="s">
         <v>223</v>
       </c>
       <c r="I24" s="7"/>
@@ -2953,7 +3011,7 @@
       <c r="M24" s="10"/>
     </row>
     <row r="25" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="45" t="s">
         <v>71</v>
       </c>
       <c r="B25" s="21" t="s">
@@ -2965,7 +3023,7 @@
       <c r="D25" s="30" t="s">
         <v>253</v>
       </c>
-      <c r="E25" s="50" t="s">
+      <c r="E25" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F25" s="30" t="s">
@@ -2974,7 +3032,7 @@
       <c r="G25" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="H25" s="51" t="s">
+      <c r="H25" s="47" t="s">
         <v>223</v>
       </c>
       <c r="I25" s="7"/>
@@ -2984,7 +3042,7 @@
       <c r="M25" s="10"/>
     </row>
     <row r="26" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="45" t="s">
         <v>74</v>
       </c>
       <c r="B26" s="21" t="s">
@@ -2996,7 +3054,7 @@
       <c r="D26" s="30" t="s">
         <v>253</v>
       </c>
-      <c r="E26" s="50" t="s">
+      <c r="E26" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F26" s="30" t="s">
@@ -3005,7 +3063,7 @@
       <c r="G26" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="H26" s="51" t="s">
+      <c r="H26" s="47" t="s">
         <v>223</v>
       </c>
       <c r="I26" s="7"/>
@@ -3015,7 +3073,7 @@
       <c r="M26" s="10"/>
     </row>
     <row r="27" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="45" t="s">
         <v>76</v>
       </c>
       <c r="B27" s="21" t="s">
@@ -3027,7 +3085,7 @@
       <c r="D27" s="30" t="s">
         <v>253</v>
       </c>
-      <c r="E27" s="50" t="s">
+      <c r="E27" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F27" s="30" t="s">
@@ -3036,7 +3094,7 @@
       <c r="G27" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="H27" s="51" t="s">
+      <c r="H27" s="47" t="s">
         <v>223</v>
       </c>
       <c r="I27" s="7"/>
@@ -3046,7 +3104,7 @@
       <c r="M27" s="10"/>
     </row>
     <row r="28" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="45" t="s">
         <v>78</v>
       </c>
       <c r="B28" s="21" t="s">
@@ -3058,7 +3116,7 @@
       <c r="D28" s="30" t="s">
         <v>253</v>
       </c>
-      <c r="E28" s="50" t="s">
+      <c r="E28" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F28" s="30" t="s">
@@ -3067,7 +3125,7 @@
       <c r="G28" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="H28" s="51" t="s">
+      <c r="H28" s="47" t="s">
         <v>223</v>
       </c>
       <c r="I28" s="7"/>
@@ -3077,7 +3135,7 @@
       <c r="M28" s="10"/>
     </row>
     <row r="29" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="45" t="s">
         <v>80</v>
       </c>
       <c r="B29" s="21" t="s">
@@ -3089,7 +3147,7 @@
       <c r="D29" s="30" t="s">
         <v>253</v>
       </c>
-      <c r="E29" s="50" t="s">
+      <c r="E29" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F29" s="30" t="s">
@@ -3098,7 +3156,7 @@
       <c r="G29" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="H29" s="51" t="s">
+      <c r="H29" s="47" t="s">
         <v>223</v>
       </c>
       <c r="I29" s="7"/>
@@ -3108,7 +3166,7 @@
       <c r="M29" s="10"/>
     </row>
     <row r="30" spans="1:13" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="48" t="s">
         <v>82</v>
       </c>
       <c r="B30" s="33" t="s">
@@ -3127,7 +3185,7 @@
       <c r="G30" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="H30" s="53" t="s">
+      <c r="H30" s="49" t="s">
         <v>223</v>
       </c>
       <c r="I30" s="29"/>
@@ -3137,7 +3195,7 @@
       <c r="M30" s="35"/>
     </row>
     <row r="31" spans="1:13" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="48" t="s">
         <v>84</v>
       </c>
       <c r="B31" s="33" t="s">
@@ -3156,7 +3214,7 @@
       <c r="G31" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="H31" s="53"/>
+      <c r="H31" s="49"/>
       <c r="I31" s="29"/>
       <c r="J31" s="29"/>
       <c r="K31" s="29"/>
@@ -3164,7 +3222,7 @@
       <c r="M31" s="35"/>
     </row>
     <row r="32" spans="1:13" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A32" s="52" t="s">
+      <c r="A32" s="48" t="s">
         <v>86</v>
       </c>
       <c r="B32" s="33" t="s">
@@ -3183,7 +3241,7 @@
       <c r="G32" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="H32" s="53"/>
+      <c r="H32" s="49"/>
       <c r="I32" s="29"/>
       <c r="J32" s="29"/>
       <c r="K32" s="29"/>
@@ -3191,7 +3249,7 @@
       <c r="M32" s="35"/>
     </row>
     <row r="33" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="45" t="s">
         <v>88</v>
       </c>
       <c r="B33" s="21" t="s">
@@ -3203,22 +3261,24 @@
       <c r="D33" s="30" t="s">
         <v>252</v>
       </c>
-      <c r="E33" s="50" t="s">
+      <c r="E33" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F33" s="22"/>
       <c r="G33" s="30"/>
-      <c r="H33" s="51" t="s">
+      <c r="H33" s="47" t="s">
         <v>223</v>
       </c>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
-      <c r="L33" s="10"/>
+      <c r="L33" s="55" t="s">
+        <v>312</v>
+      </c>
       <c r="M33" s="10"/>
     </row>
     <row r="34" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="49" t="s">
+      <c r="A34" s="45" t="s">
         <v>259</v>
       </c>
       <c r="B34" s="21" t="s">
@@ -3230,22 +3290,24 @@
       <c r="D34" s="30" t="s">
         <v>252</v>
       </c>
-      <c r="E34" s="50" t="s">
+      <c r="E34" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="30"/>
-      <c r="H34" s="51" t="s">
+      <c r="H34" s="47" t="s">
         <v>223</v>
       </c>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
-      <c r="L34" s="10"/>
+      <c r="L34" s="55" t="s">
+        <v>314</v>
+      </c>
       <c r="M34" s="10"/>
     </row>
     <row r="35" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="49" t="s">
+      <c r="A35" s="45" t="s">
         <v>260</v>
       </c>
       <c r="B35" s="21" t="s">
@@ -3257,22 +3319,24 @@
       <c r="D35" s="30" t="s">
         <v>252</v>
       </c>
-      <c r="E35" s="50" t="s">
+      <c r="E35" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="30"/>
-      <c r="H35" s="51" t="s">
+      <c r="H35" s="47" t="s">
         <v>223</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
-      <c r="L35" s="10"/>
+      <c r="L35" s="55" t="s">
+        <v>313</v>
+      </c>
       <c r="M35" s="10"/>
     </row>
     <row r="36" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="45" t="s">
         <v>261</v>
       </c>
       <c r="B36" s="21" t="s">
@@ -3284,22 +3348,24 @@
       <c r="D36" s="30" t="s">
         <v>252</v>
       </c>
-      <c r="E36" s="50" t="s">
+      <c r="E36" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F36" s="22"/>
       <c r="G36" s="30"/>
-      <c r="H36" s="51" t="s">
+      <c r="H36" s="47" t="s">
         <v>223</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
-      <c r="L36" s="10"/>
+      <c r="L36" s="55" t="s">
+        <v>315</v>
+      </c>
       <c r="M36" s="10"/>
     </row>
     <row r="37" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="49" t="s">
+      <c r="A37" s="45" t="s">
         <v>262</v>
       </c>
       <c r="B37" s="21" t="s">
@@ -3311,22 +3377,24 @@
       <c r="D37" s="30" t="s">
         <v>252</v>
       </c>
-      <c r="E37" s="50" t="s">
+      <c r="E37" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F37" s="22"/>
       <c r="G37" s="30"/>
-      <c r="H37" s="51" t="s">
+      <c r="H37" s="47" t="s">
         <v>223</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="10"/>
+      <c r="L37" s="55" t="s">
+        <v>317</v>
+      </c>
       <c r="M37" s="10"/>
     </row>
     <row r="38" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="45" t="s">
         <v>263</v>
       </c>
       <c r="B38" s="21" t="s">
@@ -3338,22 +3406,24 @@
       <c r="D38" s="30" t="s">
         <v>252</v>
       </c>
-      <c r="E38" s="50" t="s">
+      <c r="E38" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F38" s="22"/>
       <c r="G38" s="30"/>
-      <c r="H38" s="51" t="s">
+      <c r="H38" s="47" t="s">
         <v>223</v>
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
-      <c r="L38" s="10"/>
+      <c r="L38" s="55" t="s">
+        <v>316</v>
+      </c>
       <c r="M38" s="10"/>
     </row>
     <row r="39" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="49" t="s">
+      <c r="A39" s="45" t="s">
         <v>264</v>
       </c>
       <c r="B39" s="21" t="s">
@@ -3365,22 +3435,24 @@
       <c r="D39" s="30" t="s">
         <v>252</v>
       </c>
-      <c r="E39" s="50" t="s">
+      <c r="E39" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F39" s="22"/>
       <c r="G39" s="30"/>
-      <c r="H39" s="51" t="s">
+      <c r="H39" s="47" t="s">
         <v>223</v>
       </c>
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
-      <c r="L39" s="10"/>
+      <c r="L39" s="55" t="s">
+        <v>318</v>
+      </c>
       <c r="M39" s="10"/>
     </row>
     <row r="40" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="49" t="s">
+      <c r="A40" s="45" t="s">
         <v>265</v>
       </c>
       <c r="B40" s="21" t="s">
@@ -3392,22 +3464,24 @@
       <c r="D40" s="30" t="s">
         <v>252</v>
       </c>
-      <c r="E40" s="50" t="s">
+      <c r="E40" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F40" s="22"/>
       <c r="G40" s="30"/>
-      <c r="H40" s="51" t="s">
+      <c r="H40" s="47" t="s">
         <v>223</v>
       </c>
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
-      <c r="L40" s="10"/>
+      <c r="L40" s="55" t="s">
+        <v>319</v>
+      </c>
       <c r="M40" s="10"/>
     </row>
     <row r="41" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A41" s="49" t="s">
+      <c r="A41" s="45" t="s">
         <v>266</v>
       </c>
       <c r="B41" s="21" t="s">
@@ -3419,12 +3493,12 @@
       <c r="D41" s="30" t="s">
         <v>247</v>
       </c>
-      <c r="E41" s="50" t="s">
+      <c r="E41" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F41" s="30"/>
       <c r="G41" s="30"/>
-      <c r="H41" s="51" t="s">
+      <c r="H41" s="47" t="s">
         <v>224</v>
       </c>
       <c r="I41" s="7"/>
@@ -3434,7 +3508,7 @@
       <c r="M41" s="10"/>
     </row>
     <row r="42" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A42" s="49" t="s">
+      <c r="A42" s="45" t="s">
         <v>267</v>
       </c>
       <c r="B42" s="21" t="s">
@@ -3446,12 +3520,12 @@
       <c r="D42" s="30" t="s">
         <v>247</v>
       </c>
-      <c r="E42" s="50" t="s">
+      <c r="E42" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F42" s="30"/>
       <c r="G42" s="30"/>
-      <c r="H42" s="51" t="s">
+      <c r="H42" s="47" t="s">
         <v>224</v>
       </c>
       <c r="I42" s="7"/>
@@ -3461,7 +3535,7 @@
       <c r="M42" s="10"/>
     </row>
     <row r="43" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="45" t="s">
         <v>268</v>
       </c>
       <c r="B43" s="21" t="s">
@@ -3473,14 +3547,14 @@
       <c r="D43" s="30" t="s">
         <v>254</v>
       </c>
-      <c r="E43" s="50" t="s">
+      <c r="E43" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F43" s="30" t="s">
         <v>306</v>
       </c>
       <c r="G43" s="30"/>
-      <c r="H43" s="51" t="s">
+      <c r="H43" s="47" t="s">
         <v>225</v>
       </c>
       <c r="I43" s="7"/>
@@ -3490,7 +3564,7 @@
       <c r="M43" s="10"/>
     </row>
     <row r="44" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A44" s="49" t="s">
+      <c r="A44" s="45" t="s">
         <v>269</v>
       </c>
       <c r="B44" s="21" t="s">
@@ -3502,14 +3576,14 @@
       <c r="D44" s="30" t="s">
         <v>254</v>
       </c>
-      <c r="E44" s="50" t="s">
+      <c r="E44" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F44" s="30" t="s">
         <v>306</v>
       </c>
       <c r="G44" s="30"/>
-      <c r="H44" s="51" t="s">
+      <c r="H44" s="47" t="s">
         <v>225</v>
       </c>
       <c r="I44" s="7"/>
@@ -3519,7 +3593,7 @@
       <c r="M44" s="10"/>
     </row>
     <row r="45" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A45" s="49" t="s">
+      <c r="A45" s="45" t="s">
         <v>270</v>
       </c>
       <c r="B45" s="21" t="s">
@@ -3531,14 +3605,14 @@
       <c r="D45" s="30" t="s">
         <v>254</v>
       </c>
-      <c r="E45" s="50" t="s">
+      <c r="E45" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F45" s="30" t="s">
         <v>306</v>
       </c>
       <c r="G45" s="22"/>
-      <c r="H45" s="51" t="s">
+      <c r="H45" s="47" t="s">
         <v>225</v>
       </c>
       <c r="I45" s="7"/>
@@ -3548,7 +3622,7 @@
       <c r="M45" s="10"/>
     </row>
     <row r="46" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A46" s="49" t="s">
+      <c r="A46" s="45" t="s">
         <v>271</v>
       </c>
       <c r="B46" s="21" t="s">
@@ -3560,14 +3634,14 @@
       <c r="D46" s="30" t="s">
         <v>254</v>
       </c>
-      <c r="E46" s="50" t="s">
+      <c r="E46" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F46" s="30" t="s">
         <v>306</v>
       </c>
       <c r="G46" s="22"/>
-      <c r="H46" s="51" t="s">
+      <c r="H46" s="47" t="s">
         <v>225</v>
       </c>
       <c r="I46" s="7"/>
@@ -3577,7 +3651,7 @@
       <c r="M46" s="10"/>
     </row>
     <row r="47" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A47" s="49" t="s">
+      <c r="A47" s="45" t="s">
         <v>272</v>
       </c>
       <c r="B47" s="21" t="s">
@@ -3589,14 +3663,14 @@
       <c r="D47" s="30" t="s">
         <v>254</v>
       </c>
-      <c r="E47" s="50" t="s">
+      <c r="E47" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F47" s="30" t="s">
         <v>306</v>
       </c>
       <c r="G47" s="22"/>
-      <c r="H47" s="51" t="s">
+      <c r="H47" s="47" t="s">
         <v>225</v>
       </c>
       <c r="I47" s="7"/>
@@ -3606,7 +3680,7 @@
       <c r="M47" s="10"/>
     </row>
     <row r="48" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A48" s="49" t="s">
+      <c r="A48" s="45" t="s">
         <v>92</v>
       </c>
       <c r="B48" s="21" t="s">
@@ -3618,14 +3692,14 @@
       <c r="D48" s="30" t="s">
         <v>254</v>
       </c>
-      <c r="E48" s="50" t="s">
+      <c r="E48" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F48" s="30" t="s">
         <v>306</v>
       </c>
       <c r="G48" s="22"/>
-      <c r="H48" s="51" t="s">
+      <c r="H48" s="47" t="s">
         <v>225</v>
       </c>
       <c r="I48" s="7"/>
@@ -3635,7 +3709,7 @@
       <c r="M48" s="10"/>
     </row>
     <row r="49" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A49" s="49" t="s">
+      <c r="A49" s="45" t="s">
         <v>94</v>
       </c>
       <c r="B49" s="21" t="s">
@@ -3647,14 +3721,14 @@
       <c r="D49" s="30" t="s">
         <v>254</v>
       </c>
-      <c r="E49" s="50" t="s">
+      <c r="E49" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F49" s="30" t="s">
         <v>306</v>
       </c>
       <c r="G49" s="22"/>
-      <c r="H49" s="51" t="s">
+      <c r="H49" s="47" t="s">
         <v>225</v>
       </c>
       <c r="I49" s="7"/>
@@ -3664,7 +3738,7 @@
       <c r="M49" s="10"/>
     </row>
     <row r="50" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A50" s="49" t="s">
+      <c r="A50" s="45" t="s">
         <v>96</v>
       </c>
       <c r="B50" s="21" t="s">
@@ -3676,14 +3750,14 @@
       <c r="D50" s="30" t="s">
         <v>254</v>
       </c>
-      <c r="E50" s="50" t="s">
+      <c r="E50" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F50" s="30" t="s">
         <v>306</v>
       </c>
       <c r="G50" s="22"/>
-      <c r="H50" s="51" t="s">
+      <c r="H50" s="47" t="s">
         <v>225</v>
       </c>
       <c r="I50" s="7"/>
@@ -3693,7 +3767,7 @@
       <c r="M50" s="10"/>
     </row>
     <row r="51" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A51" s="49" t="s">
+      <c r="A51" s="45" t="s">
         <v>98</v>
       </c>
       <c r="B51" s="21" t="s">
@@ -3705,14 +3779,14 @@
       <c r="D51" s="30" t="s">
         <v>254</v>
       </c>
-      <c r="E51" s="50" t="s">
+      <c r="E51" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F51" s="30" t="s">
         <v>306</v>
       </c>
       <c r="G51" s="22"/>
-      <c r="H51" s="51" t="s">
+      <c r="H51" s="47" t="s">
         <v>225</v>
       </c>
       <c r="I51" s="7"/>
@@ -3722,7 +3796,7 @@
       <c r="M51" s="10"/>
     </row>
     <row r="52" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A52" s="49" t="s">
+      <c r="A52" s="45" t="s">
         <v>100</v>
       </c>
       <c r="B52" s="21" t="s">
@@ -3734,14 +3808,14 @@
       <c r="D52" s="30" t="s">
         <v>254</v>
       </c>
-      <c r="E52" s="50" t="s">
+      <c r="E52" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F52" s="30" t="s">
         <v>306</v>
       </c>
       <c r="G52" s="22"/>
-      <c r="H52" s="51" t="s">
+      <c r="H52" s="47" t="s">
         <v>225</v>
       </c>
       <c r="I52" s="7"/>
@@ -3751,7 +3825,7 @@
       <c r="M52" s="10"/>
     </row>
     <row r="53" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A53" s="49" t="s">
+      <c r="A53" s="45" t="s">
         <v>102</v>
       </c>
       <c r="B53" s="21" t="s">
@@ -3763,14 +3837,14 @@
       <c r="D53" s="30" t="s">
         <v>254</v>
       </c>
-      <c r="E53" s="50" t="s">
+      <c r="E53" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F53" s="30" t="s">
         <v>306</v>
       </c>
       <c r="G53" s="22"/>
-      <c r="H53" s="51" t="s">
+      <c r="H53" s="47" t="s">
         <v>225</v>
       </c>
       <c r="I53" s="7"/>
@@ -3780,7 +3854,7 @@
       <c r="M53" s="10"/>
     </row>
     <row r="54" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A54" s="49" t="s">
+      <c r="A54" s="45" t="s">
         <v>104</v>
       </c>
       <c r="B54" s="21" t="s">
@@ -3792,14 +3866,14 @@
       <c r="D54" s="30" t="s">
         <v>255</v>
       </c>
-      <c r="E54" s="50" t="s">
+      <c r="E54" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F54" s="30" t="s">
         <v>307</v>
       </c>
       <c r="G54" s="22"/>
-      <c r="H54" s="51" t="s">
+      <c r="H54" s="47" t="s">
         <v>226</v>
       </c>
       <c r="I54" s="7"/>
@@ -3809,7 +3883,7 @@
       <c r="M54" s="10"/>
     </row>
     <row r="55" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A55" s="49" t="s">
+      <c r="A55" s="45" t="s">
         <v>273</v>
       </c>
       <c r="B55" s="21" t="s">
@@ -3821,14 +3895,14 @@
       <c r="D55" s="30" t="s">
         <v>255</v>
       </c>
-      <c r="E55" s="50" t="s">
+      <c r="E55" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F55" s="30" t="s">
         <v>307</v>
       </c>
       <c r="G55" s="22"/>
-      <c r="H55" s="51" t="s">
+      <c r="H55" s="47" t="s">
         <v>226</v>
       </c>
       <c r="I55" s="7"/>
@@ -3838,7 +3912,7 @@
       <c r="M55" s="10"/>
     </row>
     <row r="56" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="49" t="s">
+      <c r="A56" s="45" t="s">
         <v>274</v>
       </c>
       <c r="B56" s="21" t="s">
@@ -3850,14 +3924,14 @@
       <c r="D56" s="30" t="s">
         <v>255</v>
       </c>
-      <c r="E56" s="50" t="s">
+      <c r="E56" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F56" s="30" t="s">
         <v>307</v>
       </c>
       <c r="G56" s="22"/>
-      <c r="H56" s="51" t="s">
+      <c r="H56" s="47" t="s">
         <v>226</v>
       </c>
       <c r="I56" s="7"/>
@@ -3867,7 +3941,7 @@
       <c r="M56" s="10"/>
     </row>
     <row r="57" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A57" s="49" t="s">
+      <c r="A57" s="45" t="s">
         <v>275</v>
       </c>
       <c r="B57" s="21" t="s">
@@ -3879,14 +3953,14 @@
       <c r="D57" s="30" t="s">
         <v>255</v>
       </c>
-      <c r="E57" s="50" t="s">
+      <c r="E57" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F57" s="30" t="s">
         <v>307</v>
       </c>
       <c r="G57" s="22"/>
-      <c r="H57" s="51" t="s">
+      <c r="H57" s="47" t="s">
         <v>226</v>
       </c>
       <c r="I57" s="7"/>
@@ -3896,7 +3970,7 @@
       <c r="M57" s="10"/>
     </row>
     <row r="58" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="49" t="s">
+      <c r="A58" s="45" t="s">
         <v>276</v>
       </c>
       <c r="B58" s="21" t="s">
@@ -3908,7 +3982,7 @@
       <c r="D58" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="E58" s="50" t="s">
+      <c r="E58" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F58" s="30" t="s">
@@ -3917,7 +3991,7 @@
       <c r="G58" s="30" t="s">
         <v>251</v>
       </c>
-      <c r="H58" s="51" t="s">
+      <c r="H58" s="47" t="s">
         <v>227</v>
       </c>
       <c r="I58" s="7"/>
@@ -3927,7 +4001,7 @@
       <c r="M58" s="10"/>
     </row>
     <row r="59" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="49" t="s">
+      <c r="A59" s="45" t="s">
         <v>277</v>
       </c>
       <c r="B59" s="21" t="s">
@@ -3939,7 +4013,7 @@
       <c r="D59" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="E59" s="50" t="s">
+      <c r="E59" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F59" s="30" t="s">
@@ -3948,7 +4022,7 @@
       <c r="G59" s="30" t="s">
         <v>251</v>
       </c>
-      <c r="H59" s="51" t="s">
+      <c r="H59" s="47" t="s">
         <v>227</v>
       </c>
       <c r="I59" s="7"/>
@@ -3958,7 +4032,7 @@
       <c r="M59" s="10"/>
     </row>
     <row r="60" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A60" s="49" t="s">
+      <c r="A60" s="45" t="s">
         <v>279</v>
       </c>
       <c r="B60" s="21" t="s">
@@ -3970,7 +4044,7 @@
       <c r="D60" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="E60" s="50" t="s">
+      <c r="E60" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F60" s="30" t="s">
@@ -3979,7 +4053,7 @@
       <c r="G60" s="30" t="s">
         <v>251</v>
       </c>
-      <c r="H60" s="51" t="s">
+      <c r="H60" s="47" t="s">
         <v>227</v>
       </c>
       <c r="I60" s="7"/>
@@ -3989,7 +4063,7 @@
       <c r="M60" s="10"/>
     </row>
     <row r="61" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A61" s="49" t="s">
+      <c r="A61" s="45" t="s">
         <v>280</v>
       </c>
       <c r="B61" s="21" t="s">
@@ -4001,7 +4075,7 @@
       <c r="D61" s="30" t="s">
         <v>250</v>
       </c>
-      <c r="E61" s="50" t="s">
+      <c r="E61" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F61" s="30" t="s">
@@ -4010,7 +4084,7 @@
       <c r="G61" s="30" t="s">
         <v>251</v>
       </c>
-      <c r="H61" s="51" t="s">
+      <c r="H61" s="47" t="s">
         <v>227</v>
       </c>
       <c r="I61" s="7"/>
@@ -4020,7 +4094,7 @@
       <c r="M61" s="10"/>
     </row>
     <row r="62" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A62" s="49" t="s">
+      <c r="A62" s="45" t="s">
         <v>281</v>
       </c>
       <c r="B62" s="21" t="s">
@@ -4030,12 +4104,12 @@
         <v>202</v>
       </c>
       <c r="D62" s="7"/>
-      <c r="E62" s="50" t="s">
+      <c r="E62" s="46" t="s">
         <v>237</v>
       </c>
       <c r="F62" s="22"/>
       <c r="G62" s="22"/>
-      <c r="H62" s="51" t="s">
+      <c r="H62" s="47" t="s">
         <v>222</v>
       </c>
       <c r="I62" s="7"/>
@@ -4045,7 +4119,7 @@
       <c r="M62" s="10"/>
     </row>
     <row r="63" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="49" t="s">
+      <c r="A63" s="45" t="s">
         <v>282</v>
       </c>
       <c r="B63" s="54"/>
@@ -4062,7 +4136,7 @@
       <c r="M63" s="10"/>
     </row>
     <row r="64" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A64" s="49" t="s">
+      <c r="A64" s="45" t="s">
         <v>283</v>
       </c>
       <c r="B64" s="54"/>
@@ -4079,7 +4153,7 @@
       <c r="M64" s="10"/>
     </row>
     <row r="65" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A65" s="49" t="s">
+      <c r="A65" s="45" t="s">
         <v>283</v>
       </c>
       <c r="B65" s="54"/>
@@ -4096,7 +4170,7 @@
       <c r="M65" s="10"/>
     </row>
     <row r="66" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A66" s="49" t="s">
+      <c r="A66" s="45" t="s">
         <v>284</v>
       </c>
       <c r="B66" s="54"/>
@@ -4113,7 +4187,7 @@
       <c r="M66" s="10"/>
     </row>
     <row r="67" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A67" s="49" t="s">
+      <c r="A67" s="45" t="s">
         <v>285</v>
       </c>
       <c r="B67" s="54"/>
@@ -4130,7 +4204,7 @@
       <c r="M67" s="10"/>
     </row>
     <row r="68" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A68" s="49" t="s">
+      <c r="A68" s="45" t="s">
         <v>286</v>
       </c>
       <c r="B68" s="54"/>
@@ -4147,7 +4221,7 @@
       <c r="M68" s="10"/>
     </row>
     <row r="69" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A69" s="49" t="s">
+      <c r="A69" s="45" t="s">
         <v>286</v>
       </c>
       <c r="B69" s="54"/>
@@ -4164,7 +4238,7 @@
       <c r="M69" s="10"/>
     </row>
     <row r="70" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A70" s="49" t="s">
+      <c r="A70" s="45" t="s">
         <v>287</v>
       </c>
       <c r="B70" s="54"/>
@@ -4181,7 +4255,7 @@
       <c r="M70" s="10"/>
     </row>
     <row r="71" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A71" s="49" t="s">
+      <c r="A71" s="45" t="s">
         <v>288</v>
       </c>
       <c r="B71" s="21"/>
@@ -4198,7 +4272,7 @@
       <c r="M71" s="10"/>
     </row>
     <row r="72" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A72" s="49" t="s">
+      <c r="A72" s="45" t="s">
         <v>289</v>
       </c>
       <c r="B72" s="21"/>
@@ -4215,7 +4289,7 @@
       <c r="M72" s="10"/>
     </row>
     <row r="73" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A73" s="49" t="s">
+      <c r="A73" s="45" t="s">
         <v>290</v>
       </c>
       <c r="B73" s="21"/>
@@ -4232,7 +4306,7 @@
       <c r="M73" s="10"/>
     </row>
     <row r="74" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A74" s="49" t="s">
+      <c r="A74" s="45" t="s">
         <v>291</v>
       </c>
       <c r="B74" s="21"/>
@@ -4249,7 +4323,7 @@
       <c r="M74" s="10"/>
     </row>
     <row r="75" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A75" s="49" t="s">
+      <c r="A75" s="45" t="s">
         <v>292</v>
       </c>
       <c r="B75" s="21"/>
@@ -4266,7 +4340,7 @@
       <c r="M75" s="10"/>
     </row>
     <row r="76" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A76" s="49" t="s">
+      <c r="A76" s="45" t="s">
         <v>293</v>
       </c>
       <c r="B76" s="21"/>
@@ -4283,7 +4357,7 @@
       <c r="M76" s="10"/>
     </row>
     <row r="77" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A77" s="49" t="s">
+      <c r="A77" s="45" t="s">
         <v>294</v>
       </c>
       <c r="B77" s="21"/>
@@ -4300,7 +4374,7 @@
       <c r="M77" s="10"/>
     </row>
     <row r="78" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A78" s="49" t="s">
+      <c r="A78" s="45" t="s">
         <v>295</v>
       </c>
       <c r="B78" s="21"/>
@@ -4317,7 +4391,7 @@
       <c r="M78" s="10"/>
     </row>
     <row r="79" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A79" s="49" t="s">
+      <c r="A79" s="45" t="s">
         <v>296</v>
       </c>
       <c r="B79" s="21"/>
@@ -4334,7 +4408,7 @@
       <c r="M79" s="10"/>
     </row>
     <row r="80" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A80" s="49" t="s">
+      <c r="A80" s="45" t="s">
         <v>297</v>
       </c>
       <c r="B80" s="21"/>
@@ -4351,7 +4425,7 @@
       <c r="M80" s="10"/>
     </row>
     <row r="81" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A81" s="49" t="s">
+      <c r="A81" s="45" t="s">
         <v>298</v>
       </c>
       <c r="B81" s="21"/>
@@ -4368,7 +4442,7 @@
       <c r="M81" s="10"/>
     </row>
     <row r="82" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A82" s="49" t="s">
+      <c r="A82" s="45" t="s">
         <v>299</v>
       </c>
       <c r="B82" s="21"/>
@@ -4385,7 +4459,7 @@
       <c r="M82" s="10"/>
     </row>
     <row r="83" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A83" s="49" t="s">
+      <c r="A83" s="45" t="s">
         <v>300</v>
       </c>
       <c r="B83" s="21"/>
@@ -4402,7 +4476,7 @@
       <c r="M83" s="10"/>
     </row>
     <row r="84" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A84" s="49" t="s">
+      <c r="A84" s="45" t="s">
         <v>301</v>
       </c>
       <c r="B84" s="21"/>
@@ -4419,7 +4493,7 @@
       <c r="M84" s="10"/>
     </row>
     <row r="85" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A85" s="49" t="s">
+      <c r="A85" s="45" t="s">
         <v>302</v>
       </c>
       <c r="B85" s="21"/>
@@ -4436,7 +4510,7 @@
       <c r="M85" s="10"/>
     </row>
     <row r="86" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A86" s="49" t="s">
+      <c r="A86" s="45" t="s">
         <v>120</v>
       </c>
       <c r="B86" s="21"/>
@@ -4453,7 +4527,7 @@
       <c r="M86" s="10"/>
     </row>
     <row r="87" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A87" s="49" t="s">
+      <c r="A87" s="45" t="s">
         <v>121</v>
       </c>
       <c r="B87" s="21"/>
@@ -4470,7 +4544,7 @@
       <c r="M87" s="10"/>
     </row>
     <row r="88" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A88" s="49" t="s">
+      <c r="A88" s="45" t="s">
         <v>122</v>
       </c>
       <c r="B88" s="21"/>
@@ -4487,7 +4561,7 @@
       <c r="M88" s="10"/>
     </row>
     <row r="89" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A89" s="49" t="s">
+      <c r="A89" s="45" t="s">
         <v>123</v>
       </c>
       <c r="B89" s="21"/>
@@ -4504,7 +4578,7 @@
       <c r="M89" s="10"/>
     </row>
     <row r="90" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A90" s="49" t="s">
+      <c r="A90" s="45" t="s">
         <v>124</v>
       </c>
       <c r="B90" s="21"/>
@@ -4521,7 +4595,7 @@
       <c r="M90" s="10"/>
     </row>
     <row r="91" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A91" s="49" t="s">
+      <c r="A91" s="45" t="s">
         <v>125</v>
       </c>
       <c r="B91" s="21"/>
@@ -4538,7 +4612,7 @@
       <c r="M91" s="10"/>
     </row>
     <row r="92" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A92" s="49" t="s">
+      <c r="A92" s="45" t="s">
         <v>126</v>
       </c>
       <c r="B92" s="21"/>
@@ -4555,7 +4629,7 @@
       <c r="M92" s="10"/>
     </row>
     <row r="93" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A93" s="49" t="s">
+      <c r="A93" s="45" t="s">
         <v>127</v>
       </c>
       <c r="B93" s="21"/>
@@ -4572,7 +4646,7 @@
       <c r="M93" s="10"/>
     </row>
     <row r="94" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A94" s="49" t="s">
+      <c r="A94" s="45" t="s">
         <v>128</v>
       </c>
       <c r="B94" s="21"/>
@@ -4589,7 +4663,7 @@
       <c r="M94" s="10"/>
     </row>
     <row r="95" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A95" s="49" t="s">
+      <c r="A95" s="45" t="s">
         <v>129</v>
       </c>
       <c r="B95" s="21"/>
@@ -4606,7 +4680,7 @@
       <c r="M95" s="10"/>
     </row>
     <row r="96" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A96" s="49" t="s">
+      <c r="A96" s="45" t="s">
         <v>130</v>
       </c>
       <c r="B96" s="21"/>
@@ -4623,7 +4697,7 @@
       <c r="M96" s="10"/>
     </row>
     <row r="97" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A97" s="49" t="s">
+      <c r="A97" s="45" t="s">
         <v>131</v>
       </c>
       <c r="B97" s="21"/>
@@ -4640,7 +4714,7 @@
       <c r="M97" s="10"/>
     </row>
     <row r="98" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A98" s="49" t="s">
+      <c r="A98" s="45" t="s">
         <v>132</v>
       </c>
       <c r="B98" s="21"/>
@@ -4657,7 +4731,7 @@
       <c r="M98" s="10"/>
     </row>
     <row r="99" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A99" s="49" t="s">
+      <c r="A99" s="45" t="s">
         <v>133</v>
       </c>
       <c r="B99" s="21"/>
@@ -4674,7 +4748,7 @@
       <c r="M99" s="10"/>
     </row>
     <row r="100" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A100" s="49" t="s">
+      <c r="A100" s="45" t="s">
         <v>134</v>
       </c>
       <c r="B100" s="21"/>
@@ -4691,7 +4765,7 @@
       <c r="M100" s="10"/>
     </row>
     <row r="101" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A101" s="49" t="s">
+      <c r="A101" s="45" t="s">
         <v>135</v>
       </c>
       <c r="B101" s="21"/>
@@ -4708,7 +4782,7 @@
       <c r="M101" s="10"/>
     </row>
     <row r="102" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A102" s="49" t="s">
+      <c r="A102" s="45" t="s">
         <v>136</v>
       </c>
       <c r="B102" s="21"/>
@@ -4725,7 +4799,7 @@
       <c r="M102" s="10"/>
     </row>
     <row r="103" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A103" s="49" t="s">
+      <c r="A103" s="45" t="s">
         <v>137</v>
       </c>
       <c r="B103" s="21"/>
@@ -4742,7 +4816,7 @@
       <c r="M103" s="10"/>
     </row>
     <row r="104" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A104" s="49" t="s">
+      <c r="A104" s="45" t="s">
         <v>138</v>
       </c>
       <c r="B104" s="21"/>
@@ -4759,7 +4833,7 @@
       <c r="M104" s="10"/>
     </row>
     <row r="105" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A105" s="49" t="s">
+      <c r="A105" s="45" t="s">
         <v>139</v>
       </c>
       <c r="B105" s="21"/>
@@ -4776,7 +4850,7 @@
       <c r="M105" s="10"/>
     </row>
     <row r="106" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A106" s="49" t="s">
+      <c r="A106" s="45" t="s">
         <v>140</v>
       </c>
       <c r="B106" s="21"/>
@@ -4793,7 +4867,7 @@
       <c r="M106" s="10"/>
     </row>
     <row r="107" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A107" s="49" t="s">
+      <c r="A107" s="45" t="s">
         <v>141</v>
       </c>
       <c r="B107" s="21"/>
@@ -4810,7 +4884,7 @@
       <c r="M107" s="10"/>
     </row>
     <row r="108" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A108" s="49" t="s">
+      <c r="A108" s="45" t="s">
         <v>142</v>
       </c>
       <c r="B108" s="21"/>
@@ -4827,7 +4901,7 @@
       <c r="M108" s="10"/>
     </row>
     <row r="109" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A109" s="49" t="s">
+      <c r="A109" s="45" t="s">
         <v>143</v>
       </c>
       <c r="B109" s="21"/>
@@ -4844,7 +4918,7 @@
       <c r="M109" s="10"/>
     </row>
     <row r="110" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A110" s="49" t="s">
+      <c r="A110" s="45" t="s">
         <v>144</v>
       </c>
       <c r="B110" s="21"/>
@@ -4861,7 +4935,7 @@
       <c r="M110" s="10"/>
     </row>
     <row r="111" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A111" s="49" t="s">
+      <c r="A111" s="45" t="s">
         <v>145</v>
       </c>
       <c r="B111" s="21"/>
@@ -4878,7 +4952,7 @@
       <c r="M111" s="10"/>
     </row>
     <row r="112" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A112" s="49" t="s">
+      <c r="A112" s="45" t="s">
         <v>146</v>
       </c>
       <c r="B112" s="21"/>
@@ -4895,7 +4969,7 @@
       <c r="M112" s="10"/>
     </row>
     <row r="113" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A113" s="49" t="s">
+      <c r="A113" s="45" t="s">
         <v>147</v>
       </c>
       <c r="B113" s="21"/>
@@ -4912,7 +4986,7 @@
       <c r="M113" s="10"/>
     </row>
     <row r="114" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A114" s="49" t="s">
+      <c r="A114" s="45" t="s">
         <v>148</v>
       </c>
       <c r="B114" s="21"/>
@@ -4929,7 +5003,7 @@
       <c r="M114" s="10"/>
     </row>
     <row r="115" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A115" s="49" t="s">
+      <c r="A115" s="45" t="s">
         <v>149</v>
       </c>
       <c r="B115" s="21"/>
@@ -4946,7 +5020,7 @@
       <c r="M115" s="10"/>
     </row>
     <row r="116" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A116" s="49" t="s">
+      <c r="A116" s="45" t="s">
         <v>150</v>
       </c>
       <c r="B116" s="21"/>
@@ -4963,7 +5037,7 @@
       <c r="M116" s="10"/>
     </row>
     <row r="117" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A117" s="49" t="s">
+      <c r="A117" s="45" t="s">
         <v>151</v>
       </c>
       <c r="B117" s="21"/>
@@ -4980,7 +5054,7 @@
       <c r="M117" s="10"/>
     </row>
     <row r="118" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A118" s="49" t="s">
+      <c r="A118" s="45" t="s">
         <v>152</v>
       </c>
       <c r="B118" s="21"/>
@@ -4997,7 +5071,7 @@
       <c r="M118" s="10"/>
     </row>
     <row r="119" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A119" s="49" t="s">
+      <c r="A119" s="45" t="s">
         <v>153</v>
       </c>
       <c r="B119" s="21"/>
@@ -5014,7 +5088,7 @@
       <c r="M119" s="10"/>
     </row>
     <row r="120" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A120" s="49" t="s">
+      <c r="A120" s="45" t="s">
         <v>154</v>
       </c>
       <c r="B120" s="21"/>
@@ -5031,7 +5105,7 @@
       <c r="M120" s="10"/>
     </row>
     <row r="121" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A121" s="49" t="s">
+      <c r="A121" s="45" t="s">
         <v>155</v>
       </c>
       <c r="B121" s="21"/>
@@ -5048,7 +5122,7 @@
       <c r="M121" s="10"/>
     </row>
     <row r="122" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A122" s="49" t="s">
+      <c r="A122" s="45" t="s">
         <v>156</v>
       </c>
       <c r="B122" s="21"/>
@@ -5065,7 +5139,7 @@
       <c r="M122" s="10"/>
     </row>
     <row r="123" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A123" s="49" t="s">
+      <c r="A123" s="45" t="s">
         <v>157</v>
       </c>
       <c r="B123" s="21"/>
@@ -5082,7 +5156,7 @@
       <c r="M123" s="10"/>
     </row>
     <row r="124" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A124" s="49" t="s">
+      <c r="A124" s="45" t="s">
         <v>158</v>
       </c>
       <c r="B124" s="21"/>
@@ -5099,7 +5173,7 @@
       <c r="M124" s="10"/>
     </row>
     <row r="125" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A125" s="49" t="s">
+      <c r="A125" s="45" t="s">
         <v>159</v>
       </c>
       <c r="B125" s="21"/>
@@ -5116,7 +5190,7 @@
       <c r="M125" s="10"/>
     </row>
     <row r="126" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A126" s="49" t="s">
+      <c r="A126" s="45" t="s">
         <v>160</v>
       </c>
       <c r="B126" s="21"/>
@@ -5133,7 +5207,7 @@
       <c r="M126" s="10"/>
     </row>
     <row r="127" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A127" s="49" t="s">
+      <c r="A127" s="45" t="s">
         <v>161</v>
       </c>
       <c r="B127" s="21"/>
@@ -5150,7 +5224,7 @@
       <c r="M127" s="10"/>
     </row>
     <row r="128" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A128" s="49" t="s">
+      <c r="A128" s="45" t="s">
         <v>162</v>
       </c>
       <c r="B128" s="21"/>
@@ -5167,7 +5241,7 @@
       <c r="M128" s="10"/>
     </row>
     <row r="129" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A129" s="49" t="s">
+      <c r="A129" s="45" t="s">
         <v>163</v>
       </c>
       <c r="B129" s="21"/>
@@ -5184,7 +5258,7 @@
       <c r="M129" s="10"/>
     </row>
     <row r="130" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A130" s="49" t="s">
+      <c r="A130" s="45" t="s">
         <v>164</v>
       </c>
       <c r="B130" s="21"/>
@@ -5201,7 +5275,7 @@
       <c r="M130" s="10"/>
     </row>
     <row r="131" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A131" s="49" t="s">
+      <c r="A131" s="45" t="s">
         <v>165</v>
       </c>
       <c r="B131" s="21"/>
@@ -5218,7 +5292,7 @@
       <c r="M131" s="10"/>
     </row>
     <row r="132" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A132" s="49" t="s">
+      <c r="A132" s="45" t="s">
         <v>166</v>
       </c>
       <c r="B132" s="21"/>
@@ -5235,7 +5309,7 @@
       <c r="M132" s="10"/>
     </row>
     <row r="133" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A133" s="49" t="s">
+      <c r="A133" s="45" t="s">
         <v>167</v>
       </c>
       <c r="B133" s="21"/>
@@ -5252,7 +5326,7 @@
       <c r="M133" s="10"/>
     </row>
     <row r="134" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A134" s="49" t="s">
+      <c r="A134" s="45" t="s">
         <v>168</v>
       </c>
       <c r="B134" s="21"/>
@@ -5269,7 +5343,7 @@
       <c r="M134" s="10"/>
     </row>
     <row r="135" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A135" s="49" t="s">
+      <c r="A135" s="45" t="s">
         <v>169</v>
       </c>
       <c r="B135" s="21"/>
@@ -5286,7 +5360,7 @@
       <c r="M135" s="10"/>
     </row>
     <row r="136" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A136" s="49" t="s">
+      <c r="A136" s="45" t="s">
         <v>170</v>
       </c>
       <c r="B136" s="21"/>
@@ -5303,7 +5377,7 @@
       <c r="M136" s="10"/>
     </row>
     <row r="137" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A137" s="49" t="s">
+      <c r="A137" s="45" t="s">
         <v>171</v>
       </c>
       <c r="B137" s="21"/>
@@ -5320,7 +5394,7 @@
       <c r="M137" s="10"/>
     </row>
     <row r="138" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A138" s="49" t="s">
+      <c r="A138" s="45" t="s">
         <v>172</v>
       </c>
       <c r="B138" s="21"/>
@@ -5337,7 +5411,7 @@
       <c r="M138" s="10"/>
     </row>
     <row r="139" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A139" s="49" t="s">
+      <c r="A139" s="45" t="s">
         <v>173</v>
       </c>
       <c r="B139" s="21"/>
@@ -5354,7 +5428,7 @@
       <c r="M139" s="10"/>
     </row>
     <row r="140" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A140" s="49" t="s">
+      <c r="A140" s="45" t="s">
         <v>174</v>
       </c>
       <c r="B140" s="21"/>
@@ -5371,7 +5445,7 @@
       <c r="M140" s="10"/>
     </row>
     <row r="141" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A141" s="49" t="s">
+      <c r="A141" s="45" t="s">
         <v>175</v>
       </c>
       <c r="B141" s="21"/>
@@ -5388,7 +5462,7 @@
       <c r="M141" s="10"/>
     </row>
     <row r="142" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A142" s="49" t="s">
+      <c r="A142" s="45" t="s">
         <v>176</v>
       </c>
       <c r="B142" s="21"/>
@@ -5405,7 +5479,7 @@
       <c r="M142" s="10"/>
     </row>
     <row r="143" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A143" s="49" t="s">
+      <c r="A143" s="45" t="s">
         <v>177</v>
       </c>
       <c r="B143" s="21"/>
@@ -5422,7 +5496,7 @@
       <c r="M143" s="10"/>
     </row>
     <row r="144" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A144" s="49" t="s">
+      <c r="A144" s="45" t="s">
         <v>178</v>
       </c>
       <c r="B144" s="21"/>
@@ -5439,7 +5513,7 @@
       <c r="M144" s="10"/>
     </row>
     <row r="145" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A145" s="49" t="s">
+      <c r="A145" s="45" t="s">
         <v>179</v>
       </c>
       <c r="B145" s="21"/>
@@ -5456,7 +5530,7 @@
       <c r="M145" s="10"/>
     </row>
     <row r="146" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A146" s="49" t="s">
+      <c r="A146" s="45" t="s">
         <v>180</v>
       </c>
       <c r="B146" s="21"/>
@@ -5473,7 +5547,7 @@
       <c r="M146" s="10"/>
     </row>
     <row r="147" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A147" s="49" t="s">
+      <c r="A147" s="45" t="s">
         <v>181</v>
       </c>
       <c r="B147" s="21"/>
@@ -5490,7 +5564,7 @@
       <c r="M147" s="10"/>
     </row>
     <row r="148" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A148" s="49" t="s">
+      <c r="A148" s="45" t="s">
         <v>182</v>
       </c>
       <c r="B148" s="21"/>
@@ -5507,7 +5581,7 @@
       <c r="M148" s="10"/>
     </row>
     <row r="149" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A149" s="49" t="s">
+      <c r="A149" s="45" t="s">
         <v>183</v>
       </c>
       <c r="B149" s="21"/>
@@ -5524,7 +5598,7 @@
       <c r="M149" s="10"/>
     </row>
     <row r="150" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A150" s="49" t="s">
+      <c r="A150" s="45" t="s">
         <v>184</v>
       </c>
       <c r="B150" s="21"/>
@@ -5541,7 +5615,7 @@
       <c r="M150" s="10"/>
     </row>
     <row r="151" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A151" s="49" t="s">
+      <c r="A151" s="45" t="s">
         <v>185</v>
       </c>
       <c r="B151" s="21"/>
@@ -5558,7 +5632,7 @@
       <c r="M151" s="10"/>
     </row>
     <row r="152" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A152" s="49" t="s">
+      <c r="A152" s="45" t="s">
         <v>186</v>
       </c>
       <c r="B152" s="21"/>
@@ -5575,7 +5649,7 @@
       <c r="M152" s="10"/>
     </row>
     <row r="153" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A153" s="49" t="s">
+      <c r="A153" s="45" t="s">
         <v>187</v>
       </c>
       <c r="B153" s="21"/>
@@ -5592,7 +5666,7 @@
       <c r="M153" s="10"/>
     </row>
     <row r="154" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A154" s="49" t="s">
+      <c r="A154" s="45" t="s">
         <v>188</v>
       </c>
       <c r="B154" s="21"/>
@@ -5609,7 +5683,7 @@
       <c r="M154" s="10"/>
     </row>
     <row r="155" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A155" s="49" t="s">
+      <c r="A155" s="45" t="s">
         <v>189</v>
       </c>
       <c r="B155" s="21"/>
@@ -5626,7 +5700,7 @@
       <c r="M155" s="10"/>
     </row>
     <row r="156" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A156" s="49" t="s">
+      <c r="A156" s="45" t="s">
         <v>190</v>
       </c>
       <c r="B156" s="21"/>
@@ -5643,7 +5717,7 @@
       <c r="M156" s="10"/>
     </row>
     <row r="157" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A157" s="49" t="s">
+      <c r="A157" s="45" t="s">
         <v>191</v>
       </c>
       <c r="B157" s="21"/>
@@ -5660,7 +5734,7 @@
       <c r="M157" s="10"/>
     </row>
     <row r="158" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A158" s="49" t="s">
+      <c r="A158" s="45" t="s">
         <v>192</v>
       </c>
       <c r="B158" s="21"/>
@@ -5677,7 +5751,7 @@
       <c r="M158" s="10"/>
     </row>
     <row r="159" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A159" s="49" t="s">
+      <c r="A159" s="45" t="s">
         <v>193</v>
       </c>
       <c r="B159" s="21"/>
@@ -5694,7 +5768,7 @@
       <c r="M159" s="10"/>
     </row>
     <row r="160" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A160" s="49" t="s">
+      <c r="A160" s="45" t="s">
         <v>194</v>
       </c>
       <c r="B160" s="21"/>
@@ -5711,7 +5785,7 @@
       <c r="M160" s="10"/>
     </row>
     <row r="161" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A161" s="49" t="s">
+      <c r="A161" s="45" t="s">
         <v>195</v>
       </c>
       <c r="B161" s="21"/>
@@ -5728,7 +5802,7 @@
       <c r="M161" s="10"/>
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G162" s="40"/>
+      <c r="G162" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
update RTM with navigate and delete TCs
</commit_message>
<xml_diff>
--- a/RTM/Traceability_Matrix learning hub ver 2.xlsx
+++ b/RTM/Traceability_Matrix learning hub ver 2.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed Mazrouaa\Documents\GitHub\learning-hub\RTM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC015464-71F4-4CB1-8A09-E840696A4DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" state="hidden" r:id="rId1"/>
@@ -26,12 +20,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>eze3</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="A5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +46,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -115,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -136,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="J5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -157,7 +151,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="K5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -178,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="L5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -204,7 +198,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="347">
   <si>
     <t>For detail regarding the practice of Requirements Management, please refer to the Requirements Management Practices Guide</t>
   </si>
@@ -1640,15 +1634,55 @@
 TC_LearningHub_Add_013
 TC_LearningHub_Add_014</t>
   </si>
+  <si>
+    <t>TC_LearningHub_DELETE _001 -004</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_DELETE _009 -012</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_DELETE _005 -008</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_DELETE _013 -016</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_DELETE _021 -024</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_DELETE _017 -020</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_DELETE _025 -026</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_DELETE _027</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_NAV_001 -003 
+TC_LearningHub_NAV_008 -10</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_NAV_004
+TC_LearningHub_NAV_011</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_NAV_005 -006
+TC_LearningHub_NAV_012 - 013</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_NAV_007
+TC_LearningHub_NAV_014</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1772,6 +1806,13 @@
       <sz val="8"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1952,7 +1993,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2053,13 +2094,13 @@
     <xf numFmtId="49" fontId="14" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2095,6 +2136,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2110,10 +2155,9 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2465,32 +2509,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B20"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="41" customWidth="1"/>
-    <col min="2" max="2" width="58.88671875" style="42" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="42"/>
+    <col min="1" max="1" width="5.28515625" style="41" customWidth="1"/>
+    <col min="2" max="2" width="58.85546875" style="42" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="42"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="26.4">
+    <row r="2" spans="1:2" ht="38.25">
       <c r="B2" s="43" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6">
-      <c r="A4" s="50" t="s">
+    <row r="4" spans="1:2" ht="15.75">
+      <c r="A4" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="51"/>
-    </row>
-    <row r="5" spans="1:2" ht="26.4">
+      <c r="B4" s="53"/>
+    </row>
+    <row r="5" spans="1:2" ht="25.5">
       <c r="A5" s="44" t="s">
         <v>2</v>
       </c>
@@ -2506,72 +2550,72 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="26.4">
+    <row r="7" spans="1:2" ht="25.5">
       <c r="B7" s="48" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="39.6">
+    <row r="8" spans="1:2" ht="38.25">
       <c r="B8" s="48" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="39.6">
+    <row r="9" spans="1:2" ht="51">
       <c r="B9" s="48" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="26.4">
+    <row r="10" spans="1:2" ht="25.5">
       <c r="B10" s="48" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="26.4">
+    <row r="11" spans="1:2" ht="25.5">
       <c r="B11" s="48" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="39.6">
+    <row r="12" spans="1:2" ht="38.25">
       <c r="B12" s="48" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="39.6">
+    <row r="13" spans="1:2" ht="38.25">
       <c r="B13" s="48" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="39.6">
+    <row r="14" spans="1:2" ht="38.25">
       <c r="B14" s="48" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="39.6">
+    <row r="15" spans="1:2" ht="38.25">
       <c r="B15" s="48" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="26.4">
+    <row r="16" spans="1:2" ht="25.5">
       <c r="B16" s="48" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="26.4">
+    <row r="17" spans="2:2" ht="25.5">
       <c r="B17" s="48" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="26.4">
+    <row r="18" spans="2:2" ht="38.25">
       <c r="B18" s="48" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="26.4">
+    <row r="19" spans="2:2" ht="38.25">
       <c r="B19" s="48" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="26.4">
+    <row r="20" spans="2:2" ht="25.5">
       <c r="B20" s="49" t="s">
         <v>19</v>
       </c>
@@ -2587,31 +2631,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="29.5546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="35.88671875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="55.6640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="29.109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="47.33203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="47.33203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="55.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="47.28515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="47.28515625" style="7" customWidth="1"/>
     <col min="8" max="8" width="51" style="6" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="8" customWidth="1"/>
     <col min="12" max="12" width="34" style="9" customWidth="1"/>
     <col min="13" max="13" width="86" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="29.4" customHeight="1">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="29.45" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>20</v>
       </c>
@@ -2630,40 +2674,40 @@
       <c r="L1" s="11"/>
       <c r="M1" s="11"/>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" ht="23.4" customHeight="1">
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="23.45" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="12"/>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
       <c r="K2" s="32"/>
       <c r="L2" s="32"/>
       <c r="M2" s="33"/>
     </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" ht="17.399999999999999" customHeight="1">
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="17.45" customHeight="1">
       <c r="A3" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="12"/>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
       <c r="K3" s="32"/>
       <c r="L3" s="32"/>
       <c r="M3" s="33"/>
@@ -2673,21 +2717,21 @@
         <v>25</v>
       </c>
       <c r="B4" s="12"/>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
       <c r="K4" s="32"/>
       <c r="L4" s="32"/>
       <c r="M4" s="34"/>
     </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" ht="27.6">
+    <row r="5" spans="1:13" s="3" customFormat="1" ht="30">
       <c r="A5" s="13" t="s">
         <v>27</v>
       </c>
@@ -2761,7 +2805,7 @@
       </c>
       <c r="M6" s="37"/>
     </row>
-    <row r="7" spans="1:13" ht="17.399999999999999">
+    <row r="7" spans="1:13" ht="18">
       <c r="A7" s="15" t="s">
         <v>49</v>
       </c>
@@ -2794,7 +2838,7 @@
       </c>
       <c r="M7" s="37"/>
     </row>
-    <row r="8" spans="1:13" ht="17.399999999999999">
+    <row r="8" spans="1:13" ht="18">
       <c r="A8" s="15" t="s">
         <v>51</v>
       </c>
@@ -2827,7 +2871,7 @@
       </c>
       <c r="M8" s="37"/>
     </row>
-    <row r="9" spans="1:13" ht="17.399999999999999">
+    <row r="9" spans="1:13" ht="18">
       <c r="A9" s="15" t="s">
         <v>54</v>
       </c>
@@ -2858,7 +2902,7 @@
       </c>
       <c r="M9" s="37"/>
     </row>
-    <row r="10" spans="1:13" ht="17.399999999999999">
+    <row r="10" spans="1:13" ht="18">
       <c r="A10" s="15" t="s">
         <v>58</v>
       </c>
@@ -2891,7 +2935,7 @@
       </c>
       <c r="M10" s="37"/>
     </row>
-    <row r="11" spans="1:13" ht="17.399999999999999">
+    <row r="11" spans="1:13" ht="18">
       <c r="A11" s="15" t="s">
         <v>63</v>
       </c>
@@ -2924,7 +2968,7 @@
       </c>
       <c r="M11" s="37"/>
     </row>
-    <row r="12" spans="1:13" ht="17.399999999999999">
+    <row r="12" spans="1:13" ht="18">
       <c r="A12" s="15" t="s">
         <v>66</v>
       </c>
@@ -2957,7 +3001,7 @@
       </c>
       <c r="M12" s="37"/>
     </row>
-    <row r="13" spans="1:13" ht="17.399999999999999">
+    <row r="13" spans="1:13" ht="18">
       <c r="A13" s="15" t="s">
         <v>69</v>
       </c>
@@ -3108,7 +3152,7 @@
       <c r="L17" s="36"/>
       <c r="M17" s="37"/>
     </row>
-    <row r="18" spans="1:13" ht="17.399999999999999">
+    <row r="18" spans="1:13" ht="30">
       <c r="A18" s="15" t="s">
         <v>86</v>
       </c>
@@ -3130,10 +3174,12 @@
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
-      <c r="L18" s="36"/>
+      <c r="L18" s="57" t="s">
+        <v>343</v>
+      </c>
       <c r="M18" s="37"/>
     </row>
-    <row r="19" spans="1:13" ht="17.399999999999999">
+    <row r="19" spans="1:13" ht="30">
       <c r="A19" s="15" t="s">
         <v>90</v>
       </c>
@@ -3155,10 +3201,12 @@
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
-      <c r="L19" s="36"/>
+      <c r="L19" s="57" t="s">
+        <v>344</v>
+      </c>
       <c r="M19" s="37"/>
     </row>
-    <row r="20" spans="1:13" ht="17.399999999999999">
+    <row r="20" spans="1:13" ht="30">
       <c r="A20" s="15" t="s">
         <v>93</v>
       </c>
@@ -3180,10 +3228,12 @@
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
-      <c r="L20" s="36"/>
+      <c r="L20" s="57" t="s">
+        <v>345</v>
+      </c>
       <c r="M20" s="37"/>
     </row>
-    <row r="21" spans="1:13" ht="17.399999999999999">
+    <row r="21" spans="1:13" ht="30">
       <c r="A21" s="15" t="s">
         <v>96</v>
       </c>
@@ -3205,10 +3255,12 @@
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
-      <c r="L21" s="36"/>
+      <c r="L21" s="57" t="s">
+        <v>346</v>
+      </c>
       <c r="M21" s="37"/>
     </row>
-    <row r="22" spans="1:13" ht="83.4" customHeight="1">
+    <row r="22" spans="1:13" ht="83.45" customHeight="1">
       <c r="A22" s="15" t="s">
         <v>99</v>
       </c>
@@ -3236,7 +3288,7 @@
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
-      <c r="L22" s="55" t="s">
+      <c r="L22" s="50" t="s">
         <v>330</v>
       </c>
       <c r="M22" s="37"/>
@@ -3302,12 +3354,12 @@
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
-      <c r="L24" s="55" t="s">
+      <c r="L24" s="50" t="s">
         <v>331</v>
       </c>
       <c r="M24" s="37"/>
     </row>
-    <row r="25" spans="1:13" ht="17.399999999999999">
+    <row r="25" spans="1:13" ht="18">
       <c r="A25" s="15" t="s">
         <v>112</v>
       </c>
@@ -3340,7 +3392,7 @@
       </c>
       <c r="M25" s="37"/>
     </row>
-    <row r="26" spans="1:13" ht="17.399999999999999">
+    <row r="26" spans="1:13" ht="18">
       <c r="A26" s="15" t="s">
         <v>115</v>
       </c>
@@ -3373,7 +3425,7 @@
       </c>
       <c r="M26" s="37"/>
     </row>
-    <row r="27" spans="1:13" ht="79.2">
+    <row r="27" spans="1:13" ht="76.5">
       <c r="A27" s="15" t="s">
         <v>118</v>
       </c>
@@ -3401,12 +3453,12 @@
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
-      <c r="L27" s="55" t="s">
+      <c r="L27" s="50" t="s">
         <v>331</v>
       </c>
       <c r="M27" s="37"/>
     </row>
-    <row r="28" spans="1:13" ht="17.399999999999999">
+    <row r="28" spans="1:13" ht="18">
       <c r="A28" s="15" t="s">
         <v>120</v>
       </c>
@@ -3439,7 +3491,7 @@
       </c>
       <c r="M28" s="37"/>
     </row>
-    <row r="29" spans="1:13" ht="17.399999999999999">
+    <row r="29" spans="1:13" ht="18">
       <c r="A29" s="15" t="s">
         <v>122</v>
       </c>
@@ -3472,11 +3524,11 @@
       </c>
       <c r="M29" s="37"/>
     </row>
-    <row r="30" spans="1:13" s="4" customFormat="1" ht="211.8" customHeight="1">
+    <row r="30" spans="1:13" s="4" customFormat="1" ht="211.9" customHeight="1">
       <c r="A30" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="B30" s="56" t="s">
+      <c r="B30" s="51" t="s">
         <v>125</v>
       </c>
       <c r="C30" s="29" t="s">
@@ -3496,16 +3548,16 @@
       <c r="I30" s="27"/>
       <c r="J30" s="27"/>
       <c r="K30" s="27"/>
-      <c r="L30" s="55" t="s">
+      <c r="L30" s="50" t="s">
         <v>334</v>
       </c>
       <c r="M30" s="38"/>
     </row>
-    <row r="31" spans="1:13" s="4" customFormat="1" ht="244.8" customHeight="1">
+    <row r="31" spans="1:13" s="4" customFormat="1" ht="244.9" customHeight="1">
       <c r="A31" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="51" t="s">
         <v>127</v>
       </c>
       <c r="C31" s="29"/>
@@ -3523,7 +3575,7 @@
       <c r="I31" s="27"/>
       <c r="J31" s="27"/>
       <c r="K31" s="27"/>
-      <c r="L31" s="55" t="s">
+      <c r="L31" s="50" t="s">
         <v>334</v>
       </c>
       <c r="M31" s="38"/>
@@ -3552,7 +3604,9 @@
       <c r="I32" s="18"/>
       <c r="J32" s="18"/>
       <c r="K32" s="18"/>
-      <c r="L32" s="36"/>
+      <c r="L32" s="57" t="s">
+        <v>335</v>
+      </c>
       <c r="M32" s="37"/>
     </row>
     <row r="33" spans="1:13" ht="28.5" customHeight="1">
@@ -3579,7 +3633,9 @@
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
       <c r="K33" s="18"/>
-      <c r="L33" s="36"/>
+      <c r="L33" s="57" t="s">
+        <v>336</v>
+      </c>
       <c r="M33" s="37"/>
     </row>
     <row r="34" spans="1:13" ht="27.75" customHeight="1">
@@ -3606,7 +3662,9 @@
       <c r="I34" s="18"/>
       <c r="J34" s="18"/>
       <c r="K34" s="18"/>
-      <c r="L34" s="36"/>
+      <c r="L34" s="57" t="s">
+        <v>337</v>
+      </c>
       <c r="M34" s="37"/>
     </row>
     <row r="35" spans="1:13" ht="27" customHeight="1">
@@ -3633,7 +3691,9 @@
       <c r="I35" s="18"/>
       <c r="J35" s="18"/>
       <c r="K35" s="18"/>
-      <c r="L35" s="36"/>
+      <c r="L35" s="57" t="s">
+        <v>338</v>
+      </c>
       <c r="M35" s="37"/>
     </row>
     <row r="36" spans="1:13" ht="34.5" customHeight="1">
@@ -3660,7 +3720,9 @@
       <c r="I36" s="18"/>
       <c r="J36" s="18"/>
       <c r="K36" s="18"/>
-      <c r="L36" s="36"/>
+      <c r="L36" s="57" t="s">
+        <v>339</v>
+      </c>
       <c r="M36" s="37"/>
     </row>
     <row r="37" spans="1:13" ht="26.25" customHeight="1">
@@ -3687,7 +3749,9 @@
       <c r="I37" s="18"/>
       <c r="J37" s="18"/>
       <c r="K37" s="18"/>
-      <c r="L37" s="36"/>
+      <c r="L37" s="57" t="s">
+        <v>340</v>
+      </c>
       <c r="M37" s="37"/>
     </row>
     <row r="38" spans="1:13" ht="29.25" customHeight="1">
@@ -3714,7 +3778,9 @@
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
       <c r="K38" s="18"/>
-      <c r="L38" s="36"/>
+      <c r="L38" s="57" t="s">
+        <v>341</v>
+      </c>
       <c r="M38" s="37"/>
     </row>
     <row r="39" spans="1:13" ht="30.75" customHeight="1">
@@ -3741,10 +3807,12 @@
       <c r="I39" s="18"/>
       <c r="J39" s="18"/>
       <c r="K39" s="18"/>
-      <c r="L39" s="36"/>
+      <c r="L39" s="57" t="s">
+        <v>342</v>
+      </c>
       <c r="M39" s="37"/>
     </row>
-    <row r="40" spans="1:13" ht="17.399999999999999">
+    <row r="40" spans="1:13" ht="18">
       <c r="A40" s="15" t="s">
         <v>150</v>
       </c>
@@ -3771,7 +3839,7 @@
       <c r="L40" s="36"/>
       <c r="M40" s="37"/>
     </row>
-    <row r="41" spans="1:13" ht="17.399999999999999">
+    <row r="41" spans="1:13" ht="18">
       <c r="A41" s="15" t="s">
         <v>155</v>
       </c>
@@ -3798,7 +3866,7 @@
       <c r="L41" s="36"/>
       <c r="M41" s="37"/>
     </row>
-    <row r="42" spans="1:13" ht="17.399999999999999">
+    <row r="42" spans="1:13" ht="18">
       <c r="A42" s="15" t="s">
         <v>157</v>
       </c>
@@ -3829,7 +3897,7 @@
       </c>
       <c r="M42" s="37"/>
     </row>
-    <row r="43" spans="1:13" ht="17.399999999999999">
+    <row r="43" spans="1:13" ht="18">
       <c r="A43" s="15" t="s">
         <v>163</v>
       </c>
@@ -3860,7 +3928,7 @@
       </c>
       <c r="M43" s="37"/>
     </row>
-    <row r="44" spans="1:13" ht="17.399999999999999">
+    <row r="44" spans="1:13" ht="18">
       <c r="A44" s="15" t="s">
         <v>166</v>
       </c>
@@ -3891,7 +3959,7 @@
       </c>
       <c r="M44" s="37"/>
     </row>
-    <row r="45" spans="1:13" ht="17.399999999999999">
+    <row r="45" spans="1:13" ht="18">
       <c r="A45" s="15" t="s">
         <v>169</v>
       </c>
@@ -3922,7 +3990,7 @@
       </c>
       <c r="M45" s="37"/>
     </row>
-    <row r="46" spans="1:13" ht="17.399999999999999">
+    <row r="46" spans="1:13" ht="18">
       <c r="A46" s="15" t="s">
         <v>172</v>
       </c>
@@ -3953,7 +4021,7 @@
       </c>
       <c r="M46" s="37"/>
     </row>
-    <row r="47" spans="1:13" ht="17.399999999999999">
+    <row r="47" spans="1:13" ht="18">
       <c r="A47" s="15" t="s">
         <v>175</v>
       </c>
@@ -3984,7 +4052,7 @@
       </c>
       <c r="M47" s="37"/>
     </row>
-    <row r="48" spans="1:13" ht="17.399999999999999">
+    <row r="48" spans="1:13" ht="18">
       <c r="A48" s="15" t="s">
         <v>178</v>
       </c>
@@ -4015,7 +4083,7 @@
       </c>
       <c r="M48" s="37"/>
     </row>
-    <row r="49" spans="1:13" ht="17.399999999999999">
+    <row r="49" spans="1:13" ht="18">
       <c r="A49" s="15" t="s">
         <v>181</v>
       </c>
@@ -4046,7 +4114,7 @@
       </c>
       <c r="M49" s="37"/>
     </row>
-    <row r="50" spans="1:13" ht="17.399999999999999">
+    <row r="50" spans="1:13" ht="18">
       <c r="A50" s="15" t="s">
         <v>184</v>
       </c>
@@ -4077,7 +4145,7 @@
       </c>
       <c r="M50" s="37"/>
     </row>
-    <row r="51" spans="1:13" ht="17.399999999999999">
+    <row r="51" spans="1:13" ht="18">
       <c r="A51" s="15" t="s">
         <v>188</v>
       </c>
@@ -4108,7 +4176,7 @@
       </c>
       <c r="M51" s="37"/>
     </row>
-    <row r="52" spans="1:13" ht="17.399999999999999">
+    <row r="52" spans="1:13" ht="18">
       <c r="A52" s="15" t="s">
         <v>192</v>
       </c>
@@ -4139,7 +4207,7 @@
       </c>
       <c r="M52" s="37"/>
     </row>
-    <row r="53" spans="1:13" ht="17.399999999999999">
+    <row r="53" spans="1:13" ht="18">
       <c r="A53" s="15" t="s">
         <v>194</v>
       </c>
@@ -4170,7 +4238,7 @@
       </c>
       <c r="M53" s="37"/>
     </row>
-    <row r="54" spans="1:13" ht="17.399999999999999">
+    <row r="54" spans="1:13" ht="18">
       <c r="A54" s="15" t="s">
         <v>201</v>
       </c>
@@ -4201,7 +4269,7 @@
       </c>
       <c r="M54" s="37"/>
     </row>
-    <row r="55" spans="1:13" ht="17.399999999999999">
+    <row r="55" spans="1:13" ht="18">
       <c r="A55" s="15" t="s">
         <v>205</v>
       </c>
@@ -4230,7 +4298,7 @@
       <c r="L55" s="36"/>
       <c r="M55" s="37"/>
     </row>
-    <row r="56" spans="1:13" ht="17.399999999999999">
+    <row r="56" spans="1:13" ht="18">
       <c r="A56" s="15" t="s">
         <v>208</v>
       </c>
@@ -4261,7 +4329,7 @@
       </c>
       <c r="M56" s="37"/>
     </row>
-    <row r="57" spans="1:13" ht="27">
+    <row r="57" spans="1:13" ht="26.25">
       <c r="A57" s="15" t="s">
         <v>211</v>
       </c>
@@ -4294,7 +4362,7 @@
       </c>
       <c r="M57" s="37"/>
     </row>
-    <row r="58" spans="1:13" ht="27">
+    <row r="58" spans="1:13" ht="26.25">
       <c r="A58" s="15" t="s">
         <v>219</v>
       </c>
@@ -4325,7 +4393,7 @@
       <c r="L58" s="36"/>
       <c r="M58" s="37"/>
     </row>
-    <row r="59" spans="1:13" ht="27">
+    <row r="59" spans="1:13" ht="26.25">
       <c r="A59" s="15" t="s">
         <v>222</v>
       </c>
@@ -4356,7 +4424,7 @@
       <c r="L59" s="36"/>
       <c r="M59" s="37"/>
     </row>
-    <row r="60" spans="1:13" ht="27">
+    <row r="60" spans="1:13" ht="26.25">
       <c r="A60" s="15" t="s">
         <v>224</v>
       </c>
@@ -4389,7 +4457,7 @@
       </c>
       <c r="M60" s="37"/>
     </row>
-    <row r="61" spans="1:13" ht="17.399999999999999">
+    <row r="61" spans="1:13" ht="18">
       <c r="A61" s="15" t="s">
         <v>229</v>
       </c>
@@ -4418,11 +4486,11 @@
       <c r="A62" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="B62" s="54"/>
-      <c r="C62" s="54"/>
-      <c r="D62" s="54"/>
-      <c r="E62" s="54"/>
-      <c r="F62" s="54"/>
+      <c r="B62" s="56"/>
+      <c r="C62" s="56"/>
+      <c r="D62" s="56"/>
+      <c r="E62" s="56"/>
+      <c r="F62" s="56"/>
       <c r="G62" s="31"/>
       <c r="H62" s="31"/>
       <c r="I62" s="18"/>
@@ -4431,15 +4499,15 @@
       <c r="L62" s="36"/>
       <c r="M62" s="37"/>
     </row>
-    <row r="63" spans="1:13" ht="17.399999999999999">
+    <row r="63" spans="1:13" ht="18">
       <c r="A63" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="B63" s="54"/>
-      <c r="C63" s="54"/>
-      <c r="D63" s="54"/>
-      <c r="E63" s="54"/>
-      <c r="F63" s="54"/>
+      <c r="B63" s="56"/>
+      <c r="C63" s="56"/>
+      <c r="D63" s="56"/>
+      <c r="E63" s="56"/>
+      <c r="F63" s="56"/>
       <c r="G63" s="31"/>
       <c r="H63" s="31"/>
       <c r="I63" s="18"/>
@@ -4448,15 +4516,15 @@
       <c r="L63" s="36"/>
       <c r="M63" s="37"/>
     </row>
-    <row r="64" spans="1:13" ht="17.399999999999999">
+    <row r="64" spans="1:13" ht="18">
       <c r="A64" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="B64" s="54"/>
-      <c r="C64" s="54"/>
-      <c r="D64" s="54"/>
-      <c r="E64" s="54"/>
-      <c r="F64" s="54"/>
+      <c r="B64" s="56"/>
+      <c r="C64" s="56"/>
+      <c r="D64" s="56"/>
+      <c r="E64" s="56"/>
+      <c r="F64" s="56"/>
       <c r="G64" s="31"/>
       <c r="H64" s="31"/>
       <c r="I64" s="18"/>
@@ -4465,15 +4533,15 @@
       <c r="L64" s="36"/>
       <c r="M64" s="37"/>
     </row>
-    <row r="65" spans="1:13" ht="17.399999999999999">
+    <row r="65" spans="1:13" ht="18">
       <c r="A65" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="B65" s="54"/>
-      <c r="C65" s="54"/>
-      <c r="D65" s="54"/>
-      <c r="E65" s="54"/>
-      <c r="F65" s="54"/>
+      <c r="B65" s="56"/>
+      <c r="C65" s="56"/>
+      <c r="D65" s="56"/>
+      <c r="E65" s="56"/>
+      <c r="F65" s="56"/>
       <c r="G65" s="31"/>
       <c r="H65" s="31"/>
       <c r="I65" s="18"/>
@@ -4482,15 +4550,15 @@
       <c r="L65" s="36"/>
       <c r="M65" s="37"/>
     </row>
-    <row r="66" spans="1:13" ht="17.399999999999999">
+    <row r="66" spans="1:13" ht="18">
       <c r="A66" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="B66" s="54"/>
-      <c r="C66" s="54"/>
-      <c r="D66" s="54"/>
-      <c r="E66" s="54"/>
-      <c r="F66" s="54"/>
+      <c r="B66" s="56"/>
+      <c r="C66" s="56"/>
+      <c r="D66" s="56"/>
+      <c r="E66" s="56"/>
+      <c r="F66" s="56"/>
       <c r="G66" s="31"/>
       <c r="H66" s="31"/>
       <c r="I66" s="18"/>
@@ -4499,15 +4567,15 @@
       <c r="L66" s="36"/>
       <c r="M66" s="37"/>
     </row>
-    <row r="67" spans="1:13" ht="17.399999999999999">
+    <row r="67" spans="1:13" ht="18">
       <c r="A67" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="B67" s="54"/>
-      <c r="C67" s="54"/>
-      <c r="D67" s="54"/>
-      <c r="E67" s="54"/>
-      <c r="F67" s="54"/>
+      <c r="B67" s="56"/>
+      <c r="C67" s="56"/>
+      <c r="D67" s="56"/>
+      <c r="E67" s="56"/>
+      <c r="F67" s="56"/>
       <c r="G67" s="31"/>
       <c r="H67" s="31"/>
       <c r="I67" s="18"/>
@@ -4516,15 +4584,15 @@
       <c r="L67" s="36"/>
       <c r="M67" s="37"/>
     </row>
-    <row r="68" spans="1:13" ht="17.399999999999999">
+    <row r="68" spans="1:13" ht="18">
       <c r="A68" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="B68" s="54"/>
-      <c r="C68" s="54"/>
-      <c r="D68" s="54"/>
-      <c r="E68" s="54"/>
-      <c r="F68" s="54"/>
+      <c r="B68" s="56"/>
+      <c r="C68" s="56"/>
+      <c r="D68" s="56"/>
+      <c r="E68" s="56"/>
+      <c r="F68" s="56"/>
       <c r="G68" s="31"/>
       <c r="H68" s="31"/>
       <c r="I68" s="18"/>
@@ -4533,15 +4601,15 @@
       <c r="L68" s="36"/>
       <c r="M68" s="37"/>
     </row>
-    <row r="69" spans="1:13" ht="17.399999999999999">
+    <row r="69" spans="1:13" ht="18">
       <c r="A69" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="B69" s="54"/>
-      <c r="C69" s="54"/>
-      <c r="D69" s="54"/>
-      <c r="E69" s="54"/>
-      <c r="F69" s="54"/>
+      <c r="B69" s="56"/>
+      <c r="C69" s="56"/>
+      <c r="D69" s="56"/>
+      <c r="E69" s="56"/>
+      <c r="F69" s="56"/>
       <c r="G69" s="31"/>
       <c r="H69" s="31"/>
       <c r="I69" s="18"/>
@@ -4550,7 +4618,7 @@
       <c r="L69" s="36"/>
       <c r="M69" s="37"/>
     </row>
-    <row r="70" spans="1:13" ht="17.399999999999999">
+    <row r="70" spans="1:13" ht="18">
       <c r="A70" s="15" t="s">
         <v>238</v>
       </c>
@@ -4567,7 +4635,7 @@
       <c r="L70" s="36"/>
       <c r="M70" s="37"/>
     </row>
-    <row r="71" spans="1:13" ht="17.399999999999999">
+    <row r="71" spans="1:13" ht="18">
       <c r="A71" s="15" t="s">
         <v>239</v>
       </c>
@@ -4584,7 +4652,7 @@
       <c r="L71" s="36"/>
       <c r="M71" s="37"/>
     </row>
-    <row r="72" spans="1:13" ht="17.399999999999999">
+    <row r="72" spans="1:13" ht="18">
       <c r="A72" s="15" t="s">
         <v>240</v>
       </c>
@@ -4601,7 +4669,7 @@
       <c r="L72" s="36"/>
       <c r="M72" s="37"/>
     </row>
-    <row r="73" spans="1:13" ht="17.399999999999999">
+    <row r="73" spans="1:13" ht="18">
       <c r="A73" s="15" t="s">
         <v>241</v>
       </c>
@@ -4618,7 +4686,7 @@
       <c r="L73" s="36"/>
       <c r="M73" s="37"/>
     </row>
-    <row r="74" spans="1:13" ht="17.399999999999999">
+    <row r="74" spans="1:13" ht="18">
       <c r="A74" s="15" t="s">
         <v>242</v>
       </c>
@@ -4635,7 +4703,7 @@
       <c r="L74" s="36"/>
       <c r="M74" s="37"/>
     </row>
-    <row r="75" spans="1:13" ht="17.399999999999999">
+    <row r="75" spans="1:13" ht="18">
       <c r="A75" s="15" t="s">
         <v>243</v>
       </c>
@@ -4652,7 +4720,7 @@
       <c r="L75" s="36"/>
       <c r="M75" s="37"/>
     </row>
-    <row r="76" spans="1:13" ht="17.399999999999999">
+    <row r="76" spans="1:13" ht="18">
       <c r="A76" s="15" t="s">
         <v>244</v>
       </c>
@@ -4669,7 +4737,7 @@
       <c r="L76" s="36"/>
       <c r="M76" s="37"/>
     </row>
-    <row r="77" spans="1:13" ht="17.399999999999999">
+    <row r="77" spans="1:13" ht="18">
       <c r="A77" s="15" t="s">
         <v>245</v>
       </c>
@@ -4686,7 +4754,7 @@
       <c r="L77" s="36"/>
       <c r="M77" s="37"/>
     </row>
-    <row r="78" spans="1:13" ht="17.399999999999999">
+    <row r="78" spans="1:13" ht="18">
       <c r="A78" s="15" t="s">
         <v>246</v>
       </c>
@@ -4703,7 +4771,7 @@
       <c r="L78" s="36"/>
       <c r="M78" s="37"/>
     </row>
-    <row r="79" spans="1:13" ht="17.399999999999999">
+    <row r="79" spans="1:13" ht="18">
       <c r="A79" s="15" t="s">
         <v>247</v>
       </c>
@@ -4720,7 +4788,7 @@
       <c r="L79" s="36"/>
       <c r="M79" s="37"/>
     </row>
-    <row r="80" spans="1:13" ht="17.399999999999999">
+    <row r="80" spans="1:13" ht="18">
       <c r="A80" s="15" t="s">
         <v>248</v>
       </c>
@@ -4737,7 +4805,7 @@
       <c r="L80" s="36"/>
       <c r="M80" s="37"/>
     </row>
-    <row r="81" spans="1:13" ht="17.399999999999999">
+    <row r="81" spans="1:13" ht="18">
       <c r="A81" s="15" t="s">
         <v>249</v>
       </c>
@@ -4754,7 +4822,7 @@
       <c r="L81" s="36"/>
       <c r="M81" s="37"/>
     </row>
-    <row r="82" spans="1:13" ht="17.399999999999999">
+    <row r="82" spans="1:13" ht="18">
       <c r="A82" s="15" t="s">
         <v>250</v>
       </c>
@@ -4771,7 +4839,7 @@
       <c r="L82" s="36"/>
       <c r="M82" s="37"/>
     </row>
-    <row r="83" spans="1:13" ht="17.399999999999999">
+    <row r="83" spans="1:13" ht="18">
       <c r="A83" s="15" t="s">
         <v>251</v>
       </c>
@@ -4788,7 +4856,7 @@
       <c r="L83" s="36"/>
       <c r="M83" s="37"/>
     </row>
-    <row r="84" spans="1:13" ht="17.399999999999999">
+    <row r="84" spans="1:13" ht="18">
       <c r="A84" s="15" t="s">
         <v>252</v>
       </c>
@@ -4805,7 +4873,7 @@
       <c r="L84" s="36"/>
       <c r="M84" s="37"/>
     </row>
-    <row r="85" spans="1:13" ht="17.399999999999999">
+    <row r="85" spans="1:13" ht="18">
       <c r="A85" s="15" t="s">
         <v>253</v>
       </c>
@@ -4822,7 +4890,7 @@
       <c r="L85" s="36"/>
       <c r="M85" s="37"/>
     </row>
-    <row r="86" spans="1:13" ht="17.399999999999999">
+    <row r="86" spans="1:13" ht="18">
       <c r="A86" s="15" t="s">
         <v>254</v>
       </c>
@@ -4839,7 +4907,7 @@
       <c r="L86" s="36"/>
       <c r="M86" s="37"/>
     </row>
-    <row r="87" spans="1:13" ht="17.399999999999999">
+    <row r="87" spans="1:13" ht="18">
       <c r="A87" s="15" t="s">
         <v>255</v>
       </c>
@@ -4856,7 +4924,7 @@
       <c r="L87" s="36"/>
       <c r="M87" s="37"/>
     </row>
-    <row r="88" spans="1:13" ht="17.399999999999999">
+    <row r="88" spans="1:13" ht="18">
       <c r="A88" s="15" t="s">
         <v>256</v>
       </c>
@@ -4873,7 +4941,7 @@
       <c r="L88" s="36"/>
       <c r="M88" s="37"/>
     </row>
-    <row r="89" spans="1:13" ht="17.399999999999999">
+    <row r="89" spans="1:13" ht="18">
       <c r="A89" s="15" t="s">
         <v>257</v>
       </c>
@@ -4890,7 +4958,7 @@
       <c r="L89" s="36"/>
       <c r="M89" s="37"/>
     </row>
-    <row r="90" spans="1:13" ht="17.399999999999999">
+    <row r="90" spans="1:13" ht="18">
       <c r="A90" s="15" t="s">
         <v>258</v>
       </c>
@@ -4907,7 +4975,7 @@
       <c r="L90" s="36"/>
       <c r="M90" s="37"/>
     </row>
-    <row r="91" spans="1:13" ht="17.399999999999999">
+    <row r="91" spans="1:13" ht="18">
       <c r="A91" s="15" t="s">
         <v>259</v>
       </c>
@@ -4924,7 +4992,7 @@
       <c r="L91" s="36"/>
       <c r="M91" s="37"/>
     </row>
-    <row r="92" spans="1:13" ht="17.399999999999999">
+    <row r="92" spans="1:13" ht="18">
       <c r="A92" s="15" t="s">
         <v>260</v>
       </c>
@@ -4941,7 +5009,7 @@
       <c r="L92" s="36"/>
       <c r="M92" s="37"/>
     </row>
-    <row r="93" spans="1:13" ht="17.399999999999999">
+    <row r="93" spans="1:13" ht="18">
       <c r="A93" s="15" t="s">
         <v>261</v>
       </c>
@@ -4958,7 +5026,7 @@
       <c r="L93" s="36"/>
       <c r="M93" s="37"/>
     </row>
-    <row r="94" spans="1:13" ht="17.399999999999999">
+    <row r="94" spans="1:13" ht="18">
       <c r="A94" s="15" t="s">
         <v>262</v>
       </c>
@@ -4975,7 +5043,7 @@
       <c r="L94" s="36"/>
       <c r="M94" s="37"/>
     </row>
-    <row r="95" spans="1:13" ht="17.399999999999999">
+    <row r="95" spans="1:13" ht="18">
       <c r="A95" s="15" t="s">
         <v>263</v>
       </c>
@@ -4992,7 +5060,7 @@
       <c r="L95" s="36"/>
       <c r="M95" s="37"/>
     </row>
-    <row r="96" spans="1:13" ht="17.399999999999999">
+    <row r="96" spans="1:13" ht="18">
       <c r="A96" s="15" t="s">
         <v>264</v>
       </c>
@@ -5009,7 +5077,7 @@
       <c r="L96" s="36"/>
       <c r="M96" s="37"/>
     </row>
-    <row r="97" spans="1:13" ht="17.399999999999999">
+    <row r="97" spans="1:13" ht="18">
       <c r="A97" s="15" t="s">
         <v>265</v>
       </c>
@@ -5026,7 +5094,7 @@
       <c r="L97" s="36"/>
       <c r="M97" s="37"/>
     </row>
-    <row r="98" spans="1:13" ht="17.399999999999999">
+    <row r="98" spans="1:13" ht="18">
       <c r="A98" s="15" t="s">
         <v>266</v>
       </c>
@@ -5043,7 +5111,7 @@
       <c r="L98" s="36"/>
       <c r="M98" s="37"/>
     </row>
-    <row r="99" spans="1:13" ht="17.399999999999999">
+    <row r="99" spans="1:13" ht="18">
       <c r="A99" s="15" t="s">
         <v>267</v>
       </c>
@@ -5060,7 +5128,7 @@
       <c r="L99" s="36"/>
       <c r="M99" s="37"/>
     </row>
-    <row r="100" spans="1:13" ht="17.399999999999999">
+    <row r="100" spans="1:13" ht="18">
       <c r="A100" s="15" t="s">
         <v>268</v>
       </c>
@@ -5077,7 +5145,7 @@
       <c r="L100" s="36"/>
       <c r="M100" s="37"/>
     </row>
-    <row r="101" spans="1:13" ht="17.399999999999999">
+    <row r="101" spans="1:13" ht="18">
       <c r="A101" s="15" t="s">
         <v>269</v>
       </c>
@@ -5094,7 +5162,7 @@
       <c r="L101" s="36"/>
       <c r="M101" s="37"/>
     </row>
-    <row r="102" spans="1:13" ht="17.399999999999999">
+    <row r="102" spans="1:13" ht="18">
       <c r="A102" s="15" t="s">
         <v>270</v>
       </c>
@@ -5111,7 +5179,7 @@
       <c r="L102" s="36"/>
       <c r="M102" s="37"/>
     </row>
-    <row r="103" spans="1:13" ht="17.399999999999999">
+    <row r="103" spans="1:13" ht="18">
       <c r="A103" s="15" t="s">
         <v>271</v>
       </c>
@@ -5128,7 +5196,7 @@
       <c r="L103" s="36"/>
       <c r="M103" s="37"/>
     </row>
-    <row r="104" spans="1:13" ht="17.399999999999999">
+    <row r="104" spans="1:13" ht="18">
       <c r="A104" s="15" t="s">
         <v>272</v>
       </c>
@@ -5145,7 +5213,7 @@
       <c r="L104" s="36"/>
       <c r="M104" s="37"/>
     </row>
-    <row r="105" spans="1:13" ht="17.399999999999999">
+    <row r="105" spans="1:13" ht="18">
       <c r="A105" s="15" t="s">
         <v>273</v>
       </c>
@@ -5162,7 +5230,7 @@
       <c r="L105" s="36"/>
       <c r="M105" s="37"/>
     </row>
-    <row r="106" spans="1:13" ht="17.399999999999999">
+    <row r="106" spans="1:13" ht="18">
       <c r="A106" s="15" t="s">
         <v>274</v>
       </c>
@@ -5179,7 +5247,7 @@
       <c r="L106" s="36"/>
       <c r="M106" s="37"/>
     </row>
-    <row r="107" spans="1:13" ht="17.399999999999999">
+    <row r="107" spans="1:13" ht="18">
       <c r="A107" s="15" t="s">
         <v>275</v>
       </c>
@@ -5196,7 +5264,7 @@
       <c r="L107" s="36"/>
       <c r="M107" s="37"/>
     </row>
-    <row r="108" spans="1:13" ht="17.399999999999999">
+    <row r="108" spans="1:13" ht="18">
       <c r="A108" s="15" t="s">
         <v>276</v>
       </c>
@@ -5213,7 +5281,7 @@
       <c r="L108" s="36"/>
       <c r="M108" s="37"/>
     </row>
-    <row r="109" spans="1:13" ht="17.399999999999999">
+    <row r="109" spans="1:13" ht="18">
       <c r="A109" s="15" t="s">
         <v>277</v>
       </c>
@@ -5230,7 +5298,7 @@
       <c r="L109" s="36"/>
       <c r="M109" s="37"/>
     </row>
-    <row r="110" spans="1:13" ht="17.399999999999999">
+    <row r="110" spans="1:13" ht="18">
       <c r="A110" s="15" t="s">
         <v>278</v>
       </c>
@@ -5247,7 +5315,7 @@
       <c r="L110" s="36"/>
       <c r="M110" s="37"/>
     </row>
-    <row r="111" spans="1:13" ht="17.399999999999999">
+    <row r="111" spans="1:13" ht="18">
       <c r="A111" s="15" t="s">
         <v>279</v>
       </c>
@@ -5264,7 +5332,7 @@
       <c r="L111" s="36"/>
       <c r="M111" s="37"/>
     </row>
-    <row r="112" spans="1:13" ht="17.399999999999999">
+    <row r="112" spans="1:13" ht="18">
       <c r="A112" s="15" t="s">
         <v>280</v>
       </c>
@@ -5281,7 +5349,7 @@
       <c r="L112" s="36"/>
       <c r="M112" s="37"/>
     </row>
-    <row r="113" spans="1:13" ht="17.399999999999999">
+    <row r="113" spans="1:13" ht="18">
       <c r="A113" s="15" t="s">
         <v>281</v>
       </c>
@@ -5298,7 +5366,7 @@
       <c r="L113" s="36"/>
       <c r="M113" s="37"/>
     </row>
-    <row r="114" spans="1:13" ht="17.399999999999999">
+    <row r="114" spans="1:13" ht="18">
       <c r="A114" s="15" t="s">
         <v>282</v>
       </c>
@@ -5315,7 +5383,7 @@
       <c r="L114" s="36"/>
       <c r="M114" s="37"/>
     </row>
-    <row r="115" spans="1:13" ht="17.399999999999999">
+    <row r="115" spans="1:13" ht="18">
       <c r="A115" s="15" t="s">
         <v>283</v>
       </c>
@@ -5332,7 +5400,7 @@
       <c r="L115" s="36"/>
       <c r="M115" s="37"/>
     </row>
-    <row r="116" spans="1:13" ht="17.399999999999999">
+    <row r="116" spans="1:13" ht="18">
       <c r="A116" s="15" t="s">
         <v>284</v>
       </c>
@@ -5349,7 +5417,7 @@
       <c r="L116" s="36"/>
       <c r="M116" s="37"/>
     </row>
-    <row r="117" spans="1:13" ht="17.399999999999999">
+    <row r="117" spans="1:13" ht="18">
       <c r="A117" s="15" t="s">
         <v>285</v>
       </c>
@@ -5366,7 +5434,7 @@
       <c r="L117" s="36"/>
       <c r="M117" s="37"/>
     </row>
-    <row r="118" spans="1:13" ht="17.399999999999999">
+    <row r="118" spans="1:13" ht="18">
       <c r="A118" s="15" t="s">
         <v>286</v>
       </c>
@@ -5383,7 +5451,7 @@
       <c r="L118" s="36"/>
       <c r="M118" s="37"/>
     </row>
-    <row r="119" spans="1:13" ht="17.399999999999999">
+    <row r="119" spans="1:13" ht="18">
       <c r="A119" s="15" t="s">
         <v>287</v>
       </c>
@@ -5400,7 +5468,7 @@
       <c r="L119" s="36"/>
       <c r="M119" s="37"/>
     </row>
-    <row r="120" spans="1:13" ht="17.399999999999999">
+    <row r="120" spans="1:13" ht="18">
       <c r="A120" s="15" t="s">
         <v>288</v>
       </c>
@@ -5417,7 +5485,7 @@
       <c r="L120" s="36"/>
       <c r="M120" s="37"/>
     </row>
-    <row r="121" spans="1:13" ht="17.399999999999999">
+    <row r="121" spans="1:13" ht="18">
       <c r="A121" s="15" t="s">
         <v>289</v>
       </c>
@@ -5434,7 +5502,7 @@
       <c r="L121" s="36"/>
       <c r="M121" s="37"/>
     </row>
-    <row r="122" spans="1:13" ht="17.399999999999999">
+    <row r="122" spans="1:13" ht="18">
       <c r="A122" s="15" t="s">
         <v>290</v>
       </c>
@@ -5451,7 +5519,7 @@
       <c r="L122" s="36"/>
       <c r="M122" s="37"/>
     </row>
-    <row r="123" spans="1:13" ht="17.399999999999999">
+    <row r="123" spans="1:13" ht="18">
       <c r="A123" s="15" t="s">
         <v>291</v>
       </c>
@@ -5468,7 +5536,7 @@
       <c r="L123" s="36"/>
       <c r="M123" s="37"/>
     </row>
-    <row r="124" spans="1:13" ht="17.399999999999999">
+    <row r="124" spans="1:13" ht="18">
       <c r="A124" s="15" t="s">
         <v>292</v>
       </c>
@@ -5485,7 +5553,7 @@
       <c r="L124" s="36"/>
       <c r="M124" s="37"/>
     </row>
-    <row r="125" spans="1:13" ht="17.399999999999999">
+    <row r="125" spans="1:13" ht="18">
       <c r="A125" s="15" t="s">
         <v>293</v>
       </c>
@@ -5502,7 +5570,7 @@
       <c r="L125" s="36"/>
       <c r="M125" s="37"/>
     </row>
-    <row r="126" spans="1:13" ht="17.399999999999999">
+    <row r="126" spans="1:13" ht="18">
       <c r="A126" s="15" t="s">
         <v>294</v>
       </c>
@@ -5519,7 +5587,7 @@
       <c r="L126" s="36"/>
       <c r="M126" s="37"/>
     </row>
-    <row r="127" spans="1:13" ht="17.399999999999999">
+    <row r="127" spans="1:13" ht="18">
       <c r="A127" s="15" t="s">
         <v>295</v>
       </c>
@@ -5536,7 +5604,7 @@
       <c r="L127" s="36"/>
       <c r="M127" s="37"/>
     </row>
-    <row r="128" spans="1:13" ht="17.399999999999999">
+    <row r="128" spans="1:13" ht="18">
       <c r="A128" s="15" t="s">
         <v>296</v>
       </c>
@@ -5553,7 +5621,7 @@
       <c r="L128" s="36"/>
       <c r="M128" s="37"/>
     </row>
-    <row r="129" spans="1:13" ht="17.399999999999999">
+    <row r="129" spans="1:13" ht="18">
       <c r="A129" s="15" t="s">
         <v>297</v>
       </c>
@@ -5570,7 +5638,7 @@
       <c r="L129" s="36"/>
       <c r="M129" s="37"/>
     </row>
-    <row r="130" spans="1:13" ht="17.399999999999999">
+    <row r="130" spans="1:13" ht="18">
       <c r="A130" s="15" t="s">
         <v>298</v>
       </c>
@@ -5587,7 +5655,7 @@
       <c r="L130" s="36"/>
       <c r="M130" s="37"/>
     </row>
-    <row r="131" spans="1:13" ht="17.399999999999999">
+    <row r="131" spans="1:13" ht="18">
       <c r="A131" s="15" t="s">
         <v>299</v>
       </c>
@@ -5604,7 +5672,7 @@
       <c r="L131" s="36"/>
       <c r="M131" s="37"/>
     </row>
-    <row r="132" spans="1:13" ht="17.399999999999999">
+    <row r="132" spans="1:13" ht="18">
       <c r="A132" s="15" t="s">
         <v>300</v>
       </c>
@@ -5621,7 +5689,7 @@
       <c r="L132" s="36"/>
       <c r="M132" s="37"/>
     </row>
-    <row r="133" spans="1:13" ht="17.399999999999999">
+    <row r="133" spans="1:13" ht="18">
       <c r="A133" s="15" t="s">
         <v>301</v>
       </c>
@@ -5638,7 +5706,7 @@
       <c r="L133" s="36"/>
       <c r="M133" s="37"/>
     </row>
-    <row r="134" spans="1:13" ht="17.399999999999999">
+    <row r="134" spans="1:13" ht="18">
       <c r="A134" s="15" t="s">
         <v>302</v>
       </c>
@@ -5655,7 +5723,7 @@
       <c r="L134" s="36"/>
       <c r="M134" s="37"/>
     </row>
-    <row r="135" spans="1:13" ht="17.399999999999999">
+    <row r="135" spans="1:13" ht="18">
       <c r="A135" s="15" t="s">
         <v>303</v>
       </c>
@@ -5672,7 +5740,7 @@
       <c r="L135" s="36"/>
       <c r="M135" s="37"/>
     </row>
-    <row r="136" spans="1:13" ht="17.399999999999999">
+    <row r="136" spans="1:13" ht="18">
       <c r="A136" s="15" t="s">
         <v>304</v>
       </c>
@@ -5689,7 +5757,7 @@
       <c r="L136" s="36"/>
       <c r="M136" s="37"/>
     </row>
-    <row r="137" spans="1:13" ht="17.399999999999999">
+    <row r="137" spans="1:13" ht="18">
       <c r="A137" s="15" t="s">
         <v>305</v>
       </c>
@@ -5706,7 +5774,7 @@
       <c r="L137" s="36"/>
       <c r="M137" s="37"/>
     </row>
-    <row r="138" spans="1:13" ht="17.399999999999999">
+    <row r="138" spans="1:13" ht="18">
       <c r="A138" s="15" t="s">
         <v>306</v>
       </c>
@@ -5723,7 +5791,7 @@
       <c r="L138" s="36"/>
       <c r="M138" s="37"/>
     </row>
-    <row r="139" spans="1:13" ht="17.399999999999999">
+    <row r="139" spans="1:13" ht="18">
       <c r="A139" s="15" t="s">
         <v>307</v>
       </c>
@@ -5740,7 +5808,7 @@
       <c r="L139" s="36"/>
       <c r="M139" s="37"/>
     </row>
-    <row r="140" spans="1:13" ht="17.399999999999999">
+    <row r="140" spans="1:13" ht="18">
       <c r="A140" s="15" t="s">
         <v>308</v>
       </c>
@@ -5757,7 +5825,7 @@
       <c r="L140" s="36"/>
       <c r="M140" s="37"/>
     </row>
-    <row r="141" spans="1:13" ht="17.399999999999999">
+    <row r="141" spans="1:13" ht="18">
       <c r="A141" s="15" t="s">
         <v>309</v>
       </c>
@@ -5774,7 +5842,7 @@
       <c r="L141" s="36"/>
       <c r="M141" s="37"/>
     </row>
-    <row r="142" spans="1:13" ht="17.399999999999999">
+    <row r="142" spans="1:13" ht="18">
       <c r="A142" s="15" t="s">
         <v>310</v>
       </c>
@@ -5791,7 +5859,7 @@
       <c r="L142" s="36"/>
       <c r="M142" s="37"/>
     </row>
-    <row r="143" spans="1:13" ht="17.399999999999999">
+    <row r="143" spans="1:13" ht="18">
       <c r="A143" s="15" t="s">
         <v>311</v>
       </c>
@@ -5808,7 +5876,7 @@
       <c r="L143" s="36"/>
       <c r="M143" s="37"/>
     </row>
-    <row r="144" spans="1:13" ht="17.399999999999999">
+    <row r="144" spans="1:13" ht="18">
       <c r="A144" s="15" t="s">
         <v>312</v>
       </c>
@@ -5825,7 +5893,7 @@
       <c r="L144" s="36"/>
       <c r="M144" s="37"/>
     </row>
-    <row r="145" spans="1:13" ht="17.399999999999999">
+    <row r="145" spans="1:13" ht="18">
       <c r="A145" s="15" t="s">
         <v>313</v>
       </c>
@@ -5842,7 +5910,7 @@
       <c r="L145" s="36"/>
       <c r="M145" s="37"/>
     </row>
-    <row r="146" spans="1:13" ht="17.399999999999999">
+    <row r="146" spans="1:13" ht="18">
       <c r="A146" s="15" t="s">
         <v>314</v>
       </c>
@@ -5859,7 +5927,7 @@
       <c r="L146" s="36"/>
       <c r="M146" s="37"/>
     </row>
-    <row r="147" spans="1:13" ht="17.399999999999999">
+    <row r="147" spans="1:13" ht="18">
       <c r="A147" s="15" t="s">
         <v>315</v>
       </c>
@@ -5876,7 +5944,7 @@
       <c r="L147" s="36"/>
       <c r="M147" s="37"/>
     </row>
-    <row r="148" spans="1:13" ht="17.399999999999999">
+    <row r="148" spans="1:13" ht="18">
       <c r="A148" s="15" t="s">
         <v>316</v>
       </c>
@@ -5893,7 +5961,7 @@
       <c r="L148" s="36"/>
       <c r="M148" s="37"/>
     </row>
-    <row r="149" spans="1:13" ht="17.399999999999999">
+    <row r="149" spans="1:13" ht="18">
       <c r="A149" s="15" t="s">
         <v>317</v>
       </c>
@@ -5910,7 +5978,7 @@
       <c r="L149" s="36"/>
       <c r="M149" s="37"/>
     </row>
-    <row r="150" spans="1:13" ht="17.399999999999999">
+    <row r="150" spans="1:13" ht="18">
       <c r="A150" s="15" t="s">
         <v>318</v>
       </c>
@@ -5927,7 +5995,7 @@
       <c r="L150" s="36"/>
       <c r="M150" s="37"/>
     </row>
-    <row r="151" spans="1:13" ht="17.399999999999999">
+    <row r="151" spans="1:13" ht="18">
       <c r="A151" s="15" t="s">
         <v>319</v>
       </c>
@@ -5944,7 +6012,7 @@
       <c r="L151" s="36"/>
       <c r="M151" s="37"/>
     </row>
-    <row r="152" spans="1:13" ht="17.399999999999999">
+    <row r="152" spans="1:13" ht="18">
       <c r="A152" s="15" t="s">
         <v>320</v>
       </c>
@@ -5961,7 +6029,7 @@
       <c r="L152" s="36"/>
       <c r="M152" s="37"/>
     </row>
-    <row r="153" spans="1:13" ht="17.399999999999999">
+    <row r="153" spans="1:13" ht="18">
       <c r="A153" s="15" t="s">
         <v>321</v>
       </c>
@@ -5978,7 +6046,7 @@
       <c r="L153" s="36"/>
       <c r="M153" s="37"/>
     </row>
-    <row r="154" spans="1:13" ht="17.399999999999999">
+    <row r="154" spans="1:13" ht="18">
       <c r="A154" s="15" t="s">
         <v>322</v>
       </c>
@@ -5995,7 +6063,7 @@
       <c r="L154" s="36"/>
       <c r="M154" s="37"/>
     </row>
-    <row r="155" spans="1:13" ht="17.399999999999999">
+    <row r="155" spans="1:13" ht="18">
       <c r="A155" s="15" t="s">
         <v>323</v>
       </c>
@@ -6012,7 +6080,7 @@
       <c r="L155" s="36"/>
       <c r="M155" s="37"/>
     </row>
-    <row r="156" spans="1:13" ht="17.399999999999999">
+    <row r="156" spans="1:13" ht="18">
       <c r="A156" s="15" t="s">
         <v>324</v>
       </c>
@@ -6029,7 +6097,7 @@
       <c r="L156" s="36"/>
       <c r="M156" s="37"/>
     </row>
-    <row r="157" spans="1:13" ht="17.399999999999999">
+    <row r="157" spans="1:13" ht="18">
       <c r="A157" s="15" t="s">
         <v>325</v>
       </c>
@@ -6046,7 +6114,7 @@
       <c r="L157" s="36"/>
       <c r="M157" s="37"/>
     </row>
-    <row r="158" spans="1:13" ht="17.399999999999999">
+    <row r="158" spans="1:13" ht="18">
       <c r="A158" s="15" t="s">
         <v>326</v>
       </c>
@@ -6063,7 +6131,7 @@
       <c r="L158" s="36"/>
       <c r="M158" s="37"/>
     </row>
-    <row r="159" spans="1:13" ht="17.399999999999999">
+    <row r="159" spans="1:13" ht="18">
       <c r="A159" s="15" t="s">
         <v>327</v>
       </c>
@@ -6080,7 +6148,7 @@
       <c r="L159" s="36"/>
       <c r="M159" s="37"/>
     </row>
-    <row r="160" spans="1:13" ht="17.399999999999999">
+    <row r="160" spans="1:13" ht="18">
       <c r="A160" s="15" t="s">
         <v>328</v>
       </c>
@@ -6142,7 +6210,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F70:H160" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F70:H160">
       <formula1>"In Progress, Testing, Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>